<commit_message>
EPBDS-5929 Dulicated field Region property in Repository - Property section
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="809">
   <si>
     <t>Display Name</t>
   </si>
@@ -2472,6 +2472,9 @@
   </si>
   <si>
     <t>Province pour laquelle la table devrait être utilisée</t>
+  </si>
+  <si>
+    <t>Canada Region</t>
   </si>
 </sst>
 </file>
@@ -3142,60 +3145,15 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3207,15 +3165,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3270,6 +3219,60 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
@@ -3680,215 +3683,220 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3898,11 +3906,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3919,7 +3922,7 @@
   <dimension ref="A1:AMK62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3948,157 +3951,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -4110,27 +4113,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -5791,7 +5794,7 @@
     </row>
     <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>164</v>
+        <v>808</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>801</v>
@@ -5919,40 +5922,40 @@
       </c>
     </row>
     <row r="57" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="57" t="s">
         <v>212</v>
       </c>
-      <c r="C57" s="21"/>
+      <c r="C57" s="57"/>
     </row>
     <row r="58" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="C58" s="22"/>
+      <c r="C58" s="58"/>
     </row>
     <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="C59" s="22"/>
+      <c r="C59" s="58"/>
     </row>
     <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="C60" s="23"/>
+      <c r="C60" s="59"/>
     </row>
     <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="C61" s="23"/>
+      <c r="C61" s="59"/>
     </row>
     <row r="62" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="56" t="s">
         <v>764</v>
       </c>
-      <c r="C62" s="20"/>
+      <c r="C62" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -5994,60 +5997,60 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="61" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="29"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="61"/>
+      <c r="C7" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="29"/>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="62" t="s">
         <v>223</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6082,79 +6085,79 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="56" t="s">
+      <c r="D5" s="37"/>
+      <c r="E5" s="38" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="39" t="s">
         <v>225</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="58" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="40" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="39" t="s">
         <v>134</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="40" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="39" t="s">
         <v>226</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -6163,12 +6166,12 @@
       <c r="D8" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="40" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="39" t="s">
         <v>145</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -6177,12 +6180,12 @@
       <c r="D9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="40" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="39" t="s">
         <v>229</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -6191,40 +6194,40 @@
       <c r="D10" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="40" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="41" t="s">
         <v>150</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="40" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="41" t="s">
         <v>155</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="42" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="39" t="s">
         <v>165</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -6233,12 +6236,12 @@
       <c r="D13" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="40" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="39" t="s">
         <v>768</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -6247,21 +6250,21 @@
       <c r="D14" s="3" t="s">
         <v>769</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="40" t="s">
         <v>770</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="43" t="s">
         <v>771</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="44" t="s">
         <v>772</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="45" t="s">
         <v>773</v>
       </c>
     </row>
@@ -6298,33 +6301,33 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="68" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="E2" s="39" t="s">
+      <c r="C2" s="69"/>
+      <c r="E2" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="I2" s="26" t="s">
+      <c r="F2" s="25"/>
+      <c r="I2" s="68" t="s">
         <v>232</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="69"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="20" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="20" t="s">
         <v>29</v>
       </c>
       <c r="J3" s="12" t="s">
@@ -6332,19 +6335,19 @@
       </c>
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="20" t="s">
         <v>233</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="20" t="s">
         <v>233</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="20" t="s">
         <v>233</v>
       </c>
       <c r="J4" s="12" t="s">
@@ -6352,19 +6355,19 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="21" t="s">
         <v>235</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="21" t="s">
         <v>235</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="21" t="s">
         <v>238</v>
       </c>
       <c r="J5" s="14" t="s">
@@ -6372,19 +6375,19 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="21" t="s">
         <v>240</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="21" t="s">
         <v>242</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="21" t="s">
         <v>244</v>
       </c>
       <c r="J6" s="14" t="s">
@@ -6392,19 +6395,19 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="21" t="s">
         <v>246</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="21" t="s">
         <v>250</v>
       </c>
       <c r="J7" s="14" t="s">
@@ -6412,33 +6415,33 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="21" t="s">
         <v>252</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="21" t="s">
         <v>246</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="23" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="21" t="s">
         <v>257</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="21" t="s">
         <v>259</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -6446,13 +6449,13 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="21" t="s">
         <v>261</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="21" t="s">
         <v>263</v>
       </c>
       <c r="F10" s="14" t="s">
@@ -6460,13 +6463,13 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="21" t="s">
         <v>265</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="21" t="s">
         <v>267</v>
       </c>
       <c r="F11" s="14" t="s">
@@ -6474,13 +6477,13 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="21" t="s">
         <v>269</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="21" t="s">
         <v>271</v>
       </c>
       <c r="F12" s="14" t="s">
@@ -6488,37 +6491,37 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="21" t="s">
         <v>273</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="21" t="s">
         <v>275</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="68" t="s">
         <v>277</v>
       </c>
-      <c r="J13" s="34"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="21" t="s">
         <v>278</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="21" t="s">
         <v>280</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="I14" s="35" t="s">
+      <c r="I14" s="20" t="s">
         <v>29</v>
       </c>
       <c r="J14" s="12" t="s">
@@ -6526,19 +6529,19 @@
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="21" t="s">
         <v>282</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="21" t="s">
         <v>284</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="I15" s="35" t="s">
+      <c r="I15" s="20" t="s">
         <v>233</v>
       </c>
       <c r="J15" s="12" t="s">
@@ -6546,19 +6549,19 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="21" t="s">
         <v>286</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="21" t="s">
         <v>288</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="21" t="s">
         <v>290</v>
       </c>
       <c r="J16" s="14" t="s">
@@ -6566,19 +6569,19 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="21" t="s">
         <v>259</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>292</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="21" t="s">
         <v>117</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="I17" s="36" t="s">
+      <c r="I17" s="21" t="s">
         <v>294</v>
       </c>
       <c r="J17" s="14" t="s">
@@ -6586,19 +6589,19 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="21" t="s">
         <v>296</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="21" t="s">
         <v>298</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="I18" s="36" t="s">
+      <c r="I18" s="21" t="s">
         <v>300</v>
       </c>
       <c r="J18" s="14" t="s">
@@ -6606,19 +6609,19 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="21" t="s">
         <v>302</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="21" t="s">
         <v>304</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="I19" s="36" t="s">
+      <c r="I19" s="21" t="s">
         <v>306</v>
       </c>
       <c r="J19" s="14" t="s">
@@ -6626,33 +6629,33 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="21" t="s">
         <v>263</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="21" t="s">
         <v>309</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>310</v>
       </c>
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="J20" s="38" t="s">
+      <c r="J20" s="23" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="21" t="s">
         <v>313</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="21" t="s">
         <v>315</v>
       </c>
       <c r="F21" s="14" t="s">
@@ -6660,13 +6663,13 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="21" t="s">
         <v>317</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="21" t="s">
         <v>319</v>
       </c>
       <c r="F22" s="14" t="s">
@@ -6674,37 +6677,37 @@
       </c>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="21" t="s">
         <v>321</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="21" t="s">
         <v>323</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="I23" s="68" t="s">
         <v>325</v>
       </c>
-      <c r="J23" s="34"/>
+      <c r="J23" s="69"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="21" t="s">
         <v>326</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="21" t="s">
         <v>328</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="I24" s="35" t="s">
+      <c r="I24" s="20" t="s">
         <v>29</v>
       </c>
       <c r="J24" s="12" t="s">
@@ -6712,19 +6715,19 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="21" t="s">
         <v>330</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="E25" s="36" t="s">
+      <c r="E25" s="21" t="s">
         <v>332</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="I25" s="41" t="s">
+      <c r="I25" s="26" t="s">
         <v>233</v>
       </c>
       <c r="J25" s="13" t="s">
@@ -6732,19 +6735,19 @@
       </c>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="21" t="s">
         <v>334</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="21" t="s">
         <v>336</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="21" t="s">
         <v>338</v>
       </c>
       <c r="J26" s="14" t="s">
@@ -6752,19 +6755,19 @@
       </c>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="21" t="s">
         <v>340</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="21" t="s">
         <v>342</v>
       </c>
       <c r="F27" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="I27" s="42" t="s">
+      <c r="I27" s="27" t="s">
         <v>344</v>
       </c>
       <c r="J27" s="15" t="s">
@@ -6772,33 +6775,33 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="21" t="s">
         <v>346</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="E28" s="36" t="s">
+      <c r="E28" s="21" t="s">
         <v>348</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="I28" s="43" t="s">
+      <c r="I28" s="28" t="s">
         <v>350</v>
       </c>
-      <c r="J28" s="44" t="s">
+      <c r="J28" s="29" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="21" t="s">
         <v>352</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E29" s="21" t="s">
         <v>354</v>
       </c>
       <c r="F29" s="14" t="s">
@@ -6806,13 +6809,13 @@
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="21" t="s">
         <v>356</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="E30" s="36" t="s">
+      <c r="E30" s="21" t="s">
         <v>358</v>
       </c>
       <c r="F30" s="14" t="s">
@@ -6820,13 +6823,13 @@
       </c>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="21" t="s">
         <v>360</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="E31" s="36" t="s">
+      <c r="E31" s="21" t="s">
         <v>362</v>
       </c>
       <c r="F31" s="14" t="s">
@@ -6834,37 +6837,37 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="21" t="s">
         <v>364</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="E32" s="36" t="s">
+      <c r="E32" s="21" t="s">
         <v>294</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="I32" s="26" t="s">
+      <c r="I32" s="68" t="s">
         <v>765</v>
       </c>
-      <c r="J32" s="34"/>
+      <c r="J32" s="69"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="21" t="s">
         <v>275</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>367</v>
       </c>
-      <c r="E33" s="36" t="s">
+      <c r="E33" s="21" t="s">
         <v>368</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="I33" s="35" t="s">
+      <c r="I33" s="20" t="s">
         <v>29</v>
       </c>
       <c r="J33" s="12" t="s">
@@ -6872,19 +6875,19 @@
       </c>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="21" t="s">
         <v>370</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="E34" s="36" t="s">
+      <c r="E34" s="21" t="s">
         <v>372</v>
       </c>
       <c r="F34" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="26" t="s">
         <v>233</v>
       </c>
       <c r="J34" s="13" t="s">
@@ -6892,19 +6895,19 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="21" t="s">
         <v>374</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="E35" s="36" t="s">
+      <c r="E35" s="21" t="s">
         <v>376</v>
       </c>
       <c r="F35" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="I35" s="36" t="s">
+      <c r="I35" s="21" t="s">
         <v>766</v>
       </c>
       <c r="J35" s="14" t="s">
@@ -6912,33 +6915,33 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="21" t="s">
         <v>378</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="E36" s="36" t="s">
+      <c r="E36" s="21" t="s">
         <v>380</v>
       </c>
       <c r="F36" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="I36" s="37" t="s">
+      <c r="I36" s="22" t="s">
         <v>767</v>
       </c>
-      <c r="J36" s="38" t="s">
+      <c r="J36" s="23" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="21" t="s">
         <v>382</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>383</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E37" s="21" t="s">
         <v>384</v>
       </c>
       <c r="F37" s="14" t="s">
@@ -6946,13 +6949,13 @@
       </c>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="21" t="s">
         <v>386</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>387</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="E38" s="21" t="s">
         <v>388</v>
       </c>
       <c r="F38" s="14" t="s">
@@ -6960,111 +6963,111 @@
       </c>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="21" t="s">
         <v>390</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>391</v>
       </c>
-      <c r="E39" s="36" t="s">
+      <c r="E39" s="21" t="s">
         <v>392</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="I39" s="26" t="s">
+      <c r="I39" s="68" t="s">
         <v>798</v>
       </c>
-      <c r="J39" s="34"/>
+      <c r="J39" s="69"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="21" t="s">
         <v>304</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E40" s="21" t="s">
         <v>395</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="I40" s="64" t="s">
+      <c r="I40" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="J40" s="65" t="s">
+      <c r="J40" s="47" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="21" t="s">
         <v>117</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="E41" s="36" t="s">
+      <c r="E41" s="21" t="s">
         <v>398</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>399</v>
       </c>
-      <c r="I41" s="64" t="s">
+      <c r="I41" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="J41" s="65" t="s">
+      <c r="J41" s="47" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="21" t="s">
         <v>400</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="E42" s="36" t="s">
+      <c r="E42" s="21" t="s">
         <v>402</v>
       </c>
       <c r="F42" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="I42" s="66" t="s">
+      <c r="I42" s="48" t="s">
         <v>790</v>
       </c>
-      <c r="J42" s="67" t="s">
+      <c r="J42" s="49" t="s">
         <v>791</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="21" t="s">
         <v>404</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="E43" s="36" t="s">
+      <c r="E43" s="21" t="s">
         <v>406</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="I43" s="68" t="s">
+      <c r="I43" s="50" t="s">
         <v>799</v>
       </c>
-      <c r="J43" s="69" t="s">
+      <c r="J43" s="51" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="21" t="s">
         <v>298</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="E44" s="21" t="s">
         <v>409</v>
       </c>
       <c r="F44" s="14" t="s">
@@ -7072,13 +7075,13 @@
       </c>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="21" t="s">
         <v>411</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="E45" s="36" t="s">
+      <c r="E45" s="21" t="s">
         <v>413</v>
       </c>
       <c r="F45" s="14" t="s">
@@ -7086,13 +7089,13 @@
       </c>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="21" t="s">
         <v>415</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="E46" s="36" t="s">
+      <c r="E46" s="21" t="s">
         <v>417</v>
       </c>
       <c r="F46" s="14" t="s">
@@ -7100,13 +7103,13 @@
       </c>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="21" t="s">
         <v>419</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="E47" s="36" t="s">
+      <c r="E47" s="21" t="s">
         <v>421</v>
       </c>
       <c r="F47" s="14" t="s">
@@ -7114,13 +7117,13 @@
       </c>
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="36" t="s">
+      <c r="B48" s="21" t="s">
         <v>423</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="E48" s="36" t="s">
+      <c r="E48" s="21" t="s">
         <v>425</v>
       </c>
       <c r="F48" s="14" t="s">
@@ -7128,13 +7131,13 @@
       </c>
     </row>
     <row r="49" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="36" t="s">
+      <c r="B49" s="21" t="s">
         <v>427</v>
       </c>
       <c r="C49" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="E49" s="36" t="s">
+      <c r="E49" s="21" t="s">
         <v>429</v>
       </c>
       <c r="F49" s="14" t="s">
@@ -7142,13 +7145,13 @@
       </c>
     </row>
     <row r="50" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="21" t="s">
         <v>431</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>432</v>
       </c>
-      <c r="E50" s="36" t="s">
+      <c r="E50" s="21" t="s">
         <v>433</v>
       </c>
       <c r="F50" s="14" t="s">
@@ -7156,13 +7159,13 @@
       </c>
     </row>
     <row r="51" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="21" t="s">
         <v>435</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>436</v>
       </c>
-      <c r="E51" s="36" t="s">
+      <c r="E51" s="21" t="s">
         <v>437</v>
       </c>
       <c r="F51" s="14" t="s">
@@ -7170,13 +7173,13 @@
       </c>
     </row>
     <row r="52" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="21" t="s">
         <v>439</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>440</v>
       </c>
-      <c r="E52" s="36" t="s">
+      <c r="E52" s="21" t="s">
         <v>441</v>
       </c>
       <c r="F52" s="14" t="s">
@@ -7184,13 +7187,13 @@
       </c>
     </row>
     <row r="53" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="21" t="s">
         <v>443</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="E53" s="36" t="s">
+      <c r="E53" s="21" t="s">
         <v>445</v>
       </c>
       <c r="F53" s="14" t="s">
@@ -7198,13 +7201,13 @@
       </c>
     </row>
     <row r="54" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="36" t="s">
+      <c r="B54" s="21" t="s">
         <v>447</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>448</v>
       </c>
-      <c r="E54" s="36" t="s">
+      <c r="E54" s="21" t="s">
         <v>449</v>
       </c>
       <c r="F54" s="14" t="s">
@@ -7212,13 +7215,13 @@
       </c>
     </row>
     <row r="55" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="36" t="s">
+      <c r="B55" s="21" t="s">
         <v>362</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>451</v>
       </c>
-      <c r="E55" s="36" t="s">
+      <c r="E55" s="21" t="s">
         <v>452</v>
       </c>
       <c r="F55" s="14" t="s">
@@ -7226,21 +7229,21 @@
       </c>
     </row>
     <row r="56" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="36" t="s">
+      <c r="B56" s="21" t="s">
         <v>454</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>455</v>
       </c>
-      <c r="E56" s="37" t="s">
+      <c r="E56" s="22" t="s">
         <v>456</v>
       </c>
-      <c r="F56" s="38" t="s">
+      <c r="F56" s="23" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="21" t="s">
         <v>336</v>
       </c>
       <c r="C57" s="14" t="s">
@@ -7248,7 +7251,7 @@
       </c>
     </row>
     <row r="58" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="21" t="s">
         <v>459</v>
       </c>
       <c r="C58" s="14" t="s">
@@ -7256,229 +7259,229 @@
       </c>
     </row>
     <row r="59" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="36" t="s">
+      <c r="B59" s="21" t="s">
         <v>461</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="E59" s="26" t="s">
+      <c r="E59" s="68" t="s">
         <v>774</v>
       </c>
-      <c r="F59" s="34"/>
+      <c r="F59" s="69"/>
     </row>
     <row r="60" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="21" t="s">
         <v>463</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>464</v>
       </c>
-      <c r="E60" s="64" t="s">
+      <c r="E60" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="F60" s="65" t="s">
+      <c r="F60" s="47" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="61" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="36" t="s">
+      <c r="B61" s="21" t="s">
         <v>465</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>466</v>
       </c>
-      <c r="E61" s="64" t="s">
+      <c r="E61" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="F61" s="65" t="s">
+      <c r="F61" s="47" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="36" t="s">
+      <c r="B62" s="21" t="s">
         <v>467</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>468</v>
       </c>
-      <c r="E62" s="66" t="s">
+      <c r="E62" s="48" t="s">
         <v>775</v>
       </c>
-      <c r="F62" s="67" t="s">
+      <c r="F62" s="49" t="s">
         <v>776</v>
       </c>
     </row>
     <row r="63" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="36" t="s">
+      <c r="B63" s="21" t="s">
         <v>406</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>469</v>
       </c>
-      <c r="E63" s="66" t="s">
+      <c r="E63" s="48" t="s">
         <v>777</v>
       </c>
-      <c r="F63" s="67" t="s">
+      <c r="F63" s="49" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="64" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="36" t="s">
+      <c r="B64" s="21" t="s">
         <v>470</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>471</v>
       </c>
-      <c r="E64" s="66" t="s">
+      <c r="E64" s="48" t="s">
         <v>472</v>
       </c>
-      <c r="F64" s="67" t="s">
+      <c r="F64" s="49" t="s">
         <v>779</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="21" t="s">
         <v>472</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>473</v>
       </c>
-      <c r="E65" s="66" t="s">
+      <c r="E65" s="48" t="s">
         <v>780</v>
       </c>
-      <c r="F65" s="67" t="s">
+      <c r="F65" s="49" t="s">
         <v>781</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="21" t="s">
         <v>474</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="E66" s="66" t="s">
+      <c r="E66" s="48" t="s">
         <v>782</v>
       </c>
-      <c r="F66" s="67" t="s">
+      <c r="F66" s="49" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="21" t="s">
         <v>476</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>477</v>
       </c>
-      <c r="E67" s="66" t="s">
+      <c r="E67" s="48" t="s">
         <v>784</v>
       </c>
-      <c r="F67" s="67" t="s">
+      <c r="F67" s="49" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="21" t="s">
         <v>478</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>479</v>
       </c>
-      <c r="E68" s="66" t="s">
+      <c r="E68" s="48" t="s">
         <v>786</v>
       </c>
-      <c r="F68" s="67" t="s">
+      <c r="F68" s="49" t="s">
         <v>787</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="21" t="s">
         <v>409</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="E69" s="66" t="s">
+      <c r="E69" s="48" t="s">
         <v>788</v>
       </c>
-      <c r="F69" s="67" t="s">
+      <c r="F69" s="49" t="s">
         <v>789</v>
       </c>
     </row>
     <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="36" t="s">
+      <c r="B70" s="21" t="s">
         <v>480</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>481</v>
       </c>
-      <c r="E70" s="66" t="s">
+      <c r="E70" s="48" t="s">
         <v>790</v>
       </c>
-      <c r="F70" s="67" t="s">
+      <c r="F70" s="49" t="s">
         <v>791</v>
       </c>
     </row>
     <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="36" t="s">
+      <c r="B71" s="21" t="s">
         <v>482</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>483</v>
       </c>
-      <c r="E71" s="66" t="s">
+      <c r="E71" s="48" t="s">
         <v>492</v>
       </c>
-      <c r="F71" s="67" t="s">
+      <c r="F71" s="49" t="s">
         <v>792</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="36" t="s">
+      <c r="B72" s="21" t="s">
         <v>484</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>485</v>
       </c>
-      <c r="E72" s="66" t="s">
+      <c r="E72" s="48" t="s">
         <v>459</v>
       </c>
-      <c r="F72" s="67" t="s">
+      <c r="F72" s="49" t="s">
         <v>793</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="36" t="s">
+      <c r="B73" s="21" t="s">
         <v>486</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>487</v>
       </c>
-      <c r="E73" s="66" t="s">
+      <c r="E73" s="48" t="s">
         <v>794</v>
       </c>
-      <c r="F73" s="67" t="s">
+      <c r="F73" s="49" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="36" t="s">
+      <c r="B74" s="21" t="s">
         <v>488</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>489</v>
       </c>
-      <c r="E74" s="68" t="s">
+      <c r="E74" s="50" t="s">
         <v>796</v>
       </c>
-      <c r="F74" s="69" t="s">
+      <c r="F74" s="51" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="36" t="s">
+      <c r="B75" s="21" t="s">
         <v>490</v>
       </c>
       <c r="C75" s="14" t="s">
@@ -7486,7 +7489,7 @@
       </c>
     </row>
     <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="36" t="s">
+      <c r="B76" s="21" t="s">
         <v>492</v>
       </c>
       <c r="C76" s="14" t="s">
@@ -7494,7 +7497,7 @@
       </c>
     </row>
     <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="36" t="s">
+      <c r="B77" s="21" t="s">
         <v>494</v>
       </c>
       <c r="C77" s="14" t="s">
@@ -7502,7 +7505,7 @@
       </c>
     </row>
     <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="36" t="s">
+      <c r="B78" s="21" t="s">
         <v>496</v>
       </c>
       <c r="C78" s="14" t="s">
@@ -7510,7 +7513,7 @@
       </c>
     </row>
     <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="36" t="s">
+      <c r="B79" s="21" t="s">
         <v>498</v>
       </c>
       <c r="C79" s="14" t="s">
@@ -7518,7 +7521,7 @@
       </c>
     </row>
     <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="36" t="s">
+      <c r="B80" s="21" t="s">
         <v>421</v>
       </c>
       <c r="C80" s="14" t="s">
@@ -7526,7 +7529,7 @@
       </c>
     </row>
     <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="36" t="s">
+      <c r="B81" s="21" t="s">
         <v>300</v>
       </c>
       <c r="C81" s="14" t="s">
@@ -7534,7 +7537,7 @@
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="36" t="s">
+      <c r="B82" s="21" t="s">
         <v>502</v>
       </c>
       <c r="C82" s="14" t="s">
@@ -7542,7 +7545,7 @@
       </c>
     </row>
     <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="36" t="s">
+      <c r="B83" s="21" t="s">
         <v>504</v>
       </c>
       <c r="C83" s="14" t="s">
@@ -7550,7 +7553,7 @@
       </c>
     </row>
     <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="36" t="s">
+      <c r="B84" s="21" t="s">
         <v>506</v>
       </c>
       <c r="C84" s="14" t="s">
@@ -7558,7 +7561,7 @@
       </c>
     </row>
     <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="36" t="s">
+      <c r="B85" s="21" t="s">
         <v>508</v>
       </c>
       <c r="C85" s="14" t="s">
@@ -7566,7 +7569,7 @@
       </c>
     </row>
     <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="36" t="s">
+      <c r="B86" s="21" t="s">
         <v>425</v>
       </c>
       <c r="C86" s="14" t="s">
@@ -7574,7 +7577,7 @@
       </c>
     </row>
     <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="36" t="s">
+      <c r="B87" s="21" t="s">
         <v>511</v>
       </c>
       <c r="C87" s="14" t="s">
@@ -7582,7 +7585,7 @@
       </c>
     </row>
     <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="36" t="s">
+      <c r="B88" s="21" t="s">
         <v>513</v>
       </c>
       <c r="C88" s="14" t="s">
@@ -7590,7 +7593,7 @@
       </c>
     </row>
     <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="36" t="s">
+      <c r="B89" s="21" t="s">
         <v>515</v>
       </c>
       <c r="C89" s="14" t="s">
@@ -7598,7 +7601,7 @@
       </c>
     </row>
     <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="36" t="s">
+      <c r="B90" s="21" t="s">
         <v>517</v>
       </c>
       <c r="C90" s="14" t="s">
@@ -7606,7 +7609,7 @@
       </c>
     </row>
     <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="36" t="s">
+      <c r="B91" s="21" t="s">
         <v>519</v>
       </c>
       <c r="C91" s="14" t="s">
@@ -7614,7 +7617,7 @@
       </c>
     </row>
     <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="36" t="s">
+      <c r="B92" s="21" t="s">
         <v>521</v>
       </c>
       <c r="C92" s="14" t="s">
@@ -7622,7 +7625,7 @@
       </c>
     </row>
     <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="36" t="s">
+      <c r="B93" s="21" t="s">
         <v>523</v>
       </c>
       <c r="C93" s="14" t="s">
@@ -7630,7 +7633,7 @@
       </c>
     </row>
     <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="36" t="s">
+      <c r="B94" s="21" t="s">
         <v>525</v>
       </c>
       <c r="C94" s="14" t="s">
@@ -7638,23 +7641,23 @@
       </c>
     </row>
     <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="37" t="s">
+      <c r="B95" s="22" t="s">
         <v>527</v>
       </c>
-      <c r="C95" s="38" t="s">
+      <c r="C95" s="23" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="39" t="s">
+      <c r="B99" s="24" t="s">
         <v>529</v>
       </c>
-      <c r="C99" s="40"/>
+      <c r="C99" s="25"/>
     </row>
     <row r="100" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="35" t="s">
+      <c r="B100" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C100" s="12" t="s">
@@ -7662,7 +7665,7 @@
       </c>
     </row>
     <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="35" t="s">
+      <c r="B101" s="20" t="s">
         <v>233</v>
       </c>
       <c r="C101" s="12" t="s">
@@ -7670,7 +7673,7 @@
       </c>
     </row>
     <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="36" t="s">
+      <c r="B102" s="21" t="s">
         <v>530</v>
       </c>
       <c r="C102" s="14" t="s">
@@ -7678,7 +7681,7 @@
       </c>
     </row>
     <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="36" t="s">
+      <c r="B103" s="21" t="s">
         <v>532</v>
       </c>
       <c r="C103" s="14" t="s">
@@ -7686,7 +7689,7 @@
       </c>
     </row>
     <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="36" t="s">
+      <c r="B104" s="21" t="s">
         <v>534</v>
       </c>
       <c r="C104" s="14" t="s">
@@ -7694,7 +7697,7 @@
       </c>
     </row>
     <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="36" t="s">
+      <c r="B105" s="21" t="s">
         <v>536</v>
       </c>
       <c r="C105" s="14" t="s">
@@ -7702,7 +7705,7 @@
       </c>
     </row>
     <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="36" t="s">
+      <c r="B106" s="21" t="s">
         <v>538</v>
       </c>
       <c r="C106" s="14" t="s">
@@ -7710,7 +7713,7 @@
       </c>
     </row>
     <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="36" t="s">
+      <c r="B107" s="21" t="s">
         <v>540</v>
       </c>
       <c r="C107" s="14" t="s">
@@ -7718,7 +7721,7 @@
       </c>
     </row>
     <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="36" t="s">
+      <c r="B108" s="21" t="s">
         <v>542</v>
       </c>
       <c r="C108" s="14" t="s">
@@ -7726,7 +7729,7 @@
       </c>
     </row>
     <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="36" t="s">
+      <c r="B109" s="21" t="s">
         <v>544</v>
       </c>
       <c r="C109" s="14" t="s">
@@ -7734,7 +7737,7 @@
       </c>
     </row>
     <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="36" t="s">
+      <c r="B110" s="21" t="s">
         <v>546</v>
       </c>
       <c r="C110" s="14" t="s">
@@ -7742,7 +7745,7 @@
       </c>
     </row>
     <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="36" t="s">
+      <c r="B111" s="21" t="s">
         <v>548</v>
       </c>
       <c r="C111" s="14" t="s">
@@ -7750,7 +7753,7 @@
       </c>
     </row>
     <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="36" t="s">
+      <c r="B112" s="21" t="s">
         <v>550</v>
       </c>
       <c r="C112" s="14" t="s">
@@ -7758,7 +7761,7 @@
       </c>
     </row>
     <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="36" t="s">
+      <c r="B113" s="21" t="s">
         <v>552</v>
       </c>
       <c r="C113" s="14" t="s">
@@ -7766,7 +7769,7 @@
       </c>
     </row>
     <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="36" t="s">
+      <c r="B114" s="21" t="s">
         <v>554</v>
       </c>
       <c r="C114" s="14" t="s">
@@ -7774,7 +7777,7 @@
       </c>
     </row>
     <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="36" t="s">
+      <c r="B115" s="21" t="s">
         <v>556</v>
       </c>
       <c r="C115" s="14" t="s">
@@ -7782,7 +7785,7 @@
       </c>
     </row>
     <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="36" t="s">
+      <c r="B116" s="21" t="s">
         <v>558</v>
       </c>
       <c r="C116" s="14" t="s">
@@ -7790,7 +7793,7 @@
       </c>
     </row>
     <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="36" t="s">
+      <c r="B117" s="21" t="s">
         <v>560</v>
       </c>
       <c r="C117" s="14" t="s">
@@ -7798,7 +7801,7 @@
       </c>
     </row>
     <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="36" t="s">
+      <c r="B118" s="21" t="s">
         <v>562</v>
       </c>
       <c r="C118" s="14" t="s">
@@ -7806,7 +7809,7 @@
       </c>
     </row>
     <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="36" t="s">
+      <c r="B119" s="21" t="s">
         <v>564</v>
       </c>
       <c r="C119" s="14" t="s">
@@ -7814,7 +7817,7 @@
       </c>
     </row>
     <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="36" t="s">
+      <c r="B120" s="21" t="s">
         <v>566</v>
       </c>
       <c r="C120" s="14" t="s">
@@ -7822,7 +7825,7 @@
       </c>
     </row>
     <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="36" t="s">
+      <c r="B121" s="21" t="s">
         <v>568</v>
       </c>
       <c r="C121" s="14" t="s">
@@ -7830,7 +7833,7 @@
       </c>
     </row>
     <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="36" t="s">
+      <c r="B122" s="21" t="s">
         <v>570</v>
       </c>
       <c r="C122" s="14" t="s">
@@ -7838,7 +7841,7 @@
       </c>
     </row>
     <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="36" t="s">
+      <c r="B123" s="21" t="s">
         <v>572</v>
       </c>
       <c r="C123" s="14" t="s">
@@ -7846,7 +7849,7 @@
       </c>
     </row>
     <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="36" t="s">
+      <c r="B124" s="21" t="s">
         <v>574</v>
       </c>
       <c r="C124" s="14" t="s">
@@ -7854,7 +7857,7 @@
       </c>
     </row>
     <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="36" t="s">
+      <c r="B125" s="21" t="s">
         <v>576</v>
       </c>
       <c r="C125" s="14" t="s">
@@ -7862,7 +7865,7 @@
       </c>
     </row>
     <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="36" t="s">
+      <c r="B126" s="21" t="s">
         <v>578</v>
       </c>
       <c r="C126" s="14" t="s">
@@ -7870,7 +7873,7 @@
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="36" t="s">
+      <c r="B127" s="21" t="s">
         <v>580</v>
       </c>
       <c r="C127" s="14" t="s">
@@ -7878,7 +7881,7 @@
       </c>
     </row>
     <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="36" t="s">
+      <c r="B128" s="21" t="s">
         <v>582</v>
       </c>
       <c r="C128" s="14" t="s">
@@ -7886,7 +7889,7 @@
       </c>
     </row>
     <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="36" t="s">
+      <c r="B129" s="21" t="s">
         <v>584</v>
       </c>
       <c r="C129" s="14" t="s">
@@ -7894,7 +7897,7 @@
       </c>
     </row>
     <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="36" t="s">
+      <c r="B130" s="21" t="s">
         <v>586</v>
       </c>
       <c r="C130" s="14" t="s">
@@ -7902,7 +7905,7 @@
       </c>
     </row>
     <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="36" t="s">
+      <c r="B131" s="21" t="s">
         <v>588</v>
       </c>
       <c r="C131" s="14" t="s">
@@ -7910,7 +7913,7 @@
       </c>
     </row>
     <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="36" t="s">
+      <c r="B132" s="21" t="s">
         <v>590</v>
       </c>
       <c r="C132" s="14" t="s">
@@ -7918,7 +7921,7 @@
       </c>
     </row>
     <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="36" t="s">
+      <c r="B133" s="21" t="s">
         <v>592</v>
       </c>
       <c r="C133" s="14" t="s">
@@ -7926,7 +7929,7 @@
       </c>
     </row>
     <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="36" t="s">
+      <c r="B134" s="21" t="s">
         <v>594</v>
       </c>
       <c r="C134" s="14" t="s">
@@ -7934,7 +7937,7 @@
       </c>
     </row>
     <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="36" t="s">
+      <c r="B135" s="21" t="s">
         <v>596</v>
       </c>
       <c r="C135" s="14" t="s">
@@ -7942,7 +7945,7 @@
       </c>
     </row>
     <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="36" t="s">
+      <c r="B136" s="21" t="s">
         <v>598</v>
       </c>
       <c r="C136" s="14" t="s">
@@ -7950,7 +7953,7 @@
       </c>
     </row>
     <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="36" t="s">
+      <c r="B137" s="21" t="s">
         <v>600</v>
       </c>
       <c r="C137" s="14" t="s">
@@ -7958,7 +7961,7 @@
       </c>
     </row>
     <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="36" t="s">
+      <c r="B138" s="21" t="s">
         <v>602</v>
       </c>
       <c r="C138" s="14" t="s">
@@ -7966,7 +7969,7 @@
       </c>
     </row>
     <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="36" t="s">
+      <c r="B139" s="21" t="s">
         <v>604</v>
       </c>
       <c r="C139" s="14" t="s">
@@ -7974,19 +7977,19 @@
       </c>
     </row>
     <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="37" t="s">
+      <c r="B140" s="22" t="s">
         <v>606</v>
       </c>
-      <c r="C140" s="38" t="s">
+      <c r="C140" s="23" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="24" t="s">
+      <c r="B143" s="66" t="s">
         <v>608</v>
       </c>
-      <c r="C143" s="25"/>
+      <c r="C143" s="67"/>
     </row>
     <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="8" t="s">

</xml_diff>

<commit_message>
EPBDS-5972 Rename property "Province" to "Canada Province"
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="808">
   <si>
     <t>Display Name</t>
   </si>
@@ -2460,9 +2460,6 @@
   </si>
   <si>
     <t>Région d'opération pour laquelle la table devrait être utilisée</t>
-  </si>
-  <si>
-    <t>Province</t>
   </si>
   <si>
     <t>caProvinces</t>
@@ -3222,14 +3219,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3716,16 +3713,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3761,31 +3758,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3839,13 +3836,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3854,13 +3851,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3869,34 +3866,29 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3906,6 +3898,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3922,7 +3919,7 @@
   <dimension ref="A1:AMK62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3988,18 +3985,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4039,35 +4036,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -5794,7 +5791,7 @@
     </row>
     <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>801</v>
@@ -5839,10 +5836,10 @@
     </row>
     <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>804</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>805</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>58</v>
@@ -5851,7 +5848,7 @@
         <v>140</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>78</v>
@@ -5879,7 +5876,7 @@
         <v>84</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="53" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
EPBDS-5982 Reorder properties in TablePropertyDefinition.xlsx
--HG--
branch : 5.16.x
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18900" tabRatio="410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -3219,14 +3219,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3272,39 +3272,39 @@
     </xf>
   </cellXfs>
   <cellStyles count="33">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3713,16 +3713,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3758,31 +3758,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3836,13 +3836,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3851,13 +3851,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3866,29 +3866,34 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3898,11 +3903,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3916,10 +3916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK62"/>
+  <dimension ref="A1:AMK64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3985,18 +3985,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4036,35 +4036,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -4342,10 +4342,10 @@
     </row>
     <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>58</v>
@@ -4360,12 +4360,16 @@
       <c r="H16" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="K16" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="5" t="s">
         <v>58</v>
       </c>
       <c r="M16" s="5"/>
@@ -4380,21 +4384,21 @@
         <v>64</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
@@ -4403,10 +4407,14 @@
       <c r="H17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="K17" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>58</v>
@@ -4417,41 +4425,45 @@
         <v>58</v>
       </c>
       <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
+      <c r="Q17" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="R17" s="5"/>
       <c r="S17" s="5" t="s">
         <v>64</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K18" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>58</v>
@@ -4459,26 +4471,24 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="P18" s="5"/>
-      <c r="Q18" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>58</v>
@@ -4486,19 +4496,21 @@
       <c r="E19" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="F19" s="5"/>
       <c r="G19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>58</v>
@@ -4506,7 +4518,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5" t="s">
@@ -4514,80 +4526,74 @@
       </c>
       <c r="R19" s="5"/>
       <c r="S19" s="5" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>93</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F20" s="5"/>
       <c r="G20" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="6" t="s">
         <v>58</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="P20" s="5"/>
-      <c r="Q20" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>98</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -4600,48 +4606,44 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="P21" s="5"/>
-      <c r="Q21" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G22" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>104</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
       <c r="K22" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>58</v>
@@ -4649,24 +4651,26 @@
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
+      <c r="Q22" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="R22" s="5"/>
       <c r="S22" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="T22" s="5" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>58</v>
@@ -4674,21 +4678,19 @@
       <c r="E23" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="G23" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>104</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>58</v>
@@ -4696,7 +4698,7 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" s="5" t="s">
@@ -4704,40 +4706,38 @@
       </c>
       <c r="R23" s="5"/>
       <c r="S23" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G24" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>112</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
       <c r="K24" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>58</v>
@@ -4745,24 +4745,26 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
+      <c r="Q24" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="R24" s="5"/>
       <c r="S24" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>58</v>
@@ -4770,21 +4772,19 @@
       <c r="E25" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="G25" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>112</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
       <c r="K25" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>58</v>
@@ -4792,7 +4792,7 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="P25" s="5"/>
       <c r="Q25" s="5" t="s">
@@ -4800,31 +4800,33 @@
       </c>
       <c r="R25" s="5"/>
       <c r="S25" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="T25" s="5" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>117</v>
+        <v>807</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>118</v>
+        <v>801</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>140</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>802</v>
+      </c>
       <c r="G26" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -4834,44 +4836,42 @@
       <c r="L26" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="M26" s="5" t="s">
-        <v>120</v>
-      </c>
+      <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="P26" s="5" t="s">
-        <v>122</v>
-      </c>
+        <v>772</v>
+      </c>
+      <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>123</v>
+        <v>803</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>124</v>
+        <v>770</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>125</v>
+        <v>804</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>140</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>805</v>
+      </c>
       <c r="G27" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -4884,7 +4884,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>126</v>
+        <v>769</v>
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
@@ -4893,28 +4893,30 @@
         <v>84</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>127</v>
+        <v>806</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>140</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="G28" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -4922,14 +4924,12 @@
         <v>58</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>130</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
@@ -4938,24 +4938,24 @@
         <v>84</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>78</v>
@@ -4974,24 +4974,24 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>58</v>
@@ -5000,7 +5000,7 @@
         <v>140</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>78</v>
@@ -5019,7 +5019,7 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
@@ -5028,15 +5028,15 @@
         <v>84</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>58</v>
@@ -5045,7 +5045,7 @@
         <v>140</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>78</v>
@@ -5064,7 +5064,7 @@
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
@@ -5073,24 +5073,24 @@
         <v>84</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>140</v>
+        <v>59</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>78</v>
@@ -5109,7 +5109,7 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -5118,25 +5118,23 @@
         <v>84</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>154</v>
+        <v>759</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>155</v>
+        <v>760</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>156</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
         <v>78</v>
       </c>
@@ -5149,12 +5147,14 @@
         <v>58</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M33" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>761</v>
+      </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5" t="s">
-        <v>157</v>
+        <v>762</v>
       </c>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -5163,15 +5163,15 @@
         <v>84</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>158</v>
+        <v>763</v>
       </c>
     </row>
     <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>58</v>
@@ -5180,7 +5180,7 @@
         <v>140</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>78</v>
@@ -5199,7 +5199,7 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
@@ -5208,15 +5208,15 @@
         <v>84</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>58</v>
@@ -5225,7 +5225,7 @@
         <v>140</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>78</v>
@@ -5244,16 +5244,16 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5" t="s">
-        <v>168</v>
+        <v>84</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5343,14 +5343,16 @@
     </row>
     <row r="38" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D38" s="5"/>
+        <v>118</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E38" s="5" t="s">
-        <v>176</v>
+        <v>59</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5" t="s">
@@ -5364,33 +5366,38 @@
       <c r="K38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L38" s="5"/>
+      <c r="L38" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="M38" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="N38" s="7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
+        <v>120</v>
+      </c>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="Q38" s="5"/>
       <c r="R38" s="5"/>
       <c r="S38" s="5" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="T38" s="5" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D39" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E39" s="5" t="s">
         <v>59</v>
       </c>
@@ -5406,32 +5413,34 @@
       <c r="K39" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5" t="s">
-        <v>184</v>
-      </c>
+      <c r="L39" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5" t="s">
-        <v>185</v>
+        <v>126</v>
       </c>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
       <c r="S39" s="5" t="s">
-        <v>186</v>
+        <v>84</v>
       </c>
       <c r="T39" s="5" t="s">
-        <v>187</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D40" s="5"/>
+        <v>129</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E40" s="5" t="s">
         <v>59</v>
       </c>
@@ -5447,36 +5456,36 @@
       <c r="K40" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L40" s="5"/>
+      <c r="L40" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="M40" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="N40" s="5" t="s">
-        <v>191</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="N40" s="5"/>
       <c r="O40" s="5" t="s">
-        <v>192</v>
+        <v>131</v>
       </c>
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5" t="s">
-        <v>193</v>
+        <v>84</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>194</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5" t="s">
@@ -5491,29 +5500,34 @@
         <v>58</v>
       </c>
       <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="M41" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="N41" s="7" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O41" s="5"/>
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T41" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="T41" s="5" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="42" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5" t="s">
@@ -5528,29 +5542,33 @@
         <v>58</v>
       </c>
       <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
+      <c r="M42" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="N42" s="5"/>
       <c r="O42" s="5" t="s">
-        <v>58</v>
+        <v>185</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T42" s="5"/>
+        <v>186</v>
+      </c>
+      <c r="T42" s="5" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="43" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5" t="s">
@@ -5565,31 +5583,35 @@
         <v>58</v>
       </c>
       <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
+      <c r="M43" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>191</v>
+      </c>
       <c r="O43" s="5" t="s">
-        <v>58</v>
+        <v>192</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T43" s="5"/>
+        <v>193</v>
+      </c>
+      <c r="T43" s="5" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="44" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>176</v>
+        <v>74</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5" t="s">
@@ -5606,29 +5628,27 @@
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
+      <c r="O44" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="T44" s="5" t="s">
-        <v>749</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="T44" s="5"/>
     </row>
     <row r="45" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>205</v>
+        <v>74</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5" t="s">
@@ -5646,28 +5666,26 @@
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5" t="s">
-        <v>206</v>
+        <v>58</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="T45" s="5" t="s">
-        <v>207</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="T45" s="5"/>
     </row>
     <row r="46" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>751</v>
+        <v>199</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>750</v>
+        <v>200</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5" t="s">
@@ -5682,29 +5700,25 @@
         <v>58</v>
       </c>
       <c r="L46" s="5"/>
-      <c r="M46" s="5" t="s">
-        <v>754</v>
-      </c>
+      <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5" t="s">
-        <v>753</v>
+        <v>58</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
       <c r="S46" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="T46" s="5" t="s">
-        <v>752</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="T46" s="5"/>
     </row>
     <row r="47" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>755</v>
+        <v>201</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>756</v>
+        <v>202</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>58</v>
@@ -5724,15 +5738,9 @@
       <c r="K47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L47" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M47" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="N47" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
@@ -5741,15 +5749,15 @@
         <v>84</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>758</v>
+        <v>749</v>
       </c>
     </row>
     <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>759</v>
+        <v>203</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>760</v>
+        <v>204</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>58</v>
@@ -5759,25 +5767,21 @@
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L48" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M48" s="5" t="s">
-        <v>761</v>
-      </c>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5" t="s">
-        <v>762</v>
+        <v>206</v>
       </c>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
@@ -5786,43 +5790,39 @@
         <v>84</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>763</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>807</v>
+        <v>751</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>801</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>802</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F49" s="5"/>
       <c r="G49" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L49" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5" t="s">
+        <v>754</v>
+      </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5" t="s">
-        <v>772</v>
+        <v>753</v>
       </c>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
@@ -5831,30 +5831,28 @@
         <v>84</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>803</v>
+        <v>752</v>
       </c>
     </row>
     <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>804</v>
+        <v>756</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>805</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="F50" s="5"/>
       <c r="G50" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
@@ -5864,11 +5862,13 @@
       <c r="L50" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5" t="s">
-        <v>769</v>
-      </c>
+      <c r="M50" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="N50" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O50" s="5"/>
       <c r="P50" s="5"/>
       <c r="Q50" s="5"/>
       <c r="R50" s="5"/>
@@ -5876,87 +5876,87 @@
         <v>84</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="53" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5" t="s">
+      <c r="D55" s="5"/>
+      <c r="E55" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H53" s="5" t="s">
+      <c r="F55" s="5"/>
+      <c r="G55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5" t="s">
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="5" t="s">
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="T53" s="5" t="s">
+      <c r="T55" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="57" t="s">
+    <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="57" t="s">
         <v>212</v>
       </c>
-      <c r="C57" s="57"/>
-    </row>
-    <row r="58" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="58" t="s">
+      <c r="C59" s="57"/>
+    </row>
+    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="C58" s="58"/>
-    </row>
-    <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="58" t="s">
+      <c r="C60" s="58"/>
+    </row>
+    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="C59" s="58"/>
-    </row>
-    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="59" t="s">
+      <c r="C61" s="58"/>
+    </row>
+    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="C60" s="59"/>
-    </row>
-    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="59" t="s">
+      <c r="C62" s="59"/>
+    </row>
+    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="C61" s="59"/>
-    </row>
-    <row r="62" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="56" t="s">
+      <c r="C63" s="59"/>
+    </row>
+    <row r="64" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="56" t="s">
         <v>764</v>
       </c>
-      <c r="C62" s="56"/>
+      <c r="C64" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B64:C64"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C3:L3"/>
@@ -5967,11 +5967,11 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-6043 Rewrite descriptions for Canada Province and Canada Region
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -2459,19 +2459,19 @@
     <t>contains(caRegion)</t>
   </si>
   <si>
-    <t>Région d'opération pour laquelle la table devrait être utilisée</t>
-  </si>
-  <si>
     <t>caProvinces</t>
   </si>
   <si>
     <t>contains(caProvince)</t>
   </si>
   <si>
-    <t>Province pour laquelle la table devrait être utilisée</t>
-  </si>
-  <si>
     <t>Canada Region</t>
+  </si>
+  <si>
+    <t>Canada region(s) of operation for which the table should be used</t>
+  </si>
+  <si>
+    <t>Canada province for which the table should be used</t>
   </si>
 </sst>
 </file>
@@ -3219,14 +3219,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3713,16 +3713,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3758,31 +3758,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3836,13 +3836,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3851,13 +3851,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3866,34 +3866,29 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3903,6 +3898,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3918,8 +3918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="E34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3985,18 +3985,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4036,35 +4036,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -4808,7 +4808,7 @@
     </row>
     <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>801</v>
@@ -4848,7 +4848,7 @@
         <v>84</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4856,7 +4856,7 @@
         <v>770</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>58</v>
@@ -4865,7 +4865,7 @@
         <v>140</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>78</v>
@@ -4893,7 +4893,7 @@
         <v>84</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
EPBDS-6146 Add drop down list for Validate DT: on, off, gaps, overlaps
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="Runtime Scope" sheetId="4" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="812">
   <si>
     <t>Display Name</t>
   </si>
@@ -443,12 +448,6 @@
     <t>XLS_DT, XLS_PROPERTIES</t>
   </si>
   <si>
-    <t>one of: on, off, gaps, overlaps</t>
-  </si>
-  <si>
-    <t>On/Off/Gap/Overlap validation mode for the rule table</t>
-  </si>
-  <si>
     <t>LOB</t>
   </si>
   <si>
@@ -2472,12 +2471,30 @@
   </si>
   <si>
     <t>Canada province for which the table should be used</t>
+  </si>
+  <si>
+    <t>Data EnumPropertyDefinition validateDT</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>data: validateDT</t>
+  </si>
+  <si>
+    <t>On/Off validation mode for the rule table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3272,39 +3289,39 @@
     </xf>
   </cellXfs>
   <cellStyles count="33">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3380,14 +3397,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3425,9 +3445,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3460,9 +3480,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3495,9 +3532,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3918,8 +3972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4808,19 +4862,19 @@
     </row>
     <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>78</v>
@@ -4839,7 +4893,7 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -4848,24 +4902,24 @@
         <v>84</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>78</v>
@@ -4884,7 +4938,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
@@ -4893,24 +4947,24 @@
         <v>84</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>78</v>
@@ -4929,7 +4983,7 @@
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
@@ -4938,24 +4992,24 @@
         <v>84</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>78</v>
@@ -4974,33 +5028,33 @@
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>78</v>
@@ -5019,7 +5073,7 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
@@ -5028,24 +5082,24 @@
         <v>84</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>78</v>
@@ -5064,7 +5118,7 @@
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
@@ -5073,15 +5127,15 @@
         <v>84</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>58</v>
@@ -5090,7 +5144,7 @@
         <v>59</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>78</v>
@@ -5109,7 +5163,7 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -5118,21 +5172,21 @@
         <v>84</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
@@ -5150,11 +5204,11 @@
         <v>58</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -5163,24 +5217,24 @@
         <v>84</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>78</v>
@@ -5199,7 +5253,7 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
@@ -5208,24 +5262,24 @@
         <v>84</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>78</v>
@@ -5244,7 +5298,7 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
@@ -5253,15 +5307,15 @@
         <v>84</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
@@ -5272,7 +5326,7 @@
         <v>58</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -5285,7 +5339,7 @@
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
@@ -5294,26 +5348,26 @@
         <v>64</v>
       </c>
       <c r="T36" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5" t="s">
         <v>58</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
@@ -5329,7 +5383,7 @@
         <v>1</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
@@ -5338,7 +5392,7 @@
         <v>64</v>
       </c>
       <c r="T37" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5442,7 +5496,7 @@
         <v>58</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>59</v>
+        <v>203</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5" t="s">
@@ -5464,7 +5518,7 @@
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5" t="s">
-        <v>131</v>
+        <v>810</v>
       </c>
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
@@ -5473,19 +5527,19 @@
         <v>84</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>132</v>
+        <v>811</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5" t="s">
@@ -5515,15 +5569,15 @@
         <v>84</v>
       </c>
       <c r="T41" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
@@ -5543,28 +5597,28 @@
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N42" s="5"/>
       <c r="O42" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="T42" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
@@ -5584,30 +5638,30 @@
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="O43" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="T43" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
@@ -5641,10 +5695,10 @@
     </row>
     <row r="45" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
@@ -5678,10 +5732,10 @@
     </row>
     <row r="46" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
@@ -5715,16 +5769,16 @@
     </row>
     <row r="47" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
@@ -5749,21 +5803,21 @@
         <v>84</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5" t="s">
@@ -5781,7 +5835,7 @@
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
@@ -5790,15 +5844,15 @@
         <v>84</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
@@ -5818,11 +5872,11 @@
       </c>
       <c r="L49" s="5"/>
       <c r="M49" s="5" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
@@ -5831,21 +5885,21 @@
         <v>84</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5" t="s">
@@ -5863,7 +5917,7 @@
         <v>58</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="N50" s="5" t="b">
         <v>0</v>
@@ -5876,19 +5930,19 @@
         <v>84</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="55" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5" t="s">
@@ -5904,7 +5958,7 @@
       </c>
       <c r="L55" s="5"/>
       <c r="M55" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
@@ -5915,42 +5969,42 @@
         <v>64</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="57" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C59" s="57"/>
     </row>
     <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="58" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C60" s="58"/>
     </row>
     <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="58" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C61" s="58"/>
     </row>
     <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="59" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C62" s="59"/>
     </row>
     <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="59" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C63" s="59"/>
     </row>
     <row r="64" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="56" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C64" s="56"/>
     </row>
@@ -5987,7 +6041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -5995,7 +6049,7 @@
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="60"/>
@@ -6004,10 +6058,10 @@
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -6016,7 +6070,7 @@
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
       <c r="C7" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -6025,7 +6079,7 @@
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="61"/>
       <c r="C8" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -6034,7 +6088,7 @@
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
       <c r="C9" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -6043,7 +6097,7 @@
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
       <c r="C10" s="62" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D10" s="62"/>
       <c r="E10" s="62"/>
@@ -6083,7 +6137,7 @@
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="63" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C2" s="64"/>
       <c r="D2" s="64"/>
@@ -6131,7 +6185,7 @@
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>79</v>
@@ -6143,126 +6197,126 @@
     </row>
     <row r="7" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="39" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="E9" s="40" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>152</v>
-      </c>
       <c r="E11" s="40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>157</v>
-      </c>
       <c r="E12" s="42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="E13" s="40" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="39" t="s">
+        <v>766</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="E14" s="40" t="s">
         <v>768</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="43" t="s">
+        <v>769</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>770</v>
+      </c>
+      <c r="E15" s="45" t="s">
         <v>771</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>205</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>772</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>773</v>
       </c>
     </row>
   </sheetData>
@@ -6283,8 +6337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J216"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6299,15 +6353,15 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="68" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C2" s="69"/>
       <c r="E2" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F2" s="25"/>
       <c r="I2" s="68" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J2" s="69"/>
     </row>
@@ -6333,190 +6387,190 @@
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="I5" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="J5" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="I6" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="J6" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="F7" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="I7" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="J7" s="14" t="s">
         <v>249</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="I8" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="F8" s="14" t="s">
+      <c r="J8" s="23" t="s">
         <v>254</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="F9" s="14" t="s">
         <v>258</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>262</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="F11" s="14" t="s">
         <v>266</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>270</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>271</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="F13" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="I13" s="68" t="s">
         <v>275</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="I13" s="68" t="s">
-        <v>277</v>
       </c>
       <c r="J13" s="69"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>279</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>281</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>29</v>
@@ -6527,182 +6581,182 @@
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="F15" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>285</v>
-      </c>
       <c r="I15" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="F16" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="I16" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="J16" s="14" t="s">
         <v>289</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>117</v>
       </c>
       <c r="F17" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="J17" s="14" t="s">
         <v>293</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="F18" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="I18" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="J18" s="14" t="s">
         <v>299</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="E19" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="I19" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="J19" s="14" t="s">
         <v>305</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>306</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="F20" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="I20" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="J20" s="23" t="s">
         <v>310</v>
-      </c>
-      <c r="I20" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="F21" s="14" t="s">
         <v>314</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>315</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="F22" s="14" t="s">
         <v>318</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>319</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>321</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="F23" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="I23" s="68" t="s">
         <v>323</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="I23" s="68" t="s">
-        <v>325</v>
       </c>
       <c r="J23" s="69"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="E24" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="F24" s="14" t="s">
         <v>327</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>328</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>329</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>29</v>
@@ -6713,156 +6767,156 @@
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="E25" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="F25" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>332</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>333</v>
-      </c>
       <c r="I25" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="F26" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="I26" s="21" t="s">
         <v>336</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="J26" s="14" t="s">
         <v>337</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>338</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="F27" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="I27" s="27" t="s">
         <v>342</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="J27" s="15" t="s">
         <v>343</v>
-      </c>
-      <c r="I27" s="27" t="s">
-        <v>344</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="E28" s="21" t="s">
         <v>346</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="F28" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="I28" s="28" t="s">
         <v>348</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="J28" s="29" t="s">
         <v>349</v>
-      </c>
-      <c r="I28" s="28" t="s">
-        <v>350</v>
-      </c>
-      <c r="J28" s="29" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="E29" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="F29" s="14" t="s">
         <v>353</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>354</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="E30" s="21" t="s">
         <v>356</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="F30" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>358</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="E31" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="F31" s="14" t="s">
         <v>361</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>362</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="F32" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>366</v>
-      </c>
       <c r="I32" s="68" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="J32" s="69"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="21" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C33" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F33" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>368</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>369</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>29</v>
@@ -6873,122 +6927,122 @@
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="E34" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="F34" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="E34" s="21" t="s">
-        <v>372</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>373</v>
-      </c>
       <c r="I34" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="E35" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="F35" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="E35" s="21" t="s">
-        <v>376</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>377</v>
-      </c>
       <c r="I35" s="21" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E36" s="21" t="s">
         <v>378</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="F36" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="E36" s="21" t="s">
-        <v>380</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>381</v>
-      </c>
       <c r="I36" s="22" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="E37" s="21" t="s">
         <v>382</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="F37" s="14" t="s">
         <v>383</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>384</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="E38" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="F38" s="14" t="s">
         <v>387</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>388</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="E39" s="21" t="s">
         <v>390</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="F39" s="14" t="s">
         <v>391</v>
       </c>
-      <c r="E39" s="21" t="s">
-        <v>392</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>393</v>
-      </c>
       <c r="I39" s="68" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="J39" s="69"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C40" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="F40" s="14" t="s">
         <v>394</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>395</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>396</v>
       </c>
       <c r="I40" s="46" t="s">
         <v>29</v>
@@ -7002,277 +7056,305 @@
         <v>117</v>
       </c>
       <c r="C41" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="F41" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="E41" s="21" t="s">
-        <v>398</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>399</v>
-      </c>
       <c r="I41" s="46" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J41" s="47" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="E42" s="21" t="s">
         <v>400</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="F42" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="E42" s="21" t="s">
-        <v>402</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>403</v>
-      </c>
       <c r="I42" s="48" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="J42" s="49" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="E43" s="21" t="s">
         <v>404</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="F43" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="E43" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>407</v>
-      </c>
       <c r="I43" s="50" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="J43" s="51" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="21" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C44" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="F44" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="E44" s="21" t="s">
+    </row>
+    <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="21" t="s">
         <v>409</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="C45" s="14" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="21" t="s">
+      <c r="E45" s="21" t="s">
         <v>411</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="F45" s="14" t="s">
         <v>412</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="E46" s="21" t="s">
         <v>415</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="F46" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="E46" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>418</v>
-      </c>
+      <c r="I46" s="68" t="s">
+        <v>806</v>
+      </c>
+      <c r="J46" s="69"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="E47" s="21" t="s">
         <v>419</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="F47" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="E47" s="21" t="s">
-        <v>421</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>422</v>
+      <c r="I47" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="E48" s="21" t="s">
         <v>423</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="F48" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="I48" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="J48" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="C49" s="14" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="21" t="s">
+      <c r="E49" s="21" t="s">
         <v>427</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="F49" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="I49" s="21" t="s">
+        <v>786</v>
+      </c>
+      <c r="J49" s="14" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="21" t="s">
         <v>429</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="C50" s="14" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="50" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="21" t="s">
+      <c r="E50" s="21" t="s">
         <v>431</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="F50" s="14" t="s">
         <v>432</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="I50" s="28" t="s">
+        <v>809</v>
+      </c>
+      <c r="J50" s="29" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="21" t="s">
         <v>433</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="C51" s="14" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="21" t="s">
+      <c r="E51" s="21" t="s">
         <v>435</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="F51" s="14" t="s">
         <v>436</v>
       </c>
-      <c r="E51" s="21" t="s">
+    </row>
+    <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="C52" s="14" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="52" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="21" t="s">
+      <c r="E52" s="21" t="s">
         <v>439</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="F52" s="14" t="s">
         <v>440</v>
       </c>
-      <c r="E52" s="21" t="s">
+    </row>
+    <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="21" t="s">
         <v>441</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="C53" s="14" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="53" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="21" t="s">
+      <c r="E53" s="21" t="s">
         <v>443</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="F53" s="14" t="s">
         <v>444</v>
       </c>
-      <c r="E53" s="21" t="s">
+    </row>
+    <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="21" t="s">
         <v>445</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="C54" s="14" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="54" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="21" t="s">
+      <c r="E54" s="21" t="s">
         <v>447</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="F54" s="14" t="s">
         <v>448</v>
       </c>
-      <c r="E54" s="21" t="s">
+    </row>
+    <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="C55" s="14" t="s">
         <v>449</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="E55" s="21" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="21" t="s">
-        <v>362</v>
-      </c>
-      <c r="C55" s="14" t="s">
+      <c r="F55" s="14" t="s">
         <v>451</v>
       </c>
-      <c r="E55" s="21" t="s">
+    </row>
+    <row r="56" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="21" t="s">
         <v>452</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="C56" s="14" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="21" t="s">
+      <c r="E56" s="22" t="s">
         <v>454</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="F56" s="23" t="s">
         <v>455</v>
       </c>
-      <c r="E56" s="22" t="s">
+    </row>
+    <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="C57" s="14" t="s">
         <v>456</v>
       </c>
-      <c r="F56" s="23" t="s">
+    </row>
+    <row r="58" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="21" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="57" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="21" t="s">
-        <v>336</v>
-      </c>
-      <c r="C57" s="14" t="s">
+      <c r="C58" s="14" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="21" t="s">
+    <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="21" t="s">
         <v>459</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C59" s="14" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="59" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="21" t="s">
+      <c r="E59" s="68" t="s">
+        <v>772</v>
+      </c>
+      <c r="F59" s="69"/>
+    </row>
+    <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="21" t="s">
         <v>461</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C60" s="14" t="s">
         <v>462</v>
-      </c>
-      <c r="E59" s="68" t="s">
-        <v>774</v>
-      </c>
-      <c r="F59" s="69"/>
-    </row>
-    <row r="60" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="21" t="s">
-        <v>463</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>464</v>
       </c>
       <c r="E60" s="46" t="s">
         <v>29</v>
@@ -7281,375 +7363,375 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
+        <v>463</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="E61" s="46" t="s">
+        <v>231</v>
+      </c>
+      <c r="F61" s="47" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C62" s="14" t="s">
         <v>466</v>
       </c>
-      <c r="E61" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="F61" s="47" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="21" t="s">
+      <c r="E62" s="48" t="s">
+        <v>773</v>
+      </c>
+      <c r="F62" s="49" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="C63" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="E63" s="48" t="s">
+        <v>775</v>
+      </c>
+      <c r="F63" s="49" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="21" t="s">
         <v>468</v>
       </c>
-      <c r="E62" s="48" t="s">
-        <v>775</v>
-      </c>
-      <c r="F62" s="49" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="C63" s="14" t="s">
+      <c r="C64" s="14" t="s">
         <v>469</v>
       </c>
-      <c r="E63" s="48" t="s">
+      <c r="E64" s="48" t="s">
+        <v>470</v>
+      </c>
+      <c r="F64" s="49" t="s">
         <v>777</v>
-      </c>
-      <c r="F63" s="49" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="21" t="s">
-        <v>470</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>471</v>
-      </c>
-      <c r="E64" s="48" t="s">
-        <v>472</v>
-      </c>
-      <c r="F64" s="49" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="21" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E65" s="48" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F65" s="49" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E66" s="48" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F66" s="49" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E67" s="48" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F67" s="49" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E68" s="48" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="F68" s="49" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E69" s="48" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="F69" s="49" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E70" s="48" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="F70" s="49" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E71" s="48" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F71" s="49" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="21" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E72" s="48" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F72" s="49" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="21" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E73" s="48" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F73" s="49" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="21" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E74" s="50" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="F74" s="51" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="21" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="21" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="21" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="21" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="21" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="21" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="21" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="21" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="21" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="21" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="21" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="21" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="21" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="21" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="21" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="22" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C95" s="23" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="24" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C99" s="25"/>
     </row>
@@ -7663,328 +7745,328 @@
     </row>
     <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="21" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="21" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="21" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="21" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="21" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="21" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="21" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="21" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="21" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="21" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="21" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="21" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="21" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="21" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="21" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="21" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="21" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="21" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="21" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="21" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="21" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="21" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="21" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="21" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="21" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="21" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="21" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="21" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="21" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="21" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="21" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="21" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="21" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="21" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="21" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="21" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="22" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C140" s="23" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="66" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C143" s="67"/>
     </row>
@@ -7998,575 +8080,575 @@
     </row>
     <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="10" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="10" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="10" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="10" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="150" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="10" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="151" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="10" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="152" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="10" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="153" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="10" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="154" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="10" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="155" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="10" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C155" s="11" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="156" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="10" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C156" s="11" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="157" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="10" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="158" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="10" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C158" s="11" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="159" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="10" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C159" s="11" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="160" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="10" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C160" s="11" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="161" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="10" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="162" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="10" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C162" s="11" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="163" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="10" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C163" s="11" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="164" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="10" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C164" s="11" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="165" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="10" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C165" s="11" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="166" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="10" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C166" s="11" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="167" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="10" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C167" s="11" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="168" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="10" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C168" s="11" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="169" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="10" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C169" s="11" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="170" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="10" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C170" s="11" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="171" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="10" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C171" s="11" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="172" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="10" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C172" s="11" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="173" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="10" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="174" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="10" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C174" s="11" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="10" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C175" s="11" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="10" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C176" s="11" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="177" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="10" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C177" s="11" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="178" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="10" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C178" s="11" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="179" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="10" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C179" s="11" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="180" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="10" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C180" s="11" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="181" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="10" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C181" s="11" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="182" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="10" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C182" s="11" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="183" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="10" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="C183" s="11" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="184" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="10" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C184" s="11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="185" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="10" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C185" s="11" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="186" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="10" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C186" s="11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="187" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="10" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C187" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="188" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="10" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C188" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="189" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="10" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C189" s="11" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="190" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="10" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C190" s="11" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="191" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="10" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C191" s="11" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="192" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="10" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C192" s="11" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="193" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C193" s="11" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="194" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="10" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C194" s="11" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="195" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="10" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C195" s="11" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="196" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="10" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C196" s="11" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="197" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="10" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C197" s="11" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="198" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="10" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C198" s="11" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="199" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="10" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C199" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="200" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="10" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C200" s="11" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="201" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="10" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C201" s="11" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="202" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C202" s="11" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="203" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="10" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C203" s="11" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="204" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="10" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C204" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="205" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="10" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C205" s="11" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="206" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="10" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C206" s="11" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="207" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="10" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C207" s="11" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="208" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="10" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C208" s="11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="209" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="10" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C209" s="11" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="210" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="10" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C210" s="11" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="211" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="10" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C211" s="11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="212" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="10" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C212" s="11" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="213" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="10" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C213" s="11" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="214" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="10" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C214" s="11" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="215" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="10" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C215" s="11" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="216" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="B143:C143"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I13:J13"/>
@@ -8575,6 +8657,7 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E59:F59"/>
     <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
EPBDS-6456 Turn on setting: Auto Type Discovery for spreadsheet tables
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -3128,7 +3128,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3236,14 +3236,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3286,6 +3286,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="33">
@@ -3767,16 +3770,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3812,31 +3815,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3890,13 +3893,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3905,13 +3908,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3920,29 +3923,34 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3952,11 +3960,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3972,8 +3975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK64"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4039,18 +4042,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4090,35 +4093,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -5919,8 +5922,9 @@
       <c r="M50" s="5" t="s">
         <v>755</v>
       </c>
-      <c r="N50" s="5" t="b">
-        <v>0</v>
+      <c r="N50" s="7" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
@@ -5932,6 +5936,9 @@
       <c r="T50" s="5" t="s">
         <v>756</v>
       </c>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N51" s="70"/>
     </row>
     <row r="55" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
@@ -6337,7 +6344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
       <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
EPBDS-5148 Support parallel execution for array parameter calls. Added "parallel" property.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="815">
   <si>
     <t>Display Name</t>
   </si>
@@ -2323,9 +2323,6 @@
     <t xml:space="preserve"> XLS_SPREADSHEET, XLS_PROPERTIES</t>
   </si>
   <si>
-    <t>Controls new Spreadsheet Auto Type Discovery feature. By default = false (old behaviour)</t>
-  </si>
-  <si>
     <t>Origin</t>
   </si>
   <si>
@@ -2489,6 +2486,18 @@
   </si>
   <si>
     <t>On/Off validation mode for the rule table</t>
+  </si>
+  <si>
+    <t>parallel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controls new Spreadsheet Auto Type Discovery feature. </t>
+  </si>
+  <si>
+    <t>Controls Parallel execution feature. By default = false.</t>
+  </si>
+  <si>
+    <t>Cuncurrent Execution</t>
   </si>
 </sst>
 </file>
@@ -3233,17 +3242,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3286,9 +3298,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="33">
@@ -3740,217 +3749,212 @@
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3960,6 +3964,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3973,10 +3982,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK64"/>
+  <dimension ref="A1:AMK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,7 +4002,7 @@
     <col min="10" max="10" width="22.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="19.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="39.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" style="1"/>
     <col min="15" max="15" width="20.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="8.85546875" style="1"/>
@@ -4008,154 +4017,154 @@
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -4167,27 +4176,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="58"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -4865,10 +4874,10 @@
     </row>
     <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>58</v>
@@ -4877,7 +4886,7 @@
         <v>138</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>78</v>
@@ -4896,7 +4905,7 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -4905,15 +4914,15 @@
         <v>84</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>58</v>
@@ -4922,7 +4931,7 @@
         <v>138</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>78</v>
@@ -4941,7 +4950,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
@@ -4950,7 +4959,7 @@
         <v>84</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5180,10 +5189,10 @@
     </row>
     <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>757</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>758</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>58</v>
@@ -5207,11 +5216,11 @@
         <v>58</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -5220,7 +5229,7 @@
         <v>84</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5521,7 +5530,7 @@
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
@@ -5530,7 +5539,7 @@
         <v>84</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5934,90 +5943,136 @@
         <v>84</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="N51" s="70"/>
-    </row>
-    <row r="55" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="N51" s="7" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="T51" s="5" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N52" s="52"/>
+    </row>
+    <row r="56" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5" t="s">
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H55" s="5" t="s">
+      <c r="F56" s="5"/>
+      <c r="G56" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H56" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5" t="s">
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
-      <c r="R55" s="5"/>
-      <c r="S55" s="5" t="s">
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="T55" s="5" t="s">
+      <c r="T56" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="57" t="s">
-        <v>210</v>
-      </c>
-      <c r="C59" s="57"/>
     </row>
     <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="C60" s="58"/>
+    </row>
+    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="59" t="s">
         <v>211</v>
       </c>
-      <c r="C60" s="58"/>
-    </row>
-    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="58" t="s">
-        <v>212</v>
-      </c>
-      <c r="C61" s="58"/>
+      <c r="C61" s="59"/>
     </row>
     <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" s="59"/>
+    </row>
+    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="C62" s="59"/>
-    </row>
-    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="59" t="s">
+      <c r="C63" s="60"/>
+    </row>
+    <row r="64" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="C63" s="59"/>
-    </row>
-    <row r="64" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="56" t="s">
-        <v>762</v>
-      </c>
-      <c r="C64" s="56"/>
+      <c r="C64" s="60"/>
+    </row>
+    <row r="65" spans="2:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="57" t="s">
+        <v>761</v>
+      </c>
+      <c r="C65" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C3:L3"/>
@@ -6028,11 +6083,11 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
-    <mergeCell ref="B59:C59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B61:C61"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -6055,16 +6110,16 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="61" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="62" t="s">
         <v>216</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -6075,7 +6130,7 @@
       <c r="F6" s="17"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="61"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="17" t="s">
         <v>218</v>
       </c>
@@ -6084,7 +6139,7 @@
       <c r="F7" s="17"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="61"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="17" t="s">
         <v>219</v>
       </c>
@@ -6093,7 +6148,7 @@
       <c r="F8" s="17"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="61"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="17" t="s">
         <v>220</v>
       </c>
@@ -6102,13 +6157,13 @@
       <c r="F9" s="17"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="61"/>
-      <c r="C10" s="62" t="s">
+      <c r="B10" s="62"/>
+      <c r="C10" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6143,12 +6198,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="66"/>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="30" t="s">
@@ -6300,30 +6355,30 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="39" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="E14" s="40" t="s">
         <v>767</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="43" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C15" s="44" t="s">
         <v>203</v>
       </c>
       <c r="D15" s="44" t="s">
+        <v>769</v>
+      </c>
+      <c r="E15" s="45" t="s">
         <v>770</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>771</v>
       </c>
     </row>
   </sheetData>
@@ -6344,7 +6399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J216"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
       <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
@@ -6359,18 +6414,18 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="69" t="s">
         <v>228</v>
       </c>
-      <c r="C2" s="69"/>
+      <c r="C2" s="70"/>
       <c r="E2" s="24" t="s">
         <v>229</v>
       </c>
       <c r="F2" s="25"/>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="69" t="s">
         <v>230</v>
       </c>
-      <c r="J2" s="69"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
@@ -6561,10 +6616,10 @@
       <c r="F13" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="I13" s="68" t="s">
+      <c r="I13" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="J13" s="69"/>
+      <c r="J13" s="70"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
@@ -6747,10 +6802,10 @@
       <c r="F23" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="I23" s="68" t="s">
+      <c r="I23" s="69" t="s">
         <v>323</v>
       </c>
-      <c r="J23" s="69"/>
+      <c r="J23" s="70"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
@@ -6907,10 +6962,10 @@
       <c r="F32" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="I32" s="68" t="s">
-        <v>763</v>
-      </c>
-      <c r="J32" s="69"/>
+      <c r="I32" s="69" t="s">
+        <v>762</v>
+      </c>
+      <c r="J32" s="70"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="21" t="s">
@@ -6966,10 +7021,10 @@
         <v>375</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6986,10 +7041,10 @@
         <v>379</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7033,10 +7088,10 @@
       <c r="F39" s="14" t="s">
         <v>391</v>
       </c>
-      <c r="I39" s="68" t="s">
-        <v>796</v>
-      </c>
-      <c r="J39" s="69"/>
+      <c r="I39" s="69" t="s">
+        <v>795</v>
+      </c>
+      <c r="J39" s="70"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
@@ -7092,10 +7147,10 @@
         <v>401</v>
       </c>
       <c r="I42" s="48" t="s">
+        <v>787</v>
+      </c>
+      <c r="J42" s="49" t="s">
         <v>788</v>
-      </c>
-      <c r="J42" s="49" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7112,10 +7167,10 @@
         <v>405</v>
       </c>
       <c r="I43" s="50" t="s">
+        <v>796</v>
+      </c>
+      <c r="J43" s="51" t="s">
         <v>797</v>
-      </c>
-      <c r="J43" s="51" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7159,10 +7214,10 @@
       <c r="F46" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="I46" s="68" t="s">
-        <v>806</v>
-      </c>
-      <c r="J46" s="69"/>
+      <c r="I46" s="69" t="s">
+        <v>805</v>
+      </c>
+      <c r="J46" s="70"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
@@ -7218,10 +7273,10 @@
         <v>428</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7238,10 +7293,10 @@
         <v>432</v>
       </c>
       <c r="I50" s="28" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="J50" s="29" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7351,10 +7406,10 @@
       <c r="C59" s="14" t="s">
         <v>460</v>
       </c>
-      <c r="E59" s="68" t="s">
-        <v>772</v>
-      </c>
-      <c r="F59" s="69"/>
+      <c r="E59" s="69" t="s">
+        <v>771</v>
+      </c>
+      <c r="F59" s="70"/>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="21" t="s">
@@ -7392,10 +7447,10 @@
         <v>466</v>
       </c>
       <c r="E62" s="48" t="s">
+        <v>772</v>
+      </c>
+      <c r="F62" s="49" t="s">
         <v>773</v>
-      </c>
-      <c r="F62" s="49" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7406,10 +7461,10 @@
         <v>467</v>
       </c>
       <c r="E63" s="48" t="s">
+        <v>774</v>
+      </c>
+      <c r="F63" s="49" t="s">
         <v>775</v>
-      </c>
-      <c r="F63" s="49" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7423,7 +7478,7 @@
         <v>470</v>
       </c>
       <c r="F64" s="49" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7434,10 +7489,10 @@
         <v>471</v>
       </c>
       <c r="E65" s="48" t="s">
+        <v>777</v>
+      </c>
+      <c r="F65" s="49" t="s">
         <v>778</v>
-      </c>
-      <c r="F65" s="49" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7448,10 +7503,10 @@
         <v>473</v>
       </c>
       <c r="E66" s="48" t="s">
+        <v>779</v>
+      </c>
+      <c r="F66" s="49" t="s">
         <v>780</v>
-      </c>
-      <c r="F66" s="49" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7462,10 +7517,10 @@
         <v>475</v>
       </c>
       <c r="E67" s="48" t="s">
+        <v>781</v>
+      </c>
+      <c r="F67" s="49" t="s">
         <v>782</v>
-      </c>
-      <c r="F67" s="49" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7476,10 +7531,10 @@
         <v>477</v>
       </c>
       <c r="E68" s="48" t="s">
+        <v>783</v>
+      </c>
+      <c r="F68" s="49" t="s">
         <v>784</v>
-      </c>
-      <c r="F68" s="49" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7490,10 +7545,10 @@
         <v>408</v>
       </c>
       <c r="E69" s="48" t="s">
+        <v>785</v>
+      </c>
+      <c r="F69" s="49" t="s">
         <v>786</v>
-      </c>
-      <c r="F69" s="49" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7504,10 +7559,10 @@
         <v>479</v>
       </c>
       <c r="E70" s="48" t="s">
+        <v>787</v>
+      </c>
+      <c r="F70" s="49" t="s">
         <v>788</v>
-      </c>
-      <c r="F70" s="49" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7521,7 +7576,7 @@
         <v>490</v>
       </c>
       <c r="F71" s="49" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7535,7 +7590,7 @@
         <v>457</v>
       </c>
       <c r="F72" s="49" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7546,10 +7601,10 @@
         <v>485</v>
       </c>
       <c r="E73" s="48" t="s">
+        <v>791</v>
+      </c>
+      <c r="F73" s="49" t="s">
         <v>792</v>
-      </c>
-      <c r="F73" s="49" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7560,10 +7615,10 @@
         <v>487</v>
       </c>
       <c r="E74" s="50" t="s">
+        <v>793</v>
+      </c>
+      <c r="F74" s="51" t="s">
         <v>794</v>
-      </c>
-      <c r="F74" s="51" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8072,10 +8127,10 @@
     </row>
     <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="66" t="s">
+      <c r="B143" s="67" t="s">
         <v>606</v>
       </c>
-      <c r="C143" s="67"/>
+      <c r="C143" s="68"/>
     </row>
     <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="8" t="s">

</xml_diff>

<commit_message>
"Nature" business dimensional property was added.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="820">
   <si>
     <t>Display Name</t>
   </si>
@@ -2498,6 +2498,21 @@
   </si>
   <si>
     <t>Cuncurrent Execution</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>nature</t>
+  </si>
+  <si>
+    <t>eq(nature)</t>
+  </si>
+  <si>
+    <t>list: Defined by method getNature()</t>
+  </si>
+  <si>
+    <t>Nature (type) for which this table works and should be used</t>
   </si>
 </sst>
 </file>
@@ -3137,7 +3152,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3242,9 +3257,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3749,207 +3761,207 @@
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
@@ -3985,7 +3997,7 @@
   <dimension ref="A1:AMK65"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4017,154 +4029,154 @@
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -4176,27 +4188,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="58"/>
-      <c r="S11" s="58"/>
-      <c r="T11" s="58"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -5992,8 +6004,50 @@
         <v>813</v>
       </c>
     </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="N52" s="52"/>
+    <row r="52" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5" t="s">
+        <v>818</v>
+      </c>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="T52" s="5" t="s">
+        <v>819</v>
+      </c>
     </row>
     <row r="56" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
@@ -6035,40 +6089,40 @@
       </c>
     </row>
     <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="58" t="s">
+      <c r="B60" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="C60" s="58"/>
+      <c r="C60" s="57"/>
     </row>
     <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="59" t="s">
+      <c r="B61" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="C61" s="59"/>
+      <c r="C61" s="58"/>
     </row>
     <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="59" t="s">
+      <c r="B62" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="C62" s="59"/>
+      <c r="C62" s="58"/>
     </row>
     <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="60" t="s">
+      <c r="B63" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="C63" s="60"/>
+      <c r="C63" s="59"/>
     </row>
     <row r="64" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="60" t="s">
+      <c r="B64" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="C64" s="60"/>
+      <c r="C64" s="59"/>
     </row>
     <row r="65" spans="2:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="57" t="s">
+      <c r="B65" s="56" t="s">
         <v>761</v>
       </c>
-      <c r="C65" s="57"/>
+      <c r="C65" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -6110,16 +6164,16 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="60" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="61" t="s">
         <v>216</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -6130,7 +6184,7 @@
       <c r="F6" s="17"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="62"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="17" t="s">
         <v>218</v>
       </c>
@@ -6139,7 +6193,7 @@
       <c r="F7" s="17"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="62"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="17" t="s">
         <v>219</v>
       </c>
@@ -6148,7 +6202,7 @@
       <c r="F8" s="17"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="62"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="17" t="s">
         <v>220</v>
       </c>
@@ -6157,13 +6211,13 @@
       <c r="F9" s="17"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="62"/>
-      <c r="C10" s="63" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="62" t="s">
         <v>221</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6183,10 +6237,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6198,12 +6252,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="63" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="30" t="s">
@@ -6271,113 +6325,125 @@
     </row>
     <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="39" t="s">
-        <v>224</v>
+        <v>816</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>160</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="40" t="s">
-        <v>225</v>
+        <v>815</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="39" t="s">
-        <v>143</v>
+        <v>224</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="39" t="s">
-        <v>227</v>
+        <v>143</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>136</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
-        <v>148</v>
+      <c r="B11" s="39" t="s">
+        <v>227</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>150</v>
+      <c r="D11" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
-        <v>163</v>
+      <c r="B13" s="41" t="s">
+        <v>153</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="39" t="s">
-        <v>765</v>
+        <v>163</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="39" t="s">
+        <v>765</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>766</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E15" s="40" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="43" t="s">
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="43" t="s">
         <v>768</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C16" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D16" s="44" t="s">
         <v>769</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E16" s="45" t="s">
         <v>770</v>
       </c>
     </row>
@@ -6399,7 +6465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
       <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
@@ -6414,18 +6480,18 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="68" t="s">
         <v>228</v>
       </c>
-      <c r="C2" s="70"/>
+      <c r="C2" s="69"/>
       <c r="E2" s="24" t="s">
         <v>229</v>
       </c>
       <c r="F2" s="25"/>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="68" t="s">
         <v>230</v>
       </c>
-      <c r="J2" s="70"/>
+      <c r="J2" s="69"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
@@ -6616,10 +6682,10 @@
       <c r="F13" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="I13" s="69" t="s">
+      <c r="I13" s="68" t="s">
         <v>275</v>
       </c>
-      <c r="J13" s="70"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
@@ -6802,10 +6868,10 @@
       <c r="F23" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="I23" s="69" t="s">
+      <c r="I23" s="68" t="s">
         <v>323</v>
       </c>
-      <c r="J23" s="70"/>
+      <c r="J23" s="69"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
@@ -6962,10 +7028,10 @@
       <c r="F32" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="I32" s="69" t="s">
+      <c r="I32" s="68" t="s">
         <v>762</v>
       </c>
-      <c r="J32" s="70"/>
+      <c r="J32" s="69"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="21" t="s">
@@ -7088,10 +7154,10 @@
       <c r="F39" s="14" t="s">
         <v>391</v>
       </c>
-      <c r="I39" s="69" t="s">
+      <c r="I39" s="68" t="s">
         <v>795</v>
       </c>
-      <c r="J39" s="70"/>
+      <c r="J39" s="69"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
@@ -7214,10 +7280,10 @@
       <c r="F46" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="I46" s="69" t="s">
+      <c r="I46" s="68" t="s">
         <v>805</v>
       </c>
-      <c r="J46" s="70"/>
+      <c r="J46" s="69"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
@@ -7406,10 +7472,10 @@
       <c r="C59" s="14" t="s">
         <v>460</v>
       </c>
-      <c r="E59" s="69" t="s">
+      <c r="E59" s="68" t="s">
         <v>771</v>
       </c>
-      <c r="F59" s="70"/>
+      <c r="F59" s="69"/>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="21" t="s">
@@ -8127,10 +8193,10 @@
     </row>
     <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="67" t="s">
+      <c r="B143" s="66" t="s">
         <v>606</v>
       </c>
-      <c r="C143" s="68"/>
+      <c r="C143" s="67"/>
     </row>
     <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="8" t="s">

</xml_diff>

<commit_message>
EPBDS-7439 Missed Table inheritance level for Region property
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{637E33FB-A78B-4D78-920F-4228202C56FA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="819">
   <si>
     <t>Display Name</t>
   </si>
@@ -2511,14 +2512,11 @@
   <si>
     <t>XLS_SPREADSHEET, XLS_PROPERTIES</t>
   </si>
-  <si>
-    <t>MODULE, CATEGORY</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3260,14 +3258,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3748,7 +3746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
@@ -3791,16 +3789,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3836,31 +3834,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3914,13 +3912,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3929,13 +3927,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3944,29 +3942,34 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3976,11 +3979,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3993,10 +3991,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -4063,18 +4061,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4114,35 +4112,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -5074,7 +5072,7 @@
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5" t="s">
-        <v>819</v>
+        <v>84</v>
       </c>
       <c r="T29" s="5" t="s">
         <v>166</v>
@@ -6186,7 +6184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
@@ -6268,7 +6266,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
@@ -6494,7 +6492,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:J216"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">

</xml_diff>

<commit_message>
EPBDS-7341 Only DT, SPREADSHEET, XLS_TBASIC, XLS_COLUMN_MATCH, XLS_METHOD, XLS_PROPERTIES must support business dimensional properties. Test added.
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{637E33FB-A78B-4D78-920F-4228202C56FA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{887246B2-2290-4C23-B069-2F1FE049C957}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3258,14 +3258,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3789,16 +3789,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3834,31 +3834,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3912,13 +3912,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3927,13 +3927,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3942,34 +3942,29 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3979,6 +3974,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3995,7 +3995,7 @@
   <dimension ref="A1:AMK65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="M14" sqref="M14:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,18 +4061,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4112,35 +4112,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -6063,7 +6063,7 @@
         <v>68</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>120</v>
+        <v>756</v>
       </c>
       <c r="N52" s="5"/>
       <c r="O52" s="5" t="s">
@@ -6270,7 +6270,7 @@
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B2" sqref="B2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6495,7 +6495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:J216"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
       <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
EPBDS-7442 Remove unused Custom1, Custom2 and Transactional properties.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{887246B2-2290-4C23-B069-2F1FE049C957}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EE982BF2-93E2-4BFB-910D-10F0E77145EF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="813">
   <si>
     <t>Display Name</t>
   </si>
@@ -630,24 +630,6 @@
   </si>
   <si>
     <t>The name of the package for datatype generation</t>
-  </si>
-  <si>
-    <t>Transaction Type</t>
-  </si>
-  <si>
-    <t>transaction</t>
-  </si>
-  <si>
-    <t>Custom1</t>
-  </si>
-  <si>
-    <t>custom1</t>
-  </si>
-  <si>
-    <t>Custom2</t>
-  </si>
-  <si>
-    <t>custom2</t>
   </si>
   <si>
     <t>Cacheable</t>
@@ -3258,14 +3240,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3789,16 +3771,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3834,31 +3816,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3912,13 +3894,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3927,13 +3909,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3942,29 +3924,34 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3974,11 +3961,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3992,10 +3974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK65"/>
+  <dimension ref="A1:AMK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:M21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,18 +4043,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4112,35 +4094,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -4725,7 +4707,7 @@
         <v>58</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
@@ -4774,7 +4756,7 @@
         <v>58</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5" t="s">
@@ -4823,7 +4805,7 @@
         <v>58</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N24" s="5"/>
       <c r="O24" s="5" t="s">
@@ -4872,7 +4854,7 @@
         <v>58</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5" t="s">
@@ -4892,10 +4874,10 @@
     </row>
     <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>58</v>
@@ -4904,7 +4886,7 @@
         <v>138</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>78</v>
@@ -4921,11 +4903,11 @@
         <v>58</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -4934,15 +4916,15 @@
         <v>84</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>58</v>
@@ -4951,7 +4933,7 @@
         <v>138</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>78</v>
@@ -4968,11 +4950,11 @@
         <v>58</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
@@ -4981,7 +4963,7 @@
         <v>84</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5015,7 +4997,7 @@
         <v>68</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="5" t="s">
@@ -5062,7 +5044,7 @@
         <v>68</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N29" s="5"/>
       <c r="O29" s="5" t="s">
@@ -5109,7 +5091,7 @@
         <v>68</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5" t="s">
@@ -5156,7 +5138,7 @@
         <v>68</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="5" t="s">
@@ -5203,7 +5185,7 @@
         <v>68</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="5" t="s">
@@ -5221,16 +5203,16 @@
     </row>
     <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
@@ -5248,11 +5230,11 @@
         <v>58</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -5261,7 +5243,7 @@
         <v>84</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
     </row>
     <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5295,7 +5277,7 @@
         <v>68</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N34" s="5"/>
       <c r="O34" s="5" t="s">
@@ -5342,7 +5324,7 @@
         <v>68</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N35" s="5"/>
       <c r="O35" s="5" t="s">
@@ -5544,7 +5526,7 @@
         <v>58</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5" t="s">
@@ -5566,7 +5548,7 @@
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
@@ -5575,7 +5557,7 @@
         <v>84</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5704,16 +5686,18 @@
         <v>191</v>
       </c>
     </row>
-    <row r="44" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>192</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E44" s="5" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5" t="s">
@@ -5728,18 +5712,20 @@
         <v>58</v>
       </c>
       <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
+      <c r="M44" s="5" t="s">
+        <v>750</v>
+      </c>
       <c r="N44" s="5"/>
-      <c r="O44" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="O44" s="5"/>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T44" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="T44" s="5" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="45" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
@@ -5748,9 +5734,11 @@
       <c r="C45" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E45" s="5" t="s">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5" t="s">
@@ -5765,29 +5753,33 @@
         <v>58</v>
       </c>
       <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
+      <c r="M45" s="5" t="s">
+        <v>750</v>
+      </c>
       <c r="N45" s="5"/>
       <c r="O45" s="5" t="s">
-        <v>58</v>
+        <v>197</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T45" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="T45" s="5" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="46" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>196</v>
+        <v>742</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>197</v>
+        <v>741</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5" t="s">
@@ -5802,25 +5794,29 @@
         <v>58</v>
       </c>
       <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
+      <c r="M46" s="5" t="s">
+        <v>745</v>
+      </c>
       <c r="N46" s="5"/>
       <c r="O46" s="5" t="s">
-        <v>58</v>
+        <v>744</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
       <c r="S46" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T46" s="5"/>
-    </row>
-    <row r="47" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="T46" s="5" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>198</v>
+        <v>746</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>199</v>
+        <v>747</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>58</v>
@@ -5840,11 +5836,16 @@
       <c r="K47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L47" s="5"/>
+      <c r="L47" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="M47" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="N47" s="5"/>
+        <v>812</v>
+      </c>
+      <c r="N47" s="7" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
@@ -5853,21 +5854,21 @@
         <v>84</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>746</v>
+        <v>804</v>
       </c>
     </row>
     <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>200</v>
+        <v>806</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>201</v>
+        <v>803</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5" t="s">
@@ -5881,14 +5882,17 @@
       <c r="K48" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L48" s="5"/>
+      <c r="L48" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="M48" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5" t="s">
-        <v>203</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="N48" s="7" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O48" s="5"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
       <c r="R48" s="5"/>
@@ -5896,39 +5900,45 @@
         <v>84</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>748</v>
+        <v>807</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>747</v>
-      </c>
-      <c r="D49" s="5"/>
+        <v>808</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E49" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F49" s="5"/>
+      <c r="F49" s="5" t="s">
+        <v>809</v>
+      </c>
       <c r="G49" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L49" s="5"/>
+      <c r="L49" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="M49" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5" t="s">
-        <v>750</v>
+        <v>810</v>
       </c>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
@@ -5937,226 +5947,87 @@
         <v>84</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="5" t="s">
-        <v>752</v>
-      </c>
-      <c r="C50" s="5" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="T53" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="C57" s="57"/>
+    </row>
+    <row r="58" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="C58" s="58"/>
+    </row>
+    <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="C59" s="58"/>
+    </row>
+    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="C60" s="59"/>
+    </row>
+    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="C61" s="59"/>
+    </row>
+    <row r="62" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="56" t="s">
         <v>753</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M50" s="5" t="s">
-        <v>818</v>
-      </c>
-      <c r="N50" s="7" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="T50" s="5" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="51" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
-        <v>812</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>809</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L51" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M51" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="N51" s="7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-      <c r="R51" s="5"/>
-      <c r="S51" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="T51" s="5" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="52" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="5" t="s">
-        <v>813</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>814</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>815</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5" t="s">
-        <v>816</v>
-      </c>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5"/>
-      <c r="S52" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="T52" s="5" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="56" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T56" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="57" t="s">
-        <v>209</v>
-      </c>
-      <c r="C60" s="57"/>
-    </row>
-    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="58" t="s">
-        <v>210</v>
-      </c>
-      <c r="C61" s="58"/>
-    </row>
-    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="58" t="s">
-        <v>211</v>
-      </c>
-      <c r="C62" s="58"/>
-    </row>
-    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="C63" s="59"/>
-    </row>
-    <row r="64" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="C64" s="59"/>
-    </row>
-    <row r="65" spans="2:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="56" t="s">
-        <v>759</v>
-      </c>
-      <c r="C65" s="56"/>
+      <c r="C62" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C3:L3"/>
@@ -6167,11 +6038,11 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -6195,7 +6066,7 @@
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="60"/>
@@ -6204,10 +6075,10 @@
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -6216,7 +6087,7 @@
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
       <c r="C7" s="17" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -6225,7 +6096,7 @@
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="61"/>
       <c r="C8" s="17" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -6234,7 +6105,7 @@
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
       <c r="C9" s="17" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -6243,7 +6114,7 @@
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
       <c r="C10" s="62" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D10" s="62"/>
       <c r="E10" s="62"/>
@@ -6283,7 +6154,7 @@
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="63" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C2" s="64"/>
       <c r="D2" s="64"/>
@@ -6331,7 +6202,7 @@
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="39" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>79</v>
@@ -6355,28 +6226,28 @@
     </row>
     <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="39" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="40" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="39" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6384,21 +6255,21 @@
         <v>143</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="39" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>140</v>
@@ -6412,7 +6283,7 @@
         <v>148</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D12" s="34" t="s">
         <v>150</v>
@@ -6426,7 +6297,7 @@
         <v>153</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>155</v>
@@ -6440,7 +6311,7 @@
         <v>163</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>165</v>
@@ -6451,30 +6322,30 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="39" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="43" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="E16" s="45" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
     </row>
   </sheetData>
@@ -6511,15 +6382,15 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="68" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C2" s="69"/>
       <c r="E2" s="24" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F2" s="25"/>
       <c r="I2" s="68" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="J2" s="69"/>
     </row>
@@ -6545,190 +6416,190 @@
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="I13" s="68" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="J13" s="69"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>29</v>
@@ -6739,182 +6610,182 @@
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>117</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="21" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="I23" s="68" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="J23" s="69"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>29</v>
@@ -6925,156 +6796,156 @@
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="21" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="21" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="I28" s="28" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="I32" s="68" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="J32" s="69"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="21" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>29</v>
@@ -7085,122 +6956,122 @@
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="21" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="I34" s="26" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="21" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="21" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I39" s="68" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="J39" s="69"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="I40" s="46" t="s">
         <v>29</v>
@@ -7214,119 +7085,119 @@
         <v>117</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="I41" s="46" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="J41" s="47" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="21" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="I42" s="48" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="J42" s="49" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="21" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="I43" s="50" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="J43" s="51" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="21" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="21" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="I46" s="68" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="J46" s="69"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="I47" s="20" t="s">
         <v>29</v>
@@ -7337,182 +7208,182 @@
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="21" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="I48" s="26" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="21" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="21" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="I50" s="28" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="J50" s="29" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="21" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="21" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="21" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="21" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="21" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="56" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="21" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="21" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="21" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="21" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="E59" s="68" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="F59" s="69"/>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="21" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="E60" s="46" t="s">
         <v>29</v>
@@ -7523,373 +7394,373 @@
     </row>
     <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="E61" s="46" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F61" s="47" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="21" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="E62" s="48" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="F62" s="49" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
     </row>
     <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="21" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="E63" s="48" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="F63" s="49" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="21" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="E64" s="48" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="F64" s="49" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="21" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="E65" s="48" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="F65" s="49" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="E66" s="48" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="F66" s="49" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="E67" s="48" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="F67" s="49" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="E68" s="48" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="F68" s="49" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E69" s="48" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="F69" s="49" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
     </row>
     <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E70" s="48" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="F70" s="49" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
     </row>
     <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="E71" s="48" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="F71" s="49" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="21" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="E72" s="48" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="F72" s="49" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="21" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="E73" s="48" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="F73" s="49" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="21" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="E74" s="50" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="F74" s="51" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="21" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="21" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="21" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="21" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="21" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="21" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="21" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="21" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="21" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="21" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="21" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="21" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="21" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="21" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="21" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="21" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="22" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="C95" s="23" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="24" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="C99" s="25"/>
     </row>
@@ -7903,328 +7774,328 @@
     </row>
     <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="20" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="21" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="21" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="21" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
     </row>
     <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="21" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="21" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="21" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="21" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="21" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="21" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
     </row>
     <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="21" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="21" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="21" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
     </row>
     <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="21" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="21" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
     </row>
     <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="21" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
     <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="21" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="21" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="21" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
     </row>
     <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="21" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="21" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="21" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
     </row>
     <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="21" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
     </row>
     <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="21" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="21" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
     </row>
     <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="21" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="21" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="21" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="21" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="21" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
     </row>
     <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="21" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="21" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="21" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
     </row>
     <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="21" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
     </row>
     <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="21" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="21" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
     </row>
     <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="21" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
     </row>
     <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="22" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C140" s="23" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="66" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="C143" s="67"/>
     </row>
@@ -8238,570 +8109,570 @@
     </row>
     <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="10" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
     </row>
     <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="10" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
     </row>
     <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="10" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
     </row>
     <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="10" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="150" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="10" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
     <row r="151" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="10" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
     </row>
     <row r="152" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="10" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
     <row r="153" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="10" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="154" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="10" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
     </row>
     <row r="155" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="10" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="C155" s="11" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
     </row>
     <row r="156" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="10" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="C156" s="11" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
     </row>
     <row r="157" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="10" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
     </row>
     <row r="158" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="10" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C158" s="11" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
     </row>
     <row r="159" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="10" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="C159" s="11" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="160" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="10" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C160" s="11" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="161" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="10" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="162" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="10" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="C162" s="11" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
     </row>
     <row r="163" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="10" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="C163" s="11" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
     </row>
     <row r="164" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="10" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="C164" s="11" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
     </row>
     <row r="165" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="10" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="C165" s="11" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
     </row>
     <row r="166" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="10" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="C166" s="11" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
     </row>
     <row r="167" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="10" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="C167" s="11" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="168" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="10" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="C168" s="11" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
     </row>
     <row r="169" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="10" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="C169" s="11" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
     </row>
     <row r="170" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="10" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="C170" s="11" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
     </row>
     <row r="171" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="10" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="C171" s="11" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
     </row>
     <row r="172" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="10" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="C172" s="11" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
     </row>
     <row r="173" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="10" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="174" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="10" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="C174" s="11" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
     </row>
     <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="10" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="C175" s="11" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="10" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="C176" s="11" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
     </row>
     <row r="177" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="10" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="C177" s="11" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="178" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="10" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="C178" s="11" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
     </row>
     <row r="179" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="10" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="C179" s="11" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
     </row>
     <row r="180" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="10" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="C180" s="11" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
     </row>
     <row r="181" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="10" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="C181" s="11" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
     </row>
     <row r="182" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="10" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="C182" s="11" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
     </row>
     <row r="183" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="10" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="C183" s="11" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
     </row>
     <row r="184" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="10" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="C184" s="11" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
     </row>
     <row r="185" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="10" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="C185" s="11" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
     </row>
     <row r="186" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="10" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="C186" s="11" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
     </row>
     <row r="187" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="10" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="C187" s="11" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
     </row>
     <row r="188" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="10" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="C188" s="11" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
     </row>
     <row r="189" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="10" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="C189" s="11" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
     </row>
     <row r="190" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="10" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="C190" s="11" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
     </row>
     <row r="191" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="10" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="C191" s="11" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
     </row>
     <row r="192" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="10" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="C192" s="11" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
     </row>
     <row r="193" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="10" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="C193" s="11" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
     </row>
     <row r="194" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="10" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
       <c r="C194" s="11" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
     </row>
     <row r="195" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="10" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="C195" s="11" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
     </row>
     <row r="196" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="10" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="C196" s="11" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
     </row>
     <row r="197" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="10" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="C197" s="11" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
     </row>
     <row r="198" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="10" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="C198" s="11" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
     </row>
     <row r="199" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="10" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="C199" s="11" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
     </row>
     <row r="200" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="10" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="C200" s="11" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
     </row>
     <row r="201" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="10" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="C201" s="11" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
     </row>
     <row r="202" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="10" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
       <c r="C202" s="11" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
     </row>
     <row r="203" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="10" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="C203" s="11" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
     </row>
     <row r="204" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="10" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="C204" s="11" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
     </row>
     <row r="205" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="10" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="C205" s="11" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
     </row>
     <row r="206" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="10" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="C206" s="11" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
     </row>
     <row r="207" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="10" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="C207" s="11" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
     </row>
     <row r="208" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="10" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="C208" s="11" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
     </row>
     <row r="209" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="10" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="C209" s="11" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
     </row>
     <row r="210" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="10" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="C210" s="11" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
     </row>
     <row r="211" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="10" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="C211" s="11" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
     </row>
     <row r="212" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="10" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="C212" s="11" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
     </row>
     <row r="213" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="10" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="C213" s="11" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
     </row>
     <row r="214" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="10" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="C214" s="11" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
     </row>
     <row r="215" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="10" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="C215" s="11" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
     </row>
     <row r="216" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
EPBDS-7638 Incorrect Property name - Cuncurrent execution
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EE982BF2-93E2-4BFB-910D-10F0E77145EF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DEB15F23-1281-4A96-90EE-EB3A34AB52DD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2471,12 +2471,6 @@
     <t xml:space="preserve">Controls new Spreadsheet Auto Type Discovery feature. </t>
   </si>
   <si>
-    <t>Controls Parallel execution feature. By default = false.</t>
-  </si>
-  <si>
-    <t>Cuncurrent Execution</t>
-  </si>
-  <si>
     <t>Nature</t>
   </si>
   <si>
@@ -2493,6 +2487,12 @@
   </si>
   <si>
     <t>XLS_SPREADSHEET, XLS_PROPERTIES</t>
+  </si>
+  <si>
+    <t>Controls parallel execution feature. By default = false.</t>
+  </si>
+  <si>
+    <t>Concurrent Execution</t>
   </si>
 </sst>
 </file>
@@ -3240,14 +3240,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3771,16 +3771,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3816,31 +3816,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3894,13 +3894,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3909,13 +3909,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3924,34 +3924,29 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3961,6 +3956,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3977,7 +3977,7 @@
   <dimension ref="A1:AMK62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4043,18 +4043,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4094,35 +4094,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -5840,7 +5840,7 @@
         <v>58</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="N47" s="7" t="b">
         <f>TRUE()</f>
@@ -5859,7 +5859,7 @@
     </row>
     <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>806</v>
+        <v>812</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>803</v>
@@ -5900,15 +5900,15 @@
         <v>84</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>805</v>
+        <v>811</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>58</v>
@@ -5917,7 +5917,7 @@
         <v>59</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>78</v>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
@@ -5947,7 +5947,7 @@
         <v>84</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="53" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6226,14 +6226,14 @@
     </row>
     <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="39" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="40" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
EPBDS-7891 Provide an ability to store array of Lobs and arrays of enums to the table properties, updated regex for emuns,
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openl-pub\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DEB15F23-1281-4A96-90EE-EB3A34AB52DD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -455,9 +454,6 @@
     <t>lob</t>
   </si>
   <si>
-    <t>eq(lob)</t>
-  </si>
-  <si>
     <t>list: Defined by method getLob()</t>
   </si>
   <si>
@@ -2493,12 +2489,15 @@
   </si>
   <si>
     <t>Concurrent Execution</t>
+  </si>
+  <si>
+    <t>contains(lob)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3240,14 +3239,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3484,23 +3483,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3536,23 +3518,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -3728,7 +3693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
@@ -3771,16 +3736,16 @@
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -3816,31 +3781,31 @@
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
@@ -3894,13 +3859,13 @@
       <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
@@ -3909,13 +3874,13 @@
       <c r="C13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
@@ -3924,29 +3889,34 @@
       <c r="C14" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3956,11 +3926,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3973,11 +3938,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4043,18 +4008,18 @@
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -4094,35 +4059,35 @@
       <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -4707,7 +4672,7 @@
         <v>58</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
@@ -4756,7 +4721,7 @@
         <v>58</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5" t="s">
@@ -4805,7 +4770,7 @@
         <v>58</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N24" s="5"/>
       <c r="O24" s="5" t="s">
@@ -4854,7 +4819,7 @@
         <v>58</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5" t="s">
@@ -4874,19 +4839,19 @@
     </row>
     <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>790</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>791</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>78</v>
@@ -4903,11 +4868,11 @@
         <v>58</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -4916,24 +4881,24 @@
         <v>84</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>792</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>793</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>78</v>
@@ -4950,11 +4915,11 @@
         <v>58</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
@@ -4963,24 +4928,24 @@
         <v>84</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>78</v>
@@ -4997,11 +4962,11 @@
         <v>68</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
@@ -5010,24 +4975,24 @@
         <v>84</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="D29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>78</v>
@@ -5044,11 +5009,11 @@
         <v>68</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N29" s="5"/>
       <c r="O29" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
@@ -5057,24 +5022,24 @@
         <v>84</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>78</v>
@@ -5091,11 +5056,11 @@
         <v>68</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
@@ -5104,24 +5069,24 @@
         <v>84</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>78</v>
@@ -5138,11 +5103,11 @@
         <v>68</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
@@ -5151,7 +5116,7 @@
         <v>84</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5165,10 +5130,10 @@
         <v>58</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>133</v>
+        <v>812</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>78</v>
@@ -5185,11 +5150,11 @@
         <v>68</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -5198,21 +5163,21 @@
         <v>84</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>748</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>749</v>
-      </c>
       <c r="D33" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
@@ -5230,11 +5195,11 @@
         <v>58</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -5243,24 +5208,24 @@
         <v>84</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E34" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>78</v>
@@ -5277,11 +5242,11 @@
         <v>68</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N34" s="5"/>
       <c r="O34" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
@@ -5290,24 +5255,24 @@
         <v>84</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>78</v>
@@ -5324,11 +5289,11 @@
         <v>68</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N35" s="5"/>
       <c r="O35" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
@@ -5337,15 +5302,15 @@
         <v>84</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
@@ -5356,7 +5321,7 @@
         <v>58</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -5369,7 +5334,7 @@
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
@@ -5378,26 +5343,26 @@
         <v>64</v>
       </c>
       <c r="T36" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>172</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5" t="s">
         <v>58</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
@@ -5413,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
@@ -5422,7 +5387,7 @@
         <v>64</v>
       </c>
       <c r="T37" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5526,7 +5491,7 @@
         <v>58</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5" t="s">
@@ -5548,7 +5513,7 @@
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
@@ -5557,19 +5522,19 @@
         <v>84</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5" t="s">
@@ -5599,15 +5564,15 @@
         <v>84</v>
       </c>
       <c r="T41" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
@@ -5627,28 +5592,28 @@
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N42" s="5"/>
       <c r="O42" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="T42" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="43" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
@@ -5668,36 +5633,36 @@
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="N43" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="N43" s="5" t="s">
+      <c r="O43" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="T43" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="T43" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="44" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>193</v>
-      </c>
       <c r="D44" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5" t="s">
@@ -5713,7 +5678,7 @@
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
@@ -5724,21 +5689,21 @@
         <v>84</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="45" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="D45" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5" t="s">
@@ -5754,11 +5719,11 @@
       </c>
       <c r="L45" s="5"/>
       <c r="M45" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N45" s="5"/>
       <c r="O45" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
@@ -5767,15 +5732,15 @@
         <v>84</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
@@ -5795,11 +5760,11 @@
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="N46" s="5"/>
       <c r="O46" s="5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
@@ -5808,21 +5773,21 @@
         <v>84</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="47" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>746</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>747</v>
-      </c>
       <c r="D47" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
@@ -5840,7 +5805,7 @@
         <v>58</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="N47" s="7" t="b">
         <f>TRUE()</f>
@@ -5854,21 +5819,21 @@
         <v>84</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5" t="s">
@@ -5886,7 +5851,7 @@
         <v>58</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N48" s="7" t="b">
         <f>FALSE()</f>
@@ -5900,15 +5865,15 @@
         <v>84</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>805</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>806</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>58</v>
@@ -5917,7 +5882,7 @@
         <v>59</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>78</v>
@@ -5934,11 +5899,11 @@
         <v>68</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
@@ -5947,19 +5912,19 @@
         <v>84</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="53" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5" t="s">
@@ -5975,7 +5940,7 @@
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
@@ -5986,42 +5951,42 @@
         <v>64</v>
       </c>
       <c r="T53" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="57" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C57" s="57"/>
     </row>
     <row r="58" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C58" s="58"/>
     </row>
     <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C59" s="58"/>
     </row>
     <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="59" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C60" s="59"/>
     </row>
     <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C61" s="59"/>
     </row>
     <row r="62" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="56" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C62" s="56"/>
     </row>
@@ -6055,7 +6020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
@@ -6066,7 +6031,7 @@
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="60"/>
@@ -6075,10 +6040,10 @@
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>209</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>210</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -6087,7 +6052,7 @@
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
       <c r="C7" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -6096,7 +6061,7 @@
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="61"/>
       <c r="C8" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -6105,7 +6070,7 @@
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
       <c r="C9" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -6114,7 +6079,7 @@
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
       <c r="C10" s="62" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D10" s="62"/>
       <c r="E10" s="62"/>
@@ -6137,11 +6102,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6154,7 +6119,7 @@
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="63" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2" s="64"/>
       <c r="D2" s="64"/>
@@ -6202,7 +6167,7 @@
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>79</v>
@@ -6226,126 +6191,126 @@
     </row>
     <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="39" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="40" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="40" t="s">
         <v>217</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="39" t="s">
+        <v>756</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="40" t="s">
         <v>758</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="43" t="s">
+        <v>759</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="44" t="s">
         <v>760</v>
       </c>
-      <c r="C16" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" s="44" t="s">
+      <c r="E16" s="45" t="s">
         <v>761</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>762</v>
       </c>
     </row>
   </sheetData>
@@ -6363,11 +6328,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J216"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView topLeftCell="A55" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6382,15 +6347,15 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="68" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C2" s="69"/>
       <c r="E2" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F2" s="25"/>
       <c r="I2" s="68" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J2" s="69"/>
     </row>
@@ -6416,190 +6381,190 @@
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>225</v>
-      </c>
       <c r="E4" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>225</v>
-      </c>
       <c r="I4" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="J4" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="E5" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="I5" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="J5" s="14" t="s">
         <v>229</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="E6" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="F6" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="I6" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="J6" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="E7" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="F7" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="I7" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="J7" s="14" t="s">
         <v>241</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="E8" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="F8" s="14" t="s">
+      <c r="I8" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="J8" s="23" t="s">
         <v>246</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="E9" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="F9" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="E10" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="14" t="s">
         <v>254</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="E11" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="F11" s="14" t="s">
         <v>258</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="E12" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="F12" s="14" t="s">
         <v>262</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="E13" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="I13" s="68" t="s">
         <v>267</v>
-      </c>
-      <c r="I13" s="68" t="s">
-        <v>268</v>
       </c>
       <c r="J13" s="69"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="E14" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="F14" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>272</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>29</v>
@@ -6610,182 +6575,182 @@
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="E15" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="F15" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>276</v>
-      </c>
       <c r="I15" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="J15" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="E16" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="F16" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="I16" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="J16" s="14" t="s">
         <v>281</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>117</v>
       </c>
       <c r="F17" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="I17" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="J17" s="14" t="s">
         <v>285</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="E18" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="F18" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="I18" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="J18" s="14" t="s">
         <v>291</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="E19" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="F19" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="I19" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="J19" s="14" t="s">
         <v>297</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="F20" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="I20" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="J20" s="23" t="s">
         <v>302</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="E21" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="F21" s="14" t="s">
         <v>306</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="E22" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="F22" s="14" t="s">
         <v>310</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="E23" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="F23" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="I23" s="68" t="s">
         <v>315</v>
-      </c>
-      <c r="I23" s="68" t="s">
-        <v>316</v>
       </c>
       <c r="J23" s="69"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="E24" s="21" t="s">
         <v>318</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="F24" s="14" t="s">
         <v>319</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>320</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>29</v>
@@ -6796,156 +6761,156 @@
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="E25" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="F25" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>324</v>
-      </c>
       <c r="I25" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="J25" s="13" t="s">
         <v>224</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="E26" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="F26" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="I26" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="J26" s="14" t="s">
         <v>329</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="E27" s="21" t="s">
         <v>332</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="F27" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="I27" s="27" t="s">
         <v>334</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="J27" s="15" t="s">
         <v>335</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="E28" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="F28" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="I28" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="J28" s="29" t="s">
         <v>341</v>
-      </c>
-      <c r="J28" s="29" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
+        <v>342</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="E29" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="F29" s="14" t="s">
         <v>345</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="E30" s="21" t="s">
         <v>348</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="F30" s="14" t="s">
         <v>349</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="E31" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="F31" s="14" t="s">
         <v>353</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="E32" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="F32" s="14" t="s">
         <v>356</v>
       </c>
-      <c r="E32" s="21" t="s">
-        <v>285</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>357</v>
-      </c>
       <c r="I32" s="68" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="J32" s="69"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C33" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="E33" s="21" t="s">
         <v>358</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="F33" s="14" t="s">
         <v>359</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>360</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>29</v>
@@ -6956,122 +6921,122 @@
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="E34" s="21" t="s">
         <v>362</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="F34" s="14" t="s">
         <v>363</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>364</v>
-      </c>
       <c r="I34" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="J34" s="13" t="s">
         <v>224</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="E35" s="21" t="s">
         <v>366</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="F35" s="14" t="s">
         <v>367</v>
       </c>
-      <c r="F35" s="14" t="s">
-        <v>368</v>
-      </c>
       <c r="I35" s="21" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="C36" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="E36" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="F36" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="F36" s="14" t="s">
-        <v>372</v>
-      </c>
       <c r="I36" s="22" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="C37" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="E37" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="F37" s="14" t="s">
         <v>375</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="E38" s="21" t="s">
         <v>378</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="F38" s="14" t="s">
         <v>379</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="E39" s="21" t="s">
         <v>382</v>
       </c>
-      <c r="E39" s="21" t="s">
+      <c r="F39" s="14" t="s">
         <v>383</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>384</v>
-      </c>
       <c r="I39" s="68" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J39" s="69"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C40" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="E40" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="F40" s="14" t="s">
         <v>386</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>387</v>
       </c>
       <c r="I40" s="46" t="s">
         <v>29</v>
@@ -7085,119 +7050,119 @@
         <v>117</v>
       </c>
       <c r="C41" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="E41" s="21" t="s">
         <v>388</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="F41" s="14" t="s">
         <v>389</v>
       </c>
-      <c r="F41" s="14" t="s">
-        <v>390</v>
-      </c>
       <c r="I41" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="J41" s="47" t="s">
         <v>224</v>
-      </c>
-      <c r="J41" s="47" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="21" t="s">
+        <v>390</v>
+      </c>
+      <c r="C42" s="14" t="s">
         <v>391</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="E42" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="F42" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="F42" s="14" t="s">
-        <v>394</v>
-      </c>
       <c r="I42" s="48" t="s">
+        <v>778</v>
+      </c>
+      <c r="J42" s="49" t="s">
         <v>779</v>
-      </c>
-      <c r="J42" s="49" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="E43" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="F43" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="F43" s="14" t="s">
-        <v>398</v>
-      </c>
       <c r="I43" s="50" t="s">
+        <v>787</v>
+      </c>
+      <c r="J43" s="51" t="s">
         <v>788</v>
-      </c>
-      <c r="J43" s="51" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C44" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="E44" s="21" t="s">
         <v>399</v>
       </c>
-      <c r="E44" s="21" t="s">
+      <c r="F44" s="14" t="s">
         <v>400</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="E45" s="21" t="s">
         <v>403</v>
       </c>
-      <c r="E45" s="21" t="s">
+      <c r="F45" s="14" t="s">
         <v>404</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>406</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="E46" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="F46" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="F46" s="14" t="s">
-        <v>409</v>
-      </c>
       <c r="I46" s="68" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="J46" s="69"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="C47" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="E47" s="21" t="s">
         <v>411</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="F47" s="14" t="s">
         <v>412</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>413</v>
       </c>
       <c r="I47" s="20" t="s">
         <v>29</v>
@@ -7208,182 +7173,182 @@
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="E48" s="21" t="s">
         <v>415</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="F48" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="F48" s="14" t="s">
-        <v>417</v>
-      </c>
       <c r="I48" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="J48" s="13" t="s">
         <v>224</v>
-      </c>
-      <c r="J48" s="13" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="C49" s="14" t="s">
         <v>418</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="E49" s="21" t="s">
         <v>419</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="F49" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="F49" s="14" t="s">
-        <v>421</v>
-      </c>
       <c r="I49" s="21" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="C50" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="E50" s="21" t="s">
         <v>423</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="F50" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="F50" s="14" t="s">
-        <v>425</v>
-      </c>
       <c r="I50" s="28" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="J50" s="29" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="C51" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="E51" s="21" t="s">
         <v>427</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="F51" s="14" t="s">
         <v>428</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>430</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="E52" s="21" t="s">
         <v>431</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="F52" s="14" t="s">
         <v>432</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="C53" s="14" t="s">
         <v>434</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="E53" s="21" t="s">
         <v>435</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="F53" s="14" t="s">
         <v>436</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="21" t="s">
+        <v>437</v>
+      </c>
+      <c r="C54" s="14" t="s">
         <v>438</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="E54" s="21" t="s">
         <v>439</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="F54" s="14" t="s">
         <v>440</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C55" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="E55" s="21" t="s">
         <v>442</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="F55" s="14" t="s">
         <v>443</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="56" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="21" t="s">
+        <v>444</v>
+      </c>
+      <c r="C56" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="E56" s="22" t="s">
         <v>446</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="F56" s="23" t="s">
         <v>447</v>
-      </c>
-      <c r="F56" s="23" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="21" t="s">
+        <v>449</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>450</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="C59" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="C59" s="14" t="s">
-        <v>453</v>
-      </c>
       <c r="E59" s="68" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F59" s="69"/>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="C60" s="14" t="s">
         <v>454</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>455</v>
       </c>
       <c r="E60" s="46" t="s">
         <v>29</v>
@@ -7394,373 +7359,373 @@
     </row>
     <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
+        <v>455</v>
+      </c>
+      <c r="C61" s="14" t="s">
         <v>456</v>
       </c>
-      <c r="C61" s="14" t="s">
-        <v>457</v>
-      </c>
       <c r="E61" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="F61" s="47" t="s">
         <v>224</v>
-      </c>
-      <c r="F61" s="47" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="21" t="s">
+        <v>457</v>
+      </c>
+      <c r="C62" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="C62" s="14" t="s">
-        <v>459</v>
-      </c>
       <c r="E62" s="48" t="s">
+        <v>763</v>
+      </c>
+      <c r="F62" s="49" t="s">
         <v>764</v>
-      </c>
-      <c r="F62" s="49" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E63" s="48" t="s">
+        <v>765</v>
+      </c>
+      <c r="F63" s="49" t="s">
         <v>766</v>
-      </c>
-      <c r="F63" s="49" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="C64" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="E64" s="48" t="s">
         <v>462</v>
       </c>
-      <c r="E64" s="48" t="s">
-        <v>463</v>
-      </c>
       <c r="F64" s="49" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="C65" s="14" t="s">
         <v>463</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>464</v>
-      </c>
       <c r="E65" s="48" t="s">
+        <v>768</v>
+      </c>
+      <c r="F65" s="49" t="s">
         <v>769</v>
-      </c>
-      <c r="F65" s="49" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="C66" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="C66" s="14" t="s">
-        <v>466</v>
-      </c>
       <c r="E66" s="48" t="s">
+        <v>770</v>
+      </c>
+      <c r="F66" s="49" t="s">
         <v>771</v>
-      </c>
-      <c r="F66" s="49" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="C67" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="C67" s="14" t="s">
-        <v>468</v>
-      </c>
       <c r="E67" s="48" t="s">
+        <v>772</v>
+      </c>
+      <c r="F67" s="49" t="s">
         <v>773</v>
-      </c>
-      <c r="F67" s="49" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="C68" s="14" t="s">
         <v>469</v>
       </c>
-      <c r="C68" s="14" t="s">
-        <v>470</v>
-      </c>
       <c r="E68" s="48" t="s">
+        <v>774</v>
+      </c>
+      <c r="F68" s="49" t="s">
         <v>775</v>
-      </c>
-      <c r="F68" s="49" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="C69" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="C69" s="14" t="s">
-        <v>401</v>
-      </c>
       <c r="E69" s="48" t="s">
+        <v>776</v>
+      </c>
+      <c r="F69" s="49" t="s">
         <v>777</v>
-      </c>
-      <c r="F69" s="49" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="C70" s="14" t="s">
         <v>471</v>
       </c>
-      <c r="C70" s="14" t="s">
-        <v>472</v>
-      </c>
       <c r="E70" s="48" t="s">
+        <v>778</v>
+      </c>
+      <c r="F70" s="49" t="s">
         <v>779</v>
-      </c>
-      <c r="F70" s="49" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
+        <v>472</v>
+      </c>
+      <c r="C71" s="14" t="s">
         <v>473</v>
       </c>
-      <c r="C71" s="14" t="s">
-        <v>474</v>
-      </c>
       <c r="E71" s="48" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F71" s="49" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="C72" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="C72" s="14" t="s">
-        <v>476</v>
-      </c>
       <c r="E72" s="48" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F72" s="49" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="21" t="s">
+        <v>476</v>
+      </c>
+      <c r="C73" s="14" t="s">
         <v>477</v>
       </c>
-      <c r="C73" s="14" t="s">
-        <v>478</v>
-      </c>
       <c r="E73" s="48" t="s">
+        <v>782</v>
+      </c>
+      <c r="F73" s="49" t="s">
         <v>783</v>
-      </c>
-      <c r="F73" s="49" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="21" t="s">
+        <v>478</v>
+      </c>
+      <c r="C74" s="14" t="s">
         <v>479</v>
       </c>
-      <c r="C74" s="14" t="s">
-        <v>480</v>
-      </c>
       <c r="E74" s="50" t="s">
+        <v>784</v>
+      </c>
+      <c r="F74" s="51" t="s">
         <v>785</v>
-      </c>
-      <c r="F74" s="51" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="21" t="s">
+        <v>480</v>
+      </c>
+      <c r="C75" s="14" t="s">
         <v>481</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
+        <v>482</v>
+      </c>
+      <c r="C76" s="14" t="s">
         <v>483</v>
-      </c>
-      <c r="C76" s="14" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
+        <v>484</v>
+      </c>
+      <c r="C77" s="14" t="s">
         <v>485</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="21" t="s">
+        <v>486</v>
+      </c>
+      <c r="C78" s="14" t="s">
         <v>487</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="21" t="s">
+        <v>488</v>
+      </c>
+      <c r="C79" s="14" t="s">
         <v>489</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="21" t="s">
+        <v>492</v>
+      </c>
+      <c r="C82" s="14" t="s">
         <v>493</v>
-      </c>
-      <c r="C82" s="14" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="21" t="s">
+        <v>494</v>
+      </c>
+      <c r="C83" s="14" t="s">
         <v>495</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="21" t="s">
+        <v>496</v>
+      </c>
+      <c r="C84" s="14" t="s">
         <v>497</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="21" t="s">
+        <v>498</v>
+      </c>
+      <c r="C85" s="14" t="s">
         <v>499</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="21" t="s">
+        <v>501</v>
+      </c>
+      <c r="C87" s="14" t="s">
         <v>502</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="21" t="s">
+        <v>503</v>
+      </c>
+      <c r="C88" s="14" t="s">
         <v>504</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="21" t="s">
+        <v>505</v>
+      </c>
+      <c r="C89" s="14" t="s">
         <v>506</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="21" t="s">
+        <v>507</v>
+      </c>
+      <c r="C90" s="14" t="s">
         <v>508</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
+        <v>509</v>
+      </c>
+      <c r="C91" s="14" t="s">
         <v>510</v>
-      </c>
-      <c r="C91" s="14" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
+        <v>511</v>
+      </c>
+      <c r="C92" s="14" t="s">
         <v>512</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="21" t="s">
+        <v>513</v>
+      </c>
+      <c r="C93" s="14" t="s">
         <v>514</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="21" t="s">
+        <v>515</v>
+      </c>
+      <c r="C94" s="14" t="s">
         <v>516</v>
-      </c>
-      <c r="C94" s="14" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="C95" s="23" t="s">
         <v>518</v>
-      </c>
-      <c r="C95" s="23" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="24" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C99" s="25"/>
     </row>
@@ -7774,328 +7739,328 @@
     </row>
     <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="C101" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="C101" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="21" t="s">
+        <v>520</v>
+      </c>
+      <c r="C102" s="14" t="s">
         <v>521</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="C103" s="14" t="s">
         <v>523</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C104" s="14" t="s">
         <v>525</v>
-      </c>
-      <c r="C104" s="14" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
+        <v>526</v>
+      </c>
+      <c r="C105" s="14" t="s">
         <v>527</v>
-      </c>
-      <c r="C105" s="14" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
+        <v>528</v>
+      </c>
+      <c r="C106" s="14" t="s">
         <v>529</v>
-      </c>
-      <c r="C106" s="14" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="21" t="s">
+        <v>530</v>
+      </c>
+      <c r="C107" s="14" t="s">
         <v>531</v>
-      </c>
-      <c r="C107" s="14" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="21" t="s">
+        <v>532</v>
+      </c>
+      <c r="C108" s="14" t="s">
         <v>533</v>
-      </c>
-      <c r="C108" s="14" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C109" s="14" t="s">
         <v>535</v>
-      </c>
-      <c r="C109" s="14" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="21" t="s">
+        <v>536</v>
+      </c>
+      <c r="C110" s="14" t="s">
         <v>537</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="21" t="s">
+        <v>538</v>
+      </c>
+      <c r="C111" s="14" t="s">
         <v>539</v>
-      </c>
-      <c r="C111" s="14" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="21" t="s">
+        <v>540</v>
+      </c>
+      <c r="C112" s="14" t="s">
         <v>541</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="21" t="s">
+        <v>542</v>
+      </c>
+      <c r="C113" s="14" t="s">
         <v>543</v>
-      </c>
-      <c r="C113" s="14" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="21" t="s">
+        <v>544</v>
+      </c>
+      <c r="C114" s="14" t="s">
         <v>545</v>
-      </c>
-      <c r="C114" s="14" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="21" t="s">
+        <v>546</v>
+      </c>
+      <c r="C115" s="14" t="s">
         <v>547</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="21" t="s">
+        <v>548</v>
+      </c>
+      <c r="C116" s="14" t="s">
         <v>549</v>
-      </c>
-      <c r="C116" s="14" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="21" t="s">
+        <v>550</v>
+      </c>
+      <c r="C117" s="14" t="s">
         <v>551</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="21" t="s">
+        <v>552</v>
+      </c>
+      <c r="C118" s="14" t="s">
         <v>553</v>
-      </c>
-      <c r="C118" s="14" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="21" t="s">
+        <v>554</v>
+      </c>
+      <c r="C119" s="14" t="s">
         <v>555</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="21" t="s">
+        <v>556</v>
+      </c>
+      <c r="C120" s="14" t="s">
         <v>557</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="21" t="s">
+        <v>558</v>
+      </c>
+      <c r="C121" s="14" t="s">
         <v>559</v>
-      </c>
-      <c r="C121" s="14" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="21" t="s">
+        <v>560</v>
+      </c>
+      <c r="C122" s="14" t="s">
         <v>561</v>
-      </c>
-      <c r="C122" s="14" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="21" t="s">
+        <v>562</v>
+      </c>
+      <c r="C123" s="14" t="s">
         <v>563</v>
-      </c>
-      <c r="C123" s="14" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="21" t="s">
+        <v>564</v>
+      </c>
+      <c r="C124" s="14" t="s">
         <v>565</v>
-      </c>
-      <c r="C124" s="14" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="21" t="s">
+        <v>566</v>
+      </c>
+      <c r="C125" s="14" t="s">
         <v>567</v>
-      </c>
-      <c r="C125" s="14" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="21" t="s">
+        <v>568</v>
+      </c>
+      <c r="C126" s="14" t="s">
         <v>569</v>
-      </c>
-      <c r="C126" s="14" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="21" t="s">
+        <v>570</v>
+      </c>
+      <c r="C127" s="14" t="s">
         <v>571</v>
-      </c>
-      <c r="C127" s="14" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="21" t="s">
+        <v>572</v>
+      </c>
+      <c r="C128" s="14" t="s">
         <v>573</v>
-      </c>
-      <c r="C128" s="14" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="C129" s="14" t="s">
         <v>575</v>
-      </c>
-      <c r="C129" s="14" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="21" t="s">
+        <v>576</v>
+      </c>
+      <c r="C130" s="14" t="s">
         <v>577</v>
-      </c>
-      <c r="C130" s="14" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="21" t="s">
+        <v>578</v>
+      </c>
+      <c r="C131" s="14" t="s">
         <v>579</v>
-      </c>
-      <c r="C131" s="14" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="21" t="s">
+        <v>580</v>
+      </c>
+      <c r="C132" s="14" t="s">
         <v>581</v>
-      </c>
-      <c r="C132" s="14" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="21" t="s">
+        <v>582</v>
+      </c>
+      <c r="C133" s="14" t="s">
         <v>583</v>
-      </c>
-      <c r="C133" s="14" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="21" t="s">
+        <v>584</v>
+      </c>
+      <c r="C134" s="14" t="s">
         <v>585</v>
-      </c>
-      <c r="C134" s="14" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="21" t="s">
+        <v>586</v>
+      </c>
+      <c r="C135" s="14" t="s">
         <v>587</v>
-      </c>
-      <c r="C135" s="14" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="21" t="s">
+        <v>588</v>
+      </c>
+      <c r="C136" s="14" t="s">
         <v>589</v>
-      </c>
-      <c r="C136" s="14" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="21" t="s">
+        <v>590</v>
+      </c>
+      <c r="C137" s="14" t="s">
         <v>591</v>
-      </c>
-      <c r="C137" s="14" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="21" t="s">
+        <v>592</v>
+      </c>
+      <c r="C138" s="14" t="s">
         <v>593</v>
-      </c>
-      <c r="C138" s="14" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="C139" s="14" t="s">
         <v>595</v>
-      </c>
-      <c r="C139" s="14" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="C140" s="23" t="s">
         <v>597</v>
-      </c>
-      <c r="C140" s="23" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="66" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C143" s="67"/>
     </row>
@@ -8109,570 +8074,570 @@
     </row>
     <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C145" s="9" t="s">
         <v>224</v>
-      </c>
-      <c r="C145" s="9" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="C146" s="11" t="s">
         <v>600</v>
-      </c>
-      <c r="C146" s="11" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="10" t="s">
+        <v>601</v>
+      </c>
+      <c r="C147" s="11" t="s">
         <v>602</v>
-      </c>
-      <c r="C147" s="11" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="C148" s="11" t="s">
         <v>604</v>
-      </c>
-      <c r="C148" s="11" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="C149" s="11" t="s">
         <v>606</v>
-      </c>
-      <c r="C149" s="11" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="150" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="10" t="s">
+        <v>607</v>
+      </c>
+      <c r="C150" s="11" t="s">
         <v>608</v>
-      </c>
-      <c r="C150" s="11" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="151" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="C151" s="11" t="s">
         <v>610</v>
-      </c>
-      <c r="C151" s="11" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="152" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="C152" s="11" t="s">
         <v>612</v>
-      </c>
-      <c r="C152" s="11" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="153" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="10" t="s">
+        <v>613</v>
+      </c>
+      <c r="C153" s="11" t="s">
         <v>614</v>
-      </c>
-      <c r="C153" s="11" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="154" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="C154" s="11" t="s">
         <v>616</v>
-      </c>
-      <c r="C154" s="11" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="155" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="C155" s="11" t="s">
         <v>618</v>
-      </c>
-      <c r="C155" s="11" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="156" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="C156" s="11" t="s">
         <v>620</v>
-      </c>
-      <c r="C156" s="11" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="157" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="C157" s="11" t="s">
         <v>622</v>
-      </c>
-      <c r="C157" s="11" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="158" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="C158" s="11" t="s">
         <v>624</v>
-      </c>
-      <c r="C158" s="11" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="159" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="10" t="s">
+        <v>625</v>
+      </c>
+      <c r="C159" s="11" t="s">
         <v>626</v>
-      </c>
-      <c r="C159" s="11" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="160" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="10" t="s">
+        <v>627</v>
+      </c>
+      <c r="C160" s="11" t="s">
         <v>628</v>
-      </c>
-      <c r="C160" s="11" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="161" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="C161" s="11" t="s">
         <v>630</v>
-      </c>
-      <c r="C161" s="11" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="162" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="C162" s="11" t="s">
         <v>632</v>
-      </c>
-      <c r="C162" s="11" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="163" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="10" t="s">
+        <v>633</v>
+      </c>
+      <c r="C163" s="11" t="s">
         <v>634</v>
-      </c>
-      <c r="C163" s="11" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="164" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="C164" s="11" t="s">
         <v>636</v>
-      </c>
-      <c r="C164" s="11" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="165" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="C165" s="11" t="s">
         <v>638</v>
-      </c>
-      <c r="C165" s="11" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="166" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="10" t="s">
+        <v>639</v>
+      </c>
+      <c r="C166" s="11" t="s">
         <v>640</v>
-      </c>
-      <c r="C166" s="11" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="167" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="10" t="s">
+        <v>641</v>
+      </c>
+      <c r="C167" s="11" t="s">
         <v>642</v>
-      </c>
-      <c r="C167" s="11" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="168" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="10" t="s">
+        <v>643</v>
+      </c>
+      <c r="C168" s="11" t="s">
         <v>644</v>
-      </c>
-      <c r="C168" s="11" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="169" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="10" t="s">
+        <v>645</v>
+      </c>
+      <c r="C169" s="11" t="s">
         <v>646</v>
-      </c>
-      <c r="C169" s="11" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="170" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="C170" s="11" t="s">
         <v>648</v>
-      </c>
-      <c r="C170" s="11" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="171" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="C171" s="11" t="s">
         <v>650</v>
-      </c>
-      <c r="C171" s="11" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="172" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="C172" s="11" t="s">
         <v>652</v>
-      </c>
-      <c r="C172" s="11" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="173" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="10" t="s">
+        <v>653</v>
+      </c>
+      <c r="C173" s="11" t="s">
         <v>654</v>
-      </c>
-      <c r="C173" s="11" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="174" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="C174" s="11" t="s">
         <v>656</v>
-      </c>
-      <c r="C174" s="11" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="C175" s="11" t="s">
         <v>658</v>
-      </c>
-      <c r="C175" s="11" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="10" t="s">
+        <v>659</v>
+      </c>
+      <c r="C176" s="11" t="s">
         <v>660</v>
-      </c>
-      <c r="C176" s="11" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="177" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="C177" s="11" t="s">
         <v>662</v>
-      </c>
-      <c r="C177" s="11" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="178" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="10" t="s">
+        <v>663</v>
+      </c>
+      <c r="C178" s="11" t="s">
         <v>664</v>
-      </c>
-      <c r="C178" s="11" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="179" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="C179" s="11" t="s">
         <v>666</v>
-      </c>
-      <c r="C179" s="11" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="180" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="C180" s="11" t="s">
         <v>668</v>
-      </c>
-      <c r="C180" s="11" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="181" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="C181" s="11" t="s">
         <v>670</v>
-      </c>
-      <c r="C181" s="11" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="182" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="C182" s="11" t="s">
         <v>672</v>
-      </c>
-      <c r="C182" s="11" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="183" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="C183" s="11" t="s">
         <v>674</v>
-      </c>
-      <c r="C183" s="11" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="184" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="C184" s="11" t="s">
         <v>676</v>
-      </c>
-      <c r="C184" s="11" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="185" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="C185" s="11" t="s">
         <v>678</v>
-      </c>
-      <c r="C185" s="11" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="186" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="C186" s="11" t="s">
         <v>680</v>
-      </c>
-      <c r="C186" s="11" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="187" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="C187" s="11" t="s">
         <v>682</v>
-      </c>
-      <c r="C187" s="11" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="188" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="10" t="s">
+        <v>683</v>
+      </c>
+      <c r="C188" s="11" t="s">
         <v>684</v>
-      </c>
-      <c r="C188" s="11" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="189" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="C189" s="11" t="s">
         <v>686</v>
-      </c>
-      <c r="C189" s="11" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="190" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="C190" s="11" t="s">
         <v>688</v>
-      </c>
-      <c r="C190" s="11" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="191" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="C191" s="11" t="s">
         <v>690</v>
-      </c>
-      <c r="C191" s="11" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="192" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="C192" s="11" t="s">
         <v>692</v>
-      </c>
-      <c r="C192" s="11" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="193" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="10" t="s">
+        <v>693</v>
+      </c>
+      <c r="C193" s="11" t="s">
         <v>694</v>
-      </c>
-      <c r="C193" s="11" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="194" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="C194" s="11" t="s">
         <v>696</v>
-      </c>
-      <c r="C194" s="11" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="195" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="10" t="s">
+        <v>697</v>
+      </c>
+      <c r="C195" s="11" t="s">
         <v>698</v>
-      </c>
-      <c r="C195" s="11" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="196" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="C196" s="11" t="s">
         <v>700</v>
-      </c>
-      <c r="C196" s="11" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="197" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="10" t="s">
+        <v>701</v>
+      </c>
+      <c r="C197" s="11" t="s">
         <v>702</v>
-      </c>
-      <c r="C197" s="11" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="198" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="C198" s="11" t="s">
         <v>704</v>
-      </c>
-      <c r="C198" s="11" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="199" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="C199" s="11" t="s">
         <v>706</v>
-      </c>
-      <c r="C199" s="11" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="200" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="C200" s="11" t="s">
         <v>708</v>
-      </c>
-      <c r="C200" s="11" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="201" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="10" t="s">
+        <v>709</v>
+      </c>
+      <c r="C201" s="11" t="s">
         <v>710</v>
-      </c>
-      <c r="C201" s="11" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="202" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="10" t="s">
+        <v>711</v>
+      </c>
+      <c r="C202" s="11" t="s">
         <v>712</v>
-      </c>
-      <c r="C202" s="11" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="203" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="C203" s="11" t="s">
         <v>714</v>
-      </c>
-      <c r="C203" s="11" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="204" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="10" t="s">
+        <v>715</v>
+      </c>
+      <c r="C204" s="11" t="s">
         <v>716</v>
-      </c>
-      <c r="C204" s="11" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="205" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="10" t="s">
+        <v>717</v>
+      </c>
+      <c r="C205" s="11" t="s">
         <v>718</v>
-      </c>
-      <c r="C205" s="11" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="206" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="10" t="s">
+        <v>719</v>
+      </c>
+      <c r="C206" s="11" t="s">
         <v>720</v>
-      </c>
-      <c r="C206" s="11" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="207" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="C207" s="11" t="s">
         <v>722</v>
-      </c>
-      <c r="C207" s="11" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="208" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="10" t="s">
+        <v>723</v>
+      </c>
+      <c r="C208" s="11" t="s">
         <v>724</v>
-      </c>
-      <c r="C208" s="11" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="209" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="10" t="s">
+        <v>725</v>
+      </c>
+      <c r="C209" s="11" t="s">
         <v>726</v>
-      </c>
-      <c r="C209" s="11" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="210" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="10" t="s">
+        <v>727</v>
+      </c>
+      <c r="C210" s="11" t="s">
         <v>728</v>
-      </c>
-      <c r="C210" s="11" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="211" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="10" t="s">
+        <v>729</v>
+      </c>
+      <c r="C211" s="11" t="s">
         <v>730</v>
-      </c>
-      <c r="C211" s="11" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="212" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="C212" s="11" t="s">
         <v>732</v>
-      </c>
-      <c r="C212" s="11" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="213" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="10" t="s">
+        <v>733</v>
+      </c>
+      <c r="C213" s="11" t="s">
         <v>734</v>
-      </c>
-      <c r="C213" s="11" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="214" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="C214" s="11" t="s">
         <v>736</v>
-      </c>
-      <c r="C214" s="11" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="215" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="10" t="s">
+        <v>737</v>
+      </c>
+      <c r="C215" s="11" t="s">
         <v>738</v>
-      </c>
-      <c r="C215" s="11" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="216" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
EPBDS-8161 Create a new property "calculateAllCells" for Spreadsheets that returns a particular type
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openl-pub\DEV\org.openl.rules\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC74937-A46D-4BA3-9128-B9CD08AC28F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Runtime Scope" sheetId="4" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="181029" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="817">
   <si>
     <t>Display Name</t>
   </si>
@@ -2493,11 +2494,23 @@
   <si>
     <t>contains(lob)</t>
   </si>
+  <si>
+    <t>XLS_SPREADSHEET</t>
+  </si>
+  <si>
+    <t>calculateAllCells</t>
+  </si>
+  <si>
+    <t>Calculate All Cells</t>
+  </si>
+  <si>
+    <t>If true calculates all cells in the Spreadsheet, otherwise calculates only cells these are requred for a result. By default = true.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3483,6 +3496,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3518,6 +3548,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -3693,7 +3740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
@@ -3938,11 +3985,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="F40" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5824,10 +5871,10 @@
     </row>
     <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>802</v>
+        <v>814</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>58</v>
@@ -5851,11 +5898,11 @@
         <v>58</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>749</v>
+        <v>813</v>
       </c>
       <c r="N48" s="7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
@@ -5865,30 +5912,28 @@
         <v>84</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="49" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>804</v>
+        <v>811</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>806</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="F49" s="5"/>
       <c r="G49" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
@@ -5896,15 +5941,16 @@
         <v>58</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="M49" s="5" t="s">
         <v>749</v>
       </c>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5" t="s">
-        <v>807</v>
-      </c>
+      <c r="N49" s="7" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O49" s="5"/>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
@@ -5912,87 +5958,134 @@
         <v>84</v>
       </c>
       <c r="T49" s="5" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M50" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="T50" s="5" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="53" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
+    <row r="54" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5" t="s">
+      <c r="D54" s="5"/>
+      <c r="E54" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H53" s="5" t="s">
+      <c r="F54" s="5"/>
+      <c r="G54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H54" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5" t="s">
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="5" t="s">
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="T53" s="5" t="s">
+      <c r="T54" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="57" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="57" t="s">
+    <row r="58" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="C57" s="57"/>
-    </row>
-    <row r="58" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="58" t="s">
-        <v>203</v>
-      </c>
-      <c r="C58" s="58"/>
+      <c r="C58" s="57"/>
     </row>
     <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" s="58"/>
+    </row>
+    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="C59" s="58"/>
-    </row>
-    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="59" t="s">
-        <v>205</v>
-      </c>
-      <c r="C60" s="59"/>
+      <c r="C60" s="58"/>
     </row>
     <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="59" t="s">
+        <v>205</v>
+      </c>
+      <c r="C61" s="59"/>
+    </row>
+    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="59" t="s">
         <v>206</v>
       </c>
-      <c r="C61" s="59"/>
-    </row>
-    <row r="62" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="56" t="s">
+      <c r="C62" s="59"/>
+    </row>
+    <row r="63" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="56" t="s">
         <v>752</v>
       </c>
-      <c r="C62" s="56"/>
+      <c r="C63" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C3:L3"/>
@@ -6003,11 +6096,11 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
-    <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -6020,7 +6113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
@@ -6102,7 +6195,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
@@ -6328,7 +6421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:J216"/>
   <sheetViews>
     <sheetView topLeftCell="A55" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">

</xml_diff>

<commit_message>
EPBDS-8354 Property 'calculateAllCells' can't be defined in Properties Table
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC74937-A46D-4BA3-9128-B9CD08AC28F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2BFD19-6912-4E51-8D73-50FA3D77E7E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="816">
   <si>
     <t>Display Name</t>
   </si>
@@ -2493,9 +2493,6 @@
   </si>
   <si>
     <t>contains(lob)</t>
-  </si>
-  <si>
-    <t>XLS_SPREADSHEET</t>
   </si>
   <si>
     <t>calculateAllCells</t>
@@ -3144,7 +3141,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3152,19 +3149,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3178,7 +3172,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3189,8 +3183,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3207,25 +3201,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3234,32 +3216,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3270,16 +3251,16 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3750,220 +3731,215 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3973,6 +3949,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3988,8 +3969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F40" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4018,157 +3999,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -4180,27 +4161,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -5420,7 +5401,7 @@
       <c r="M37" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="N37" s="7" t="b">
+      <c r="N37" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
@@ -5599,7 +5580,7 @@
       <c r="M41" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="N41" s="7" t="b">
+      <c r="N41" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -5854,7 +5835,7 @@
       <c r="M47" s="5" t="s">
         <v>809</v>
       </c>
-      <c r="N47" s="7" t="b">
+      <c r="N47" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
@@ -5871,10 +5852,10 @@
     </row>
     <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>58</v>
@@ -5898,9 +5879,9 @@
         <v>58</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>813</v>
-      </c>
-      <c r="N48" s="7" t="b">
+        <v>809</v>
+      </c>
+      <c r="N48" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
@@ -5912,7 +5893,7 @@
         <v>84</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5946,7 +5927,7 @@
       <c r="M49" s="5" t="s">
         <v>749</v>
       </c>
-      <c r="N49" s="7" t="b">
+      <c r="N49" s="5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -6048,40 +6029,40 @@
       </c>
     </row>
     <row r="58" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="57" t="s">
+      <c r="B58" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="C58" s="57"/>
+      <c r="C58" s="51"/>
     </row>
     <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="58" t="s">
+      <c r="B59" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="C59" s="58"/>
+      <c r="C59" s="52"/>
     </row>
     <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="58" t="s">
+      <c r="B60" s="52" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="58"/>
+      <c r="C60" s="52"/>
     </row>
     <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="59" t="s">
+      <c r="B61" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="C61" s="59"/>
+      <c r="C61" s="53"/>
     </row>
     <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="59" t="s">
+      <c r="B62" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="C62" s="59"/>
+      <c r="C62" s="53"/>
     </row>
     <row r="63" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="50" t="s">
         <v>752</v>
       </c>
-      <c r="C63" s="56"/>
+      <c r="C63" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -6123,60 +6104,60 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="54" t="s">
         <v>207</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="61"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="61"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="55"/>
+      <c r="C8" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="61"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="55"/>
+      <c r="C9" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="61"/>
-      <c r="C10" s="62" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6211,91 +6192,91 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="57" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="30" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="36" t="s">
         <v>215</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="37" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="36" t="s">
         <v>132</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="37" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="36" t="s">
         <v>805</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="37" t="s">
         <v>804</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="36" t="s">
         <v>216</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -6304,12 +6285,12 @@
       <c r="D9" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="37" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="36" t="s">
         <v>142</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -6318,12 +6299,12 @@
       <c r="D10" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="37" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="36" t="s">
         <v>219</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -6332,40 +6313,40 @@
       <c r="D11" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="37" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="36" t="s">
         <v>147</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="37" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="36" t="s">
         <v>152</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="37" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="36" t="s">
         <v>162</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -6374,12 +6355,12 @@
       <c r="D14" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="37" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="36" t="s">
         <v>756</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -6388,21 +6369,21 @@
       <c r="D15" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="37" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="38" t="s">
         <v>759</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="39" t="s">
         <v>760</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="40" t="s">
         <v>761</v>
       </c>
     </row>
@@ -6439,2297 +6420,2297 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="63"/>
+      <c r="E2" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="I2" s="68" t="s">
+      <c r="F2" s="24"/>
+      <c r="I2" s="62" t="s">
         <v>222</v>
       </c>
-      <c r="J2" s="69"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="22" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="I13" s="68" t="s">
+      <c r="I13" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="J13" s="69"/>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="13" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="13" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="I18" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="13" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="13" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="I20" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="J20" s="22" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="13" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="13" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="I23" s="68" t="s">
+      <c r="I23" s="62" t="s">
         <v>315</v>
       </c>
-      <c r="J23" s="69"/>
+      <c r="J23" s="63"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>320</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="I25" s="26" t="s">
+      <c r="I25" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="12" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="I26" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="J26" s="13" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>330</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="20" t="s">
         <v>332</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="26" t="s">
         <v>334</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="J27" s="14" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="I28" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="J28" s="29" t="s">
+      <c r="J28" s="28" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="13" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="13" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="I32" s="68" t="s">
+      <c r="I32" s="62" t="s">
         <v>753</v>
       </c>
-      <c r="J32" s="69"/>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="E33" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="I33" s="20" t="s">
+      <c r="I33" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="E34" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="I34" s="26" t="s">
+      <c r="I34" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="12" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>364</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>365</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="I35" s="20" t="s">
         <v>754</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="13" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="I36" s="22" t="s">
+      <c r="I36" s="21" t="s">
         <v>755</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="J36" s="22" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="20" t="s">
         <v>374</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="13" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="20" t="s">
         <v>376</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="13" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="20" t="s">
         <v>380</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="E39" s="21" t="s">
+      <c r="E39" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="I39" s="68" t="s">
+      <c r="I39" s="62" t="s">
         <v>786</v>
       </c>
-      <c r="J39" s="69"/>
+      <c r="J39" s="63"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="20" t="s">
         <v>385</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="13" t="s">
         <v>386</v>
       </c>
-      <c r="I40" s="46" t="s">
+      <c r="I40" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="J40" s="47" t="s">
+      <c r="J40" s="42" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="20" t="s">
         <v>388</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="I41" s="46" t="s">
+      <c r="I41" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="J41" s="47" t="s">
+      <c r="J41" s="42" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="20" t="s">
         <v>392</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="I42" s="48" t="s">
+      <c r="I42" s="43" t="s">
         <v>778</v>
       </c>
-      <c r="J42" s="49" t="s">
+      <c r="J42" s="44" t="s">
         <v>779</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="20" t="s">
         <v>394</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>395</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="13" t="s">
         <v>397</v>
       </c>
-      <c r="I43" s="50" t="s">
+      <c r="I43" s="27" t="s">
         <v>787</v>
       </c>
-      <c r="J43" s="51" t="s">
+      <c r="J43" s="45" t="s">
         <v>788</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="E44" s="21" t="s">
+      <c r="E44" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="13" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="E45" s="21" t="s">
+      <c r="E45" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="13" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="20" t="s">
         <v>405</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="I46" s="68" t="s">
+      <c r="I46" s="62" t="s">
         <v>796</v>
       </c>
-      <c r="J46" s="69"/>
+      <c r="J46" s="63"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="20" t="s">
         <v>409</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E47" s="20" t="s">
         <v>411</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="I47" s="20" t="s">
+      <c r="I47" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J47" s="12" t="s">
+      <c r="J47" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="20" t="s">
         <v>413</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="I48" s="26" t="s">
+      <c r="I48" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="J48" s="13" t="s">
+      <c r="J48" s="12" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="E49" s="20" t="s">
         <v>419</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="F49" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="I49" s="21" t="s">
+      <c r="I49" s="20" t="s">
         <v>776</v>
       </c>
-      <c r="J49" s="14" t="s">
+      <c r="J49" s="13" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="20" t="s">
         <v>421</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="E50" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="F50" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="I50" s="28" t="s">
+      <c r="I50" s="27" t="s">
         <v>799</v>
       </c>
-      <c r="J50" s="29" t="s">
+      <c r="J50" s="28" t="s">
         <v>798</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="20" t="s">
         <v>425</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="E51" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="13" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="20" t="s">
         <v>429</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="E52" s="20" t="s">
         <v>431</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="13" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="13" t="s">
         <v>434</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="E53" s="20" t="s">
         <v>435</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F53" s="13" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="20" t="s">
         <v>437</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="13" t="s">
         <v>438</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E54" s="20" t="s">
         <v>439</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="13" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="13" t="s">
         <v>441</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="E55" s="20" t="s">
         <v>442</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="F55" s="13" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="56" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="20" t="s">
         <v>444</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="13" t="s">
         <v>445</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="E56" s="21" t="s">
         <v>446</v>
       </c>
-      <c r="F56" s="23" t="s">
+      <c r="F56" s="22" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="13" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="20" t="s">
         <v>449</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="13" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="20" t="s">
         <v>451</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="E59" s="68" t="s">
+      <c r="E59" s="62" t="s">
         <v>762</v>
       </c>
-      <c r="F59" s="69"/>
+      <c r="F59" s="63"/>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="E60" s="46" t="s">
+      <c r="E60" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F60" s="47" t="s">
+      <c r="F60" s="42" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="21" t="s">
+      <c r="B61" s="20" t="s">
         <v>455</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C61" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="E61" s="46" t="s">
+      <c r="E61" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="F61" s="47" t="s">
+      <c r="F61" s="42" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="20" t="s">
         <v>457</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="E62" s="48" t="s">
+      <c r="E62" s="43" t="s">
         <v>763</v>
       </c>
-      <c r="F62" s="49" t="s">
+      <c r="F62" s="44" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="21" t="s">
+      <c r="B63" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C63" s="13" t="s">
         <v>459</v>
       </c>
-      <c r="E63" s="48" t="s">
+      <c r="E63" s="43" t="s">
         <v>765</v>
       </c>
-      <c r="F63" s="49" t="s">
+      <c r="F63" s="44" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="20" t="s">
         <v>460</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="E64" s="48" t="s">
+      <c r="E64" s="43" t="s">
         <v>462</v>
       </c>
-      <c r="F64" s="49" t="s">
+      <c r="F64" s="44" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="21" t="s">
+      <c r="B65" s="20" t="s">
         <v>462</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="13" t="s">
         <v>463</v>
       </c>
-      <c r="E65" s="48" t="s">
+      <c r="E65" s="43" t="s">
         <v>768</v>
       </c>
-      <c r="F65" s="49" t="s">
+      <c r="F65" s="44" t="s">
         <v>769</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="21" t="s">
+      <c r="B66" s="20" t="s">
         <v>464</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="13" t="s">
         <v>465</v>
       </c>
-      <c r="E66" s="48" t="s">
+      <c r="E66" s="43" t="s">
         <v>770</v>
       </c>
-      <c r="F66" s="49" t="s">
+      <c r="F66" s="44" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="21" t="s">
+      <c r="B67" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="C67" s="14" t="s">
+      <c r="C67" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="E67" s="48" t="s">
+      <c r="E67" s="43" t="s">
         <v>772</v>
       </c>
-      <c r="F67" s="49" t="s">
+      <c r="F67" s="44" t="s">
         <v>773</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="21" t="s">
+      <c r="B68" s="20" t="s">
         <v>468</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="13" t="s">
         <v>469</v>
       </c>
-      <c r="E68" s="48" t="s">
+      <c r="E68" s="43" t="s">
         <v>774</v>
       </c>
-      <c r="F68" s="49" t="s">
+      <c r="F68" s="44" t="s">
         <v>775</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="E69" s="48" t="s">
+      <c r="E69" s="43" t="s">
         <v>776</v>
       </c>
-      <c r="F69" s="49" t="s">
+      <c r="F69" s="44" t="s">
         <v>777</v>
       </c>
     </row>
     <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="13" t="s">
         <v>471</v>
       </c>
-      <c r="E70" s="48" t="s">
+      <c r="E70" s="43" t="s">
         <v>778</v>
       </c>
-      <c r="F70" s="49" t="s">
+      <c r="F70" s="44" t="s">
         <v>779</v>
       </c>
     </row>
     <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="20" t="s">
         <v>472</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="E71" s="48" t="s">
+      <c r="E71" s="43" t="s">
         <v>482</v>
       </c>
-      <c r="F71" s="49" t="s">
+      <c r="F71" s="44" t="s">
         <v>780</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="20" t="s">
         <v>474</v>
       </c>
-      <c r="C72" s="14" t="s">
+      <c r="C72" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="E72" s="48" t="s">
+      <c r="E72" s="43" t="s">
         <v>449</v>
       </c>
-      <c r="F72" s="49" t="s">
+      <c r="F72" s="44" t="s">
         <v>781</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="21" t="s">
+      <c r="B73" s="20" t="s">
         <v>476</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" s="13" t="s">
         <v>477</v>
       </c>
-      <c r="E73" s="48" t="s">
+      <c r="E73" s="43" t="s">
         <v>782</v>
       </c>
-      <c r="F73" s="49" t="s">
+      <c r="F73" s="44" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="21" t="s">
+      <c r="B74" s="20" t="s">
         <v>478</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="E74" s="50" t="s">
+      <c r="E74" s="27" t="s">
         <v>784</v>
       </c>
-      <c r="F74" s="51" t="s">
+      <c r="F74" s="45" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="C75" s="14" t="s">
+      <c r="C75" s="13" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="21" t="s">
+      <c r="B76" s="20" t="s">
         <v>482</v>
       </c>
-      <c r="C76" s="14" t="s">
+      <c r="C76" s="13" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C77" s="13" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="21" t="s">
+      <c r="B78" s="20" t="s">
         <v>486</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" s="13" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="21" t="s">
+      <c r="B79" s="20" t="s">
         <v>488</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="13" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="21" t="s">
+      <c r="B80" s="20" t="s">
         <v>411</v>
       </c>
-      <c r="C80" s="14" t="s">
+      <c r="C80" s="13" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="21" t="s">
+      <c r="B81" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="C81" s="14" t="s">
+      <c r="C81" s="13" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="21" t="s">
+      <c r="B82" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="C82" s="14" t="s">
+      <c r="C82" s="13" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="21" t="s">
+      <c r="B83" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" s="13" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="21" t="s">
+      <c r="B84" s="20" t="s">
         <v>496</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" s="13" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="20" t="s">
         <v>498</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C85" s="13" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="21" t="s">
+      <c r="B86" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C86" s="13" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="21" t="s">
+      <c r="B87" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C87" s="13" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="21" t="s">
+      <c r="B88" s="20" t="s">
         <v>503</v>
       </c>
-      <c r="C88" s="14" t="s">
+      <c r="C88" s="13" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="21" t="s">
+      <c r="B89" s="20" t="s">
         <v>505</v>
       </c>
-      <c r="C89" s="14" t="s">
+      <c r="C89" s="13" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="21" t="s">
+      <c r="B90" s="20" t="s">
         <v>507</v>
       </c>
-      <c r="C90" s="14" t="s">
+      <c r="C90" s="13" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="21" t="s">
+      <c r="B91" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="C91" s="14" t="s">
+      <c r="C91" s="13" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="21" t="s">
+      <c r="B92" s="20" t="s">
         <v>511</v>
       </c>
-      <c r="C92" s="14" t="s">
+      <c r="C92" s="13" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="21" t="s">
+      <c r="B93" s="20" t="s">
         <v>513</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C93" s="13" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="21" t="s">
+      <c r="B94" s="20" t="s">
         <v>515</v>
       </c>
-      <c r="C94" s="14" t="s">
+      <c r="C94" s="13" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="22" t="s">
+      <c r="B95" s="21" t="s">
         <v>517</v>
       </c>
-      <c r="C95" s="23" t="s">
+      <c r="C95" s="22" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="24" t="s">
+      <c r="B99" s="23" t="s">
         <v>519</v>
       </c>
-      <c r="C99" s="25"/>
+      <c r="C99" s="24"/>
     </row>
     <row r="100" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="20" t="s">
+      <c r="B100" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C100" s="12" t="s">
+      <c r="C100" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="20" t="s">
+      <c r="B101" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="C101" s="12" t="s">
+      <c r="C101" s="11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="21" t="s">
+      <c r="B102" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="C102" s="14" t="s">
+      <c r="C102" s="13" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="21" t="s">
+      <c r="B103" s="20" t="s">
         <v>522</v>
       </c>
-      <c r="C103" s="14" t="s">
+      <c r="C103" s="13" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="21" t="s">
+      <c r="B104" s="20" t="s">
         <v>524</v>
       </c>
-      <c r="C104" s="14" t="s">
+      <c r="C104" s="13" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="21" t="s">
+      <c r="B105" s="20" t="s">
         <v>526</v>
       </c>
-      <c r="C105" s="14" t="s">
+      <c r="C105" s="13" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="21" t="s">
+      <c r="B106" s="20" t="s">
         <v>528</v>
       </c>
-      <c r="C106" s="14" t="s">
+      <c r="C106" s="13" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="21" t="s">
+      <c r="B107" s="20" t="s">
         <v>530</v>
       </c>
-      <c r="C107" s="14" t="s">
+      <c r="C107" s="13" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="21" t="s">
+      <c r="B108" s="20" t="s">
         <v>532</v>
       </c>
-      <c r="C108" s="14" t="s">
+      <c r="C108" s="13" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="20" t="s">
         <v>534</v>
       </c>
-      <c r="C109" s="14" t="s">
+      <c r="C109" s="13" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="21" t="s">
+      <c r="B110" s="20" t="s">
         <v>536</v>
       </c>
-      <c r="C110" s="14" t="s">
+      <c r="C110" s="13" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="21" t="s">
+      <c r="B111" s="20" t="s">
         <v>538</v>
       </c>
-      <c r="C111" s="14" t="s">
+      <c r="C111" s="13" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="21" t="s">
+      <c r="B112" s="20" t="s">
         <v>540</v>
       </c>
-      <c r="C112" s="14" t="s">
+      <c r="C112" s="13" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="21" t="s">
+      <c r="B113" s="20" t="s">
         <v>542</v>
       </c>
-      <c r="C113" s="14" t="s">
+      <c r="C113" s="13" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="21" t="s">
+      <c r="B114" s="20" t="s">
         <v>544</v>
       </c>
-      <c r="C114" s="14" t="s">
+      <c r="C114" s="13" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="21" t="s">
+      <c r="B115" s="20" t="s">
         <v>546</v>
       </c>
-      <c r="C115" s="14" t="s">
+      <c r="C115" s="13" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="21" t="s">
+      <c r="B116" s="20" t="s">
         <v>548</v>
       </c>
-      <c r="C116" s="14" t="s">
+      <c r="C116" s="13" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="21" t="s">
+      <c r="B117" s="20" t="s">
         <v>550</v>
       </c>
-      <c r="C117" s="14" t="s">
+      <c r="C117" s="13" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="21" t="s">
+      <c r="B118" s="20" t="s">
         <v>552</v>
       </c>
-      <c r="C118" s="14" t="s">
+      <c r="C118" s="13" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="21" t="s">
+      <c r="B119" s="20" t="s">
         <v>554</v>
       </c>
-      <c r="C119" s="14" t="s">
+      <c r="C119" s="13" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="21" t="s">
+      <c r="B120" s="20" t="s">
         <v>556</v>
       </c>
-      <c r="C120" s="14" t="s">
+      <c r="C120" s="13" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="21" t="s">
+      <c r="B121" s="20" t="s">
         <v>558</v>
       </c>
-      <c r="C121" s="14" t="s">
+      <c r="C121" s="13" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="21" t="s">
+      <c r="B122" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="C122" s="14" t="s">
+      <c r="C122" s="13" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="21" t="s">
+      <c r="B123" s="20" t="s">
         <v>562</v>
       </c>
-      <c r="C123" s="14" t="s">
+      <c r="C123" s="13" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="21" t="s">
+      <c r="B124" s="20" t="s">
         <v>564</v>
       </c>
-      <c r="C124" s="14" t="s">
+      <c r="C124" s="13" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="21" t="s">
+      <c r="B125" s="20" t="s">
         <v>566</v>
       </c>
-      <c r="C125" s="14" t="s">
+      <c r="C125" s="13" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="21" t="s">
+      <c r="B126" s="20" t="s">
         <v>568</v>
       </c>
-      <c r="C126" s="14" t="s">
+      <c r="C126" s="13" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="21" t="s">
+      <c r="B127" s="20" t="s">
         <v>570</v>
       </c>
-      <c r="C127" s="14" t="s">
+      <c r="C127" s="13" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="21" t="s">
+      <c r="B128" s="20" t="s">
         <v>572</v>
       </c>
-      <c r="C128" s="14" t="s">
+      <c r="C128" s="13" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="21" t="s">
+      <c r="B129" s="20" t="s">
         <v>574</v>
       </c>
-      <c r="C129" s="14" t="s">
+      <c r="C129" s="13" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="21" t="s">
+      <c r="B130" s="20" t="s">
         <v>576</v>
       </c>
-      <c r="C130" s="14" t="s">
+      <c r="C130" s="13" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="21" t="s">
+      <c r="B131" s="20" t="s">
         <v>578</v>
       </c>
-      <c r="C131" s="14" t="s">
+      <c r="C131" s="13" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="21" t="s">
+      <c r="B132" s="20" t="s">
         <v>580</v>
       </c>
-      <c r="C132" s="14" t="s">
+      <c r="C132" s="13" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="21" t="s">
+      <c r="B133" s="20" t="s">
         <v>582</v>
       </c>
-      <c r="C133" s="14" t="s">
+      <c r="C133" s="13" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="21" t="s">
+      <c r="B134" s="20" t="s">
         <v>584</v>
       </c>
-      <c r="C134" s="14" t="s">
+      <c r="C134" s="13" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="21" t="s">
+      <c r="B135" s="20" t="s">
         <v>586</v>
       </c>
-      <c r="C135" s="14" t="s">
+      <c r="C135" s="13" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="21" t="s">
+      <c r="B136" s="20" t="s">
         <v>588</v>
       </c>
-      <c r="C136" s="14" t="s">
+      <c r="C136" s="13" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="21" t="s">
+      <c r="B137" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="C137" s="14" t="s">
+      <c r="C137" s="13" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="21" t="s">
+      <c r="B138" s="20" t="s">
         <v>592</v>
       </c>
-      <c r="C138" s="14" t="s">
+      <c r="C138" s="13" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="21" t="s">
+      <c r="B139" s="20" t="s">
         <v>594</v>
       </c>
-      <c r="C139" s="14" t="s">
+      <c r="C139" s="13" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="22" t="s">
+      <c r="B140" s="21" t="s">
         <v>596</v>
       </c>
-      <c r="C140" s="23" t="s">
+      <c r="C140" s="22" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="66" t="s">
+      <c r="B143" s="60" t="s">
         <v>598</v>
       </c>
-      <c r="C143" s="67"/>
+      <c r="C143" s="61"/>
     </row>
     <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="8" t="s">
+      <c r="B144" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C144" s="9" t="s">
+      <c r="C144" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="8" t="s">
+      <c r="B145" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="C145" s="9" t="s">
+      <c r="C145" s="8" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="10" t="s">
+      <c r="B146" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C146" s="10" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="10" t="s">
+      <c r="B147" s="9" t="s">
         <v>601</v>
       </c>
-      <c r="C147" s="11" t="s">
+      <c r="C147" s="10" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="10" t="s">
+      <c r="B148" s="9" t="s">
         <v>603</v>
       </c>
-      <c r="C148" s="11" t="s">
+      <c r="C148" s="10" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="10" t="s">
+      <c r="B149" s="9" t="s">
         <v>605</v>
       </c>
-      <c r="C149" s="11" t="s">
+      <c r="C149" s="10" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="150" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="10" t="s">
+      <c r="B150" s="9" t="s">
         <v>607</v>
       </c>
-      <c r="C150" s="11" t="s">
+      <c r="C150" s="10" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="151" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="10" t="s">
+      <c r="B151" s="9" t="s">
         <v>609</v>
       </c>
-      <c r="C151" s="11" t="s">
+      <c r="C151" s="10" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="152" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="10" t="s">
+      <c r="B152" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="C152" s="11" t="s">
+      <c r="C152" s="10" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="153" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="10" t="s">
+      <c r="B153" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="C153" s="11" t="s">
+      <c r="C153" s="10" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="154" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="10" t="s">
+      <c r="B154" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="C154" s="11" t="s">
+      <c r="C154" s="10" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="155" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="10" t="s">
+      <c r="B155" s="9" t="s">
         <v>617</v>
       </c>
-      <c r="C155" s="11" t="s">
+      <c r="C155" s="10" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="156" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="10" t="s">
+      <c r="B156" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="C156" s="11" t="s">
+      <c r="C156" s="10" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="157" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="10" t="s">
+      <c r="B157" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="C157" s="11" t="s">
+      <c r="C157" s="10" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="158" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="10" t="s">
+      <c r="B158" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="C158" s="11" t="s">
+      <c r="C158" s="10" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="159" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="10" t="s">
+      <c r="B159" s="9" t="s">
         <v>625</v>
       </c>
-      <c r="C159" s="11" t="s">
+      <c r="C159" s="10" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="160" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="10" t="s">
+      <c r="B160" s="9" t="s">
         <v>627</v>
       </c>
-      <c r="C160" s="11" t="s">
+      <c r="C160" s="10" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="161" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="10" t="s">
+      <c r="B161" s="9" t="s">
         <v>629</v>
       </c>
-      <c r="C161" s="11" t="s">
+      <c r="C161" s="10" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="162" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="10" t="s">
+      <c r="B162" s="9" t="s">
         <v>631</v>
       </c>
-      <c r="C162" s="11" t="s">
+      <c r="C162" s="10" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="163" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="10" t="s">
+      <c r="B163" s="9" t="s">
         <v>633</v>
       </c>
-      <c r="C163" s="11" t="s">
+      <c r="C163" s="10" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="164" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="10" t="s">
+      <c r="B164" s="9" t="s">
         <v>635</v>
       </c>
-      <c r="C164" s="11" t="s">
+      <c r="C164" s="10" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="165" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B165" s="10" t="s">
+      <c r="B165" s="9" t="s">
         <v>637</v>
       </c>
-      <c r="C165" s="11" t="s">
+      <c r="C165" s="10" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="166" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="10" t="s">
+      <c r="B166" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="C166" s="11" t="s">
+      <c r="C166" s="10" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="167" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="10" t="s">
+      <c r="B167" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="C167" s="11" t="s">
+      <c r="C167" s="10" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="168" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="10" t="s">
+      <c r="B168" s="9" t="s">
         <v>643</v>
       </c>
-      <c r="C168" s="11" t="s">
+      <c r="C168" s="10" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="169" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="10" t="s">
+      <c r="B169" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="C169" s="11" t="s">
+      <c r="C169" s="10" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="170" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="10" t="s">
+      <c r="B170" s="9" t="s">
         <v>647</v>
       </c>
-      <c r="C170" s="11" t="s">
+      <c r="C170" s="10" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="171" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B171" s="10" t="s">
+      <c r="B171" s="9" t="s">
         <v>649</v>
       </c>
-      <c r="C171" s="11" t="s">
+      <c r="C171" s="10" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="172" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="10" t="s">
+      <c r="B172" s="9" t="s">
         <v>651</v>
       </c>
-      <c r="C172" s="11" t="s">
+      <c r="C172" s="10" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="173" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="10" t="s">
+      <c r="B173" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="C173" s="11" t="s">
+      <c r="C173" s="10" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="174" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="10" t="s">
+      <c r="B174" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="C174" s="11" t="s">
+      <c r="C174" s="10" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="10" t="s">
+      <c r="B175" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="C175" s="11" t="s">
+      <c r="C175" s="10" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="10" t="s">
+      <c r="B176" s="9" t="s">
         <v>659</v>
       </c>
-      <c r="C176" s="11" t="s">
+      <c r="C176" s="10" t="s">
         <v>660</v>
       </c>
     </row>
     <row r="177" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="10" t="s">
+      <c r="B177" s="9" t="s">
         <v>661</v>
       </c>
-      <c r="C177" s="11" t="s">
+      <c r="C177" s="10" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="178" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="10" t="s">
+      <c r="B178" s="9" t="s">
         <v>663</v>
       </c>
-      <c r="C178" s="11" t="s">
+      <c r="C178" s="10" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="179" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="10" t="s">
+      <c r="B179" s="9" t="s">
         <v>665</v>
       </c>
-      <c r="C179" s="11" t="s">
+      <c r="C179" s="10" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="180" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B180" s="10" t="s">
+      <c r="B180" s="9" t="s">
         <v>667</v>
       </c>
-      <c r="C180" s="11" t="s">
+      <c r="C180" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="181" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B181" s="10" t="s">
+      <c r="B181" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="C181" s="11" t="s">
+      <c r="C181" s="10" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="182" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B182" s="10" t="s">
+      <c r="B182" s="9" t="s">
         <v>671</v>
       </c>
-      <c r="C182" s="11" t="s">
+      <c r="C182" s="10" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="183" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B183" s="10" t="s">
+      <c r="B183" s="9" t="s">
         <v>673</v>
       </c>
-      <c r="C183" s="11" t="s">
+      <c r="C183" s="10" t="s">
         <v>674</v>
       </c>
     </row>
     <row r="184" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="10" t="s">
+      <c r="B184" s="9" t="s">
         <v>675</v>
       </c>
-      <c r="C184" s="11" t="s">
+      <c r="C184" s="10" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="185" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="10" t="s">
+      <c r="B185" s="9" t="s">
         <v>677</v>
       </c>
-      <c r="C185" s="11" t="s">
+      <c r="C185" s="10" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="186" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="10" t="s">
+      <c r="B186" s="9" t="s">
         <v>679</v>
       </c>
-      <c r="C186" s="11" t="s">
+      <c r="C186" s="10" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="187" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="10" t="s">
+      <c r="B187" s="9" t="s">
         <v>681</v>
       </c>
-      <c r="C187" s="11" t="s">
+      <c r="C187" s="10" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="188" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="10" t="s">
+      <c r="B188" s="9" t="s">
         <v>683</v>
       </c>
-      <c r="C188" s="11" t="s">
+      <c r="C188" s="10" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="189" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="10" t="s">
+      <c r="B189" s="9" t="s">
         <v>685</v>
       </c>
-      <c r="C189" s="11" t="s">
+      <c r="C189" s="10" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="190" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="10" t="s">
+      <c r="B190" s="9" t="s">
         <v>687</v>
       </c>
-      <c r="C190" s="11" t="s">
+      <c r="C190" s="10" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="191" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="10" t="s">
+      <c r="B191" s="9" t="s">
         <v>689</v>
       </c>
-      <c r="C191" s="11" t="s">
+      <c r="C191" s="10" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="192" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="10" t="s">
+      <c r="B192" s="9" t="s">
         <v>691</v>
       </c>
-      <c r="C192" s="11" t="s">
+      <c r="C192" s="10" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="193" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="10" t="s">
+      <c r="B193" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="C193" s="11" t="s">
+      <c r="C193" s="10" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="194" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="10" t="s">
+      <c r="B194" s="9" t="s">
         <v>695</v>
       </c>
-      <c r="C194" s="11" t="s">
+      <c r="C194" s="10" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="195" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="10" t="s">
+      <c r="B195" s="9" t="s">
         <v>697</v>
       </c>
-      <c r="C195" s="11" t="s">
+      <c r="C195" s="10" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="196" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="10" t="s">
+      <c r="B196" s="9" t="s">
         <v>699</v>
       </c>
-      <c r="C196" s="11" t="s">
+      <c r="C196" s="10" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="197" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="10" t="s">
+      <c r="B197" s="9" t="s">
         <v>701</v>
       </c>
-      <c r="C197" s="11" t="s">
+      <c r="C197" s="10" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="198" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="10" t="s">
+      <c r="B198" s="9" t="s">
         <v>703</v>
       </c>
-      <c r="C198" s="11" t="s">
+      <c r="C198" s="10" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="199" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="10" t="s">
+      <c r="B199" s="9" t="s">
         <v>705</v>
       </c>
-      <c r="C199" s="11" t="s">
+      <c r="C199" s="10" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="200" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="10" t="s">
+      <c r="B200" s="9" t="s">
         <v>707</v>
       </c>
-      <c r="C200" s="11" t="s">
+      <c r="C200" s="10" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="201" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="10" t="s">
+      <c r="B201" s="9" t="s">
         <v>709</v>
       </c>
-      <c r="C201" s="11" t="s">
+      <c r="C201" s="10" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="202" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="10" t="s">
+      <c r="B202" s="9" t="s">
         <v>711</v>
       </c>
-      <c r="C202" s="11" t="s">
+      <c r="C202" s="10" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="203" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="10" t="s">
+      <c r="B203" s="9" t="s">
         <v>713</v>
       </c>
-      <c r="C203" s="11" t="s">
+      <c r="C203" s="10" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="204" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="10" t="s">
+      <c r="B204" s="9" t="s">
         <v>715</v>
       </c>
-      <c r="C204" s="11" t="s">
+      <c r="C204" s="10" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="205" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="10" t="s">
+      <c r="B205" s="9" t="s">
         <v>717</v>
       </c>
-      <c r="C205" s="11" t="s">
+      <c r="C205" s="10" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="206" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="10" t="s">
+      <c r="B206" s="9" t="s">
         <v>719</v>
       </c>
-      <c r="C206" s="11" t="s">
+      <c r="C206" s="10" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="207" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="10" t="s">
+      <c r="B207" s="9" t="s">
         <v>721</v>
       </c>
-      <c r="C207" s="11" t="s">
+      <c r="C207" s="10" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="208" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="10" t="s">
+      <c r="B208" s="9" t="s">
         <v>723</v>
       </c>
-      <c r="C208" s="11" t="s">
+      <c r="C208" s="10" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="209" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B209" s="10" t="s">
+      <c r="B209" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="C209" s="11" t="s">
+      <c r="C209" s="10" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="210" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B210" s="10" t="s">
+      <c r="B210" s="9" t="s">
         <v>727</v>
       </c>
-      <c r="C210" s="11" t="s">
+      <c r="C210" s="10" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="211" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B211" s="10" t="s">
+      <c r="B211" s="9" t="s">
         <v>729</v>
       </c>
-      <c r="C211" s="11" t="s">
+      <c r="C211" s="10" t="s">
         <v>730</v>
       </c>
     </row>
     <row r="212" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B212" s="10" t="s">
+      <c r="B212" s="9" t="s">
         <v>731</v>
       </c>
-      <c r="C212" s="11" t="s">
+      <c r="C212" s="10" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="213" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B213" s="10" t="s">
+      <c r="B213" s="9" t="s">
         <v>733</v>
       </c>
-      <c r="C213" s="11" t="s">
+      <c r="C213" s="10" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="214" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B214" s="10" t="s">
+      <c r="B214" s="9" t="s">
         <v>735</v>
       </c>
-      <c r="C214" s="11" t="s">
+      <c r="C214" s="10" t="s">
         <v>736</v>
       </c>
     </row>
     <row r="215" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B215" s="10" t="s">
+      <c r="B215" s="9" t="s">
         <v>737</v>
       </c>
-      <c r="C215" s="11" t="s">
+      <c r="C215" s="10" t="s">
         <v>738</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-8844 Customizing output of a SpreadsheetResult.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2BFD19-6912-4E51-8D73-50FA3D77E7E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B992E2-2A25-44B7-A81A-300DACD4BC93}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8295" yWindow="450" windowWidth="28845" windowHeight="20115" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,13 @@
     <sheet name="Runtime Scope" sheetId="4" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterate="1" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="819">
   <si>
     <t>Display Name</t>
   </si>
@@ -2502,6 +2507,15 @@
   </si>
   <si>
     <t>If true calculates all cells in the Spreadsheet, otherwise calculates only cells these are requred for a result. By default = true.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controls generation additional fields in an output model for the Spreadsheet. </t>
+  </si>
+  <si>
+    <t>verboseOutputModel</t>
+  </si>
+  <si>
+    <t>Verbose Output Model</t>
   </si>
 </sst>
 </file>
@@ -3141,7 +3155,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3230,6 +3244,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3734,207 +3751,207 @@
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
@@ -3967,10 +3984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK63"/>
+  <dimension ref="A1:AMK64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4002,154 +4019,154 @@
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -4161,27 +4178,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="51"/>
-      <c r="T11" s="51"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
+      <c r="T11" s="52"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -5194,7 +5211,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>747</v>
       </c>
@@ -5239,7 +5256,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>135</v>
       </c>
@@ -5286,7 +5303,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>156</v>
       </c>
@@ -5333,7 +5350,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>166</v>
       </c>
@@ -5374,7 +5391,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>170</v>
       </c>
@@ -5418,7 +5435,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>117</v>
       </c>
@@ -5465,7 +5482,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>124</v>
       </c>
@@ -5508,7 +5525,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>128</v>
       </c>
@@ -5553,7 +5570,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="41" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>175</v>
       </c>
@@ -5595,7 +5612,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>178</v>
       </c>
@@ -5636,7 +5653,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>184</v>
       </c>
@@ -5679,7 +5696,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1025" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>191</v>
       </c>
@@ -5720,7 +5737,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="45" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>193</v>
       </c>
@@ -5763,7 +5780,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>741</v>
       </c>
@@ -5804,12 +5821,13 @@
         <v>742</v>
       </c>
     </row>
-    <row r="47" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="46"/>
       <c r="B47" s="5" t="s">
-        <v>745</v>
+        <v>818</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>746</v>
+        <v>817</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>58</v>
@@ -5836,8 +5854,8 @@
         <v>809</v>
       </c>
       <c r="N47" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
@@ -5847,15 +5865,1020 @@
         <v>84</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>816</v>
+      </c>
+      <c r="U47" s="46"/>
+      <c r="V47" s="46"/>
+      <c r="W47" s="46"/>
+      <c r="X47" s="46"/>
+      <c r="Y47" s="46"/>
+      <c r="Z47" s="46"/>
+      <c r="AA47" s="46"/>
+      <c r="AB47" s="46"/>
+      <c r="AC47" s="46"/>
+      <c r="AD47" s="46"/>
+      <c r="AE47" s="46"/>
+      <c r="AF47" s="46"/>
+      <c r="AG47" s="46"/>
+      <c r="AH47" s="46"/>
+      <c r="AI47" s="46"/>
+      <c r="AJ47" s="46"/>
+      <c r="AK47" s="46"/>
+      <c r="AL47" s="46"/>
+      <c r="AM47" s="46"/>
+      <c r="AN47" s="46"/>
+      <c r="AO47" s="46"/>
+      <c r="AP47" s="46"/>
+      <c r="AQ47" s="46"/>
+      <c r="AR47" s="46"/>
+      <c r="AS47" s="46"/>
+      <c r="AT47" s="46"/>
+      <c r="AU47" s="46"/>
+      <c r="AV47" s="46"/>
+      <c r="AW47" s="46"/>
+      <c r="AX47" s="46"/>
+      <c r="AY47" s="46"/>
+      <c r="AZ47" s="46"/>
+      <c r="BA47" s="46"/>
+      <c r="BB47" s="46"/>
+      <c r="BC47" s="46"/>
+      <c r="BD47" s="46"/>
+      <c r="BE47" s="46"/>
+      <c r="BF47" s="46"/>
+      <c r="BG47" s="46"/>
+      <c r="BH47" s="46"/>
+      <c r="BI47" s="46"/>
+      <c r="BJ47" s="46"/>
+      <c r="BK47" s="46"/>
+      <c r="BL47" s="46"/>
+      <c r="BM47" s="46"/>
+      <c r="BN47" s="46"/>
+      <c r="BO47" s="46"/>
+      <c r="BP47" s="46"/>
+      <c r="BQ47" s="46"/>
+      <c r="BR47" s="46"/>
+      <c r="BS47" s="46"/>
+      <c r="BT47" s="46"/>
+      <c r="BU47" s="46"/>
+      <c r="BV47" s="46"/>
+      <c r="BW47" s="46"/>
+      <c r="BX47" s="46"/>
+      <c r="BY47" s="46"/>
+      <c r="BZ47" s="46"/>
+      <c r="CA47" s="46"/>
+      <c r="CB47" s="46"/>
+      <c r="CC47" s="46"/>
+      <c r="CD47" s="46"/>
+      <c r="CE47" s="46"/>
+      <c r="CF47" s="46"/>
+      <c r="CG47" s="46"/>
+      <c r="CH47" s="46"/>
+      <c r="CI47" s="46"/>
+      <c r="CJ47" s="46"/>
+      <c r="CK47" s="46"/>
+      <c r="CL47" s="46"/>
+      <c r="CM47" s="46"/>
+      <c r="CN47" s="46"/>
+      <c r="CO47" s="46"/>
+      <c r="CP47" s="46"/>
+      <c r="CQ47" s="46"/>
+      <c r="CR47" s="46"/>
+      <c r="CS47" s="46"/>
+      <c r="CT47" s="46"/>
+      <c r="CU47" s="46"/>
+      <c r="CV47" s="46"/>
+      <c r="CW47" s="46"/>
+      <c r="CX47" s="46"/>
+      <c r="CY47" s="46"/>
+      <c r="CZ47" s="46"/>
+      <c r="DA47" s="46"/>
+      <c r="DB47" s="46"/>
+      <c r="DC47" s="46"/>
+      <c r="DD47" s="46"/>
+      <c r="DE47" s="46"/>
+      <c r="DF47" s="46"/>
+      <c r="DG47" s="46"/>
+      <c r="DH47" s="46"/>
+      <c r="DI47" s="46"/>
+      <c r="DJ47" s="46"/>
+      <c r="DK47" s="46"/>
+      <c r="DL47" s="46"/>
+      <c r="DM47" s="46"/>
+      <c r="DN47" s="46"/>
+      <c r="DO47" s="46"/>
+      <c r="DP47" s="46"/>
+      <c r="DQ47" s="46"/>
+      <c r="DR47" s="46"/>
+      <c r="DS47" s="46"/>
+      <c r="DT47" s="46"/>
+      <c r="DU47" s="46"/>
+      <c r="DV47" s="46"/>
+      <c r="DW47" s="46"/>
+      <c r="DX47" s="46"/>
+      <c r="DY47" s="46"/>
+      <c r="DZ47" s="46"/>
+      <c r="EA47" s="46"/>
+      <c r="EB47" s="46"/>
+      <c r="EC47" s="46"/>
+      <c r="ED47" s="46"/>
+      <c r="EE47" s="46"/>
+      <c r="EF47" s="46"/>
+      <c r="EG47" s="46"/>
+      <c r="EH47" s="46"/>
+      <c r="EI47" s="46"/>
+      <c r="EJ47" s="46"/>
+      <c r="EK47" s="46"/>
+      <c r="EL47" s="46"/>
+      <c r="EM47" s="46"/>
+      <c r="EN47" s="46"/>
+      <c r="EO47" s="46"/>
+      <c r="EP47" s="46"/>
+      <c r="EQ47" s="46"/>
+      <c r="ER47" s="46"/>
+      <c r="ES47" s="46"/>
+      <c r="ET47" s="46"/>
+      <c r="EU47" s="46"/>
+      <c r="EV47" s="46"/>
+      <c r="EW47" s="46"/>
+      <c r="EX47" s="46"/>
+      <c r="EY47" s="46"/>
+      <c r="EZ47" s="46"/>
+      <c r="FA47" s="46"/>
+      <c r="FB47" s="46"/>
+      <c r="FC47" s="46"/>
+      <c r="FD47" s="46"/>
+      <c r="FE47" s="46"/>
+      <c r="FF47" s="46"/>
+      <c r="FG47" s="46"/>
+      <c r="FH47" s="46"/>
+      <c r="FI47" s="46"/>
+      <c r="FJ47" s="46"/>
+      <c r="FK47" s="46"/>
+      <c r="FL47" s="46"/>
+      <c r="FM47" s="46"/>
+      <c r="FN47" s="46"/>
+      <c r="FO47" s="46"/>
+      <c r="FP47" s="46"/>
+      <c r="FQ47" s="46"/>
+      <c r="FR47" s="46"/>
+      <c r="FS47" s="46"/>
+      <c r="FT47" s="46"/>
+      <c r="FU47" s="46"/>
+      <c r="FV47" s="46"/>
+      <c r="FW47" s="46"/>
+      <c r="FX47" s="46"/>
+      <c r="FY47" s="46"/>
+      <c r="FZ47" s="46"/>
+      <c r="GA47" s="46"/>
+      <c r="GB47" s="46"/>
+      <c r="GC47" s="46"/>
+      <c r="GD47" s="46"/>
+      <c r="GE47" s="46"/>
+      <c r="GF47" s="46"/>
+      <c r="GG47" s="46"/>
+      <c r="GH47" s="46"/>
+      <c r="GI47" s="46"/>
+      <c r="GJ47" s="46"/>
+      <c r="GK47" s="46"/>
+      <c r="GL47" s="46"/>
+      <c r="GM47" s="46"/>
+      <c r="GN47" s="46"/>
+      <c r="GO47" s="46"/>
+      <c r="GP47" s="46"/>
+      <c r="GQ47" s="46"/>
+      <c r="GR47" s="46"/>
+      <c r="GS47" s="46"/>
+      <c r="GT47" s="46"/>
+      <c r="GU47" s="46"/>
+      <c r="GV47" s="46"/>
+      <c r="GW47" s="46"/>
+      <c r="GX47" s="46"/>
+      <c r="GY47" s="46"/>
+      <c r="GZ47" s="46"/>
+      <c r="HA47" s="46"/>
+      <c r="HB47" s="46"/>
+      <c r="HC47" s="46"/>
+      <c r="HD47" s="46"/>
+      <c r="HE47" s="46"/>
+      <c r="HF47" s="46"/>
+      <c r="HG47" s="46"/>
+      <c r="HH47" s="46"/>
+      <c r="HI47" s="46"/>
+      <c r="HJ47" s="46"/>
+      <c r="HK47" s="46"/>
+      <c r="HL47" s="46"/>
+      <c r="HM47" s="46"/>
+      <c r="HN47" s="46"/>
+      <c r="HO47" s="46"/>
+      <c r="HP47" s="46"/>
+      <c r="HQ47" s="46"/>
+      <c r="HR47" s="46"/>
+      <c r="HS47" s="46"/>
+      <c r="HT47" s="46"/>
+      <c r="HU47" s="46"/>
+      <c r="HV47" s="46"/>
+      <c r="HW47" s="46"/>
+      <c r="HX47" s="46"/>
+      <c r="HY47" s="46"/>
+      <c r="HZ47" s="46"/>
+      <c r="IA47" s="46"/>
+      <c r="IB47" s="46"/>
+      <c r="IC47" s="46"/>
+      <c r="ID47" s="46"/>
+      <c r="IE47" s="46"/>
+      <c r="IF47" s="46"/>
+      <c r="IG47" s="46"/>
+      <c r="IH47" s="46"/>
+      <c r="II47" s="46"/>
+      <c r="IJ47" s="46"/>
+      <c r="IK47" s="46"/>
+      <c r="IL47" s="46"/>
+      <c r="IM47" s="46"/>
+      <c r="IN47" s="46"/>
+      <c r="IO47" s="46"/>
+      <c r="IP47" s="46"/>
+      <c r="IQ47" s="46"/>
+      <c r="IR47" s="46"/>
+      <c r="IS47" s="46"/>
+      <c r="IT47" s="46"/>
+      <c r="IU47" s="46"/>
+      <c r="IV47" s="46"/>
+      <c r="IW47" s="46"/>
+      <c r="IX47" s="46"/>
+      <c r="IY47" s="46"/>
+      <c r="IZ47" s="46"/>
+      <c r="JA47" s="46"/>
+      <c r="JB47" s="46"/>
+      <c r="JC47" s="46"/>
+      <c r="JD47" s="46"/>
+      <c r="JE47" s="46"/>
+      <c r="JF47" s="46"/>
+      <c r="JG47" s="46"/>
+      <c r="JH47" s="46"/>
+      <c r="JI47" s="46"/>
+      <c r="JJ47" s="46"/>
+      <c r="JK47" s="46"/>
+      <c r="JL47" s="46"/>
+      <c r="JM47" s="46"/>
+      <c r="JN47" s="46"/>
+      <c r="JO47" s="46"/>
+      <c r="JP47" s="46"/>
+      <c r="JQ47" s="46"/>
+      <c r="JR47" s="46"/>
+      <c r="JS47" s="46"/>
+      <c r="JT47" s="46"/>
+      <c r="JU47" s="46"/>
+      <c r="JV47" s="46"/>
+      <c r="JW47" s="46"/>
+      <c r="JX47" s="46"/>
+      <c r="JY47" s="46"/>
+      <c r="JZ47" s="46"/>
+      <c r="KA47" s="46"/>
+      <c r="KB47" s="46"/>
+      <c r="KC47" s="46"/>
+      <c r="KD47" s="46"/>
+      <c r="KE47" s="46"/>
+      <c r="KF47" s="46"/>
+      <c r="KG47" s="46"/>
+      <c r="KH47" s="46"/>
+      <c r="KI47" s="46"/>
+      <c r="KJ47" s="46"/>
+      <c r="KK47" s="46"/>
+      <c r="KL47" s="46"/>
+      <c r="KM47" s="46"/>
+      <c r="KN47" s="46"/>
+      <c r="KO47" s="46"/>
+      <c r="KP47" s="46"/>
+      <c r="KQ47" s="46"/>
+      <c r="KR47" s="46"/>
+      <c r="KS47" s="46"/>
+      <c r="KT47" s="46"/>
+      <c r="KU47" s="46"/>
+      <c r="KV47" s="46"/>
+      <c r="KW47" s="46"/>
+      <c r="KX47" s="46"/>
+      <c r="KY47" s="46"/>
+      <c r="KZ47" s="46"/>
+      <c r="LA47" s="46"/>
+      <c r="LB47" s="46"/>
+      <c r="LC47" s="46"/>
+      <c r="LD47" s="46"/>
+      <c r="LE47" s="46"/>
+      <c r="LF47" s="46"/>
+      <c r="LG47" s="46"/>
+      <c r="LH47" s="46"/>
+      <c r="LI47" s="46"/>
+      <c r="LJ47" s="46"/>
+      <c r="LK47" s="46"/>
+      <c r="LL47" s="46"/>
+      <c r="LM47" s="46"/>
+      <c r="LN47" s="46"/>
+      <c r="LO47" s="46"/>
+      <c r="LP47" s="46"/>
+      <c r="LQ47" s="46"/>
+      <c r="LR47" s="46"/>
+      <c r="LS47" s="46"/>
+      <c r="LT47" s="46"/>
+      <c r="LU47" s="46"/>
+      <c r="LV47" s="46"/>
+      <c r="LW47" s="46"/>
+      <c r="LX47" s="46"/>
+      <c r="LY47" s="46"/>
+      <c r="LZ47" s="46"/>
+      <c r="MA47" s="46"/>
+      <c r="MB47" s="46"/>
+      <c r="MC47" s="46"/>
+      <c r="MD47" s="46"/>
+      <c r="ME47" s="46"/>
+      <c r="MF47" s="46"/>
+      <c r="MG47" s="46"/>
+      <c r="MH47" s="46"/>
+      <c r="MI47" s="46"/>
+      <c r="MJ47" s="46"/>
+      <c r="MK47" s="46"/>
+      <c r="ML47" s="46"/>
+      <c r="MM47" s="46"/>
+      <c r="MN47" s="46"/>
+      <c r="MO47" s="46"/>
+      <c r="MP47" s="46"/>
+      <c r="MQ47" s="46"/>
+      <c r="MR47" s="46"/>
+      <c r="MS47" s="46"/>
+      <c r="MT47" s="46"/>
+      <c r="MU47" s="46"/>
+      <c r="MV47" s="46"/>
+      <c r="MW47" s="46"/>
+      <c r="MX47" s="46"/>
+      <c r="MY47" s="46"/>
+      <c r="MZ47" s="46"/>
+      <c r="NA47" s="46"/>
+      <c r="NB47" s="46"/>
+      <c r="NC47" s="46"/>
+      <c r="ND47" s="46"/>
+      <c r="NE47" s="46"/>
+      <c r="NF47" s="46"/>
+      <c r="NG47" s="46"/>
+      <c r="NH47" s="46"/>
+      <c r="NI47" s="46"/>
+      <c r="NJ47" s="46"/>
+      <c r="NK47" s="46"/>
+      <c r="NL47" s="46"/>
+      <c r="NM47" s="46"/>
+      <c r="NN47" s="46"/>
+      <c r="NO47" s="46"/>
+      <c r="NP47" s="46"/>
+      <c r="NQ47" s="46"/>
+      <c r="NR47" s="46"/>
+      <c r="NS47" s="46"/>
+      <c r="NT47" s="46"/>
+      <c r="NU47" s="46"/>
+      <c r="NV47" s="46"/>
+      <c r="NW47" s="46"/>
+      <c r="NX47" s="46"/>
+      <c r="NY47" s="46"/>
+      <c r="NZ47" s="46"/>
+      <c r="OA47" s="46"/>
+      <c r="OB47" s="46"/>
+      <c r="OC47" s="46"/>
+      <c r="OD47" s="46"/>
+      <c r="OE47" s="46"/>
+      <c r="OF47" s="46"/>
+      <c r="OG47" s="46"/>
+      <c r="OH47" s="46"/>
+      <c r="OI47" s="46"/>
+      <c r="OJ47" s="46"/>
+      <c r="OK47" s="46"/>
+      <c r="OL47" s="46"/>
+      <c r="OM47" s="46"/>
+      <c r="ON47" s="46"/>
+      <c r="OO47" s="46"/>
+      <c r="OP47" s="46"/>
+      <c r="OQ47" s="46"/>
+      <c r="OR47" s="46"/>
+      <c r="OS47" s="46"/>
+      <c r="OT47" s="46"/>
+      <c r="OU47" s="46"/>
+      <c r="OV47" s="46"/>
+      <c r="OW47" s="46"/>
+      <c r="OX47" s="46"/>
+      <c r="OY47" s="46"/>
+      <c r="OZ47" s="46"/>
+      <c r="PA47" s="46"/>
+      <c r="PB47" s="46"/>
+      <c r="PC47" s="46"/>
+      <c r="PD47" s="46"/>
+      <c r="PE47" s="46"/>
+      <c r="PF47" s="46"/>
+      <c r="PG47" s="46"/>
+      <c r="PH47" s="46"/>
+      <c r="PI47" s="46"/>
+      <c r="PJ47" s="46"/>
+      <c r="PK47" s="46"/>
+      <c r="PL47" s="46"/>
+      <c r="PM47" s="46"/>
+      <c r="PN47" s="46"/>
+      <c r="PO47" s="46"/>
+      <c r="PP47" s="46"/>
+      <c r="PQ47" s="46"/>
+      <c r="PR47" s="46"/>
+      <c r="PS47" s="46"/>
+      <c r="PT47" s="46"/>
+      <c r="PU47" s="46"/>
+      <c r="PV47" s="46"/>
+      <c r="PW47" s="46"/>
+      <c r="PX47" s="46"/>
+      <c r="PY47" s="46"/>
+      <c r="PZ47" s="46"/>
+      <c r="QA47" s="46"/>
+      <c r="QB47" s="46"/>
+      <c r="QC47" s="46"/>
+      <c r="QD47" s="46"/>
+      <c r="QE47" s="46"/>
+      <c r="QF47" s="46"/>
+      <c r="QG47" s="46"/>
+      <c r="QH47" s="46"/>
+      <c r="QI47" s="46"/>
+      <c r="QJ47" s="46"/>
+      <c r="QK47" s="46"/>
+      <c r="QL47" s="46"/>
+      <c r="QM47" s="46"/>
+      <c r="QN47" s="46"/>
+      <c r="QO47" s="46"/>
+      <c r="QP47" s="46"/>
+      <c r="QQ47" s="46"/>
+      <c r="QR47" s="46"/>
+      <c r="QS47" s="46"/>
+      <c r="QT47" s="46"/>
+      <c r="QU47" s="46"/>
+      <c r="QV47" s="46"/>
+      <c r="QW47" s="46"/>
+      <c r="QX47" s="46"/>
+      <c r="QY47" s="46"/>
+      <c r="QZ47" s="46"/>
+      <c r="RA47" s="46"/>
+      <c r="RB47" s="46"/>
+      <c r="RC47" s="46"/>
+      <c r="RD47" s="46"/>
+      <c r="RE47" s="46"/>
+      <c r="RF47" s="46"/>
+      <c r="RG47" s="46"/>
+      <c r="RH47" s="46"/>
+      <c r="RI47" s="46"/>
+      <c r="RJ47" s="46"/>
+      <c r="RK47" s="46"/>
+      <c r="RL47" s="46"/>
+      <c r="RM47" s="46"/>
+      <c r="RN47" s="46"/>
+      <c r="RO47" s="46"/>
+      <c r="RP47" s="46"/>
+      <c r="RQ47" s="46"/>
+      <c r="RR47" s="46"/>
+      <c r="RS47" s="46"/>
+      <c r="RT47" s="46"/>
+      <c r="RU47" s="46"/>
+      <c r="RV47" s="46"/>
+      <c r="RW47" s="46"/>
+      <c r="RX47" s="46"/>
+      <c r="RY47" s="46"/>
+      <c r="RZ47" s="46"/>
+      <c r="SA47" s="46"/>
+      <c r="SB47" s="46"/>
+      <c r="SC47" s="46"/>
+      <c r="SD47" s="46"/>
+      <c r="SE47" s="46"/>
+      <c r="SF47" s="46"/>
+      <c r="SG47" s="46"/>
+      <c r="SH47" s="46"/>
+      <c r="SI47" s="46"/>
+      <c r="SJ47" s="46"/>
+      <c r="SK47" s="46"/>
+      <c r="SL47" s="46"/>
+      <c r="SM47" s="46"/>
+      <c r="SN47" s="46"/>
+      <c r="SO47" s="46"/>
+      <c r="SP47" s="46"/>
+      <c r="SQ47" s="46"/>
+      <c r="SR47" s="46"/>
+      <c r="SS47" s="46"/>
+      <c r="ST47" s="46"/>
+      <c r="SU47" s="46"/>
+      <c r="SV47" s="46"/>
+      <c r="SW47" s="46"/>
+      <c r="SX47" s="46"/>
+      <c r="SY47" s="46"/>
+      <c r="SZ47" s="46"/>
+      <c r="TA47" s="46"/>
+      <c r="TB47" s="46"/>
+      <c r="TC47" s="46"/>
+      <c r="TD47" s="46"/>
+      <c r="TE47" s="46"/>
+      <c r="TF47" s="46"/>
+      <c r="TG47" s="46"/>
+      <c r="TH47" s="46"/>
+      <c r="TI47" s="46"/>
+      <c r="TJ47" s="46"/>
+      <c r="TK47" s="46"/>
+      <c r="TL47" s="46"/>
+      <c r="TM47" s="46"/>
+      <c r="TN47" s="46"/>
+      <c r="TO47" s="46"/>
+      <c r="TP47" s="46"/>
+      <c r="TQ47" s="46"/>
+      <c r="TR47" s="46"/>
+      <c r="TS47" s="46"/>
+      <c r="TT47" s="46"/>
+      <c r="TU47" s="46"/>
+      <c r="TV47" s="46"/>
+      <c r="TW47" s="46"/>
+      <c r="TX47" s="46"/>
+      <c r="TY47" s="46"/>
+      <c r="TZ47" s="46"/>
+      <c r="UA47" s="46"/>
+      <c r="UB47" s="46"/>
+      <c r="UC47" s="46"/>
+      <c r="UD47" s="46"/>
+      <c r="UE47" s="46"/>
+      <c r="UF47" s="46"/>
+      <c r="UG47" s="46"/>
+      <c r="UH47" s="46"/>
+      <c r="UI47" s="46"/>
+      <c r="UJ47" s="46"/>
+      <c r="UK47" s="46"/>
+      <c r="UL47" s="46"/>
+      <c r="UM47" s="46"/>
+      <c r="UN47" s="46"/>
+      <c r="UO47" s="46"/>
+      <c r="UP47" s="46"/>
+      <c r="UQ47" s="46"/>
+      <c r="UR47" s="46"/>
+      <c r="US47" s="46"/>
+      <c r="UT47" s="46"/>
+      <c r="UU47" s="46"/>
+      <c r="UV47" s="46"/>
+      <c r="UW47" s="46"/>
+      <c r="UX47" s="46"/>
+      <c r="UY47" s="46"/>
+      <c r="UZ47" s="46"/>
+      <c r="VA47" s="46"/>
+      <c r="VB47" s="46"/>
+      <c r="VC47" s="46"/>
+      <c r="VD47" s="46"/>
+      <c r="VE47" s="46"/>
+      <c r="VF47" s="46"/>
+      <c r="VG47" s="46"/>
+      <c r="VH47" s="46"/>
+      <c r="VI47" s="46"/>
+      <c r="VJ47" s="46"/>
+      <c r="VK47" s="46"/>
+      <c r="VL47" s="46"/>
+      <c r="VM47" s="46"/>
+      <c r="VN47" s="46"/>
+      <c r="VO47" s="46"/>
+      <c r="VP47" s="46"/>
+      <c r="VQ47" s="46"/>
+      <c r="VR47" s="46"/>
+      <c r="VS47" s="46"/>
+      <c r="VT47" s="46"/>
+      <c r="VU47" s="46"/>
+      <c r="VV47" s="46"/>
+      <c r="VW47" s="46"/>
+      <c r="VX47" s="46"/>
+      <c r="VY47" s="46"/>
+      <c r="VZ47" s="46"/>
+      <c r="WA47" s="46"/>
+      <c r="WB47" s="46"/>
+      <c r="WC47" s="46"/>
+      <c r="WD47" s="46"/>
+      <c r="WE47" s="46"/>
+      <c r="WF47" s="46"/>
+      <c r="WG47" s="46"/>
+      <c r="WH47" s="46"/>
+      <c r="WI47" s="46"/>
+      <c r="WJ47" s="46"/>
+      <c r="WK47" s="46"/>
+      <c r="WL47" s="46"/>
+      <c r="WM47" s="46"/>
+      <c r="WN47" s="46"/>
+      <c r="WO47" s="46"/>
+      <c r="WP47" s="46"/>
+      <c r="WQ47" s="46"/>
+      <c r="WR47" s="46"/>
+      <c r="WS47" s="46"/>
+      <c r="WT47" s="46"/>
+      <c r="WU47" s="46"/>
+      <c r="WV47" s="46"/>
+      <c r="WW47" s="46"/>
+      <c r="WX47" s="46"/>
+      <c r="WY47" s="46"/>
+      <c r="WZ47" s="46"/>
+      <c r="XA47" s="46"/>
+      <c r="XB47" s="46"/>
+      <c r="XC47" s="46"/>
+      <c r="XD47" s="46"/>
+      <c r="XE47" s="46"/>
+      <c r="XF47" s="46"/>
+      <c r="XG47" s="46"/>
+      <c r="XH47" s="46"/>
+      <c r="XI47" s="46"/>
+      <c r="XJ47" s="46"/>
+      <c r="XK47" s="46"/>
+      <c r="XL47" s="46"/>
+      <c r="XM47" s="46"/>
+      <c r="XN47" s="46"/>
+      <c r="XO47" s="46"/>
+      <c r="XP47" s="46"/>
+      <c r="XQ47" s="46"/>
+      <c r="XR47" s="46"/>
+      <c r="XS47" s="46"/>
+      <c r="XT47" s="46"/>
+      <c r="XU47" s="46"/>
+      <c r="XV47" s="46"/>
+      <c r="XW47" s="46"/>
+      <c r="XX47" s="46"/>
+      <c r="XY47" s="46"/>
+      <c r="XZ47" s="46"/>
+      <c r="YA47" s="46"/>
+      <c r="YB47" s="46"/>
+      <c r="YC47" s="46"/>
+      <c r="YD47" s="46"/>
+      <c r="YE47" s="46"/>
+      <c r="YF47" s="46"/>
+      <c r="YG47" s="46"/>
+      <c r="YH47" s="46"/>
+      <c r="YI47" s="46"/>
+      <c r="YJ47" s="46"/>
+      <c r="YK47" s="46"/>
+      <c r="YL47" s="46"/>
+      <c r="YM47" s="46"/>
+      <c r="YN47" s="46"/>
+      <c r="YO47" s="46"/>
+      <c r="YP47" s="46"/>
+      <c r="YQ47" s="46"/>
+      <c r="YR47" s="46"/>
+      <c r="YS47" s="46"/>
+      <c r="YT47" s="46"/>
+      <c r="YU47" s="46"/>
+      <c r="YV47" s="46"/>
+      <c r="YW47" s="46"/>
+      <c r="YX47" s="46"/>
+      <c r="YY47" s="46"/>
+      <c r="YZ47" s="46"/>
+      <c r="ZA47" s="46"/>
+      <c r="ZB47" s="46"/>
+      <c r="ZC47" s="46"/>
+      <c r="ZD47" s="46"/>
+      <c r="ZE47" s="46"/>
+      <c r="ZF47" s="46"/>
+      <c r="ZG47" s="46"/>
+      <c r="ZH47" s="46"/>
+      <c r="ZI47" s="46"/>
+      <c r="ZJ47" s="46"/>
+      <c r="ZK47" s="46"/>
+      <c r="ZL47" s="46"/>
+      <c r="ZM47" s="46"/>
+      <c r="ZN47" s="46"/>
+      <c r="ZO47" s="46"/>
+      <c r="ZP47" s="46"/>
+      <c r="ZQ47" s="46"/>
+      <c r="ZR47" s="46"/>
+      <c r="ZS47" s="46"/>
+      <c r="ZT47" s="46"/>
+      <c r="ZU47" s="46"/>
+      <c r="ZV47" s="46"/>
+      <c r="ZW47" s="46"/>
+      <c r="ZX47" s="46"/>
+      <c r="ZY47" s="46"/>
+      <c r="ZZ47" s="46"/>
+      <c r="AAA47" s="46"/>
+      <c r="AAB47" s="46"/>
+      <c r="AAC47" s="46"/>
+      <c r="AAD47" s="46"/>
+      <c r="AAE47" s="46"/>
+      <c r="AAF47" s="46"/>
+      <c r="AAG47" s="46"/>
+      <c r="AAH47" s="46"/>
+      <c r="AAI47" s="46"/>
+      <c r="AAJ47" s="46"/>
+      <c r="AAK47" s="46"/>
+      <c r="AAL47" s="46"/>
+      <c r="AAM47" s="46"/>
+      <c r="AAN47" s="46"/>
+      <c r="AAO47" s="46"/>
+      <c r="AAP47" s="46"/>
+      <c r="AAQ47" s="46"/>
+      <c r="AAR47" s="46"/>
+      <c r="AAS47" s="46"/>
+      <c r="AAT47" s="46"/>
+      <c r="AAU47" s="46"/>
+      <c r="AAV47" s="46"/>
+      <c r="AAW47" s="46"/>
+      <c r="AAX47" s="46"/>
+      <c r="AAY47" s="46"/>
+      <c r="AAZ47" s="46"/>
+      <c r="ABA47" s="46"/>
+      <c r="ABB47" s="46"/>
+      <c r="ABC47" s="46"/>
+      <c r="ABD47" s="46"/>
+      <c r="ABE47" s="46"/>
+      <c r="ABF47" s="46"/>
+      <c r="ABG47" s="46"/>
+      <c r="ABH47" s="46"/>
+      <c r="ABI47" s="46"/>
+      <c r="ABJ47" s="46"/>
+      <c r="ABK47" s="46"/>
+      <c r="ABL47" s="46"/>
+      <c r="ABM47" s="46"/>
+      <c r="ABN47" s="46"/>
+      <c r="ABO47" s="46"/>
+      <c r="ABP47" s="46"/>
+      <c r="ABQ47" s="46"/>
+      <c r="ABR47" s="46"/>
+      <c r="ABS47" s="46"/>
+      <c r="ABT47" s="46"/>
+      <c r="ABU47" s="46"/>
+      <c r="ABV47" s="46"/>
+      <c r="ABW47" s="46"/>
+      <c r="ABX47" s="46"/>
+      <c r="ABY47" s="46"/>
+      <c r="ABZ47" s="46"/>
+      <c r="ACA47" s="46"/>
+      <c r="ACB47" s="46"/>
+      <c r="ACC47" s="46"/>
+      <c r="ACD47" s="46"/>
+      <c r="ACE47" s="46"/>
+      <c r="ACF47" s="46"/>
+      <c r="ACG47" s="46"/>
+      <c r="ACH47" s="46"/>
+      <c r="ACI47" s="46"/>
+      <c r="ACJ47" s="46"/>
+      <c r="ACK47" s="46"/>
+      <c r="ACL47" s="46"/>
+      <c r="ACM47" s="46"/>
+      <c r="ACN47" s="46"/>
+      <c r="ACO47" s="46"/>
+      <c r="ACP47" s="46"/>
+      <c r="ACQ47" s="46"/>
+      <c r="ACR47" s="46"/>
+      <c r="ACS47" s="46"/>
+      <c r="ACT47" s="46"/>
+      <c r="ACU47" s="46"/>
+      <c r="ACV47" s="46"/>
+      <c r="ACW47" s="46"/>
+      <c r="ACX47" s="46"/>
+      <c r="ACY47" s="46"/>
+      <c r="ACZ47" s="46"/>
+      <c r="ADA47" s="46"/>
+      <c r="ADB47" s="46"/>
+      <c r="ADC47" s="46"/>
+      <c r="ADD47" s="46"/>
+      <c r="ADE47" s="46"/>
+      <c r="ADF47" s="46"/>
+      <c r="ADG47" s="46"/>
+      <c r="ADH47" s="46"/>
+      <c r="ADI47" s="46"/>
+      <c r="ADJ47" s="46"/>
+      <c r="ADK47" s="46"/>
+      <c r="ADL47" s="46"/>
+      <c r="ADM47" s="46"/>
+      <c r="ADN47" s="46"/>
+      <c r="ADO47" s="46"/>
+      <c r="ADP47" s="46"/>
+      <c r="ADQ47" s="46"/>
+      <c r="ADR47" s="46"/>
+      <c r="ADS47" s="46"/>
+      <c r="ADT47" s="46"/>
+      <c r="ADU47" s="46"/>
+      <c r="ADV47" s="46"/>
+      <c r="ADW47" s="46"/>
+      <c r="ADX47" s="46"/>
+      <c r="ADY47" s="46"/>
+      <c r="ADZ47" s="46"/>
+      <c r="AEA47" s="46"/>
+      <c r="AEB47" s="46"/>
+      <c r="AEC47" s="46"/>
+      <c r="AED47" s="46"/>
+      <c r="AEE47" s="46"/>
+      <c r="AEF47" s="46"/>
+      <c r="AEG47" s="46"/>
+      <c r="AEH47" s="46"/>
+      <c r="AEI47" s="46"/>
+      <c r="AEJ47" s="46"/>
+      <c r="AEK47" s="46"/>
+      <c r="AEL47" s="46"/>
+      <c r="AEM47" s="46"/>
+      <c r="AEN47" s="46"/>
+      <c r="AEO47" s="46"/>
+      <c r="AEP47" s="46"/>
+      <c r="AEQ47" s="46"/>
+      <c r="AER47" s="46"/>
+      <c r="AES47" s="46"/>
+      <c r="AET47" s="46"/>
+      <c r="AEU47" s="46"/>
+      <c r="AEV47" s="46"/>
+      <c r="AEW47" s="46"/>
+      <c r="AEX47" s="46"/>
+      <c r="AEY47" s="46"/>
+      <c r="AEZ47" s="46"/>
+      <c r="AFA47" s="46"/>
+      <c r="AFB47" s="46"/>
+      <c r="AFC47" s="46"/>
+      <c r="AFD47" s="46"/>
+      <c r="AFE47" s="46"/>
+      <c r="AFF47" s="46"/>
+      <c r="AFG47" s="46"/>
+      <c r="AFH47" s="46"/>
+      <c r="AFI47" s="46"/>
+      <c r="AFJ47" s="46"/>
+      <c r="AFK47" s="46"/>
+      <c r="AFL47" s="46"/>
+      <c r="AFM47" s="46"/>
+      <c r="AFN47" s="46"/>
+      <c r="AFO47" s="46"/>
+      <c r="AFP47" s="46"/>
+      <c r="AFQ47" s="46"/>
+      <c r="AFR47" s="46"/>
+      <c r="AFS47" s="46"/>
+      <c r="AFT47" s="46"/>
+      <c r="AFU47" s="46"/>
+      <c r="AFV47" s="46"/>
+      <c r="AFW47" s="46"/>
+      <c r="AFX47" s="46"/>
+      <c r="AFY47" s="46"/>
+      <c r="AFZ47" s="46"/>
+      <c r="AGA47" s="46"/>
+      <c r="AGB47" s="46"/>
+      <c r="AGC47" s="46"/>
+      <c r="AGD47" s="46"/>
+      <c r="AGE47" s="46"/>
+      <c r="AGF47" s="46"/>
+      <c r="AGG47" s="46"/>
+      <c r="AGH47" s="46"/>
+      <c r="AGI47" s="46"/>
+      <c r="AGJ47" s="46"/>
+      <c r="AGK47" s="46"/>
+      <c r="AGL47" s="46"/>
+      <c r="AGM47" s="46"/>
+      <c r="AGN47" s="46"/>
+      <c r="AGO47" s="46"/>
+      <c r="AGP47" s="46"/>
+      <c r="AGQ47" s="46"/>
+      <c r="AGR47" s="46"/>
+      <c r="AGS47" s="46"/>
+      <c r="AGT47" s="46"/>
+      <c r="AGU47" s="46"/>
+      <c r="AGV47" s="46"/>
+      <c r="AGW47" s="46"/>
+      <c r="AGX47" s="46"/>
+      <c r="AGY47" s="46"/>
+      <c r="AGZ47" s="46"/>
+      <c r="AHA47" s="46"/>
+      <c r="AHB47" s="46"/>
+      <c r="AHC47" s="46"/>
+      <c r="AHD47" s="46"/>
+      <c r="AHE47" s="46"/>
+      <c r="AHF47" s="46"/>
+      <c r="AHG47" s="46"/>
+      <c r="AHH47" s="46"/>
+      <c r="AHI47" s="46"/>
+      <c r="AHJ47" s="46"/>
+      <c r="AHK47" s="46"/>
+      <c r="AHL47" s="46"/>
+      <c r="AHM47" s="46"/>
+      <c r="AHN47" s="46"/>
+      <c r="AHO47" s="46"/>
+      <c r="AHP47" s="46"/>
+      <c r="AHQ47" s="46"/>
+      <c r="AHR47" s="46"/>
+      <c r="AHS47" s="46"/>
+      <c r="AHT47" s="46"/>
+      <c r="AHU47" s="46"/>
+      <c r="AHV47" s="46"/>
+      <c r="AHW47" s="46"/>
+      <c r="AHX47" s="46"/>
+      <c r="AHY47" s="46"/>
+      <c r="AHZ47" s="46"/>
+      <c r="AIA47" s="46"/>
+      <c r="AIB47" s="46"/>
+      <c r="AIC47" s="46"/>
+      <c r="AID47" s="46"/>
+      <c r="AIE47" s="46"/>
+      <c r="AIF47" s="46"/>
+      <c r="AIG47" s="46"/>
+      <c r="AIH47" s="46"/>
+      <c r="AII47" s="46"/>
+      <c r="AIJ47" s="46"/>
+      <c r="AIK47" s="46"/>
+      <c r="AIL47" s="46"/>
+      <c r="AIM47" s="46"/>
+      <c r="AIN47" s="46"/>
+      <c r="AIO47" s="46"/>
+      <c r="AIP47" s="46"/>
+      <c r="AIQ47" s="46"/>
+      <c r="AIR47" s="46"/>
+      <c r="AIS47" s="46"/>
+      <c r="AIT47" s="46"/>
+      <c r="AIU47" s="46"/>
+      <c r="AIV47" s="46"/>
+      <c r="AIW47" s="46"/>
+      <c r="AIX47" s="46"/>
+      <c r="AIY47" s="46"/>
+      <c r="AIZ47" s="46"/>
+      <c r="AJA47" s="46"/>
+      <c r="AJB47" s="46"/>
+      <c r="AJC47" s="46"/>
+      <c r="AJD47" s="46"/>
+      <c r="AJE47" s="46"/>
+      <c r="AJF47" s="46"/>
+      <c r="AJG47" s="46"/>
+      <c r="AJH47" s="46"/>
+      <c r="AJI47" s="46"/>
+      <c r="AJJ47" s="46"/>
+      <c r="AJK47" s="46"/>
+      <c r="AJL47" s="46"/>
+      <c r="AJM47" s="46"/>
+      <c r="AJN47" s="46"/>
+      <c r="AJO47" s="46"/>
+      <c r="AJP47" s="46"/>
+      <c r="AJQ47" s="46"/>
+      <c r="AJR47" s="46"/>
+      <c r="AJS47" s="46"/>
+      <c r="AJT47" s="46"/>
+      <c r="AJU47" s="46"/>
+      <c r="AJV47" s="46"/>
+      <c r="AJW47" s="46"/>
+      <c r="AJX47" s="46"/>
+      <c r="AJY47" s="46"/>
+      <c r="AJZ47" s="46"/>
+      <c r="AKA47" s="46"/>
+      <c r="AKB47" s="46"/>
+      <c r="AKC47" s="46"/>
+      <c r="AKD47" s="46"/>
+      <c r="AKE47" s="46"/>
+      <c r="AKF47" s="46"/>
+      <c r="AKG47" s="46"/>
+      <c r="AKH47" s="46"/>
+      <c r="AKI47" s="46"/>
+      <c r="AKJ47" s="46"/>
+      <c r="AKK47" s="46"/>
+      <c r="AKL47" s="46"/>
+      <c r="AKM47" s="46"/>
+      <c r="AKN47" s="46"/>
+      <c r="AKO47" s="46"/>
+      <c r="AKP47" s="46"/>
+      <c r="AKQ47" s="46"/>
+      <c r="AKR47" s="46"/>
+      <c r="AKS47" s="46"/>
+      <c r="AKT47" s="46"/>
+      <c r="AKU47" s="46"/>
+      <c r="AKV47" s="46"/>
+      <c r="AKW47" s="46"/>
+      <c r="AKX47" s="46"/>
+      <c r="AKY47" s="46"/>
+      <c r="AKZ47" s="46"/>
+      <c r="ALA47" s="46"/>
+      <c r="ALB47" s="46"/>
+      <c r="ALC47" s="46"/>
+      <c r="ALD47" s="46"/>
+      <c r="ALE47" s="46"/>
+      <c r="ALF47" s="46"/>
+      <c r="ALG47" s="46"/>
+      <c r="ALH47" s="46"/>
+      <c r="ALI47" s="46"/>
+      <c r="ALJ47" s="46"/>
+      <c r="ALK47" s="46"/>
+      <c r="ALL47" s="46"/>
+      <c r="ALM47" s="46"/>
+      <c r="ALN47" s="46"/>
+      <c r="ALO47" s="46"/>
+      <c r="ALP47" s="46"/>
+      <c r="ALQ47" s="46"/>
+      <c r="ALR47" s="46"/>
+      <c r="ALS47" s="46"/>
+      <c r="ALT47" s="46"/>
+      <c r="ALU47" s="46"/>
+      <c r="ALV47" s="46"/>
+      <c r="ALW47" s="46"/>
+      <c r="ALX47" s="46"/>
+      <c r="ALY47" s="46"/>
+      <c r="ALZ47" s="46"/>
+      <c r="AMA47" s="46"/>
+      <c r="AMB47" s="46"/>
+      <c r="AMC47" s="46"/>
+      <c r="AMD47" s="46"/>
+      <c r="AME47" s="46"/>
+      <c r="AMF47" s="46"/>
+      <c r="AMG47" s="46"/>
+      <c r="AMH47" s="46"/>
+      <c r="AMI47" s="46"/>
+      <c r="AMJ47" s="46"/>
+      <c r="AMK47" s="46"/>
+    </row>
+    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>814</v>
+        <v>745</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>813</v>
+        <v>746</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>58</v>
@@ -5893,15 +6916,15 @@
         <v>84</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>815</v>
+        <v>803</v>
       </c>
     </row>
     <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>802</v>
+        <v>813</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>58</v>
@@ -5925,11 +6948,11 @@
         <v>58</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>749</v>
+        <v>809</v>
       </c>
       <c r="N49" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
@@ -5939,30 +6962,28 @@
         <v>84</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="50" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>804</v>
+        <v>811</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>806</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="F50" s="5"/>
       <c r="G50" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
@@ -5970,15 +6991,16 @@
         <v>58</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="M50" s="5" t="s">
         <v>749</v>
       </c>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5" t="s">
-        <v>807</v>
-      </c>
+      <c r="N50" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O50" s="5"/>
       <c r="P50" s="5"/>
       <c r="Q50" s="5"/>
       <c r="R50" s="5"/>
@@ -5986,87 +7008,134 @@
         <v>84</v>
       </c>
       <c r="T50" s="5" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="T51" s="5" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="54" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
+    <row r="55" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5" t="s">
+      <c r="D55" s="5"/>
+      <c r="E55" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H54" s="5" t="s">
+      <c r="F55" s="5"/>
+      <c r="G55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5" t="s">
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="5"/>
-      <c r="R54" s="5"/>
-      <c r="S54" s="5" t="s">
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="T54" s="5" t="s">
+      <c r="T55" s="5" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="58" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="51" t="s">
-        <v>202</v>
-      </c>
-      <c r="C58" s="51"/>
     </row>
     <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="C59" s="52"/>
+    </row>
+    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="53" t="s">
         <v>203</v>
       </c>
-      <c r="C59" s="52"/>
-    </row>
-    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="52" t="s">
-        <v>204</v>
-      </c>
-      <c r="C60" s="52"/>
+      <c r="C60" s="53"/>
     </row>
     <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="53" t="s">
+        <v>204</v>
+      </c>
+      <c r="C61" s="53"/>
+    </row>
+    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="54" t="s">
         <v>205</v>
       </c>
-      <c r="C61" s="53"/>
-    </row>
-    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="53" t="s">
+      <c r="C62" s="54"/>
+    </row>
+    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="54" t="s">
         <v>206</v>
       </c>
-      <c r="C62" s="53"/>
-    </row>
-    <row r="63" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="50" t="s">
+      <c r="C63" s="54"/>
+    </row>
+    <row r="64" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="51" t="s">
         <v>752</v>
       </c>
-      <c r="C63" s="50"/>
+      <c r="C64" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C3:L3"/>
@@ -6077,11 +7146,11 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
-    <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B61:C61"/>
     <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -6104,16 +7173,16 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>208</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -6124,7 +7193,7 @@
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="55"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="16" t="s">
         <v>210</v>
       </c>
@@ -6133,7 +7202,7 @@
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="55"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="16" t="s">
         <v>211</v>
       </c>
@@ -6142,7 +7211,7 @@
       <c r="F8" s="16"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="55"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="16" t="s">
         <v>212</v>
       </c>
@@ -6151,13 +7220,13 @@
       <c r="F9" s="16"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="55"/>
-      <c r="C10" s="56" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="57" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6192,12 +7261,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
@@ -6420,18 +7489,18 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="63"/>
+      <c r="C2" s="64"/>
       <c r="E2" s="23" t="s">
         <v>221</v>
       </c>
       <c r="F2" s="24"/>
-      <c r="I2" s="62" t="s">
+      <c r="I2" s="63" t="s">
         <v>222</v>
       </c>
-      <c r="J2" s="63"/>
+      <c r="J2" s="64"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
@@ -6622,10 +7691,10 @@
       <c r="F13" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="63" t="s">
         <v>267</v>
       </c>
-      <c r="J13" s="63"/>
+      <c r="J13" s="64"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
@@ -6808,10 +7877,10 @@
       <c r="F23" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="I23" s="62" t="s">
+      <c r="I23" s="63" t="s">
         <v>315</v>
       </c>
-      <c r="J23" s="63"/>
+      <c r="J23" s="64"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
@@ -6968,10 +8037,10 @@
       <c r="F32" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="I32" s="62" t="s">
+      <c r="I32" s="63" t="s">
         <v>753</v>
       </c>
-      <c r="J32" s="63"/>
+      <c r="J32" s="64"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="20" t="s">
@@ -7094,10 +8163,10 @@
       <c r="F39" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="I39" s="62" t="s">
+      <c r="I39" s="63" t="s">
         <v>786</v>
       </c>
-      <c r="J39" s="63"/>
+      <c r="J39" s="64"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="20" t="s">
@@ -7220,10 +8289,10 @@
       <c r="F46" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="I46" s="62" t="s">
+      <c r="I46" s="63" t="s">
         <v>796</v>
       </c>
-      <c r="J46" s="63"/>
+      <c r="J46" s="64"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="20" t="s">
@@ -7412,10 +8481,10 @@
       <c r="C59" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="E59" s="62" t="s">
+      <c r="E59" s="63" t="s">
         <v>762</v>
       </c>
-      <c r="F59" s="63"/>
+      <c r="F59" s="64"/>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="20" t="s">
@@ -8133,10 +9202,10 @@
     </row>
     <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="60" t="s">
+      <c r="B143" s="61" t="s">
         <v>598</v>
       </c>
-      <c r="C143" s="61"/>
+      <c r="C143" s="62"/>
     </row>
     <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="7" t="s">

</xml_diff>

<commit_message>
EPBDS-8844 Customizing output of a SpreadsheetResult. Refactoring.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B992E2-2A25-44B7-A81A-300DACD4BC93}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1F7495-25B4-44BD-ADCF-239C08E1694E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8295" yWindow="450" windowWidth="28845" windowHeight="20115" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="1470" windowWidth="28875" windowHeight="17610" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -2509,13 +2509,13 @@
     <t>If true calculates all cells in the Spreadsheet, otherwise calculates only cells these are requred for a result. By default = true.</t>
   </si>
   <si>
-    <t xml:space="preserve">Controls generation additional fields in an output model for the Spreadsheet. </t>
-  </si>
-  <si>
-    <t>verboseOutputModel</t>
-  </si>
-  <si>
-    <t>Verbose Output Model</t>
+    <t xml:space="preserve">Controls generation additional fields in an plain model for the Spreadsheet. </t>
+  </si>
+  <si>
+    <t>Detaled Plain Model</t>
+  </si>
+  <si>
+    <t>detailedPlainModel</t>
   </si>
 </sst>
 </file>
@@ -3987,7 +3987,7 @@
   <dimension ref="A1:AMK64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5824,10 +5824,10 @@
     <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="46"/>
       <c r="B47" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>818</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>817</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
EPBDS-9556 Fix merge conflict in binary file.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\openl\DEV\org.openl.rules\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AFD273-97BE-4C9A-9CAE-872561C7C575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437664F7-2FC3-4F3D-9670-08DE60001F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,12 @@
     <sheet name="Runtime Scope" sheetId="4" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="181029" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="823">
   <si>
     <t>Display Name</t>
   </si>
@@ -2519,6 +2517,18 @@
   </si>
   <si>
     <t>MM/dd/yyyy hh:mm a</t>
+  </si>
+  <si>
+    <t>Spreadsheet Result Package</t>
+  </si>
+  <si>
+    <t>org.openl.generated.spreadsheetresults</t>
+  </si>
+  <si>
+    <t>The name of the package for spreadsheet result beans generation</t>
+  </si>
+  <si>
+    <t>spreadsheetResultPackage</t>
   </si>
 </sst>
 </file>
@@ -3158,7 +3168,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3247,6 +3257,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3748,213 +3761,213 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-    </row>
-    <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+    </row>
+    <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-    </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+    </row>
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-    </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+    </row>
+    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-    </row>
-    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-    </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+    </row>
+    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-    </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+    </row>
+    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-    </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+    </row>
+    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-    </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+    </row>
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-    </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+    </row>
+    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-    </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+    </row>
+    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="49" t="s">
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
@@ -3987,191 +4000,191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK64"/>
+  <dimension ref="A1:AMK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="17.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="1"/>
+    <col min="2" max="2" width="17.46484375" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="19.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.53125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.86328125" style="1"/>
+    <col min="6" max="6" width="19.1328125" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.86328125" style="1" customWidth="1"/>
     <col min="9" max="9" width="24.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="39.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="22.86328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="39.46484375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.86328125" style="1"/>
     <col min="15" max="15" width="20.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="8.86328125" style="1"/>
     <col min="17" max="17" width="14" style="1" customWidth="1"/>
     <col min="18" max="18" width="13.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="26.88671875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="45.88671875" style="1" customWidth="1"/>
-    <col min="21" max="1025" width="8.88671875" style="1"/>
+    <col min="19" max="19" width="26.86328125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="45.86328125" style="1" customWidth="1"/>
+    <col min="21" max="1025" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-    </row>
-    <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+    </row>
+    <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-    </row>
-    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+    </row>
+    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-    </row>
-    <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+    </row>
+    <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-    </row>
-    <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+    </row>
+    <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-    </row>
-    <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+    </row>
+    <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-    </row>
-    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+    </row>
+    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-    </row>
-    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+    </row>
+    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-    </row>
-    <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+    </row>
+    <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-    </row>
-    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+    </row>
+    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -4180,30 +4193,30 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="52" t="s">
+    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-    </row>
-    <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
+      <c r="T11" s="53"/>
+    </row>
+    <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
@@ -4262,7 +4275,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
@@ -4321,7 +4334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
@@ -4368,7 +4381,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="5" t="s">
         <v>66</v>
       </c>
@@ -4411,7 +4424,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="5" t="s">
         <v>100</v>
       </c>
@@ -4458,7 +4471,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="5" t="s">
         <v>105</v>
       </c>
@@ -4507,7 +4520,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="5" t="s">
         <v>109</v>
       </c>
@@ -4554,7 +4567,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
         <v>113</v>
       </c>
@@ -4603,7 +4616,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
@@ -4646,7 +4659,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
         <v>72</v>
       </c>
@@ -4689,7 +4702,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="5" t="s">
         <v>76</v>
       </c>
@@ -4738,7 +4751,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -4787,7 +4800,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="5" t="s">
         <v>90</v>
       </c>
@@ -4836,7 +4849,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="5" t="s">
         <v>95</v>
       </c>
@@ -4885,7 +4898,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
         <v>792</v>
       </c>
@@ -4932,7 +4945,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="5" t="s">
         <v>757</v>
       </c>
@@ -4979,7 +4992,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="5" t="s">
         <v>140</v>
       </c>
@@ -5026,7 +5039,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="5" t="s">
         <v>160</v>
       </c>
@@ -5073,7 +5086,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="5" t="s">
         <v>145</v>
       </c>
@@ -5120,7 +5133,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="5" t="s">
         <v>150</v>
       </c>
@@ -5167,7 +5180,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="5" t="s">
         <v>130</v>
       </c>
@@ -5214,7 +5227,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="5" t="s">
         <v>746</v>
       </c>
@@ -5259,7 +5272,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="5" t="s">
         <v>134</v>
       </c>
@@ -5306,7 +5319,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="5" t="s">
         <v>155</v>
       </c>
@@ -5353,7 +5366,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="5" t="s">
         <v>165</v>
       </c>
@@ -5394,7 +5407,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="5" t="s">
         <v>169</v>
       </c>
@@ -5438,7 +5451,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="5" t="s">
         <v>116</v>
       </c>
@@ -5485,7 +5498,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B39" s="5" t="s">
         <v>123</v>
       </c>
@@ -5528,7 +5541,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B40" s="5" t="s">
         <v>127</v>
       </c>
@@ -5573,7 +5586,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" s="5" t="s">
         <v>174</v>
       </c>
@@ -5615,7 +5628,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42" s="5" t="s">
         <v>177</v>
       </c>
@@ -5656,7 +5669,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B43" s="5" t="s">
         <v>183</v>
       </c>
@@ -5699,18 +5712,17 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1025" ht="57" x14ac:dyDescent="0.45">
+      <c r="A44" s="47"/>
       <c r="B44" s="5" t="s">
-        <v>190</v>
+        <v>819</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>822</v>
+      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5" t="s">
@@ -5726,32 +5738,37 @@
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="5" t="s">
-        <v>748</v>
-      </c>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
+        <v>808</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>187</v>
+      </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5" t="s">
-        <v>83</v>
+        <v>188</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>821</v>
+      </c>
+      <c r="U44" s="47"/>
+    </row>
+    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5" t="s">
@@ -5770,9 +5787,7 @@
         <v>748</v>
       </c>
       <c r="N45" s="5"/>
-      <c r="O45" s="5" t="s">
-        <v>195</v>
-      </c>
+      <c r="O45" s="5"/>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
@@ -5780,19 +5795,21 @@
         <v>83</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="5" t="s">
-        <v>740</v>
+        <v>192</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>739</v>
-      </c>
-      <c r="D46" s="5"/>
+        <v>193</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E46" s="5" t="s">
-        <v>59</v>
+        <v>194</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5" t="s">
@@ -5808,11 +5825,11 @@
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
       <c r="N46" s="5"/>
       <c r="O46" s="5" t="s">
-        <v>742</v>
+        <v>195</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
@@ -5821,22 +5838,19 @@
         <v>83</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="46"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="5" t="s">
-        <v>816</v>
+        <v>740</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>817</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>739</v>
+      </c>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
@@ -5850,17 +5864,14 @@
       <c r="K47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L47" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="L47" s="5"/>
       <c r="M47" s="5" t="s">
-        <v>808</v>
-      </c>
-      <c r="N47" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O47" s="5"/>
+        <v>743</v>
+      </c>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5" t="s">
+        <v>742</v>
+      </c>
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
@@ -5868,9 +5879,8 @@
         <v>83</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>815</v>
-      </c>
-      <c r="U47" s="46"/>
+        <v>741</v>
+      </c>
       <c r="V47" s="46"/>
       <c r="W47" s="46"/>
       <c r="X47" s="46"/>
@@ -6876,12 +6886,13 @@
       <c r="AMJ47" s="46"/>
       <c r="AMK47" s="46"/>
     </row>
-    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="46"/>
       <c r="B48" s="5" t="s">
-        <v>744</v>
+        <v>816</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>745</v>
+        <v>817</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>58</v>
@@ -6908,8 +6919,8 @@
         <v>808</v>
       </c>
       <c r="N48" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
@@ -6919,15 +6930,16 @@
         <v>83</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>815</v>
+      </c>
+      <c r="U48" s="46"/>
+    </row>
+    <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="5" t="s">
-        <v>813</v>
+        <v>744</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>812</v>
+        <v>745</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>58</v>
@@ -6965,15 +6977,15 @@
         <v>83</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="5" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>801</v>
+        <v>812</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>58</v>
@@ -6997,11 +7009,11 @@
         <v>58</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>748</v>
+        <v>808</v>
       </c>
       <c r="N50" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
@@ -7011,30 +7023,28 @@
         <v>83</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="51" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="5" t="s">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>805</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="F51" s="5"/>
       <c r="G51" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
@@ -7042,15 +7052,16 @@
         <v>58</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>748</v>
       </c>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5" t="s">
-        <v>806</v>
-      </c>
+      <c r="N51" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O51" s="5"/>
       <c r="P51" s="5"/>
       <c r="Q51" s="5"/>
       <c r="R51" s="5"/>
@@ -7058,87 +7069,136 @@
         <v>83</v>
       </c>
       <c r="T51" s="5" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" ht="57" x14ac:dyDescent="0.45">
+      <c r="B52" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="T52" s="5" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="55" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="5" t="s">
+    <row r="55" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="B56" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5" t="s">
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H55" s="5" t="s">
+      <c r="F56" s="5"/>
+      <c r="G56" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H56" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5" t="s">
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
-      <c r="R55" s="5"/>
-      <c r="S55" s="5" t="s">
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="T55" s="5" t="s">
+      <c r="T56" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="52" t="s">
+    <row r="59" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B60" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="C59" s="52"/>
-    </row>
-    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="53" t="s">
+      <c r="C60" s="53"/>
+    </row>
+    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="C60" s="53"/>
-    </row>
-    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="53" t="s">
+      <c r="C61" s="54"/>
+    </row>
+    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="C61" s="53"/>
-    </row>
-    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="54" t="s">
+      <c r="C62" s="54"/>
+    </row>
+    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="C62" s="54"/>
-    </row>
-    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="54" t="s">
+      <c r="C63" s="55"/>
+    </row>
+    <row r="64" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B64" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="C63" s="54"/>
-    </row>
-    <row r="64" spans="2:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="51" t="s">
+      <c r="C64" s="55"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" s="52" t="s">
         <v>751</v>
       </c>
-      <c r="C64" s="51"/>
+      <c r="C65" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C3:L3"/>
@@ -7149,11 +7209,11 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
-    <mergeCell ref="B59:C59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B61:C61"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -7173,19 +7233,19 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="55" t="s">
+    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-    </row>
-    <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="56" t="s">
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+    </row>
+    <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="57" t="s">
         <v>207</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -7195,8 +7255,8 @@
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="56"/>
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="57"/>
       <c r="C7" s="16" t="s">
         <v>209</v>
       </c>
@@ -7204,8 +7264,8 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="56"/>
+    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="57"/>
       <c r="C8" s="16" t="s">
         <v>210</v>
       </c>
@@ -7213,8 +7273,8 @@
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
     </row>
-    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="56"/>
+    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="57"/>
       <c r="C9" s="16" t="s">
         <v>211</v>
       </c>
@@ -7222,14 +7282,14 @@
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="56"/>
-      <c r="C10" s="57" t="s">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="57"/>
+      <c r="C10" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7255,23 +7315,23 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.53125" customWidth="1"/>
+    <col min="5" max="5" width="19.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="58" t="s">
+    <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="60"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="29" t="s">
         <v>29</v>
       </c>
@@ -7285,7 +7345,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
@@ -7299,7 +7359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="33" t="s">
         <v>107</v>
       </c>
@@ -7311,7 +7371,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="36" t="s">
         <v>214</v>
       </c>
@@ -7323,7 +7383,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="36" t="s">
         <v>131</v>
       </c>
@@ -7335,7 +7395,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="36" t="s">
         <v>804</v>
       </c>
@@ -7347,7 +7407,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="36" t="s">
         <v>215</v>
       </c>
@@ -7361,7 +7421,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="36" t="s">
         <v>141</v>
       </c>
@@ -7375,7 +7435,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="36" t="s">
         <v>218</v>
       </c>
@@ -7389,7 +7449,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="36" t="s">
         <v>146</v>
       </c>
@@ -7403,7 +7463,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="36" t="s">
         <v>151</v>
       </c>
@@ -7417,7 +7477,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="36" t="s">
         <v>161</v>
       </c>
@@ -7431,7 +7491,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B15" s="36" t="s">
         <v>755</v>
       </c>
@@ -7445,7 +7505,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B16" s="38" t="s">
         <v>758</v>
       </c>
@@ -7481,31 +7541,31 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="31.46484375" customWidth="1"/>
     <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="9" max="9" width="24.88671875" customWidth="1"/>
+    <col min="9" max="9" width="24.86328125" customWidth="1"/>
     <col min="10" max="10" width="33.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="11" max="11" width="23.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+    <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B2" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="64"/>
+      <c r="C2" s="65"/>
       <c r="E2" s="23" t="s">
         <v>220</v>
       </c>
       <c r="F2" s="24"/>
-      <c r="I2" s="63" t="s">
+      <c r="I2" s="64" t="s">
         <v>221</v>
       </c>
-      <c r="J2" s="64"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="65"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="19" t="s">
         <v>29</v>
       </c>
@@ -7525,7 +7585,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="19" t="s">
         <v>222</v>
       </c>
@@ -7545,7 +7605,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="20" t="s">
         <v>224</v>
       </c>
@@ -7565,7 +7625,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="20" t="s">
         <v>229</v>
       </c>
@@ -7585,7 +7645,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="20" t="s">
         <v>235</v>
       </c>
@@ -7605,7 +7665,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="20" t="s">
         <v>241</v>
       </c>
@@ -7625,7 +7685,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="20" t="s">
         <v>246</v>
       </c>
@@ -7639,7 +7699,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="20" t="s">
         <v>250</v>
       </c>
@@ -7653,7 +7713,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="20" t="s">
         <v>254</v>
       </c>
@@ -7667,7 +7727,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="20" t="s">
         <v>258</v>
       </c>
@@ -7681,7 +7741,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="20" t="s">
         <v>262</v>
       </c>
@@ -7694,12 +7754,12 @@
       <c r="F13" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="I13" s="63" t="s">
+      <c r="I13" s="64" t="s">
         <v>266</v>
       </c>
-      <c r="J13" s="64"/>
-    </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="65"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="20" t="s">
         <v>267</v>
       </c>
@@ -7719,7 +7779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="20" t="s">
         <v>271</v>
       </c>
@@ -7739,7 +7799,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="20" t="s">
         <v>275</v>
       </c>
@@ -7759,7 +7819,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="20" t="s">
         <v>248</v>
       </c>
@@ -7779,7 +7839,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="20" t="s">
         <v>285</v>
       </c>
@@ -7799,7 +7859,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="20" t="s">
         <v>291</v>
       </c>
@@ -7819,7 +7879,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B20" s="20" t="s">
         <v>252</v>
       </c>
@@ -7839,7 +7899,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="20" t="s">
         <v>302</v>
       </c>
@@ -7853,7 +7913,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="20" t="s">
         <v>306</v>
       </c>
@@ -7867,7 +7927,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="20" t="s">
         <v>310</v>
       </c>
@@ -7880,12 +7940,12 @@
       <c r="F23" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="I23" s="63" t="s">
+      <c r="I23" s="64" t="s">
         <v>314</v>
       </c>
-      <c r="J23" s="64"/>
-    </row>
-    <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="65"/>
+    </row>
+    <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="20" t="s">
         <v>315</v>
       </c>
@@ -7905,7 +7965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="20" t="s">
         <v>319</v>
       </c>
@@ -7925,7 +7985,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="20" t="s">
         <v>323</v>
       </c>
@@ -7945,7 +8005,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="20" t="s">
         <v>329</v>
       </c>
@@ -7965,7 +8025,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B28" s="20" t="s">
         <v>335</v>
       </c>
@@ -7985,7 +8045,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="20" t="s">
         <v>341</v>
       </c>
@@ -7999,7 +8059,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="20" t="s">
         <v>345</v>
       </c>
@@ -8013,7 +8073,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="20" t="s">
         <v>349</v>
       </c>
@@ -8027,7 +8087,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="20" t="s">
         <v>353</v>
       </c>
@@ -8040,12 +8100,12 @@
       <c r="F32" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="I32" s="63" t="s">
+      <c r="I32" s="64" t="s">
         <v>752</v>
       </c>
-      <c r="J32" s="64"/>
-    </row>
-    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J32" s="65"/>
+    </row>
+    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="20" t="s">
         <v>264</v>
       </c>
@@ -8065,7 +8125,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="20" t="s">
         <v>359</v>
       </c>
@@ -8085,7 +8145,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="20" t="s">
         <v>363</v>
       </c>
@@ -8105,7 +8165,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B36" s="20" t="s">
         <v>367</v>
       </c>
@@ -8125,7 +8185,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="20" t="s">
         <v>371</v>
       </c>
@@ -8139,7 +8199,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B38" s="20" t="s">
         <v>375</v>
       </c>
@@ -8153,7 +8213,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B39" s="20" t="s">
         <v>379</v>
       </c>
@@ -8166,12 +8226,12 @@
       <c r="F39" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="I39" s="63" t="s">
+      <c r="I39" s="64" t="s">
         <v>785</v>
       </c>
-      <c r="J39" s="64"/>
-    </row>
-    <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="65"/>
+    </row>
+    <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B40" s="20" t="s">
         <v>293</v>
       </c>
@@ -8191,7 +8251,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" s="20" t="s">
         <v>116</v>
       </c>
@@ -8211,7 +8271,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42" s="20" t="s">
         <v>389</v>
       </c>
@@ -8231,7 +8291,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B43" s="20" t="s">
         <v>393</v>
       </c>
@@ -8251,7 +8311,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B44" s="20" t="s">
         <v>287</v>
       </c>
@@ -8265,7 +8325,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B45" s="20" t="s">
         <v>400</v>
       </c>
@@ -8279,7 +8339,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="20" t="s">
         <v>404</v>
       </c>
@@ -8292,12 +8352,12 @@
       <c r="F46" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="I46" s="63" t="s">
+      <c r="I46" s="64" t="s">
         <v>795</v>
       </c>
-      <c r="J46" s="64"/>
-    </row>
-    <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="65"/>
+    </row>
+    <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="20" t="s">
         <v>408</v>
       </c>
@@ -8317,7 +8377,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="20" t="s">
         <v>412</v>
       </c>
@@ -8337,7 +8397,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="20" t="s">
         <v>416</v>
       </c>
@@ -8357,7 +8417,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B50" s="20" t="s">
         <v>420</v>
       </c>
@@ -8377,7 +8437,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="20" t="s">
         <v>424</v>
       </c>
@@ -8391,7 +8451,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="20" t="s">
         <v>428</v>
       </c>
@@ -8405,7 +8465,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="20" t="s">
         <v>432</v>
       </c>
@@ -8419,7 +8479,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B54" s="20" t="s">
         <v>436</v>
       </c>
@@ -8433,7 +8493,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B55" s="20" t="s">
         <v>351</v>
       </c>
@@ -8447,7 +8507,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="56" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B56" s="20" t="s">
         <v>443</v>
       </c>
@@ -8461,7 +8521,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="20" t="s">
         <v>325</v>
       </c>
@@ -8469,7 +8529,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="58" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B58" s="20" t="s">
         <v>448</v>
       </c>
@@ -8477,19 +8537,19 @@
         <v>449</v>
       </c>
     </row>
-    <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B59" s="20" t="s">
         <v>450</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="E59" s="63" t="s">
+      <c r="E59" s="64" t="s">
         <v>761</v>
       </c>
-      <c r="F59" s="64"/>
-    </row>
-    <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F59" s="65"/>
+    </row>
+    <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="20" t="s">
         <v>452</v>
       </c>
@@ -8503,7 +8563,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B61" s="20" t="s">
         <v>454</v>
       </c>
@@ -8517,7 +8577,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="20" t="s">
         <v>456</v>
       </c>
@@ -8531,7 +8591,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B63" s="20" t="s">
         <v>395</v>
       </c>
@@ -8545,7 +8605,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B64" s="20" t="s">
         <v>459</v>
       </c>
@@ -8559,7 +8619,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B65" s="20" t="s">
         <v>461</v>
       </c>
@@ -8573,7 +8633,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B66" s="20" t="s">
         <v>463</v>
       </c>
@@ -8587,7 +8647,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B67" s="20" t="s">
         <v>465</v>
       </c>
@@ -8601,7 +8661,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B68" s="20" t="s">
         <v>467</v>
       </c>
@@ -8615,7 +8675,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B69" s="20" t="s">
         <v>398</v>
       </c>
@@ -8629,7 +8689,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B70" s="20" t="s">
         <v>469</v>
       </c>
@@ -8643,7 +8703,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B71" s="20" t="s">
         <v>471</v>
       </c>
@@ -8657,7 +8717,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B72" s="20" t="s">
         <v>473</v>
       </c>
@@ -8671,7 +8731,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B73" s="20" t="s">
         <v>475</v>
       </c>
@@ -8685,7 +8745,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B74" s="20" t="s">
         <v>477</v>
       </c>
@@ -8699,7 +8759,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B75" s="20" t="s">
         <v>479</v>
       </c>
@@ -8707,7 +8767,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B76" s="20" t="s">
         <v>481</v>
       </c>
@@ -8715,7 +8775,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B77" s="20" t="s">
         <v>483</v>
       </c>
@@ -8723,7 +8783,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B78" s="20" t="s">
         <v>485</v>
       </c>
@@ -8731,7 +8791,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B79" s="20" t="s">
         <v>487</v>
       </c>
@@ -8739,7 +8799,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B80" s="20" t="s">
         <v>410</v>
       </c>
@@ -8747,7 +8807,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B81" s="20" t="s">
         <v>289</v>
       </c>
@@ -8755,7 +8815,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B82" s="20" t="s">
         <v>491</v>
       </c>
@@ -8763,7 +8823,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B83" s="20" t="s">
         <v>493</v>
       </c>
@@ -8771,7 +8831,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B84" s="20" t="s">
         <v>495</v>
       </c>
@@ -8779,7 +8839,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B85" s="20" t="s">
         <v>497</v>
       </c>
@@ -8787,7 +8847,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B86" s="20" t="s">
         <v>414</v>
       </c>
@@ -8795,7 +8855,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B87" s="20" t="s">
         <v>500</v>
       </c>
@@ -8803,7 +8863,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" s="20" t="s">
         <v>502</v>
       </c>
@@ -8811,7 +8871,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B89" s="20" t="s">
         <v>504</v>
       </c>
@@ -8819,7 +8879,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B90" s="20" t="s">
         <v>506</v>
       </c>
@@ -8827,7 +8887,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B91" s="20" t="s">
         <v>508</v>
       </c>
@@ -8835,7 +8895,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B92" s="20" t="s">
         <v>510</v>
       </c>
@@ -8843,7 +8903,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B93" s="20" t="s">
         <v>512</v>
       </c>
@@ -8851,7 +8911,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B94" s="20" t="s">
         <v>514</v>
       </c>
@@ -8859,7 +8919,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B95" s="21" t="s">
         <v>516</v>
       </c>
@@ -8867,15 +8927,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="98" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B99" s="23" t="s">
         <v>518</v>
       </c>
       <c r="C99" s="24"/>
     </row>
-    <row r="100" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B100" s="19" t="s">
         <v>29</v>
       </c>
@@ -8883,7 +8943,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B101" s="19" t="s">
         <v>222</v>
       </c>
@@ -8891,7 +8951,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B102" s="20" t="s">
         <v>519</v>
       </c>
@@ -8899,7 +8959,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B103" s="20" t="s">
         <v>521</v>
       </c>
@@ -8907,7 +8967,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B104" s="20" t="s">
         <v>523</v>
       </c>
@@ -8915,7 +8975,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B105" s="20" t="s">
         <v>525</v>
       </c>
@@ -8923,7 +8983,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B106" s="20" t="s">
         <v>527</v>
       </c>
@@ -8931,7 +8991,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B107" s="20" t="s">
         <v>529</v>
       </c>
@@ -8939,7 +8999,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B108" s="20" t="s">
         <v>531</v>
       </c>
@@ -8947,7 +9007,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B109" s="20" t="s">
         <v>533</v>
       </c>
@@ -8955,7 +9015,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B110" s="20" t="s">
         <v>535</v>
       </c>
@@ -8963,7 +9023,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B111" s="20" t="s">
         <v>537</v>
       </c>
@@ -8971,7 +9031,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B112" s="20" t="s">
         <v>539</v>
       </c>
@@ -8979,7 +9039,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B113" s="20" t="s">
         <v>541</v>
       </c>
@@ -8987,7 +9047,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B114" s="20" t="s">
         <v>543</v>
       </c>
@@ -8995,7 +9055,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B115" s="20" t="s">
         <v>545</v>
       </c>
@@ -9003,7 +9063,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B116" s="20" t="s">
         <v>547</v>
       </c>
@@ -9011,7 +9071,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B117" s="20" t="s">
         <v>549</v>
       </c>
@@ -9019,7 +9079,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B118" s="20" t="s">
         <v>551</v>
       </c>
@@ -9027,7 +9087,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B119" s="20" t="s">
         <v>553</v>
       </c>
@@ -9035,7 +9095,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B120" s="20" t="s">
         <v>555</v>
       </c>
@@ -9043,7 +9103,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B121" s="20" t="s">
         <v>557</v>
       </c>
@@ -9051,7 +9111,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B122" s="20" t="s">
         <v>559</v>
       </c>
@@ -9059,7 +9119,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B123" s="20" t="s">
         <v>561</v>
       </c>
@@ -9067,7 +9127,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B124" s="20" t="s">
         <v>563</v>
       </c>
@@ -9075,7 +9135,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B125" s="20" t="s">
         <v>565</v>
       </c>
@@ -9083,7 +9143,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B126" s="20" t="s">
         <v>567</v>
       </c>
@@ -9091,7 +9151,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B127" s="20" t="s">
         <v>569</v>
       </c>
@@ -9099,7 +9159,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B128" s="20" t="s">
         <v>571</v>
       </c>
@@ -9107,7 +9167,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B129" s="20" t="s">
         <v>573</v>
       </c>
@@ -9115,7 +9175,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B130" s="20" t="s">
         <v>575</v>
       </c>
@@ -9123,7 +9183,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B131" s="20" t="s">
         <v>577</v>
       </c>
@@ -9131,7 +9191,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B132" s="20" t="s">
         <v>579</v>
       </c>
@@ -9139,7 +9199,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B133" s="20" t="s">
         <v>581</v>
       </c>
@@ -9147,7 +9207,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B134" s="20" t="s">
         <v>583</v>
       </c>
@@ -9155,7 +9215,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B135" s="20" t="s">
         <v>585</v>
       </c>
@@ -9163,7 +9223,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B136" s="20" t="s">
         <v>587</v>
       </c>
@@ -9171,7 +9231,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B137" s="20" t="s">
         <v>589</v>
       </c>
@@ -9179,7 +9239,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B138" s="20" t="s">
         <v>591</v>
       </c>
@@ -9187,7 +9247,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B139" s="20" t="s">
         <v>593</v>
       </c>
@@ -9195,7 +9255,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B140" s="21" t="s">
         <v>595</v>
       </c>
@@ -9203,14 +9263,14 @@
         <v>596</v>
       </c>
     </row>
-    <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B143" s="61" t="s">
+    <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B143" s="62" t="s">
         <v>597</v>
       </c>
-      <c r="C143" s="62"/>
-    </row>
-    <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C143" s="63"/>
+    </row>
+    <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B144" s="7" t="s">
         <v>29</v>
       </c>
@@ -9218,7 +9278,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B145" s="7" t="s">
         <v>222</v>
       </c>
@@ -9226,7 +9286,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B146" s="9" t="s">
         <v>598</v>
       </c>
@@ -9234,7 +9294,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B147" s="9" t="s">
         <v>600</v>
       </c>
@@ -9242,7 +9302,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B148" s="9" t="s">
         <v>602</v>
       </c>
@@ -9250,7 +9310,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B149" s="9" t="s">
         <v>604</v>
       </c>
@@ -9258,7 +9318,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="150" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B150" s="9" t="s">
         <v>606</v>
       </c>
@@ -9266,7 +9326,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="151" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B151" s="9" t="s">
         <v>608</v>
       </c>
@@ -9274,7 +9334,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="152" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B152" s="9" t="s">
         <v>610</v>
       </c>
@@ -9282,7 +9342,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="153" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B153" s="9" t="s">
         <v>612</v>
       </c>
@@ -9290,7 +9350,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="154" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B154" s="9" t="s">
         <v>614</v>
       </c>
@@ -9298,7 +9358,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="155" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B155" s="9" t="s">
         <v>616</v>
       </c>
@@ -9306,7 +9366,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="156" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B156" s="9" t="s">
         <v>618</v>
       </c>
@@ -9314,7 +9374,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="157" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B157" s="9" t="s">
         <v>620</v>
       </c>
@@ -9322,7 +9382,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="158" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B158" s="9" t="s">
         <v>622</v>
       </c>
@@ -9330,7 +9390,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="159" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B159" s="9" t="s">
         <v>624</v>
       </c>
@@ -9338,7 +9398,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="160" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B160" s="9" t="s">
         <v>626</v>
       </c>
@@ -9346,7 +9406,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="161" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B161" s="9" t="s">
         <v>628</v>
       </c>
@@ -9354,7 +9414,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="162" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B162" s="9" t="s">
         <v>630</v>
       </c>
@@ -9362,7 +9422,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="163" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B163" s="9" t="s">
         <v>632</v>
       </c>
@@ -9370,7 +9430,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="164" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B164" s="9" t="s">
         <v>634</v>
       </c>
@@ -9378,7 +9438,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="165" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B165" s="9" t="s">
         <v>636</v>
       </c>
@@ -9386,7 +9446,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="166" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B166" s="9" t="s">
         <v>638</v>
       </c>
@@ -9394,7 +9454,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="167" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B167" s="9" t="s">
         <v>640</v>
       </c>
@@ -9402,7 +9462,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="168" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B168" s="9" t="s">
         <v>642</v>
       </c>
@@ -9410,7 +9470,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="169" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B169" s="9" t="s">
         <v>644</v>
       </c>
@@ -9418,7 +9478,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="170" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B170" s="9" t="s">
         <v>646</v>
       </c>
@@ -9426,7 +9486,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="171" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B171" s="9" t="s">
         <v>648</v>
       </c>
@@ -9434,7 +9494,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="172" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B172" s="9" t="s">
         <v>650</v>
       </c>
@@ -9442,7 +9502,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="173" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B173" s="9" t="s">
         <v>652</v>
       </c>
@@ -9450,7 +9510,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="174" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B174" s="9" t="s">
         <v>654</v>
       </c>
@@ -9458,7 +9518,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B175" s="9" t="s">
         <v>656</v>
       </c>
@@ -9466,7 +9526,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B176" s="9" t="s">
         <v>658</v>
       </c>
@@ -9474,7 +9534,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="177" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B177" s="9" t="s">
         <v>660</v>
       </c>
@@ -9482,7 +9542,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="178" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B178" s="9" t="s">
         <v>662</v>
       </c>
@@ -9490,7 +9550,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="179" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B179" s="9" t="s">
         <v>664</v>
       </c>
@@ -9498,7 +9558,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="180" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B180" s="9" t="s">
         <v>666</v>
       </c>
@@ -9506,7 +9566,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="181" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B181" s="9" t="s">
         <v>668</v>
       </c>
@@ -9514,7 +9574,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="182" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B182" s="9" t="s">
         <v>670</v>
       </c>
@@ -9522,7 +9582,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="183" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B183" s="9" t="s">
         <v>672</v>
       </c>
@@ -9530,7 +9590,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="184" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B184" s="9" t="s">
         <v>674</v>
       </c>
@@ -9538,7 +9598,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="185" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B185" s="9" t="s">
         <v>676</v>
       </c>
@@ -9546,7 +9606,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="186" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B186" s="9" t="s">
         <v>678</v>
       </c>
@@ -9554,7 +9614,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="187" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B187" s="9" t="s">
         <v>680</v>
       </c>
@@ -9562,7 +9622,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="188" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B188" s="9" t="s">
         <v>682</v>
       </c>
@@ -9570,7 +9630,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="189" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B189" s="9" t="s">
         <v>684</v>
       </c>
@@ -9578,7 +9638,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="190" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B190" s="9" t="s">
         <v>686</v>
       </c>
@@ -9586,7 +9646,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="191" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B191" s="9" t="s">
         <v>688</v>
       </c>
@@ -9594,7 +9654,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="192" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B192" s="9" t="s">
         <v>690</v>
       </c>
@@ -9602,7 +9662,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="193" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B193" s="9" t="s">
         <v>692</v>
       </c>
@@ -9610,7 +9670,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="194" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B194" s="9" t="s">
         <v>694</v>
       </c>
@@ -9618,7 +9678,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="195" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B195" s="9" t="s">
         <v>696</v>
       </c>
@@ -9626,7 +9686,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="196" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B196" s="9" t="s">
         <v>698</v>
       </c>
@@ -9634,7 +9694,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="197" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B197" s="9" t="s">
         <v>700</v>
       </c>
@@ -9642,7 +9702,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="198" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B198" s="9" t="s">
         <v>702</v>
       </c>
@@ -9650,7 +9710,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="199" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B199" s="9" t="s">
         <v>704</v>
       </c>
@@ -9658,7 +9718,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="200" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B200" s="9" t="s">
         <v>706</v>
       </c>
@@ -9666,7 +9726,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="201" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B201" s="9" t="s">
         <v>708</v>
       </c>
@@ -9674,7 +9734,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="202" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B202" s="9" t="s">
         <v>710</v>
       </c>
@@ -9682,7 +9742,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="203" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B203" s="9" t="s">
         <v>712</v>
       </c>
@@ -9690,7 +9750,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="204" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B204" s="9" t="s">
         <v>714</v>
       </c>
@@ -9698,7 +9758,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="205" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B205" s="9" t="s">
         <v>716</v>
       </c>
@@ -9706,7 +9766,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="206" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B206" s="9" t="s">
         <v>718</v>
       </c>
@@ -9714,7 +9774,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="207" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B207" s="9" t="s">
         <v>720</v>
       </c>
@@ -9722,7 +9782,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="208" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B208" s="9" t="s">
         <v>722</v>
       </c>
@@ -9730,7 +9790,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="209" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B209" s="9" t="s">
         <v>724</v>
       </c>
@@ -9738,7 +9798,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="210" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B210" s="9" t="s">
         <v>726</v>
       </c>
@@ -9746,7 +9806,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="211" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B211" s="9" t="s">
         <v>728</v>
       </c>
@@ -9754,7 +9814,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="212" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B212" s="9" t="s">
         <v>730</v>
       </c>
@@ -9762,7 +9822,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="213" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B213" s="9" t="s">
         <v>732</v>
       </c>
@@ -9770,7 +9830,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="214" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B214" s="9" t="s">
         <v>734</v>
       </c>
@@ -9778,7 +9838,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="215" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B215" s="9" t="s">
         <v>736</v>
       </c>
@@ -9786,7 +9846,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="216" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B143:C143"/>

</xml_diff>

<commit_message>
EPBDS-9556 Simplify configuration package for output model
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437664F7-2FC3-4F3D-9670-08DE60001F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EF3F5A-E320-4212-9529-79C4EECC4FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="824">
   <si>
     <t>Display Name</t>
   </si>
@@ -2529,6 +2529,9 @@
   </si>
   <si>
     <t>spreadsheetResultPackage</t>
+  </si>
+  <si>
+    <t>MODULE</t>
   </si>
 </sst>
 </file>
@@ -3266,14 +3269,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3797,16 +3800,16 @@
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="15" t="s">
@@ -3842,31 +3845,31 @@
       <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="15" t="s">
@@ -3920,13 +3923,13 @@
       <c r="C12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="15" t="s">
@@ -3935,13 +3938,13 @@
       <c r="C13" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="15" t="s">
@@ -3950,34 +3953,29 @@
       <c r="C14" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3987,6 +3985,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4002,8 +4005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="H37" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4069,18 +4072,18 @@
       <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="15" t="s">
@@ -4120,35 +4123,35 @@
       <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="15" t="s">
@@ -5738,7 +5741,7 @@
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="5" t="s">
-        <v>808</v>
+        <v>179</v>
       </c>
       <c r="N44" s="5" t="s">
         <v>820</v>
@@ -5750,7 +5753,7 @@
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5" t="s">
-        <v>188</v>
+        <v>823</v>
       </c>
       <c r="T44" s="5" t="s">
         <v>821</v>

</xml_diff>

<commit_message>
EPBDS-9519 Swagger: response example has the different case than declared in the Spreadsheet
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EF3F5A-E320-4212-9529-79C4EECC4FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF3F917-2E2B-45DB-825B-4813D48C0D6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Runtime Scope" sheetId="4" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3269,14 +3269,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3800,16 +3800,16 @@
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="15" t="s">
@@ -3845,31 +3845,31 @@
       <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="15" t="s">
@@ -3923,13 +3923,13 @@
       <c r="C12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="15" t="s">
@@ -3938,13 +3938,13 @@
       <c r="C13" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="15" t="s">
@@ -3953,29 +3953,34 @@
       <c r="C14" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -3985,11 +3990,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4005,8 +4005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H37" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4072,18 +4072,18 @@
       <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="15" t="s">
@@ -4123,35 +4123,35 @@
       <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="15" t="s">

</xml_diff>

<commit_message>
EPBDS-10183 Select Rule with the newest effectiveDate
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66C107D-E3B4-451E-9B92-035EDE877C87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF5CD3-E0FA-46E4-B905-D3B24770A48C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,15 @@
     <sheet name="Runtime Scope" sheetId="4" r:id="rId4"/>
     <sheet name="Data Enums" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="829">
   <si>
     <t>Display Name</t>
   </si>
@@ -2544,6 +2547,9 @@
   </si>
   <si>
     <t>The priority for for global properties</t>
+  </si>
+  <si>
+    <t>max(effectiveDate)</t>
   </si>
 </sst>
 </file>
@@ -3183,7 +3189,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3282,16 +3288,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3337,39 +3346,39 @@
     </xf>
   </cellXfs>
   <cellStyles count="33">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3453,9 +3462,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3493,7 +3502,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3599,7 +3608,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3779,163 +3788,163 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-    </row>
-    <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+    </row>
+    <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-    </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+    </row>
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-    </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+    </row>
+    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-    </row>
-    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+    </row>
+    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-    </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+    </row>
+    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-    </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+    </row>
+    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-    </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+    </row>
+    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-    </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="50" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="51"/>
@@ -3946,11 +3955,11 @@
       <c r="I12" s="51"/>
       <c r="J12" s="51"/>
     </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="50" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="51"/>
@@ -3961,11 +3970,11 @@
       <c r="I13" s="51"/>
       <c r="J13" s="51"/>
     </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="50" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="51"/>
@@ -3976,7 +3985,7 @@
       <c r="I14" s="51"/>
       <c r="J14" s="51"/>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
         <v>26</v>
       </c>
@@ -3991,6 +4000,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -4000,11 +4014,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4018,191 +4027,191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK66"/>
+  <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H31" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" style="1"/>
-    <col min="2" max="2" width="17.46484375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.53125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.86328125" style="1"/>
-    <col min="6" max="6" width="19.1328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.86328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.86328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1328125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="39.46484375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.86328125" style="1"/>
-    <col min="15" max="15" width="20.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.86328125" style="1"/>
+    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="19.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="39.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1"/>
+    <col min="15" max="15" width="20.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="1"/>
     <col min="17" max="17" width="14" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="26.86328125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="45.86328125" style="1" customWidth="1"/>
-    <col min="21" max="1025" width="8.86328125" style="1"/>
+    <col min="18" max="18" width="13.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="26.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="45.85546875" style="1" customWidth="1"/>
+    <col min="21" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-    </row>
-    <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+    </row>
+    <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-    </row>
-    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+    </row>
+    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-    </row>
-    <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+    </row>
+    <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-    </row>
-    <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+    </row>
+    <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-    </row>
-    <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+    </row>
+    <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-    </row>
-    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+    </row>
+    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-    </row>
-    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+    </row>
+    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-    </row>
-    <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+    </row>
+    <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-    </row>
-    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+    </row>
+    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -4211,30 +4220,30 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="54" t="s">
+    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="54"/>
-    </row>
-    <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="55"/>
+    </row>
+    <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
@@ -4293,7 +4302,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
@@ -4352,7 +4361,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
@@ -4399,7 +4408,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>66</v>
       </c>
@@ -4442,7 +4451,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>100</v>
       </c>
@@ -4489,7 +4498,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>105</v>
       </c>
@@ -4538,7 +4547,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>109</v>
       </c>
@@ -4585,7 +4594,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>113</v>
       </c>
@@ -4634,7 +4643,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
@@ -4677,7 +4686,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>72</v>
       </c>
@@ -4720,7 +4729,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>76</v>
       </c>
@@ -4769,7 +4778,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -4818,7 +4827,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>90</v>
       </c>
@@ -4867,7 +4876,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>95</v>
       </c>
@@ -4916,7 +4925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>790</v>
       </c>
@@ -4963,7 +4972,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>755</v>
       </c>
@@ -5010,7 +5019,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>140</v>
       </c>
@@ -5057,7 +5066,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>160</v>
       </c>
@@ -5104,7 +5113,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>145</v>
       </c>
@@ -5151,7 +5160,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>150</v>
       </c>
@@ -5198,7 +5207,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>130</v>
       </c>
@@ -5245,7 +5254,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>744</v>
       </c>
@@ -5290,7 +5299,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>134</v>
       </c>
@@ -5337,7 +5346,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>155</v>
       </c>
@@ -5384,7 +5393,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>165</v>
       </c>
@@ -5425,7 +5434,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>169</v>
       </c>
@@ -5469,7 +5478,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>116</v>
       </c>
@@ -5516,7 +5525,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>123</v>
       </c>
@@ -5559,7 +5568,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>127</v>
       </c>
@@ -5604,7 +5613,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>174</v>
       </c>
@@ -5646,7 +5655,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>177</v>
       </c>
@@ -5687,7 +5696,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48"/>
       <c r="B43" s="5" t="s">
         <v>823</v>
@@ -5731,7 +5740,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>182</v>
       </c>
@@ -5775,7 +5784,7 @@
       </c>
       <c r="U44" s="47"/>
     </row>
-    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="47"/>
       <c r="B45" s="5" t="s">
         <v>817</v>
@@ -5819,7 +5828,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>188</v>
       </c>
@@ -5860,7 +5869,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>190</v>
       </c>
@@ -6907,7 +6916,7 @@
       <c r="AMJ47" s="46"/>
       <c r="AMK47" s="46"/>
     </row>
-    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>738</v>
       </c>
@@ -6949,7 +6958,7 @@
       </c>
       <c r="U48" s="46"/>
     </row>
-    <row r="49" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="46"/>
       <c r="B49" s="5" t="s">
         <v>814</v>
@@ -6996,7 +7005,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>742</v>
       </c>
@@ -7042,7 +7051,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>811</v>
       </c>
@@ -7088,7 +7097,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>808</v>
       </c>
@@ -7134,7 +7143,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="57" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>801</v>
       </c>
@@ -7181,8 +7190,8 @@
         <v>805</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>195</v>
       </c>
@@ -7221,47 +7230,1077 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="54" t="s">
+    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="55" t="s">
         <v>199</v>
       </c>
-      <c r="C61" s="54"/>
-    </row>
-    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="55" t="s">
+      <c r="C61" s="55"/>
+    </row>
+    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="C62" s="55"/>
-    </row>
-    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B63" s="55" t="s">
+      <c r="C62" s="56"/>
+    </row>
+    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="C63" s="55"/>
-    </row>
-    <row r="64" spans="1:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B64" s="56" t="s">
+      <c r="C63" s="56"/>
+    </row>
+    <row r="64" spans="1:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="C64" s="56"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B65" s="56" t="s">
+      <c r="C64" s="57"/>
+    </row>
+    <row r="65" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="B65" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="C65" s="56"/>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B66" s="53" t="s">
+      <c r="C65" s="57"/>
+    </row>
+    <row r="66" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="A66" s="49"/>
+      <c r="B66" s="57" t="s">
+        <v>828</v>
+      </c>
+      <c r="C66" s="57"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="49"/>
+      <c r="J66" s="49"/>
+      <c r="K66" s="49"/>
+      <c r="L66" s="49"/>
+      <c r="M66" s="49"/>
+      <c r="N66" s="49"/>
+      <c r="O66" s="49"/>
+      <c r="P66" s="49"/>
+      <c r="Q66" s="49"/>
+      <c r="R66" s="49"/>
+      <c r="S66" s="49"/>
+      <c r="T66" s="49"/>
+      <c r="U66" s="49"/>
+      <c r="V66" s="49"/>
+      <c r="W66" s="49"/>
+      <c r="X66" s="49"/>
+      <c r="Y66" s="49"/>
+      <c r="Z66" s="49"/>
+      <c r="AA66" s="49"/>
+      <c r="AB66" s="49"/>
+      <c r="AC66" s="49"/>
+      <c r="AD66" s="49"/>
+      <c r="AE66" s="49"/>
+      <c r="AF66" s="49"/>
+      <c r="AG66" s="49"/>
+      <c r="AH66" s="49"/>
+      <c r="AI66" s="49"/>
+      <c r="AJ66" s="49"/>
+      <c r="AK66" s="49"/>
+      <c r="AL66" s="49"/>
+      <c r="AM66" s="49"/>
+      <c r="AN66" s="49"/>
+      <c r="AO66" s="49"/>
+      <c r="AP66" s="49"/>
+      <c r="AQ66" s="49"/>
+      <c r="AR66" s="49"/>
+      <c r="AS66" s="49"/>
+      <c r="AT66" s="49"/>
+      <c r="AU66" s="49"/>
+      <c r="AV66" s="49"/>
+      <c r="AW66" s="49"/>
+      <c r="AX66" s="49"/>
+      <c r="AY66" s="49"/>
+      <c r="AZ66" s="49"/>
+      <c r="BA66" s="49"/>
+      <c r="BB66" s="49"/>
+      <c r="BC66" s="49"/>
+      <c r="BD66" s="49"/>
+      <c r="BE66" s="49"/>
+      <c r="BF66" s="49"/>
+      <c r="BG66" s="49"/>
+      <c r="BH66" s="49"/>
+      <c r="BI66" s="49"/>
+      <c r="BJ66" s="49"/>
+      <c r="BK66" s="49"/>
+      <c r="BL66" s="49"/>
+      <c r="BM66" s="49"/>
+      <c r="BN66" s="49"/>
+      <c r="BO66" s="49"/>
+      <c r="BP66" s="49"/>
+      <c r="BQ66" s="49"/>
+      <c r="BR66" s="49"/>
+      <c r="BS66" s="49"/>
+      <c r="BT66" s="49"/>
+      <c r="BU66" s="49"/>
+      <c r="BV66" s="49"/>
+      <c r="BW66" s="49"/>
+      <c r="BX66" s="49"/>
+      <c r="BY66" s="49"/>
+      <c r="BZ66" s="49"/>
+      <c r="CA66" s="49"/>
+      <c r="CB66" s="49"/>
+      <c r="CC66" s="49"/>
+      <c r="CD66" s="49"/>
+      <c r="CE66" s="49"/>
+      <c r="CF66" s="49"/>
+      <c r="CG66" s="49"/>
+      <c r="CH66" s="49"/>
+      <c r="CI66" s="49"/>
+      <c r="CJ66" s="49"/>
+      <c r="CK66" s="49"/>
+      <c r="CL66" s="49"/>
+      <c r="CM66" s="49"/>
+      <c r="CN66" s="49"/>
+      <c r="CO66" s="49"/>
+      <c r="CP66" s="49"/>
+      <c r="CQ66" s="49"/>
+      <c r="CR66" s="49"/>
+      <c r="CS66" s="49"/>
+      <c r="CT66" s="49"/>
+      <c r="CU66" s="49"/>
+      <c r="CV66" s="49"/>
+      <c r="CW66" s="49"/>
+      <c r="CX66" s="49"/>
+      <c r="CY66" s="49"/>
+      <c r="CZ66" s="49"/>
+      <c r="DA66" s="49"/>
+      <c r="DB66" s="49"/>
+      <c r="DC66" s="49"/>
+      <c r="DD66" s="49"/>
+      <c r="DE66" s="49"/>
+      <c r="DF66" s="49"/>
+      <c r="DG66" s="49"/>
+      <c r="DH66" s="49"/>
+      <c r="DI66" s="49"/>
+      <c r="DJ66" s="49"/>
+      <c r="DK66" s="49"/>
+      <c r="DL66" s="49"/>
+      <c r="DM66" s="49"/>
+      <c r="DN66" s="49"/>
+      <c r="DO66" s="49"/>
+      <c r="DP66" s="49"/>
+      <c r="DQ66" s="49"/>
+      <c r="DR66" s="49"/>
+      <c r="DS66" s="49"/>
+      <c r="DT66" s="49"/>
+      <c r="DU66" s="49"/>
+      <c r="DV66" s="49"/>
+      <c r="DW66" s="49"/>
+      <c r="DX66" s="49"/>
+      <c r="DY66" s="49"/>
+      <c r="DZ66" s="49"/>
+      <c r="EA66" s="49"/>
+      <c r="EB66" s="49"/>
+      <c r="EC66" s="49"/>
+      <c r="ED66" s="49"/>
+      <c r="EE66" s="49"/>
+      <c r="EF66" s="49"/>
+      <c r="EG66" s="49"/>
+      <c r="EH66" s="49"/>
+      <c r="EI66" s="49"/>
+      <c r="EJ66" s="49"/>
+      <c r="EK66" s="49"/>
+      <c r="EL66" s="49"/>
+      <c r="EM66" s="49"/>
+      <c r="EN66" s="49"/>
+      <c r="EO66" s="49"/>
+      <c r="EP66" s="49"/>
+      <c r="EQ66" s="49"/>
+      <c r="ER66" s="49"/>
+      <c r="ES66" s="49"/>
+      <c r="ET66" s="49"/>
+      <c r="EU66" s="49"/>
+      <c r="EV66" s="49"/>
+      <c r="EW66" s="49"/>
+      <c r="EX66" s="49"/>
+      <c r="EY66" s="49"/>
+      <c r="EZ66" s="49"/>
+      <c r="FA66" s="49"/>
+      <c r="FB66" s="49"/>
+      <c r="FC66" s="49"/>
+      <c r="FD66" s="49"/>
+      <c r="FE66" s="49"/>
+      <c r="FF66" s="49"/>
+      <c r="FG66" s="49"/>
+      <c r="FH66" s="49"/>
+      <c r="FI66" s="49"/>
+      <c r="FJ66" s="49"/>
+      <c r="FK66" s="49"/>
+      <c r="FL66" s="49"/>
+      <c r="FM66" s="49"/>
+      <c r="FN66" s="49"/>
+      <c r="FO66" s="49"/>
+      <c r="FP66" s="49"/>
+      <c r="FQ66" s="49"/>
+      <c r="FR66" s="49"/>
+      <c r="FS66" s="49"/>
+      <c r="FT66" s="49"/>
+      <c r="FU66" s="49"/>
+      <c r="FV66" s="49"/>
+      <c r="FW66" s="49"/>
+      <c r="FX66" s="49"/>
+      <c r="FY66" s="49"/>
+      <c r="FZ66" s="49"/>
+      <c r="GA66" s="49"/>
+      <c r="GB66" s="49"/>
+      <c r="GC66" s="49"/>
+      <c r="GD66" s="49"/>
+      <c r="GE66" s="49"/>
+      <c r="GF66" s="49"/>
+      <c r="GG66" s="49"/>
+      <c r="GH66" s="49"/>
+      <c r="GI66" s="49"/>
+      <c r="GJ66" s="49"/>
+      <c r="GK66" s="49"/>
+      <c r="GL66" s="49"/>
+      <c r="GM66" s="49"/>
+      <c r="GN66" s="49"/>
+      <c r="GO66" s="49"/>
+      <c r="GP66" s="49"/>
+      <c r="GQ66" s="49"/>
+      <c r="GR66" s="49"/>
+      <c r="GS66" s="49"/>
+      <c r="GT66" s="49"/>
+      <c r="GU66" s="49"/>
+      <c r="GV66" s="49"/>
+      <c r="GW66" s="49"/>
+      <c r="GX66" s="49"/>
+      <c r="GY66" s="49"/>
+      <c r="GZ66" s="49"/>
+      <c r="HA66" s="49"/>
+      <c r="HB66" s="49"/>
+      <c r="HC66" s="49"/>
+      <c r="HD66" s="49"/>
+      <c r="HE66" s="49"/>
+      <c r="HF66" s="49"/>
+      <c r="HG66" s="49"/>
+      <c r="HH66" s="49"/>
+      <c r="HI66" s="49"/>
+      <c r="HJ66" s="49"/>
+      <c r="HK66" s="49"/>
+      <c r="HL66" s="49"/>
+      <c r="HM66" s="49"/>
+      <c r="HN66" s="49"/>
+      <c r="HO66" s="49"/>
+      <c r="HP66" s="49"/>
+      <c r="HQ66" s="49"/>
+      <c r="HR66" s="49"/>
+      <c r="HS66" s="49"/>
+      <c r="HT66" s="49"/>
+      <c r="HU66" s="49"/>
+      <c r="HV66" s="49"/>
+      <c r="HW66" s="49"/>
+      <c r="HX66" s="49"/>
+      <c r="HY66" s="49"/>
+      <c r="HZ66" s="49"/>
+      <c r="IA66" s="49"/>
+      <c r="IB66" s="49"/>
+      <c r="IC66" s="49"/>
+      <c r="ID66" s="49"/>
+      <c r="IE66" s="49"/>
+      <c r="IF66" s="49"/>
+      <c r="IG66" s="49"/>
+      <c r="IH66" s="49"/>
+      <c r="II66" s="49"/>
+      <c r="IJ66" s="49"/>
+      <c r="IK66" s="49"/>
+      <c r="IL66" s="49"/>
+      <c r="IM66" s="49"/>
+      <c r="IN66" s="49"/>
+      <c r="IO66" s="49"/>
+      <c r="IP66" s="49"/>
+      <c r="IQ66" s="49"/>
+      <c r="IR66" s="49"/>
+      <c r="IS66" s="49"/>
+      <c r="IT66" s="49"/>
+      <c r="IU66" s="49"/>
+      <c r="IV66" s="49"/>
+      <c r="IW66" s="49"/>
+      <c r="IX66" s="49"/>
+      <c r="IY66" s="49"/>
+      <c r="IZ66" s="49"/>
+      <c r="JA66" s="49"/>
+      <c r="JB66" s="49"/>
+      <c r="JC66" s="49"/>
+      <c r="JD66" s="49"/>
+      <c r="JE66" s="49"/>
+      <c r="JF66" s="49"/>
+      <c r="JG66" s="49"/>
+      <c r="JH66" s="49"/>
+      <c r="JI66" s="49"/>
+      <c r="JJ66" s="49"/>
+      <c r="JK66" s="49"/>
+      <c r="JL66" s="49"/>
+      <c r="JM66" s="49"/>
+      <c r="JN66" s="49"/>
+      <c r="JO66" s="49"/>
+      <c r="JP66" s="49"/>
+      <c r="JQ66" s="49"/>
+      <c r="JR66" s="49"/>
+      <c r="JS66" s="49"/>
+      <c r="JT66" s="49"/>
+      <c r="JU66" s="49"/>
+      <c r="JV66" s="49"/>
+      <c r="JW66" s="49"/>
+      <c r="JX66" s="49"/>
+      <c r="JY66" s="49"/>
+      <c r="JZ66" s="49"/>
+      <c r="KA66" s="49"/>
+      <c r="KB66" s="49"/>
+      <c r="KC66" s="49"/>
+      <c r="KD66" s="49"/>
+      <c r="KE66" s="49"/>
+      <c r="KF66" s="49"/>
+      <c r="KG66" s="49"/>
+      <c r="KH66" s="49"/>
+      <c r="KI66" s="49"/>
+      <c r="KJ66" s="49"/>
+      <c r="KK66" s="49"/>
+      <c r="KL66" s="49"/>
+      <c r="KM66" s="49"/>
+      <c r="KN66" s="49"/>
+      <c r="KO66" s="49"/>
+      <c r="KP66" s="49"/>
+      <c r="KQ66" s="49"/>
+      <c r="KR66" s="49"/>
+      <c r="KS66" s="49"/>
+      <c r="KT66" s="49"/>
+      <c r="KU66" s="49"/>
+      <c r="KV66" s="49"/>
+      <c r="KW66" s="49"/>
+      <c r="KX66" s="49"/>
+      <c r="KY66" s="49"/>
+      <c r="KZ66" s="49"/>
+      <c r="LA66" s="49"/>
+      <c r="LB66" s="49"/>
+      <c r="LC66" s="49"/>
+      <c r="LD66" s="49"/>
+      <c r="LE66" s="49"/>
+      <c r="LF66" s="49"/>
+      <c r="LG66" s="49"/>
+      <c r="LH66" s="49"/>
+      <c r="LI66" s="49"/>
+      <c r="LJ66" s="49"/>
+      <c r="LK66" s="49"/>
+      <c r="LL66" s="49"/>
+      <c r="LM66" s="49"/>
+      <c r="LN66" s="49"/>
+      <c r="LO66" s="49"/>
+      <c r="LP66" s="49"/>
+      <c r="LQ66" s="49"/>
+      <c r="LR66" s="49"/>
+      <c r="LS66" s="49"/>
+      <c r="LT66" s="49"/>
+      <c r="LU66" s="49"/>
+      <c r="LV66" s="49"/>
+      <c r="LW66" s="49"/>
+      <c r="LX66" s="49"/>
+      <c r="LY66" s="49"/>
+      <c r="LZ66" s="49"/>
+      <c r="MA66" s="49"/>
+      <c r="MB66" s="49"/>
+      <c r="MC66" s="49"/>
+      <c r="MD66" s="49"/>
+      <c r="ME66" s="49"/>
+      <c r="MF66" s="49"/>
+      <c r="MG66" s="49"/>
+      <c r="MH66" s="49"/>
+      <c r="MI66" s="49"/>
+      <c r="MJ66" s="49"/>
+      <c r="MK66" s="49"/>
+      <c r="ML66" s="49"/>
+      <c r="MM66" s="49"/>
+      <c r="MN66" s="49"/>
+      <c r="MO66" s="49"/>
+      <c r="MP66" s="49"/>
+      <c r="MQ66" s="49"/>
+      <c r="MR66" s="49"/>
+      <c r="MS66" s="49"/>
+      <c r="MT66" s="49"/>
+      <c r="MU66" s="49"/>
+      <c r="MV66" s="49"/>
+      <c r="MW66" s="49"/>
+      <c r="MX66" s="49"/>
+      <c r="MY66" s="49"/>
+      <c r="MZ66" s="49"/>
+      <c r="NA66" s="49"/>
+      <c r="NB66" s="49"/>
+      <c r="NC66" s="49"/>
+      <c r="ND66" s="49"/>
+      <c r="NE66" s="49"/>
+      <c r="NF66" s="49"/>
+      <c r="NG66" s="49"/>
+      <c r="NH66" s="49"/>
+      <c r="NI66" s="49"/>
+      <c r="NJ66" s="49"/>
+      <c r="NK66" s="49"/>
+      <c r="NL66" s="49"/>
+      <c r="NM66" s="49"/>
+      <c r="NN66" s="49"/>
+      <c r="NO66" s="49"/>
+      <c r="NP66" s="49"/>
+      <c r="NQ66" s="49"/>
+      <c r="NR66" s="49"/>
+      <c r="NS66" s="49"/>
+      <c r="NT66" s="49"/>
+      <c r="NU66" s="49"/>
+      <c r="NV66" s="49"/>
+      <c r="NW66" s="49"/>
+      <c r="NX66" s="49"/>
+      <c r="NY66" s="49"/>
+      <c r="NZ66" s="49"/>
+      <c r="OA66" s="49"/>
+      <c r="OB66" s="49"/>
+      <c r="OC66" s="49"/>
+      <c r="OD66" s="49"/>
+      <c r="OE66" s="49"/>
+      <c r="OF66" s="49"/>
+      <c r="OG66" s="49"/>
+      <c r="OH66" s="49"/>
+      <c r="OI66" s="49"/>
+      <c r="OJ66" s="49"/>
+      <c r="OK66" s="49"/>
+      <c r="OL66" s="49"/>
+      <c r="OM66" s="49"/>
+      <c r="ON66" s="49"/>
+      <c r="OO66" s="49"/>
+      <c r="OP66" s="49"/>
+      <c r="OQ66" s="49"/>
+      <c r="OR66" s="49"/>
+      <c r="OS66" s="49"/>
+      <c r="OT66" s="49"/>
+      <c r="OU66" s="49"/>
+      <c r="OV66" s="49"/>
+      <c r="OW66" s="49"/>
+      <c r="OX66" s="49"/>
+      <c r="OY66" s="49"/>
+      <c r="OZ66" s="49"/>
+      <c r="PA66" s="49"/>
+      <c r="PB66" s="49"/>
+      <c r="PC66" s="49"/>
+      <c r="PD66" s="49"/>
+      <c r="PE66" s="49"/>
+      <c r="PF66" s="49"/>
+      <c r="PG66" s="49"/>
+      <c r="PH66" s="49"/>
+      <c r="PI66" s="49"/>
+      <c r="PJ66" s="49"/>
+      <c r="PK66" s="49"/>
+      <c r="PL66" s="49"/>
+      <c r="PM66" s="49"/>
+      <c r="PN66" s="49"/>
+      <c r="PO66" s="49"/>
+      <c r="PP66" s="49"/>
+      <c r="PQ66" s="49"/>
+      <c r="PR66" s="49"/>
+      <c r="PS66" s="49"/>
+      <c r="PT66" s="49"/>
+      <c r="PU66" s="49"/>
+      <c r="PV66" s="49"/>
+      <c r="PW66" s="49"/>
+      <c r="PX66" s="49"/>
+      <c r="PY66" s="49"/>
+      <c r="PZ66" s="49"/>
+      <c r="QA66" s="49"/>
+      <c r="QB66" s="49"/>
+      <c r="QC66" s="49"/>
+      <c r="QD66" s="49"/>
+      <c r="QE66" s="49"/>
+      <c r="QF66" s="49"/>
+      <c r="QG66" s="49"/>
+      <c r="QH66" s="49"/>
+      <c r="QI66" s="49"/>
+      <c r="QJ66" s="49"/>
+      <c r="QK66" s="49"/>
+      <c r="QL66" s="49"/>
+      <c r="QM66" s="49"/>
+      <c r="QN66" s="49"/>
+      <c r="QO66" s="49"/>
+      <c r="QP66" s="49"/>
+      <c r="QQ66" s="49"/>
+      <c r="QR66" s="49"/>
+      <c r="QS66" s="49"/>
+      <c r="QT66" s="49"/>
+      <c r="QU66" s="49"/>
+      <c r="QV66" s="49"/>
+      <c r="QW66" s="49"/>
+      <c r="QX66" s="49"/>
+      <c r="QY66" s="49"/>
+      <c r="QZ66" s="49"/>
+      <c r="RA66" s="49"/>
+      <c r="RB66" s="49"/>
+      <c r="RC66" s="49"/>
+      <c r="RD66" s="49"/>
+      <c r="RE66" s="49"/>
+      <c r="RF66" s="49"/>
+      <c r="RG66" s="49"/>
+      <c r="RH66" s="49"/>
+      <c r="RI66" s="49"/>
+      <c r="RJ66" s="49"/>
+      <c r="RK66" s="49"/>
+      <c r="RL66" s="49"/>
+      <c r="RM66" s="49"/>
+      <c r="RN66" s="49"/>
+      <c r="RO66" s="49"/>
+      <c r="RP66" s="49"/>
+      <c r="RQ66" s="49"/>
+      <c r="RR66" s="49"/>
+      <c r="RS66" s="49"/>
+      <c r="RT66" s="49"/>
+      <c r="RU66" s="49"/>
+      <c r="RV66" s="49"/>
+      <c r="RW66" s="49"/>
+      <c r="RX66" s="49"/>
+      <c r="RY66" s="49"/>
+      <c r="RZ66" s="49"/>
+      <c r="SA66" s="49"/>
+      <c r="SB66" s="49"/>
+      <c r="SC66" s="49"/>
+      <c r="SD66" s="49"/>
+      <c r="SE66" s="49"/>
+      <c r="SF66" s="49"/>
+      <c r="SG66" s="49"/>
+      <c r="SH66" s="49"/>
+      <c r="SI66" s="49"/>
+      <c r="SJ66" s="49"/>
+      <c r="SK66" s="49"/>
+      <c r="SL66" s="49"/>
+      <c r="SM66" s="49"/>
+      <c r="SN66" s="49"/>
+      <c r="SO66" s="49"/>
+      <c r="SP66" s="49"/>
+      <c r="SQ66" s="49"/>
+      <c r="SR66" s="49"/>
+      <c r="SS66" s="49"/>
+      <c r="ST66" s="49"/>
+      <c r="SU66" s="49"/>
+      <c r="SV66" s="49"/>
+      <c r="SW66" s="49"/>
+      <c r="SX66" s="49"/>
+      <c r="SY66" s="49"/>
+      <c r="SZ66" s="49"/>
+      <c r="TA66" s="49"/>
+      <c r="TB66" s="49"/>
+      <c r="TC66" s="49"/>
+      <c r="TD66" s="49"/>
+      <c r="TE66" s="49"/>
+      <c r="TF66" s="49"/>
+      <c r="TG66" s="49"/>
+      <c r="TH66" s="49"/>
+      <c r="TI66" s="49"/>
+      <c r="TJ66" s="49"/>
+      <c r="TK66" s="49"/>
+      <c r="TL66" s="49"/>
+      <c r="TM66" s="49"/>
+      <c r="TN66" s="49"/>
+      <c r="TO66" s="49"/>
+      <c r="TP66" s="49"/>
+      <c r="TQ66" s="49"/>
+      <c r="TR66" s="49"/>
+      <c r="TS66" s="49"/>
+      <c r="TT66" s="49"/>
+      <c r="TU66" s="49"/>
+      <c r="TV66" s="49"/>
+      <c r="TW66" s="49"/>
+      <c r="TX66" s="49"/>
+      <c r="TY66" s="49"/>
+      <c r="TZ66" s="49"/>
+      <c r="UA66" s="49"/>
+      <c r="UB66" s="49"/>
+      <c r="UC66" s="49"/>
+      <c r="UD66" s="49"/>
+      <c r="UE66" s="49"/>
+      <c r="UF66" s="49"/>
+      <c r="UG66" s="49"/>
+      <c r="UH66" s="49"/>
+      <c r="UI66" s="49"/>
+      <c r="UJ66" s="49"/>
+      <c r="UK66" s="49"/>
+      <c r="UL66" s="49"/>
+      <c r="UM66" s="49"/>
+      <c r="UN66" s="49"/>
+      <c r="UO66" s="49"/>
+      <c r="UP66" s="49"/>
+      <c r="UQ66" s="49"/>
+      <c r="UR66" s="49"/>
+      <c r="US66" s="49"/>
+      <c r="UT66" s="49"/>
+      <c r="UU66" s="49"/>
+      <c r="UV66" s="49"/>
+      <c r="UW66" s="49"/>
+      <c r="UX66" s="49"/>
+      <c r="UY66" s="49"/>
+      <c r="UZ66" s="49"/>
+      <c r="VA66" s="49"/>
+      <c r="VB66" s="49"/>
+      <c r="VC66" s="49"/>
+      <c r="VD66" s="49"/>
+      <c r="VE66" s="49"/>
+      <c r="VF66" s="49"/>
+      <c r="VG66" s="49"/>
+      <c r="VH66" s="49"/>
+      <c r="VI66" s="49"/>
+      <c r="VJ66" s="49"/>
+      <c r="VK66" s="49"/>
+      <c r="VL66" s="49"/>
+      <c r="VM66" s="49"/>
+      <c r="VN66" s="49"/>
+      <c r="VO66" s="49"/>
+      <c r="VP66" s="49"/>
+      <c r="VQ66" s="49"/>
+      <c r="VR66" s="49"/>
+      <c r="VS66" s="49"/>
+      <c r="VT66" s="49"/>
+      <c r="VU66" s="49"/>
+      <c r="VV66" s="49"/>
+      <c r="VW66" s="49"/>
+      <c r="VX66" s="49"/>
+      <c r="VY66" s="49"/>
+      <c r="VZ66" s="49"/>
+      <c r="WA66" s="49"/>
+      <c r="WB66" s="49"/>
+      <c r="WC66" s="49"/>
+      <c r="WD66" s="49"/>
+      <c r="WE66" s="49"/>
+      <c r="WF66" s="49"/>
+      <c r="WG66" s="49"/>
+      <c r="WH66" s="49"/>
+      <c r="WI66" s="49"/>
+      <c r="WJ66" s="49"/>
+      <c r="WK66" s="49"/>
+      <c r="WL66" s="49"/>
+      <c r="WM66" s="49"/>
+      <c r="WN66" s="49"/>
+      <c r="WO66" s="49"/>
+      <c r="WP66" s="49"/>
+      <c r="WQ66" s="49"/>
+      <c r="WR66" s="49"/>
+      <c r="WS66" s="49"/>
+      <c r="WT66" s="49"/>
+      <c r="WU66" s="49"/>
+      <c r="WV66" s="49"/>
+      <c r="WW66" s="49"/>
+      <c r="WX66" s="49"/>
+      <c r="WY66" s="49"/>
+      <c r="WZ66" s="49"/>
+      <c r="XA66" s="49"/>
+      <c r="XB66" s="49"/>
+      <c r="XC66" s="49"/>
+      <c r="XD66" s="49"/>
+      <c r="XE66" s="49"/>
+      <c r="XF66" s="49"/>
+      <c r="XG66" s="49"/>
+      <c r="XH66" s="49"/>
+      <c r="XI66" s="49"/>
+      <c r="XJ66" s="49"/>
+      <c r="XK66" s="49"/>
+      <c r="XL66" s="49"/>
+      <c r="XM66" s="49"/>
+      <c r="XN66" s="49"/>
+      <c r="XO66" s="49"/>
+      <c r="XP66" s="49"/>
+      <c r="XQ66" s="49"/>
+      <c r="XR66" s="49"/>
+      <c r="XS66" s="49"/>
+      <c r="XT66" s="49"/>
+      <c r="XU66" s="49"/>
+      <c r="XV66" s="49"/>
+      <c r="XW66" s="49"/>
+      <c r="XX66" s="49"/>
+      <c r="XY66" s="49"/>
+      <c r="XZ66" s="49"/>
+      <c r="YA66" s="49"/>
+      <c r="YB66" s="49"/>
+      <c r="YC66" s="49"/>
+      <c r="YD66" s="49"/>
+      <c r="YE66" s="49"/>
+      <c r="YF66" s="49"/>
+      <c r="YG66" s="49"/>
+      <c r="YH66" s="49"/>
+      <c r="YI66" s="49"/>
+      <c r="YJ66" s="49"/>
+      <c r="YK66" s="49"/>
+      <c r="YL66" s="49"/>
+      <c r="YM66" s="49"/>
+      <c r="YN66" s="49"/>
+      <c r="YO66" s="49"/>
+      <c r="YP66" s="49"/>
+      <c r="YQ66" s="49"/>
+      <c r="YR66" s="49"/>
+      <c r="YS66" s="49"/>
+      <c r="YT66" s="49"/>
+      <c r="YU66" s="49"/>
+      <c r="YV66" s="49"/>
+      <c r="YW66" s="49"/>
+      <c r="YX66" s="49"/>
+      <c r="YY66" s="49"/>
+      <c r="YZ66" s="49"/>
+      <c r="ZA66" s="49"/>
+      <c r="ZB66" s="49"/>
+      <c r="ZC66" s="49"/>
+      <c r="ZD66" s="49"/>
+      <c r="ZE66" s="49"/>
+      <c r="ZF66" s="49"/>
+      <c r="ZG66" s="49"/>
+      <c r="ZH66" s="49"/>
+      <c r="ZI66" s="49"/>
+      <c r="ZJ66" s="49"/>
+      <c r="ZK66" s="49"/>
+      <c r="ZL66" s="49"/>
+      <c r="ZM66" s="49"/>
+      <c r="ZN66" s="49"/>
+      <c r="ZO66" s="49"/>
+      <c r="ZP66" s="49"/>
+      <c r="ZQ66" s="49"/>
+      <c r="ZR66" s="49"/>
+      <c r="ZS66" s="49"/>
+      <c r="ZT66" s="49"/>
+      <c r="ZU66" s="49"/>
+      <c r="ZV66" s="49"/>
+      <c r="ZW66" s="49"/>
+      <c r="ZX66" s="49"/>
+      <c r="ZY66" s="49"/>
+      <c r="ZZ66" s="49"/>
+      <c r="AAA66" s="49"/>
+      <c r="AAB66" s="49"/>
+      <c r="AAC66" s="49"/>
+      <c r="AAD66" s="49"/>
+      <c r="AAE66" s="49"/>
+      <c r="AAF66" s="49"/>
+      <c r="AAG66" s="49"/>
+      <c r="AAH66" s="49"/>
+      <c r="AAI66" s="49"/>
+      <c r="AAJ66" s="49"/>
+      <c r="AAK66" s="49"/>
+      <c r="AAL66" s="49"/>
+      <c r="AAM66" s="49"/>
+      <c r="AAN66" s="49"/>
+      <c r="AAO66" s="49"/>
+      <c r="AAP66" s="49"/>
+      <c r="AAQ66" s="49"/>
+      <c r="AAR66" s="49"/>
+      <c r="AAS66" s="49"/>
+      <c r="AAT66" s="49"/>
+      <c r="AAU66" s="49"/>
+      <c r="AAV66" s="49"/>
+      <c r="AAW66" s="49"/>
+      <c r="AAX66" s="49"/>
+      <c r="AAY66" s="49"/>
+      <c r="AAZ66" s="49"/>
+      <c r="ABA66" s="49"/>
+      <c r="ABB66" s="49"/>
+      <c r="ABC66" s="49"/>
+      <c r="ABD66" s="49"/>
+      <c r="ABE66" s="49"/>
+      <c r="ABF66" s="49"/>
+      <c r="ABG66" s="49"/>
+      <c r="ABH66" s="49"/>
+      <c r="ABI66" s="49"/>
+      <c r="ABJ66" s="49"/>
+      <c r="ABK66" s="49"/>
+      <c r="ABL66" s="49"/>
+      <c r="ABM66" s="49"/>
+      <c r="ABN66" s="49"/>
+      <c r="ABO66" s="49"/>
+      <c r="ABP66" s="49"/>
+      <c r="ABQ66" s="49"/>
+      <c r="ABR66" s="49"/>
+      <c r="ABS66" s="49"/>
+      <c r="ABT66" s="49"/>
+      <c r="ABU66" s="49"/>
+      <c r="ABV66" s="49"/>
+      <c r="ABW66" s="49"/>
+      <c r="ABX66" s="49"/>
+      <c r="ABY66" s="49"/>
+      <c r="ABZ66" s="49"/>
+      <c r="ACA66" s="49"/>
+      <c r="ACB66" s="49"/>
+      <c r="ACC66" s="49"/>
+      <c r="ACD66" s="49"/>
+      <c r="ACE66" s="49"/>
+      <c r="ACF66" s="49"/>
+      <c r="ACG66" s="49"/>
+      <c r="ACH66" s="49"/>
+      <c r="ACI66" s="49"/>
+      <c r="ACJ66" s="49"/>
+      <c r="ACK66" s="49"/>
+      <c r="ACL66" s="49"/>
+      <c r="ACM66" s="49"/>
+      <c r="ACN66" s="49"/>
+      <c r="ACO66" s="49"/>
+      <c r="ACP66" s="49"/>
+      <c r="ACQ66" s="49"/>
+      <c r="ACR66" s="49"/>
+      <c r="ACS66" s="49"/>
+      <c r="ACT66" s="49"/>
+      <c r="ACU66" s="49"/>
+      <c r="ACV66" s="49"/>
+      <c r="ACW66" s="49"/>
+      <c r="ACX66" s="49"/>
+      <c r="ACY66" s="49"/>
+      <c r="ACZ66" s="49"/>
+      <c r="ADA66" s="49"/>
+      <c r="ADB66" s="49"/>
+      <c r="ADC66" s="49"/>
+      <c r="ADD66" s="49"/>
+      <c r="ADE66" s="49"/>
+      <c r="ADF66" s="49"/>
+      <c r="ADG66" s="49"/>
+      <c r="ADH66" s="49"/>
+      <c r="ADI66" s="49"/>
+      <c r="ADJ66" s="49"/>
+      <c r="ADK66" s="49"/>
+      <c r="ADL66" s="49"/>
+      <c r="ADM66" s="49"/>
+      <c r="ADN66" s="49"/>
+      <c r="ADO66" s="49"/>
+      <c r="ADP66" s="49"/>
+      <c r="ADQ66" s="49"/>
+      <c r="ADR66" s="49"/>
+      <c r="ADS66" s="49"/>
+      <c r="ADT66" s="49"/>
+      <c r="ADU66" s="49"/>
+      <c r="ADV66" s="49"/>
+      <c r="ADW66" s="49"/>
+      <c r="ADX66" s="49"/>
+      <c r="ADY66" s="49"/>
+      <c r="ADZ66" s="49"/>
+      <c r="AEA66" s="49"/>
+      <c r="AEB66" s="49"/>
+      <c r="AEC66" s="49"/>
+      <c r="AED66" s="49"/>
+      <c r="AEE66" s="49"/>
+      <c r="AEF66" s="49"/>
+      <c r="AEG66" s="49"/>
+      <c r="AEH66" s="49"/>
+      <c r="AEI66" s="49"/>
+      <c r="AEJ66" s="49"/>
+      <c r="AEK66" s="49"/>
+      <c r="AEL66" s="49"/>
+      <c r="AEM66" s="49"/>
+      <c r="AEN66" s="49"/>
+      <c r="AEO66" s="49"/>
+      <c r="AEP66" s="49"/>
+      <c r="AEQ66" s="49"/>
+      <c r="AER66" s="49"/>
+      <c r="AES66" s="49"/>
+      <c r="AET66" s="49"/>
+      <c r="AEU66" s="49"/>
+      <c r="AEV66" s="49"/>
+      <c r="AEW66" s="49"/>
+      <c r="AEX66" s="49"/>
+      <c r="AEY66" s="49"/>
+      <c r="AEZ66" s="49"/>
+      <c r="AFA66" s="49"/>
+      <c r="AFB66" s="49"/>
+      <c r="AFC66" s="49"/>
+      <c r="AFD66" s="49"/>
+      <c r="AFE66" s="49"/>
+      <c r="AFF66" s="49"/>
+      <c r="AFG66" s="49"/>
+      <c r="AFH66" s="49"/>
+      <c r="AFI66" s="49"/>
+      <c r="AFJ66" s="49"/>
+      <c r="AFK66" s="49"/>
+      <c r="AFL66" s="49"/>
+      <c r="AFM66" s="49"/>
+      <c r="AFN66" s="49"/>
+      <c r="AFO66" s="49"/>
+      <c r="AFP66" s="49"/>
+      <c r="AFQ66" s="49"/>
+      <c r="AFR66" s="49"/>
+      <c r="AFS66" s="49"/>
+      <c r="AFT66" s="49"/>
+      <c r="AFU66" s="49"/>
+      <c r="AFV66" s="49"/>
+      <c r="AFW66" s="49"/>
+      <c r="AFX66" s="49"/>
+      <c r="AFY66" s="49"/>
+      <c r="AFZ66" s="49"/>
+      <c r="AGA66" s="49"/>
+      <c r="AGB66" s="49"/>
+      <c r="AGC66" s="49"/>
+      <c r="AGD66" s="49"/>
+      <c r="AGE66" s="49"/>
+      <c r="AGF66" s="49"/>
+      <c r="AGG66" s="49"/>
+      <c r="AGH66" s="49"/>
+      <c r="AGI66" s="49"/>
+      <c r="AGJ66" s="49"/>
+      <c r="AGK66" s="49"/>
+      <c r="AGL66" s="49"/>
+      <c r="AGM66" s="49"/>
+      <c r="AGN66" s="49"/>
+      <c r="AGO66" s="49"/>
+      <c r="AGP66" s="49"/>
+      <c r="AGQ66" s="49"/>
+      <c r="AGR66" s="49"/>
+      <c r="AGS66" s="49"/>
+      <c r="AGT66" s="49"/>
+      <c r="AGU66" s="49"/>
+      <c r="AGV66" s="49"/>
+      <c r="AGW66" s="49"/>
+      <c r="AGX66" s="49"/>
+      <c r="AGY66" s="49"/>
+      <c r="AGZ66" s="49"/>
+      <c r="AHA66" s="49"/>
+      <c r="AHB66" s="49"/>
+      <c r="AHC66" s="49"/>
+      <c r="AHD66" s="49"/>
+      <c r="AHE66" s="49"/>
+      <c r="AHF66" s="49"/>
+      <c r="AHG66" s="49"/>
+      <c r="AHH66" s="49"/>
+      <c r="AHI66" s="49"/>
+      <c r="AHJ66" s="49"/>
+      <c r="AHK66" s="49"/>
+      <c r="AHL66" s="49"/>
+      <c r="AHM66" s="49"/>
+      <c r="AHN66" s="49"/>
+      <c r="AHO66" s="49"/>
+      <c r="AHP66" s="49"/>
+      <c r="AHQ66" s="49"/>
+      <c r="AHR66" s="49"/>
+      <c r="AHS66" s="49"/>
+      <c r="AHT66" s="49"/>
+      <c r="AHU66" s="49"/>
+      <c r="AHV66" s="49"/>
+      <c r="AHW66" s="49"/>
+      <c r="AHX66" s="49"/>
+      <c r="AHY66" s="49"/>
+      <c r="AHZ66" s="49"/>
+      <c r="AIA66" s="49"/>
+      <c r="AIB66" s="49"/>
+      <c r="AIC66" s="49"/>
+      <c r="AID66" s="49"/>
+      <c r="AIE66" s="49"/>
+      <c r="AIF66" s="49"/>
+      <c r="AIG66" s="49"/>
+      <c r="AIH66" s="49"/>
+      <c r="AII66" s="49"/>
+      <c r="AIJ66" s="49"/>
+      <c r="AIK66" s="49"/>
+      <c r="AIL66" s="49"/>
+      <c r="AIM66" s="49"/>
+      <c r="AIN66" s="49"/>
+      <c r="AIO66" s="49"/>
+      <c r="AIP66" s="49"/>
+      <c r="AIQ66" s="49"/>
+      <c r="AIR66" s="49"/>
+      <c r="AIS66" s="49"/>
+      <c r="AIT66" s="49"/>
+      <c r="AIU66" s="49"/>
+      <c r="AIV66" s="49"/>
+      <c r="AIW66" s="49"/>
+      <c r="AIX66" s="49"/>
+      <c r="AIY66" s="49"/>
+      <c r="AIZ66" s="49"/>
+      <c r="AJA66" s="49"/>
+      <c r="AJB66" s="49"/>
+      <c r="AJC66" s="49"/>
+      <c r="AJD66" s="49"/>
+      <c r="AJE66" s="49"/>
+      <c r="AJF66" s="49"/>
+      <c r="AJG66" s="49"/>
+      <c r="AJH66" s="49"/>
+      <c r="AJI66" s="49"/>
+      <c r="AJJ66" s="49"/>
+      <c r="AJK66" s="49"/>
+      <c r="AJL66" s="49"/>
+      <c r="AJM66" s="49"/>
+      <c r="AJN66" s="49"/>
+      <c r="AJO66" s="49"/>
+      <c r="AJP66" s="49"/>
+      <c r="AJQ66" s="49"/>
+      <c r="AJR66" s="49"/>
+      <c r="AJS66" s="49"/>
+      <c r="AJT66" s="49"/>
+      <c r="AJU66" s="49"/>
+      <c r="AJV66" s="49"/>
+      <c r="AJW66" s="49"/>
+      <c r="AJX66" s="49"/>
+      <c r="AJY66" s="49"/>
+      <c r="AJZ66" s="49"/>
+      <c r="AKA66" s="49"/>
+      <c r="AKB66" s="49"/>
+      <c r="AKC66" s="49"/>
+      <c r="AKD66" s="49"/>
+      <c r="AKE66" s="49"/>
+      <c r="AKF66" s="49"/>
+      <c r="AKG66" s="49"/>
+      <c r="AKH66" s="49"/>
+      <c r="AKI66" s="49"/>
+      <c r="AKJ66" s="49"/>
+      <c r="AKK66" s="49"/>
+      <c r="AKL66" s="49"/>
+      <c r="AKM66" s="49"/>
+      <c r="AKN66" s="49"/>
+      <c r="AKO66" s="49"/>
+      <c r="AKP66" s="49"/>
+      <c r="AKQ66" s="49"/>
+      <c r="AKR66" s="49"/>
+      <c r="AKS66" s="49"/>
+      <c r="AKT66" s="49"/>
+      <c r="AKU66" s="49"/>
+      <c r="AKV66" s="49"/>
+      <c r="AKW66" s="49"/>
+      <c r="AKX66" s="49"/>
+      <c r="AKY66" s="49"/>
+      <c r="AKZ66" s="49"/>
+      <c r="ALA66" s="49"/>
+      <c r="ALB66" s="49"/>
+      <c r="ALC66" s="49"/>
+      <c r="ALD66" s="49"/>
+      <c r="ALE66" s="49"/>
+      <c r="ALF66" s="49"/>
+      <c r="ALG66" s="49"/>
+      <c r="ALH66" s="49"/>
+      <c r="ALI66" s="49"/>
+      <c r="ALJ66" s="49"/>
+      <c r="ALK66" s="49"/>
+      <c r="ALL66" s="49"/>
+      <c r="ALM66" s="49"/>
+      <c r="ALN66" s="49"/>
+      <c r="ALO66" s="49"/>
+      <c r="ALP66" s="49"/>
+      <c r="ALQ66" s="49"/>
+      <c r="ALR66" s="49"/>
+      <c r="ALS66" s="49"/>
+      <c r="ALT66" s="49"/>
+      <c r="ALU66" s="49"/>
+      <c r="ALV66" s="49"/>
+      <c r="ALW66" s="49"/>
+      <c r="ALX66" s="49"/>
+      <c r="ALY66" s="49"/>
+      <c r="ALZ66" s="49"/>
+      <c r="AMA66" s="49"/>
+      <c r="AMB66" s="49"/>
+      <c r="AMC66" s="49"/>
+      <c r="AMD66" s="49"/>
+      <c r="AME66" s="49"/>
+      <c r="AMF66" s="49"/>
+      <c r="AMG66" s="49"/>
+      <c r="AMH66" s="49"/>
+      <c r="AMI66" s="49"/>
+      <c r="AMJ66" s="49"/>
+      <c r="AMK66" s="49"/>
+    </row>
+    <row r="67" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="B67" s="54" t="s">
         <v>749</v>
       </c>
-      <c r="C66" s="53"/>
+      <c r="C67" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C3:L3"/>
@@ -7296,19 +8335,19 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="57" t="s">
+    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-    </row>
-    <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="58" t="s">
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+    </row>
+    <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="59" t="s">
         <v>205</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -7318,8 +8357,8 @@
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="58"/>
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="59"/>
       <c r="C7" s="16" t="s">
         <v>207</v>
       </c>
@@ -7327,8 +8366,8 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="58"/>
+    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="59"/>
       <c r="C8" s="16" t="s">
         <v>208</v>
       </c>
@@ -7336,8 +8375,8 @@
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
     </row>
-    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="58"/>
+    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="59"/>
       <c r="C9" s="16" t="s">
         <v>209</v>
       </c>
@@ -7345,14 +8384,14 @@
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="58"/>
-      <c r="C10" s="59" t="s">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="59"/>
+      <c r="C10" s="60" t="s">
         <v>210</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7378,23 +8417,23 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.53125" customWidth="1"/>
-    <col min="5" max="5" width="19.53125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="60" t="s">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="61" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
         <v>29</v>
       </c>
@@ -7408,7 +8447,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
@@ -7422,7 +8461,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>107</v>
       </c>
@@ -7434,7 +8473,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
         <v>212</v>
       </c>
@@ -7446,7 +8485,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36" t="s">
         <v>131</v>
       </c>
@@ -7458,7 +8497,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="36" t="s">
         <v>802</v>
       </c>
@@ -7470,7 +8509,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="36" t="s">
         <v>213</v>
       </c>
@@ -7484,7 +8523,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="36" t="s">
         <v>141</v>
       </c>
@@ -7498,7 +8537,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="36" t="s">
         <v>216</v>
       </c>
@@ -7512,7 +8551,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="36" t="s">
         <v>146</v>
       </c>
@@ -7526,7 +8565,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="36" t="s">
         <v>151</v>
       </c>
@@ -7540,7 +8579,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="36" t="s">
         <v>161</v>
       </c>
@@ -7554,7 +8593,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="36" t="s">
         <v>753</v>
       </c>
@@ -7568,7 +8607,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
         <v>756</v>
       </c>
@@ -7604,31 +8643,31 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.46484375" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="9" max="9" width="24.86328125" customWidth="1"/>
-    <col min="10" max="10" width="33.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.46484375" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="65" t="s">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="66" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="66"/>
+      <c r="C2" s="67"/>
       <c r="E2" s="23" t="s">
         <v>218</v>
       </c>
       <c r="F2" s="24"/>
-      <c r="I2" s="65" t="s">
+      <c r="I2" s="66" t="s">
         <v>219</v>
       </c>
-      <c r="J2" s="66"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J2" s="67"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>29</v>
       </c>
@@ -7648,7 +8687,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>220</v>
       </c>
@@ -7668,7 +8707,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>222</v>
       </c>
@@ -7688,7 +8727,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>227</v>
       </c>
@@ -7708,7 +8747,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>233</v>
       </c>
@@ -7728,7 +8767,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
         <v>239</v>
       </c>
@@ -7748,7 +8787,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>244</v>
       </c>
@@ -7762,7 +8801,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>248</v>
       </c>
@@ -7776,7 +8815,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
         <v>252</v>
       </c>
@@ -7790,7 +8829,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
         <v>256</v>
       </c>
@@ -7804,7 +8843,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
         <v>260</v>
       </c>
@@ -7817,12 +8856,12 @@
       <c r="F13" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="I13" s="65" t="s">
+      <c r="I13" s="66" t="s">
         <v>264</v>
       </c>
-      <c r="J13" s="66"/>
-    </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J13" s="67"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
         <v>265</v>
       </c>
@@ -7842,7 +8881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
         <v>269</v>
       </c>
@@ -7862,7 +8901,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
         <v>273</v>
       </c>
@@ -7882,7 +8921,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
         <v>246</v>
       </c>
@@ -7902,7 +8941,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
         <v>283</v>
       </c>
@@ -7922,7 +8961,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
         <v>289</v>
       </c>
@@ -7942,7 +8981,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="20" t="s">
         <v>250</v>
       </c>
@@ -7962,7 +9001,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>300</v>
       </c>
@@ -7976,7 +9015,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="20" t="s">
         <v>304</v>
       </c>
@@ -7990,7 +9029,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
         <v>308</v>
       </c>
@@ -8003,12 +9042,12 @@
       <c r="F23" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="I23" s="65" t="s">
+      <c r="I23" s="66" t="s">
         <v>312</v>
       </c>
-      <c r="J23" s="66"/>
-    </row>
-    <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J23" s="67"/>
+    </row>
+    <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
         <v>313</v>
       </c>
@@ -8028,7 +9067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
         <v>317</v>
       </c>
@@ -8048,7 +9087,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
         <v>321</v>
       </c>
@@ -8068,7 +9107,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
         <v>327</v>
       </c>
@@ -8088,7 +9127,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="20" t="s">
         <v>333</v>
       </c>
@@ -8108,7 +9147,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>339</v>
       </c>
@@ -8122,7 +9161,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
         <v>343</v>
       </c>
@@ -8136,7 +9175,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
         <v>347</v>
       </c>
@@ -8150,7 +9189,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="20" t="s">
         <v>351</v>
       </c>
@@ -8163,12 +9202,12 @@
       <c r="F32" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="I32" s="65" t="s">
+      <c r="I32" s="66" t="s">
         <v>750</v>
       </c>
-      <c r="J32" s="66"/>
-    </row>
-    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J32" s="67"/>
+    </row>
+    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="20" t="s">
         <v>262</v>
       </c>
@@ -8188,7 +9227,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="20" t="s">
         <v>357</v>
       </c>
@@ -8208,7 +9247,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="20" t="s">
         <v>361</v>
       </c>
@@ -8228,7 +9267,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="20" t="s">
         <v>365</v>
       </c>
@@ -8248,7 +9287,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
         <v>369</v>
       </c>
@@ -8262,7 +9301,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="20" t="s">
         <v>373</v>
       </c>
@@ -8276,7 +9315,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="20" t="s">
         <v>377</v>
       </c>
@@ -8289,12 +9328,12 @@
       <c r="F39" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="I39" s="65" t="s">
+      <c r="I39" s="66" t="s">
         <v>783</v>
       </c>
-      <c r="J39" s="66"/>
-    </row>
-    <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J39" s="67"/>
+    </row>
+    <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="20" t="s">
         <v>291</v>
       </c>
@@ -8314,7 +9353,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="20" t="s">
         <v>116</v>
       </c>
@@ -8334,7 +9373,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="20" t="s">
         <v>387</v>
       </c>
@@ -8354,7 +9393,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="20" t="s">
         <v>391</v>
       </c>
@@ -8374,7 +9413,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="20" t="s">
         <v>285</v>
       </c>
@@ -8388,7 +9427,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="20" t="s">
         <v>398</v>
       </c>
@@ -8402,7 +9441,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="20" t="s">
         <v>402</v>
       </c>
@@ -8415,12 +9454,12 @@
       <c r="F46" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="I46" s="65" t="s">
+      <c r="I46" s="66" t="s">
         <v>793</v>
       </c>
-      <c r="J46" s="66"/>
-    </row>
-    <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J46" s="67"/>
+    </row>
+    <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="20" t="s">
         <v>406</v>
       </c>
@@ -8440,7 +9479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="20" t="s">
         <v>410</v>
       </c>
@@ -8460,7 +9499,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="20" t="s">
         <v>414</v>
       </c>
@@ -8480,7 +9519,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="20" t="s">
         <v>418</v>
       </c>
@@ -8500,7 +9539,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="20" t="s">
         <v>422</v>
       </c>
@@ -8514,7 +9553,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>426</v>
       </c>
@@ -8528,7 +9567,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="20" t="s">
         <v>430</v>
       </c>
@@ -8542,7 +9581,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>434</v>
       </c>
@@ -8556,7 +9595,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="20" t="s">
         <v>349</v>
       </c>
@@ -8570,7 +9609,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="56" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="20" t="s">
         <v>441</v>
       </c>
@@ -8584,7 +9623,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="20" t="s">
         <v>323</v>
       </c>
@@ -8592,7 +9631,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="58" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="20" t="s">
         <v>446</v>
       </c>
@@ -8600,19 +9639,19 @@
         <v>447</v>
       </c>
     </row>
-    <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="20" t="s">
         <v>448</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="E59" s="65" t="s">
+      <c r="E59" s="66" t="s">
         <v>759</v>
       </c>
-      <c r="F59" s="66"/>
-    </row>
-    <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F59" s="67"/>
+    </row>
+    <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="20" t="s">
         <v>450</v>
       </c>
@@ -8626,7 +9665,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="20" t="s">
         <v>452</v>
       </c>
@@ -8640,7 +9679,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="20" t="s">
         <v>454</v>
       </c>
@@ -8654,7 +9693,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="20" t="s">
         <v>393</v>
       </c>
@@ -8668,7 +9707,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="20" t="s">
         <v>457</v>
       </c>
@@ -8682,7 +9721,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="20" t="s">
         <v>459</v>
       </c>
@@ -8696,7 +9735,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="20" t="s">
         <v>461</v>
       </c>
@@ -8710,7 +9749,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="20" t="s">
         <v>463</v>
       </c>
@@ -8724,7 +9763,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="20" t="s">
         <v>465</v>
       </c>
@@ -8738,7 +9777,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="20" t="s">
         <v>396</v>
       </c>
@@ -8752,7 +9791,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="20" t="s">
         <v>467</v>
       </c>
@@ -8766,7 +9805,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="20" t="s">
         <v>469</v>
       </c>
@@ -8780,7 +9819,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="20" t="s">
         <v>471</v>
       </c>
@@ -8794,7 +9833,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="20" t="s">
         <v>473</v>
       </c>
@@ -8808,7 +9847,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="20" t="s">
         <v>475</v>
       </c>
@@ -8822,7 +9861,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="20" t="s">
         <v>477</v>
       </c>
@@ -8830,7 +9869,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="20" t="s">
         <v>479</v>
       </c>
@@ -8838,7 +9877,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="20" t="s">
         <v>481</v>
       </c>
@@ -8846,7 +9885,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="20" t="s">
         <v>483</v>
       </c>
@@ -8854,7 +9893,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="20" t="s">
         <v>485</v>
       </c>
@@ -8862,7 +9901,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="20" t="s">
         <v>408</v>
       </c>
@@ -8870,7 +9909,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="20" t="s">
         <v>287</v>
       </c>
@@ -8878,7 +9917,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="20" t="s">
         <v>489</v>
       </c>
@@ -8886,7 +9925,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="20" t="s">
         <v>491</v>
       </c>
@@ -8894,7 +9933,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="20" t="s">
         <v>493</v>
       </c>
@@ -8902,7 +9941,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="20" t="s">
         <v>495</v>
       </c>
@@ -8910,7 +9949,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="20" t="s">
         <v>412</v>
       </c>
@@ -8918,7 +9957,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="20" t="s">
         <v>498</v>
       </c>
@@ -8926,7 +9965,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="20" t="s">
         <v>500</v>
       </c>
@@ -8934,7 +9973,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="20" t="s">
         <v>502</v>
       </c>
@@ -8942,7 +9981,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="20" t="s">
         <v>504</v>
       </c>
@@ -8950,7 +9989,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="20" t="s">
         <v>506</v>
       </c>
@@ -8958,7 +9997,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="20" t="s">
         <v>508</v>
       </c>
@@ -8966,7 +10005,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="20" t="s">
         <v>510</v>
       </c>
@@ -8974,7 +10013,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="20" t="s">
         <v>512</v>
       </c>
@@ -8982,7 +10021,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="21" t="s">
         <v>514</v>
       </c>
@@ -8990,15 +10029,15 @@
         <v>515</v>
       </c>
     </row>
-    <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="23" t="s">
         <v>516</v>
       </c>
       <c r="C99" s="24"/>
     </row>
-    <row r="100" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="19" t="s">
         <v>29</v>
       </c>
@@ -9006,7 +10045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="19" t="s">
         <v>220</v>
       </c>
@@ -9014,7 +10053,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="20" t="s">
         <v>517</v>
       </c>
@@ -9022,7 +10061,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="20" t="s">
         <v>519</v>
       </c>
@@ -9030,7 +10069,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="20" t="s">
         <v>521</v>
       </c>
@@ -9038,7 +10077,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="20" t="s">
         <v>523</v>
       </c>
@@ -9046,7 +10085,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="20" t="s">
         <v>525</v>
       </c>
@@ -9054,7 +10093,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="20" t="s">
         <v>527</v>
       </c>
@@ -9062,7 +10101,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="20" t="s">
         <v>529</v>
       </c>
@@ -9070,7 +10109,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="20" t="s">
         <v>531</v>
       </c>
@@ -9078,7 +10117,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="20" t="s">
         <v>533</v>
       </c>
@@ -9086,7 +10125,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="20" t="s">
         <v>535</v>
       </c>
@@ -9094,7 +10133,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="20" t="s">
         <v>537</v>
       </c>
@@ -9102,7 +10141,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="20" t="s">
         <v>539</v>
       </c>
@@ -9110,7 +10149,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="20" t="s">
         <v>541</v>
       </c>
@@ -9118,7 +10157,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="20" t="s">
         <v>543</v>
       </c>
@@ -9126,7 +10165,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="20" t="s">
         <v>545</v>
       </c>
@@ -9134,7 +10173,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="20" t="s">
         <v>547</v>
       </c>
@@ -9142,7 +10181,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="20" t="s">
         <v>549</v>
       </c>
@@ -9150,7 +10189,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="20" t="s">
         <v>551</v>
       </c>
@@ -9158,7 +10197,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="20" t="s">
         <v>553</v>
       </c>
@@ -9166,7 +10205,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="20" t="s">
         <v>555</v>
       </c>
@@ -9174,7 +10213,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="20" t="s">
         <v>557</v>
       </c>
@@ -9182,7 +10221,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="20" t="s">
         <v>559</v>
       </c>
@@ -9190,7 +10229,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="20" t="s">
         <v>561</v>
       </c>
@@ -9198,7 +10237,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="20" t="s">
         <v>563</v>
       </c>
@@ -9206,7 +10245,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="20" t="s">
         <v>565</v>
       </c>
@@ -9214,7 +10253,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="20" t="s">
         <v>567</v>
       </c>
@@ -9222,7 +10261,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="20" t="s">
         <v>569</v>
       </c>
@@ -9230,7 +10269,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="20" t="s">
         <v>571</v>
       </c>
@@ -9238,7 +10277,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="20" t="s">
         <v>573</v>
       </c>
@@ -9246,7 +10285,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="20" t="s">
         <v>575</v>
       </c>
@@ -9254,7 +10293,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="20" t="s">
         <v>577</v>
       </c>
@@ -9262,7 +10301,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="20" t="s">
         <v>579</v>
       </c>
@@ -9270,7 +10309,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="20" t="s">
         <v>581</v>
       </c>
@@ -9278,7 +10317,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="20" t="s">
         <v>583</v>
       </c>
@@ -9286,7 +10325,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="20" t="s">
         <v>585</v>
       </c>
@@ -9294,7 +10333,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="20" t="s">
         <v>587</v>
       </c>
@@ -9302,7 +10341,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="20" t="s">
         <v>589</v>
       </c>
@@ -9310,7 +10349,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="20" t="s">
         <v>591</v>
       </c>
@@ -9318,7 +10357,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="140" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="21" t="s">
         <v>593</v>
       </c>
@@ -9326,14 +10365,14 @@
         <v>594</v>
       </c>
     </row>
-    <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B143" s="63" t="s">
+    <row r="141" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" s="64" t="s">
         <v>595</v>
       </c>
-      <c r="C143" s="64"/>
-    </row>
-    <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C143" s="65"/>
+    </row>
+    <row r="144" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="7" t="s">
         <v>29</v>
       </c>
@@ -9341,7 +10380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="7" t="s">
         <v>220</v>
       </c>
@@ -9349,7 +10388,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="9" t="s">
         <v>596</v>
       </c>
@@ -9357,7 +10396,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="9" t="s">
         <v>598</v>
       </c>
@@ -9365,7 +10404,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="9" t="s">
         <v>600</v>
       </c>
@@ -9373,7 +10412,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="9" t="s">
         <v>602</v>
       </c>
@@ -9381,7 +10420,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="150" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="9" t="s">
         <v>604</v>
       </c>
@@ -9389,7 +10428,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="151" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="9" t="s">
         <v>606</v>
       </c>
@@ -9397,7 +10436,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="152" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="152" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="9" t="s">
         <v>608</v>
       </c>
@@ -9405,7 +10444,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="153" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="9" t="s">
         <v>610</v>
       </c>
@@ -9413,7 +10452,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="154" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="9" t="s">
         <v>612</v>
       </c>
@@ -9421,7 +10460,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="155" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="9" t="s">
         <v>614</v>
       </c>
@@ -9429,7 +10468,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="156" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="156" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="9" t="s">
         <v>616</v>
       </c>
@@ -9437,7 +10476,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="157" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="9" t="s">
         <v>618</v>
       </c>
@@ -9445,7 +10484,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="158" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="158" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="9" t="s">
         <v>620</v>
       </c>
@@ -9453,7 +10492,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="159" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="9" t="s">
         <v>622</v>
       </c>
@@ -9461,7 +10500,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="160" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="160" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="9" t="s">
         <v>624</v>
       </c>
@@ -9469,7 +10508,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="161" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="9" t="s">
         <v>626</v>
       </c>
@@ -9477,7 +10516,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="162" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="162" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="9" t="s">
         <v>628</v>
       </c>
@@ -9485,7 +10524,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="163" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="163" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="9" t="s">
         <v>630</v>
       </c>
@@ -9493,7 +10532,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="164" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="164" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="9" t="s">
         <v>632</v>
       </c>
@@ -9501,7 +10540,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="165" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="165" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="9" t="s">
         <v>634</v>
       </c>
@@ -9509,7 +10548,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="166" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="9" t="s">
         <v>636</v>
       </c>
@@ -9517,7 +10556,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="167" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="167" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="9" t="s">
         <v>638</v>
       </c>
@@ -9525,7 +10564,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="168" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="9" t="s">
         <v>640</v>
       </c>
@@ -9533,7 +10572,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="169" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="9" t="s">
         <v>642</v>
       </c>
@@ -9541,7 +10580,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="170" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="9" t="s">
         <v>644</v>
       </c>
@@ -9549,7 +10588,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="171" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="171" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="9" t="s">
         <v>646</v>
       </c>
@@ -9557,7 +10596,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="172" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="172" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="9" t="s">
         <v>648</v>
       </c>
@@ -9565,7 +10604,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="173" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="9" t="s">
         <v>650</v>
       </c>
@@ -9573,7 +10612,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="174" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="9" t="s">
         <v>652</v>
       </c>
@@ -9581,7 +10620,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="9" t="s">
         <v>654</v>
       </c>
@@ -9589,7 +10628,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="9" t="s">
         <v>656</v>
       </c>
@@ -9597,7 +10636,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="177" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="9" t="s">
         <v>658</v>
       </c>
@@ -9605,7 +10644,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="178" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="178" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="9" t="s">
         <v>660</v>
       </c>
@@ -9613,7 +10652,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="179" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="179" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="9" t="s">
         <v>662</v>
       </c>
@@ -9621,7 +10660,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="180" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="180" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="9" t="s">
         <v>664</v>
       </c>
@@ -9629,7 +10668,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="181" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="181" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="9" t="s">
         <v>666</v>
       </c>
@@ -9637,7 +10676,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="182" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="182" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="9" t="s">
         <v>668</v>
       </c>
@@ -9645,7 +10684,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="183" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="183" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="9" t="s">
         <v>670</v>
       </c>
@@ -9653,7 +10692,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="184" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="9" t="s">
         <v>672</v>
       </c>
@@ -9661,7 +10700,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="185" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="9" t="s">
         <v>674</v>
       </c>
@@ -9669,7 +10708,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="186" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="9" t="s">
         <v>676</v>
       </c>
@@ -9677,7 +10716,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="187" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
         <v>678</v>
       </c>
@@ -9685,7 +10724,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="188" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="188" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="9" t="s">
         <v>680</v>
       </c>
@@ -9693,7 +10732,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="189" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="9" t="s">
         <v>682</v>
       </c>
@@ -9701,7 +10740,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="190" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="9" t="s">
         <v>684</v>
       </c>
@@ -9709,7 +10748,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="191" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="9" t="s">
         <v>686</v>
       </c>
@@ -9717,7 +10756,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="192" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="9" t="s">
         <v>688</v>
       </c>
@@ -9725,7 +10764,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="193" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="9" t="s">
         <v>690</v>
       </c>
@@ -9733,7 +10772,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="194" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="194" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="9" t="s">
         <v>692</v>
       </c>
@@ -9741,7 +10780,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="195" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="9" t="s">
         <v>694</v>
       </c>
@@ -9749,7 +10788,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="196" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="196" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="9" t="s">
         <v>696</v>
       </c>
@@ -9757,7 +10796,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="197" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="197" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="9" t="s">
         <v>698</v>
       </c>
@@ -9765,7 +10804,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="198" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="198" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="9" t="s">
         <v>700</v>
       </c>
@@ -9773,7 +10812,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="199" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="199" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="9" t="s">
         <v>702</v>
       </c>
@@ -9781,7 +10820,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="200" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="200" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="9" t="s">
         <v>704</v>
       </c>
@@ -9789,7 +10828,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="201" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="201" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="9" t="s">
         <v>706</v>
       </c>
@@ -9797,7 +10836,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="202" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="202" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="9" t="s">
         <v>708</v>
       </c>
@@ -9805,7 +10844,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="203" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="203" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="9" t="s">
         <v>710</v>
       </c>
@@ -9813,7 +10852,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="204" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="204" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="9" t="s">
         <v>712</v>
       </c>
@@ -9821,7 +10860,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="205" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="205" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="9" t="s">
         <v>714</v>
       </c>
@@ -9829,7 +10868,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="206" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="206" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="9" t="s">
         <v>716</v>
       </c>
@@ -9837,7 +10876,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="207" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="207" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="9" t="s">
         <v>718</v>
       </c>
@@ -9845,7 +10884,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="208" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="208" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="9" t="s">
         <v>720</v>
       </c>
@@ -9853,7 +10892,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="209" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="209" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="9" t="s">
         <v>722</v>
       </c>
@@ -9861,7 +10900,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="210" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="210" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="9" t="s">
         <v>724</v>
       </c>
@@ -9869,7 +10908,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="211" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="9" t="s">
         <v>726</v>
       </c>
@@ -9877,7 +10916,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="212" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="212" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="9" t="s">
         <v>728</v>
       </c>
@@ -9885,7 +10924,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="213" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="213" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="9" t="s">
         <v>730</v>
       </c>
@@ -9893,7 +10932,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="214" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="214" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="9" t="s">
         <v>732</v>
       </c>
@@ -9901,7 +10940,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="215" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="215" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="9" t="s">
         <v>734</v>
       </c>
@@ -9909,7 +10948,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="216" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="216" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B143:C143"/>

</xml_diff>

<commit_message>
EPBDS-8844 Rename "detailedPlainModel" to "tableStructureDetails"
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\DEV\org.openl.rules\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2916C47F-BFCA-4D7A-995E-926684D6BD3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D714BA69-4AAE-498E-A968-CFBAF5D65551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6110" yWindow="2130" windowWidth="24340" windowHeight="15820" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -805,15 +796,6 @@
     <t>If true calculates all cells in the Spreadsheet, otherwise calculates only cells these are requred for a result. By default = true.</t>
   </si>
   <si>
-    <t xml:space="preserve">Controls generation additional fields in an plain model for the Spreadsheet. </t>
-  </si>
-  <si>
-    <t>Detaled Plain Model</t>
-  </si>
-  <si>
-    <t>detailedPlainModel</t>
-  </si>
-  <si>
     <t>MM/dd/yyyy hh:mm a</t>
   </si>
   <si>
@@ -908,6 +890,15 @@
   </si>
   <si>
     <t>CaProvincesEnum</t>
+  </si>
+  <si>
+    <t>Table Structure Details</t>
+  </si>
+  <si>
+    <t>tableStructureDetails</t>
+  </si>
+  <si>
+    <t>Controls generation additional properties with table structure details in an output model</t>
   </si>
 </sst>
 </file>
@@ -1414,6 +1405,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1421,9 +1415,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1446,39 +1437,39 @@
     </xf>
   </cellXfs>
   <cellStyles count="33">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1562,9 +1553,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1602,7 +1593,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1708,7 +1699,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1888,12 +1879,12 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1908,7 +1899,7 @@
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
     </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1923,7 +1914,7 @@
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
     </row>
-    <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1938,7 +1929,7 @@
       <c r="I4" s="30"/>
       <c r="J4" s="30"/>
     </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1953,7 +1944,7 @@
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
     </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1968,7 +1959,7 @@
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
     </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1983,7 +1974,7 @@
       <c r="I7" s="30"/>
       <c r="J7" s="30"/>
     </row>
-    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1998,7 +1989,7 @@
       <c r="I8" s="30"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
@@ -2013,7 +2004,7 @@
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
     </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
@@ -2028,7 +2019,7 @@
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
     </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
@@ -2043,7 +2034,7 @@
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
@@ -2058,7 +2049,7 @@
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
     </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
@@ -2073,7 +2064,7 @@
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
     </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
@@ -2088,7 +2079,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="29" t="s">
         <v>26</v>
       </c>
@@ -2132,36 +2123,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="49.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="73.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="1025" width="8.85546875" style="1"/>
+    <col min="16" max="16" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="73.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2178,7 +2169,7 @@
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
     </row>
-    <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -2195,7 +2186,7 @@
       <c r="K2" s="27"/>
       <c r="L2" s="27"/>
     </row>
-    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2212,7 +2203,7 @@
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
     </row>
-    <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -2229,7 +2220,7 @@
       <c r="K4" s="27"/>
       <c r="L4" s="27"/>
     </row>
-    <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2246,7 +2237,7 @@
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
     </row>
-    <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -2263,7 +2254,7 @@
       <c r="K6" s="30"/>
       <c r="L6" s="30"/>
     </row>
-    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
@@ -2280,7 +2271,7 @@
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
     </row>
-    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
@@ -2297,7 +2288,7 @@
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
     </row>
-    <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
@@ -2314,7 +2305,7 @@
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
     </row>
-    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2323,30 +2314,30 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
+    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-    </row>
-    <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+    </row>
+    <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
@@ -2405,7 +2396,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
@@ -2464,7 +2455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
@@ -2511,7 +2502,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>66</v>
       </c>
@@ -2554,7 +2545,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>100</v>
       </c>
@@ -2601,7 +2592,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>105</v>
       </c>
@@ -2640,7 +2631,7 @@
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R17" s="5"/>
       <c r="S17" s="5" t="s">
@@ -2650,7 +2641,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>109</v>
       </c>
@@ -2697,7 +2688,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
         <v>113</v>
       </c>
@@ -2736,7 +2727,7 @@
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R19" s="5"/>
       <c r="S19" s="5" t="s">
@@ -2746,7 +2737,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
@@ -2789,7 +2780,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>72</v>
       </c>
@@ -2832,7 +2823,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
         <v>76</v>
       </c>
@@ -2871,7 +2862,7 @@
       </c>
       <c r="P22" s="5"/>
       <c r="Q22" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R22" s="5"/>
       <c r="S22" s="5" t="s">
@@ -2881,7 +2872,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -2920,7 +2911,7 @@
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R23" s="5"/>
       <c r="S23" s="5" t="s">
@@ -2930,7 +2921,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>90</v>
       </c>
@@ -2969,7 +2960,7 @@
       </c>
       <c r="P24" s="5"/>
       <c r="Q24" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R24" s="5"/>
       <c r="S24" s="5" t="s">
@@ -2979,7 +2970,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>95</v>
       </c>
@@ -3018,7 +3009,7 @@
       </c>
       <c r="P25" s="5"/>
       <c r="Q25" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R25" s="5"/>
       <c r="S25" s="5" t="s">
@@ -3028,7 +3019,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
         <v>229</v>
       </c>
@@ -3039,7 +3030,7 @@
         <v>58</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>226</v>
@@ -3073,7 +3064,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
         <v>222</v>
       </c>
@@ -3084,7 +3075,7 @@
         <v>58</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>228</v>
@@ -3118,7 +3109,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="5" t="s">
         <v>138</v>
       </c>
@@ -3129,7 +3120,7 @@
         <v>58</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>140</v>
@@ -3163,7 +3154,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="5" t="s">
         <v>154</v>
       </c>
@@ -3174,7 +3165,7 @@
         <v>58</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>156</v>
@@ -3208,7 +3199,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="5" t="s">
         <v>142</v>
       </c>
@@ -3219,7 +3210,7 @@
         <v>58</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>144</v>
@@ -3253,7 +3244,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
         <v>146</v>
       </c>
@@ -3264,7 +3255,7 @@
         <v>58</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>148</v>
@@ -3298,7 +3289,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="5" t="s">
         <v>130</v>
       </c>
@@ -3345,7 +3336,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
         <v>216</v>
       </c>
@@ -3356,7 +3347,7 @@
         <v>58</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5" t="s">
@@ -3388,7 +3379,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="5" t="s">
         <v>134</v>
       </c>
@@ -3399,7 +3390,7 @@
         <v>58</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>136</v>
@@ -3433,7 +3424,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
         <v>150</v>
       </c>
@@ -3444,7 +3435,7 @@
         <v>58</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>152</v>
@@ -3478,7 +3469,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="5" t="s">
         <v>158</v>
       </c>
@@ -3519,7 +3510,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="5" t="s">
         <v>162</v>
       </c>
@@ -3563,7 +3554,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="5" t="s">
         <v>116</v>
       </c>
@@ -3610,7 +3601,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="5" t="s">
         <v>123</v>
       </c>
@@ -3653,7 +3644,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="5" t="s">
         <v>127</v>
       </c>
@@ -3664,7 +3655,7 @@
         <v>58</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5" t="s">
@@ -3696,7 +3687,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="5" t="s">
         <v>167</v>
       </c>
@@ -3738,7 +3729,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="5" t="s">
         <v>170</v>
       </c>
@@ -3773,23 +3764,23 @@
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T42" s="5" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="25"/>
       <c r="B43" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5" t="s">
@@ -3817,13 +3808,13 @@
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="T43" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1025" ht="60" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1025" ht="29" x14ac:dyDescent="0.35">
       <c r="B44" s="5" t="s">
         <v>175</v>
       </c>
@@ -3860,20 +3851,20 @@
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="T44" s="5" t="s">
         <v>180</v>
       </c>
       <c r="U44" s="24"/>
     </row>
-    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="24"/>
       <c r="B45" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>251</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
@@ -3896,7 +3887,7 @@
         <v>172</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O45" s="5" t="s">
         <v>179</v>
@@ -3905,13 +3896,13 @@
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
       <c r="S45" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="5" t="s">
         <v>181</v>
       </c>
@@ -3952,7 +3943,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="5" t="s">
         <v>183</v>
       </c>
@@ -3963,7 +3954,7 @@
         <v>58</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
@@ -4997,7 +4988,7 @@
       <c r="AMJ47" s="23"/>
       <c r="AMK47" s="23"/>
     </row>
-    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="5" t="s">
         <v>210</v>
       </c>
@@ -5039,13 +5030,13 @@
       </c>
       <c r="U48" s="23"/>
     </row>
-    <row r="49" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="23"/>
       <c r="B49" s="5" t="s">
-        <v>248</v>
+        <v>279</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>58</v>
@@ -5083,10 +5074,10 @@
         <v>83</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="5" t="s">
         <v>214</v>
       </c>
@@ -5132,7 +5123,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
         <v>245</v>
       </c>
@@ -5178,7 +5169,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="B52" s="5" t="s">
         <v>242</v>
       </c>
@@ -5224,7 +5215,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="B53" s="5" t="s">
         <v>235</v>
       </c>
@@ -5271,8 +5262,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B57" s="5" t="s">
         <v>186</v>
       </c>
@@ -5311,44 +5302,44 @@
         <v>189</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="33" t="s">
+    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="C61" s="33"/>
-    </row>
-    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="34" t="s">
+      <c r="C61" s="34"/>
+    </row>
+    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="C62" s="34"/>
-    </row>
-    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="34" t="s">
+      <c r="C62" s="31"/>
+    </row>
+    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="34"/>
-    </row>
-    <row r="64" spans="1:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="31" t="s">
+      <c r="C63" s="31"/>
+    </row>
+    <row r="64" spans="1:20" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="C64" s="31"/>
-    </row>
-    <row r="65" spans="1:1025" x14ac:dyDescent="0.25">
-      <c r="B65" s="31" t="s">
+      <c r="C64" s="32"/>
+    </row>
+    <row r="65" spans="1:1025" x14ac:dyDescent="0.35">
+      <c r="B65" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="C65" s="31"/>
-    </row>
-    <row r="66" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="C65" s="32"/>
+    </row>
+    <row r="66" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A66" s="26"/>
-      <c r="B66" s="31" t="s">
-        <v>262</v>
-      </c>
-      <c r="C66" s="31"/>
+      <c r="B66" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="C66" s="32"/>
       <c r="D66" s="26"/>
       <c r="E66" s="26"/>
       <c r="F66" s="26"/>
@@ -6372,31 +6363,31 @@
       <c r="AMJ66" s="26"/>
       <c r="AMK66" s="26"/>
     </row>
-    <row r="67" spans="1:1025" x14ac:dyDescent="0.25">
-      <c r="B67" s="32" t="s">
+    <row r="67" spans="1:1025" x14ac:dyDescent="0.35">
+      <c r="B67" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="C67" s="32"/>
+      <c r="C67" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="C6:L6"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="B11:T11"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="C5:L5"/>
-    <mergeCell ref="C6:L6"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="B11:T11"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -6416,9 +6407,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="35" t="s">
         <v>195</v>
       </c>
@@ -6427,7 +6418,7 @@
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
     </row>
-    <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="36" t="s">
         <v>196</v>
       </c>
@@ -6438,7 +6429,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="36"/>
       <c r="C7" s="8" t="s">
         <v>198</v>
@@ -6447,7 +6438,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="36"/>
       <c r="C8" s="8" t="s">
         <v>199</v>
@@ -6456,7 +6447,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="36"/>
       <c r="C9" s="8" t="s">
         <v>200</v>
@@ -6465,7 +6456,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="36"/>
       <c r="C10" s="37" t="s">
         <v>201</v>
@@ -6498,22 +6489,22 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="38" t="s">
         <v>202</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
@@ -6524,7 +6515,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
@@ -6535,7 +6526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="15" t="s">
         <v>107</v>
       </c>
@@ -6546,7 +6537,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="18" t="s">
         <v>203</v>
       </c>
@@ -6557,7 +6548,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="18" t="s">
         <v>131</v>
       </c>
@@ -6568,7 +6559,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="18" t="s">
         <v>236</v>
       </c>
@@ -6579,89 +6570,89 @@
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="18" t="s">
         <v>204</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="18" t="s">
         <v>139</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="18" t="s">
         <v>207</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="18" t="s">
         <v>143</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="18" t="s">
         <v>147</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="18" t="s">
         <v>155</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="18" t="s">
         <v>221</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="20" t="s">
         <v>223</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>224</v>

</xml_diff>

<commit_message>
EPBDS-7066 Add new dev property to control a possibility of returning empty result
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D714BA69-4AAE-498E-A968-CFBAF5D65551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F001C1F-B47F-41A1-B5B2-4936384EDFD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6110" yWindow="2130" windowWidth="24340" windowHeight="15820" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="287">
   <si>
     <t>Display Name</t>
   </si>
@@ -899,6 +899,21 @@
   </si>
   <si>
     <t>Controls generation additional properties with table structure details in an output model</t>
+  </si>
+  <si>
+    <t>Calculation Mode</t>
+  </si>
+  <si>
+    <t>The way of calculation of the DT table</t>
+  </si>
+  <si>
+    <t>DTCalculationModeEnum</t>
+  </si>
+  <si>
+    <t>calculationMode</t>
+  </si>
+  <si>
+    <t>AVOID_EMPTY_RESULT</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1330,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1379,6 +1394,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1888,207 +1906,207 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
@@ -2121,10 +2139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK67"/>
+  <dimension ref="A1:AMK68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2156,154 +2174,154 @@
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
@@ -2315,27 +2333,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
@@ -4989,15 +5007,18 @@
       <c r="AMK47" s="23"/>
     </row>
     <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="27"/>
       <c r="B48" s="5" t="s">
-        <v>210</v>
+        <v>282</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D48" s="5"/>
+        <v>285</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E48" s="5" t="s">
-        <v>59</v>
+        <v>284</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5" t="s">
@@ -5013,12 +5034,12 @@
       </c>
       <c r="L48" s="5"/>
       <c r="M48" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5" t="s">
-        <v>212</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="N48" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="O48" s="5"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
       <c r="R48" s="5"/>
@@ -5026,23 +5047,1024 @@
         <v>83</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="U48" s="23"/>
-    </row>
-    <row r="49" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="23"/>
+        <v>283</v>
+      </c>
+      <c r="U48" s="27"/>
+      <c r="V48" s="27"/>
+      <c r="W48" s="27"/>
+      <c r="X48" s="27"/>
+      <c r="Y48" s="27"/>
+      <c r="Z48" s="27"/>
+      <c r="AA48" s="27"/>
+      <c r="AB48" s="27"/>
+      <c r="AC48" s="27"/>
+      <c r="AD48" s="27"/>
+      <c r="AE48" s="27"/>
+      <c r="AF48" s="27"/>
+      <c r="AG48" s="27"/>
+      <c r="AH48" s="27"/>
+      <c r="AI48" s="27"/>
+      <c r="AJ48" s="27"/>
+      <c r="AK48" s="27"/>
+      <c r="AL48" s="27"/>
+      <c r="AM48" s="27"/>
+      <c r="AN48" s="27"/>
+      <c r="AO48" s="27"/>
+      <c r="AP48" s="27"/>
+      <c r="AQ48" s="27"/>
+      <c r="AR48" s="27"/>
+      <c r="AS48" s="27"/>
+      <c r="AT48" s="27"/>
+      <c r="AU48" s="27"/>
+      <c r="AV48" s="27"/>
+      <c r="AW48" s="27"/>
+      <c r="AX48" s="27"/>
+      <c r="AY48" s="27"/>
+      <c r="AZ48" s="27"/>
+      <c r="BA48" s="27"/>
+      <c r="BB48" s="27"/>
+      <c r="BC48" s="27"/>
+      <c r="BD48" s="27"/>
+      <c r="BE48" s="27"/>
+      <c r="BF48" s="27"/>
+      <c r="BG48" s="27"/>
+      <c r="BH48" s="27"/>
+      <c r="BI48" s="27"/>
+      <c r="BJ48" s="27"/>
+      <c r="BK48" s="27"/>
+      <c r="BL48" s="27"/>
+      <c r="BM48" s="27"/>
+      <c r="BN48" s="27"/>
+      <c r="BO48" s="27"/>
+      <c r="BP48" s="27"/>
+      <c r="BQ48" s="27"/>
+      <c r="BR48" s="27"/>
+      <c r="BS48" s="27"/>
+      <c r="BT48" s="27"/>
+      <c r="BU48" s="27"/>
+      <c r="BV48" s="27"/>
+      <c r="BW48" s="27"/>
+      <c r="BX48" s="27"/>
+      <c r="BY48" s="27"/>
+      <c r="BZ48" s="27"/>
+      <c r="CA48" s="27"/>
+      <c r="CB48" s="27"/>
+      <c r="CC48" s="27"/>
+      <c r="CD48" s="27"/>
+      <c r="CE48" s="27"/>
+      <c r="CF48" s="27"/>
+      <c r="CG48" s="27"/>
+      <c r="CH48" s="27"/>
+      <c r="CI48" s="27"/>
+      <c r="CJ48" s="27"/>
+      <c r="CK48" s="27"/>
+      <c r="CL48" s="27"/>
+      <c r="CM48" s="27"/>
+      <c r="CN48" s="27"/>
+      <c r="CO48" s="27"/>
+      <c r="CP48" s="27"/>
+      <c r="CQ48" s="27"/>
+      <c r="CR48" s="27"/>
+      <c r="CS48" s="27"/>
+      <c r="CT48" s="27"/>
+      <c r="CU48" s="27"/>
+      <c r="CV48" s="27"/>
+      <c r="CW48" s="27"/>
+      <c r="CX48" s="27"/>
+      <c r="CY48" s="27"/>
+      <c r="CZ48" s="27"/>
+      <c r="DA48" s="27"/>
+      <c r="DB48" s="27"/>
+      <c r="DC48" s="27"/>
+      <c r="DD48" s="27"/>
+      <c r="DE48" s="27"/>
+      <c r="DF48" s="27"/>
+      <c r="DG48" s="27"/>
+      <c r="DH48" s="27"/>
+      <c r="DI48" s="27"/>
+      <c r="DJ48" s="27"/>
+      <c r="DK48" s="27"/>
+      <c r="DL48" s="27"/>
+      <c r="DM48" s="27"/>
+      <c r="DN48" s="27"/>
+      <c r="DO48" s="27"/>
+      <c r="DP48" s="27"/>
+      <c r="DQ48" s="27"/>
+      <c r="DR48" s="27"/>
+      <c r="DS48" s="27"/>
+      <c r="DT48" s="27"/>
+      <c r="DU48" s="27"/>
+      <c r="DV48" s="27"/>
+      <c r="DW48" s="27"/>
+      <c r="DX48" s="27"/>
+      <c r="DY48" s="27"/>
+      <c r="DZ48" s="27"/>
+      <c r="EA48" s="27"/>
+      <c r="EB48" s="27"/>
+      <c r="EC48" s="27"/>
+      <c r="ED48" s="27"/>
+      <c r="EE48" s="27"/>
+      <c r="EF48" s="27"/>
+      <c r="EG48" s="27"/>
+      <c r="EH48" s="27"/>
+      <c r="EI48" s="27"/>
+      <c r="EJ48" s="27"/>
+      <c r="EK48" s="27"/>
+      <c r="EL48" s="27"/>
+      <c r="EM48" s="27"/>
+      <c r="EN48" s="27"/>
+      <c r="EO48" s="27"/>
+      <c r="EP48" s="27"/>
+      <c r="EQ48" s="27"/>
+      <c r="ER48" s="27"/>
+      <c r="ES48" s="27"/>
+      <c r="ET48" s="27"/>
+      <c r="EU48" s="27"/>
+      <c r="EV48" s="27"/>
+      <c r="EW48" s="27"/>
+      <c r="EX48" s="27"/>
+      <c r="EY48" s="27"/>
+      <c r="EZ48" s="27"/>
+      <c r="FA48" s="27"/>
+      <c r="FB48" s="27"/>
+      <c r="FC48" s="27"/>
+      <c r="FD48" s="27"/>
+      <c r="FE48" s="27"/>
+      <c r="FF48" s="27"/>
+      <c r="FG48" s="27"/>
+      <c r="FH48" s="27"/>
+      <c r="FI48" s="27"/>
+      <c r="FJ48" s="27"/>
+      <c r="FK48" s="27"/>
+      <c r="FL48" s="27"/>
+      <c r="FM48" s="27"/>
+      <c r="FN48" s="27"/>
+      <c r="FO48" s="27"/>
+      <c r="FP48" s="27"/>
+      <c r="FQ48" s="27"/>
+      <c r="FR48" s="27"/>
+      <c r="FS48" s="27"/>
+      <c r="FT48" s="27"/>
+      <c r="FU48" s="27"/>
+      <c r="FV48" s="27"/>
+      <c r="FW48" s="27"/>
+      <c r="FX48" s="27"/>
+      <c r="FY48" s="27"/>
+      <c r="FZ48" s="27"/>
+      <c r="GA48" s="27"/>
+      <c r="GB48" s="27"/>
+      <c r="GC48" s="27"/>
+      <c r="GD48" s="27"/>
+      <c r="GE48" s="27"/>
+      <c r="GF48" s="27"/>
+      <c r="GG48" s="27"/>
+      <c r="GH48" s="27"/>
+      <c r="GI48" s="27"/>
+      <c r="GJ48" s="27"/>
+      <c r="GK48" s="27"/>
+      <c r="GL48" s="27"/>
+      <c r="GM48" s="27"/>
+      <c r="GN48" s="27"/>
+      <c r="GO48" s="27"/>
+      <c r="GP48" s="27"/>
+      <c r="GQ48" s="27"/>
+      <c r="GR48" s="27"/>
+      <c r="GS48" s="27"/>
+      <c r="GT48" s="27"/>
+      <c r="GU48" s="27"/>
+      <c r="GV48" s="27"/>
+      <c r="GW48" s="27"/>
+      <c r="GX48" s="27"/>
+      <c r="GY48" s="27"/>
+      <c r="GZ48" s="27"/>
+      <c r="HA48" s="27"/>
+      <c r="HB48" s="27"/>
+      <c r="HC48" s="27"/>
+      <c r="HD48" s="27"/>
+      <c r="HE48" s="27"/>
+      <c r="HF48" s="27"/>
+      <c r="HG48" s="27"/>
+      <c r="HH48" s="27"/>
+      <c r="HI48" s="27"/>
+      <c r="HJ48" s="27"/>
+      <c r="HK48" s="27"/>
+      <c r="HL48" s="27"/>
+      <c r="HM48" s="27"/>
+      <c r="HN48" s="27"/>
+      <c r="HO48" s="27"/>
+      <c r="HP48" s="27"/>
+      <c r="HQ48" s="27"/>
+      <c r="HR48" s="27"/>
+      <c r="HS48" s="27"/>
+      <c r="HT48" s="27"/>
+      <c r="HU48" s="27"/>
+      <c r="HV48" s="27"/>
+      <c r="HW48" s="27"/>
+      <c r="HX48" s="27"/>
+      <c r="HY48" s="27"/>
+      <c r="HZ48" s="27"/>
+      <c r="IA48" s="27"/>
+      <c r="IB48" s="27"/>
+      <c r="IC48" s="27"/>
+      <c r="ID48" s="27"/>
+      <c r="IE48" s="27"/>
+      <c r="IF48" s="27"/>
+      <c r="IG48" s="27"/>
+      <c r="IH48" s="27"/>
+      <c r="II48" s="27"/>
+      <c r="IJ48" s="27"/>
+      <c r="IK48" s="27"/>
+      <c r="IL48" s="27"/>
+      <c r="IM48" s="27"/>
+      <c r="IN48" s="27"/>
+      <c r="IO48" s="27"/>
+      <c r="IP48" s="27"/>
+      <c r="IQ48" s="27"/>
+      <c r="IR48" s="27"/>
+      <c r="IS48" s="27"/>
+      <c r="IT48" s="27"/>
+      <c r="IU48" s="27"/>
+      <c r="IV48" s="27"/>
+      <c r="IW48" s="27"/>
+      <c r="IX48" s="27"/>
+      <c r="IY48" s="27"/>
+      <c r="IZ48" s="27"/>
+      <c r="JA48" s="27"/>
+      <c r="JB48" s="27"/>
+      <c r="JC48" s="27"/>
+      <c r="JD48" s="27"/>
+      <c r="JE48" s="27"/>
+      <c r="JF48" s="27"/>
+      <c r="JG48" s="27"/>
+      <c r="JH48" s="27"/>
+      <c r="JI48" s="27"/>
+      <c r="JJ48" s="27"/>
+      <c r="JK48" s="27"/>
+      <c r="JL48" s="27"/>
+      <c r="JM48" s="27"/>
+      <c r="JN48" s="27"/>
+      <c r="JO48" s="27"/>
+      <c r="JP48" s="27"/>
+      <c r="JQ48" s="27"/>
+      <c r="JR48" s="27"/>
+      <c r="JS48" s="27"/>
+      <c r="JT48" s="27"/>
+      <c r="JU48" s="27"/>
+      <c r="JV48" s="27"/>
+      <c r="JW48" s="27"/>
+      <c r="JX48" s="27"/>
+      <c r="JY48" s="27"/>
+      <c r="JZ48" s="27"/>
+      <c r="KA48" s="27"/>
+      <c r="KB48" s="27"/>
+      <c r="KC48" s="27"/>
+      <c r="KD48" s="27"/>
+      <c r="KE48" s="27"/>
+      <c r="KF48" s="27"/>
+      <c r="KG48" s="27"/>
+      <c r="KH48" s="27"/>
+      <c r="KI48" s="27"/>
+      <c r="KJ48" s="27"/>
+      <c r="KK48" s="27"/>
+      <c r="KL48" s="27"/>
+      <c r="KM48" s="27"/>
+      <c r="KN48" s="27"/>
+      <c r="KO48" s="27"/>
+      <c r="KP48" s="27"/>
+      <c r="KQ48" s="27"/>
+      <c r="KR48" s="27"/>
+      <c r="KS48" s="27"/>
+      <c r="KT48" s="27"/>
+      <c r="KU48" s="27"/>
+      <c r="KV48" s="27"/>
+      <c r="KW48" s="27"/>
+      <c r="KX48" s="27"/>
+      <c r="KY48" s="27"/>
+      <c r="KZ48" s="27"/>
+      <c r="LA48" s="27"/>
+      <c r="LB48" s="27"/>
+      <c r="LC48" s="27"/>
+      <c r="LD48" s="27"/>
+      <c r="LE48" s="27"/>
+      <c r="LF48" s="27"/>
+      <c r="LG48" s="27"/>
+      <c r="LH48" s="27"/>
+      <c r="LI48" s="27"/>
+      <c r="LJ48" s="27"/>
+      <c r="LK48" s="27"/>
+      <c r="LL48" s="27"/>
+      <c r="LM48" s="27"/>
+      <c r="LN48" s="27"/>
+      <c r="LO48" s="27"/>
+      <c r="LP48" s="27"/>
+      <c r="LQ48" s="27"/>
+      <c r="LR48" s="27"/>
+      <c r="LS48" s="27"/>
+      <c r="LT48" s="27"/>
+      <c r="LU48" s="27"/>
+      <c r="LV48" s="27"/>
+      <c r="LW48" s="27"/>
+      <c r="LX48" s="27"/>
+      <c r="LY48" s="27"/>
+      <c r="LZ48" s="27"/>
+      <c r="MA48" s="27"/>
+      <c r="MB48" s="27"/>
+      <c r="MC48" s="27"/>
+      <c r="MD48" s="27"/>
+      <c r="ME48" s="27"/>
+      <c r="MF48" s="27"/>
+      <c r="MG48" s="27"/>
+      <c r="MH48" s="27"/>
+      <c r="MI48" s="27"/>
+      <c r="MJ48" s="27"/>
+      <c r="MK48" s="27"/>
+      <c r="ML48" s="27"/>
+      <c r="MM48" s="27"/>
+      <c r="MN48" s="27"/>
+      <c r="MO48" s="27"/>
+      <c r="MP48" s="27"/>
+      <c r="MQ48" s="27"/>
+      <c r="MR48" s="27"/>
+      <c r="MS48" s="27"/>
+      <c r="MT48" s="27"/>
+      <c r="MU48" s="27"/>
+      <c r="MV48" s="27"/>
+      <c r="MW48" s="27"/>
+      <c r="MX48" s="27"/>
+      <c r="MY48" s="27"/>
+      <c r="MZ48" s="27"/>
+      <c r="NA48" s="27"/>
+      <c r="NB48" s="27"/>
+      <c r="NC48" s="27"/>
+      <c r="ND48" s="27"/>
+      <c r="NE48" s="27"/>
+      <c r="NF48" s="27"/>
+      <c r="NG48" s="27"/>
+      <c r="NH48" s="27"/>
+      <c r="NI48" s="27"/>
+      <c r="NJ48" s="27"/>
+      <c r="NK48" s="27"/>
+      <c r="NL48" s="27"/>
+      <c r="NM48" s="27"/>
+      <c r="NN48" s="27"/>
+      <c r="NO48" s="27"/>
+      <c r="NP48" s="27"/>
+      <c r="NQ48" s="27"/>
+      <c r="NR48" s="27"/>
+      <c r="NS48" s="27"/>
+      <c r="NT48" s="27"/>
+      <c r="NU48" s="27"/>
+      <c r="NV48" s="27"/>
+      <c r="NW48" s="27"/>
+      <c r="NX48" s="27"/>
+      <c r="NY48" s="27"/>
+      <c r="NZ48" s="27"/>
+      <c r="OA48" s="27"/>
+      <c r="OB48" s="27"/>
+      <c r="OC48" s="27"/>
+      <c r="OD48" s="27"/>
+      <c r="OE48" s="27"/>
+      <c r="OF48" s="27"/>
+      <c r="OG48" s="27"/>
+      <c r="OH48" s="27"/>
+      <c r="OI48" s="27"/>
+      <c r="OJ48" s="27"/>
+      <c r="OK48" s="27"/>
+      <c r="OL48" s="27"/>
+      <c r="OM48" s="27"/>
+      <c r="ON48" s="27"/>
+      <c r="OO48" s="27"/>
+      <c r="OP48" s="27"/>
+      <c r="OQ48" s="27"/>
+      <c r="OR48" s="27"/>
+      <c r="OS48" s="27"/>
+      <c r="OT48" s="27"/>
+      <c r="OU48" s="27"/>
+      <c r="OV48" s="27"/>
+      <c r="OW48" s="27"/>
+      <c r="OX48" s="27"/>
+      <c r="OY48" s="27"/>
+      <c r="OZ48" s="27"/>
+      <c r="PA48" s="27"/>
+      <c r="PB48" s="27"/>
+      <c r="PC48" s="27"/>
+      <c r="PD48" s="27"/>
+      <c r="PE48" s="27"/>
+      <c r="PF48" s="27"/>
+      <c r="PG48" s="27"/>
+      <c r="PH48" s="27"/>
+      <c r="PI48" s="27"/>
+      <c r="PJ48" s="27"/>
+      <c r="PK48" s="27"/>
+      <c r="PL48" s="27"/>
+      <c r="PM48" s="27"/>
+      <c r="PN48" s="27"/>
+      <c r="PO48" s="27"/>
+      <c r="PP48" s="27"/>
+      <c r="PQ48" s="27"/>
+      <c r="PR48" s="27"/>
+      <c r="PS48" s="27"/>
+      <c r="PT48" s="27"/>
+      <c r="PU48" s="27"/>
+      <c r="PV48" s="27"/>
+      <c r="PW48" s="27"/>
+      <c r="PX48" s="27"/>
+      <c r="PY48" s="27"/>
+      <c r="PZ48" s="27"/>
+      <c r="QA48" s="27"/>
+      <c r="QB48" s="27"/>
+      <c r="QC48" s="27"/>
+      <c r="QD48" s="27"/>
+      <c r="QE48" s="27"/>
+      <c r="QF48" s="27"/>
+      <c r="QG48" s="27"/>
+      <c r="QH48" s="27"/>
+      <c r="QI48" s="27"/>
+      <c r="QJ48" s="27"/>
+      <c r="QK48" s="27"/>
+      <c r="QL48" s="27"/>
+      <c r="QM48" s="27"/>
+      <c r="QN48" s="27"/>
+      <c r="QO48" s="27"/>
+      <c r="QP48" s="27"/>
+      <c r="QQ48" s="27"/>
+      <c r="QR48" s="27"/>
+      <c r="QS48" s="27"/>
+      <c r="QT48" s="27"/>
+      <c r="QU48" s="27"/>
+      <c r="QV48" s="27"/>
+      <c r="QW48" s="27"/>
+      <c r="QX48" s="27"/>
+      <c r="QY48" s="27"/>
+      <c r="QZ48" s="27"/>
+      <c r="RA48" s="27"/>
+      <c r="RB48" s="27"/>
+      <c r="RC48" s="27"/>
+      <c r="RD48" s="27"/>
+      <c r="RE48" s="27"/>
+      <c r="RF48" s="27"/>
+      <c r="RG48" s="27"/>
+      <c r="RH48" s="27"/>
+      <c r="RI48" s="27"/>
+      <c r="RJ48" s="27"/>
+      <c r="RK48" s="27"/>
+      <c r="RL48" s="27"/>
+      <c r="RM48" s="27"/>
+      <c r="RN48" s="27"/>
+      <c r="RO48" s="27"/>
+      <c r="RP48" s="27"/>
+      <c r="RQ48" s="27"/>
+      <c r="RR48" s="27"/>
+      <c r="RS48" s="27"/>
+      <c r="RT48" s="27"/>
+      <c r="RU48" s="27"/>
+      <c r="RV48" s="27"/>
+      <c r="RW48" s="27"/>
+      <c r="RX48" s="27"/>
+      <c r="RY48" s="27"/>
+      <c r="RZ48" s="27"/>
+      <c r="SA48" s="27"/>
+      <c r="SB48" s="27"/>
+      <c r="SC48" s="27"/>
+      <c r="SD48" s="27"/>
+      <c r="SE48" s="27"/>
+      <c r="SF48" s="27"/>
+      <c r="SG48" s="27"/>
+      <c r="SH48" s="27"/>
+      <c r="SI48" s="27"/>
+      <c r="SJ48" s="27"/>
+      <c r="SK48" s="27"/>
+      <c r="SL48" s="27"/>
+      <c r="SM48" s="27"/>
+      <c r="SN48" s="27"/>
+      <c r="SO48" s="27"/>
+      <c r="SP48" s="27"/>
+      <c r="SQ48" s="27"/>
+      <c r="SR48" s="27"/>
+      <c r="SS48" s="27"/>
+      <c r="ST48" s="27"/>
+      <c r="SU48" s="27"/>
+      <c r="SV48" s="27"/>
+      <c r="SW48" s="27"/>
+      <c r="SX48" s="27"/>
+      <c r="SY48" s="27"/>
+      <c r="SZ48" s="27"/>
+      <c r="TA48" s="27"/>
+      <c r="TB48" s="27"/>
+      <c r="TC48" s="27"/>
+      <c r="TD48" s="27"/>
+      <c r="TE48" s="27"/>
+      <c r="TF48" s="27"/>
+      <c r="TG48" s="27"/>
+      <c r="TH48" s="27"/>
+      <c r="TI48" s="27"/>
+      <c r="TJ48" s="27"/>
+      <c r="TK48" s="27"/>
+      <c r="TL48" s="27"/>
+      <c r="TM48" s="27"/>
+      <c r="TN48" s="27"/>
+      <c r="TO48" s="27"/>
+      <c r="TP48" s="27"/>
+      <c r="TQ48" s="27"/>
+      <c r="TR48" s="27"/>
+      <c r="TS48" s="27"/>
+      <c r="TT48" s="27"/>
+      <c r="TU48" s="27"/>
+      <c r="TV48" s="27"/>
+      <c r="TW48" s="27"/>
+      <c r="TX48" s="27"/>
+      <c r="TY48" s="27"/>
+      <c r="TZ48" s="27"/>
+      <c r="UA48" s="27"/>
+      <c r="UB48" s="27"/>
+      <c r="UC48" s="27"/>
+      <c r="UD48" s="27"/>
+      <c r="UE48" s="27"/>
+      <c r="UF48" s="27"/>
+      <c r="UG48" s="27"/>
+      <c r="UH48" s="27"/>
+      <c r="UI48" s="27"/>
+      <c r="UJ48" s="27"/>
+      <c r="UK48" s="27"/>
+      <c r="UL48" s="27"/>
+      <c r="UM48" s="27"/>
+      <c r="UN48" s="27"/>
+      <c r="UO48" s="27"/>
+      <c r="UP48" s="27"/>
+      <c r="UQ48" s="27"/>
+      <c r="UR48" s="27"/>
+      <c r="US48" s="27"/>
+      <c r="UT48" s="27"/>
+      <c r="UU48" s="27"/>
+      <c r="UV48" s="27"/>
+      <c r="UW48" s="27"/>
+      <c r="UX48" s="27"/>
+      <c r="UY48" s="27"/>
+      <c r="UZ48" s="27"/>
+      <c r="VA48" s="27"/>
+      <c r="VB48" s="27"/>
+      <c r="VC48" s="27"/>
+      <c r="VD48" s="27"/>
+      <c r="VE48" s="27"/>
+      <c r="VF48" s="27"/>
+      <c r="VG48" s="27"/>
+      <c r="VH48" s="27"/>
+      <c r="VI48" s="27"/>
+      <c r="VJ48" s="27"/>
+      <c r="VK48" s="27"/>
+      <c r="VL48" s="27"/>
+      <c r="VM48" s="27"/>
+      <c r="VN48" s="27"/>
+      <c r="VO48" s="27"/>
+      <c r="VP48" s="27"/>
+      <c r="VQ48" s="27"/>
+      <c r="VR48" s="27"/>
+      <c r="VS48" s="27"/>
+      <c r="VT48" s="27"/>
+      <c r="VU48" s="27"/>
+      <c r="VV48" s="27"/>
+      <c r="VW48" s="27"/>
+      <c r="VX48" s="27"/>
+      <c r="VY48" s="27"/>
+      <c r="VZ48" s="27"/>
+      <c r="WA48" s="27"/>
+      <c r="WB48" s="27"/>
+      <c r="WC48" s="27"/>
+      <c r="WD48" s="27"/>
+      <c r="WE48" s="27"/>
+      <c r="WF48" s="27"/>
+      <c r="WG48" s="27"/>
+      <c r="WH48" s="27"/>
+      <c r="WI48" s="27"/>
+      <c r="WJ48" s="27"/>
+      <c r="WK48" s="27"/>
+      <c r="WL48" s="27"/>
+      <c r="WM48" s="27"/>
+      <c r="WN48" s="27"/>
+      <c r="WO48" s="27"/>
+      <c r="WP48" s="27"/>
+      <c r="WQ48" s="27"/>
+      <c r="WR48" s="27"/>
+      <c r="WS48" s="27"/>
+      <c r="WT48" s="27"/>
+      <c r="WU48" s="27"/>
+      <c r="WV48" s="27"/>
+      <c r="WW48" s="27"/>
+      <c r="WX48" s="27"/>
+      <c r="WY48" s="27"/>
+      <c r="WZ48" s="27"/>
+      <c r="XA48" s="27"/>
+      <c r="XB48" s="27"/>
+      <c r="XC48" s="27"/>
+      <c r="XD48" s="27"/>
+      <c r="XE48" s="27"/>
+      <c r="XF48" s="27"/>
+      <c r="XG48" s="27"/>
+      <c r="XH48" s="27"/>
+      <c r="XI48" s="27"/>
+      <c r="XJ48" s="27"/>
+      <c r="XK48" s="27"/>
+      <c r="XL48" s="27"/>
+      <c r="XM48" s="27"/>
+      <c r="XN48" s="27"/>
+      <c r="XO48" s="27"/>
+      <c r="XP48" s="27"/>
+      <c r="XQ48" s="27"/>
+      <c r="XR48" s="27"/>
+      <c r="XS48" s="27"/>
+      <c r="XT48" s="27"/>
+      <c r="XU48" s="27"/>
+      <c r="XV48" s="27"/>
+      <c r="XW48" s="27"/>
+      <c r="XX48" s="27"/>
+      <c r="XY48" s="27"/>
+      <c r="XZ48" s="27"/>
+      <c r="YA48" s="27"/>
+      <c r="YB48" s="27"/>
+      <c r="YC48" s="27"/>
+      <c r="YD48" s="27"/>
+      <c r="YE48" s="27"/>
+      <c r="YF48" s="27"/>
+      <c r="YG48" s="27"/>
+      <c r="YH48" s="27"/>
+      <c r="YI48" s="27"/>
+      <c r="YJ48" s="27"/>
+      <c r="YK48" s="27"/>
+      <c r="YL48" s="27"/>
+      <c r="YM48" s="27"/>
+      <c r="YN48" s="27"/>
+      <c r="YO48" s="27"/>
+      <c r="YP48" s="27"/>
+      <c r="YQ48" s="27"/>
+      <c r="YR48" s="27"/>
+      <c r="YS48" s="27"/>
+      <c r="YT48" s="27"/>
+      <c r="YU48" s="27"/>
+      <c r="YV48" s="27"/>
+      <c r="YW48" s="27"/>
+      <c r="YX48" s="27"/>
+      <c r="YY48" s="27"/>
+      <c r="YZ48" s="27"/>
+      <c r="ZA48" s="27"/>
+      <c r="ZB48" s="27"/>
+      <c r="ZC48" s="27"/>
+      <c r="ZD48" s="27"/>
+      <c r="ZE48" s="27"/>
+      <c r="ZF48" s="27"/>
+      <c r="ZG48" s="27"/>
+      <c r="ZH48" s="27"/>
+      <c r="ZI48" s="27"/>
+      <c r="ZJ48" s="27"/>
+      <c r="ZK48" s="27"/>
+      <c r="ZL48" s="27"/>
+      <c r="ZM48" s="27"/>
+      <c r="ZN48" s="27"/>
+      <c r="ZO48" s="27"/>
+      <c r="ZP48" s="27"/>
+      <c r="ZQ48" s="27"/>
+      <c r="ZR48" s="27"/>
+      <c r="ZS48" s="27"/>
+      <c r="ZT48" s="27"/>
+      <c r="ZU48" s="27"/>
+      <c r="ZV48" s="27"/>
+      <c r="ZW48" s="27"/>
+      <c r="ZX48" s="27"/>
+      <c r="ZY48" s="27"/>
+      <c r="ZZ48" s="27"/>
+      <c r="AAA48" s="27"/>
+      <c r="AAB48" s="27"/>
+      <c r="AAC48" s="27"/>
+      <c r="AAD48" s="27"/>
+      <c r="AAE48" s="27"/>
+      <c r="AAF48" s="27"/>
+      <c r="AAG48" s="27"/>
+      <c r="AAH48" s="27"/>
+      <c r="AAI48" s="27"/>
+      <c r="AAJ48" s="27"/>
+      <c r="AAK48" s="27"/>
+      <c r="AAL48" s="27"/>
+      <c r="AAM48" s="27"/>
+      <c r="AAN48" s="27"/>
+      <c r="AAO48" s="27"/>
+      <c r="AAP48" s="27"/>
+      <c r="AAQ48" s="27"/>
+      <c r="AAR48" s="27"/>
+      <c r="AAS48" s="27"/>
+      <c r="AAT48" s="27"/>
+      <c r="AAU48" s="27"/>
+      <c r="AAV48" s="27"/>
+      <c r="AAW48" s="27"/>
+      <c r="AAX48" s="27"/>
+      <c r="AAY48" s="27"/>
+      <c r="AAZ48" s="27"/>
+      <c r="ABA48" s="27"/>
+      <c r="ABB48" s="27"/>
+      <c r="ABC48" s="27"/>
+      <c r="ABD48" s="27"/>
+      <c r="ABE48" s="27"/>
+      <c r="ABF48" s="27"/>
+      <c r="ABG48" s="27"/>
+      <c r="ABH48" s="27"/>
+      <c r="ABI48" s="27"/>
+      <c r="ABJ48" s="27"/>
+      <c r="ABK48" s="27"/>
+      <c r="ABL48" s="27"/>
+      <c r="ABM48" s="27"/>
+      <c r="ABN48" s="27"/>
+      <c r="ABO48" s="27"/>
+      <c r="ABP48" s="27"/>
+      <c r="ABQ48" s="27"/>
+      <c r="ABR48" s="27"/>
+      <c r="ABS48" s="27"/>
+      <c r="ABT48" s="27"/>
+      <c r="ABU48" s="27"/>
+      <c r="ABV48" s="27"/>
+      <c r="ABW48" s="27"/>
+      <c r="ABX48" s="27"/>
+      <c r="ABY48" s="27"/>
+      <c r="ABZ48" s="27"/>
+      <c r="ACA48" s="27"/>
+      <c r="ACB48" s="27"/>
+      <c r="ACC48" s="27"/>
+      <c r="ACD48" s="27"/>
+      <c r="ACE48" s="27"/>
+      <c r="ACF48" s="27"/>
+      <c r="ACG48" s="27"/>
+      <c r="ACH48" s="27"/>
+      <c r="ACI48" s="27"/>
+      <c r="ACJ48" s="27"/>
+      <c r="ACK48" s="27"/>
+      <c r="ACL48" s="27"/>
+      <c r="ACM48" s="27"/>
+      <c r="ACN48" s="27"/>
+      <c r="ACO48" s="27"/>
+      <c r="ACP48" s="27"/>
+      <c r="ACQ48" s="27"/>
+      <c r="ACR48" s="27"/>
+      <c r="ACS48" s="27"/>
+      <c r="ACT48" s="27"/>
+      <c r="ACU48" s="27"/>
+      <c r="ACV48" s="27"/>
+      <c r="ACW48" s="27"/>
+      <c r="ACX48" s="27"/>
+      <c r="ACY48" s="27"/>
+      <c r="ACZ48" s="27"/>
+      <c r="ADA48" s="27"/>
+      <c r="ADB48" s="27"/>
+      <c r="ADC48" s="27"/>
+      <c r="ADD48" s="27"/>
+      <c r="ADE48" s="27"/>
+      <c r="ADF48" s="27"/>
+      <c r="ADG48" s="27"/>
+      <c r="ADH48" s="27"/>
+      <c r="ADI48" s="27"/>
+      <c r="ADJ48" s="27"/>
+      <c r="ADK48" s="27"/>
+      <c r="ADL48" s="27"/>
+      <c r="ADM48" s="27"/>
+      <c r="ADN48" s="27"/>
+      <c r="ADO48" s="27"/>
+      <c r="ADP48" s="27"/>
+      <c r="ADQ48" s="27"/>
+      <c r="ADR48" s="27"/>
+      <c r="ADS48" s="27"/>
+      <c r="ADT48" s="27"/>
+      <c r="ADU48" s="27"/>
+      <c r="ADV48" s="27"/>
+      <c r="ADW48" s="27"/>
+      <c r="ADX48" s="27"/>
+      <c r="ADY48" s="27"/>
+      <c r="ADZ48" s="27"/>
+      <c r="AEA48" s="27"/>
+      <c r="AEB48" s="27"/>
+      <c r="AEC48" s="27"/>
+      <c r="AED48" s="27"/>
+      <c r="AEE48" s="27"/>
+      <c r="AEF48" s="27"/>
+      <c r="AEG48" s="27"/>
+      <c r="AEH48" s="27"/>
+      <c r="AEI48" s="27"/>
+      <c r="AEJ48" s="27"/>
+      <c r="AEK48" s="27"/>
+      <c r="AEL48" s="27"/>
+      <c r="AEM48" s="27"/>
+      <c r="AEN48" s="27"/>
+      <c r="AEO48" s="27"/>
+      <c r="AEP48" s="27"/>
+      <c r="AEQ48" s="27"/>
+      <c r="AER48" s="27"/>
+      <c r="AES48" s="27"/>
+      <c r="AET48" s="27"/>
+      <c r="AEU48" s="27"/>
+      <c r="AEV48" s="27"/>
+      <c r="AEW48" s="27"/>
+      <c r="AEX48" s="27"/>
+      <c r="AEY48" s="27"/>
+      <c r="AEZ48" s="27"/>
+      <c r="AFA48" s="27"/>
+      <c r="AFB48" s="27"/>
+      <c r="AFC48" s="27"/>
+      <c r="AFD48" s="27"/>
+      <c r="AFE48" s="27"/>
+      <c r="AFF48" s="27"/>
+      <c r="AFG48" s="27"/>
+      <c r="AFH48" s="27"/>
+      <c r="AFI48" s="27"/>
+      <c r="AFJ48" s="27"/>
+      <c r="AFK48" s="27"/>
+      <c r="AFL48" s="27"/>
+      <c r="AFM48" s="27"/>
+      <c r="AFN48" s="27"/>
+      <c r="AFO48" s="27"/>
+      <c r="AFP48" s="27"/>
+      <c r="AFQ48" s="27"/>
+      <c r="AFR48" s="27"/>
+      <c r="AFS48" s="27"/>
+      <c r="AFT48" s="27"/>
+      <c r="AFU48" s="27"/>
+      <c r="AFV48" s="27"/>
+      <c r="AFW48" s="27"/>
+      <c r="AFX48" s="27"/>
+      <c r="AFY48" s="27"/>
+      <c r="AFZ48" s="27"/>
+      <c r="AGA48" s="27"/>
+      <c r="AGB48" s="27"/>
+      <c r="AGC48" s="27"/>
+      <c r="AGD48" s="27"/>
+      <c r="AGE48" s="27"/>
+      <c r="AGF48" s="27"/>
+      <c r="AGG48" s="27"/>
+      <c r="AGH48" s="27"/>
+      <c r="AGI48" s="27"/>
+      <c r="AGJ48" s="27"/>
+      <c r="AGK48" s="27"/>
+      <c r="AGL48" s="27"/>
+      <c r="AGM48" s="27"/>
+      <c r="AGN48" s="27"/>
+      <c r="AGO48" s="27"/>
+      <c r="AGP48" s="27"/>
+      <c r="AGQ48" s="27"/>
+      <c r="AGR48" s="27"/>
+      <c r="AGS48" s="27"/>
+      <c r="AGT48" s="27"/>
+      <c r="AGU48" s="27"/>
+      <c r="AGV48" s="27"/>
+      <c r="AGW48" s="27"/>
+      <c r="AGX48" s="27"/>
+      <c r="AGY48" s="27"/>
+      <c r="AGZ48" s="27"/>
+      <c r="AHA48" s="27"/>
+      <c r="AHB48" s="27"/>
+      <c r="AHC48" s="27"/>
+      <c r="AHD48" s="27"/>
+      <c r="AHE48" s="27"/>
+      <c r="AHF48" s="27"/>
+      <c r="AHG48" s="27"/>
+      <c r="AHH48" s="27"/>
+      <c r="AHI48" s="27"/>
+      <c r="AHJ48" s="27"/>
+      <c r="AHK48" s="27"/>
+      <c r="AHL48" s="27"/>
+      <c r="AHM48" s="27"/>
+      <c r="AHN48" s="27"/>
+      <c r="AHO48" s="27"/>
+      <c r="AHP48" s="27"/>
+      <c r="AHQ48" s="27"/>
+      <c r="AHR48" s="27"/>
+      <c r="AHS48" s="27"/>
+      <c r="AHT48" s="27"/>
+      <c r="AHU48" s="27"/>
+      <c r="AHV48" s="27"/>
+      <c r="AHW48" s="27"/>
+      <c r="AHX48" s="27"/>
+      <c r="AHY48" s="27"/>
+      <c r="AHZ48" s="27"/>
+      <c r="AIA48" s="27"/>
+      <c r="AIB48" s="27"/>
+      <c r="AIC48" s="27"/>
+      <c r="AID48" s="27"/>
+      <c r="AIE48" s="27"/>
+      <c r="AIF48" s="27"/>
+      <c r="AIG48" s="27"/>
+      <c r="AIH48" s="27"/>
+      <c r="AII48" s="27"/>
+      <c r="AIJ48" s="27"/>
+      <c r="AIK48" s="27"/>
+      <c r="AIL48" s="27"/>
+      <c r="AIM48" s="27"/>
+      <c r="AIN48" s="27"/>
+      <c r="AIO48" s="27"/>
+      <c r="AIP48" s="27"/>
+      <c r="AIQ48" s="27"/>
+      <c r="AIR48" s="27"/>
+      <c r="AIS48" s="27"/>
+      <c r="AIT48" s="27"/>
+      <c r="AIU48" s="27"/>
+      <c r="AIV48" s="27"/>
+      <c r="AIW48" s="27"/>
+      <c r="AIX48" s="27"/>
+      <c r="AIY48" s="27"/>
+      <c r="AIZ48" s="27"/>
+      <c r="AJA48" s="27"/>
+      <c r="AJB48" s="27"/>
+      <c r="AJC48" s="27"/>
+      <c r="AJD48" s="27"/>
+      <c r="AJE48" s="27"/>
+      <c r="AJF48" s="27"/>
+      <c r="AJG48" s="27"/>
+      <c r="AJH48" s="27"/>
+      <c r="AJI48" s="27"/>
+      <c r="AJJ48" s="27"/>
+      <c r="AJK48" s="27"/>
+      <c r="AJL48" s="27"/>
+      <c r="AJM48" s="27"/>
+      <c r="AJN48" s="27"/>
+      <c r="AJO48" s="27"/>
+      <c r="AJP48" s="27"/>
+      <c r="AJQ48" s="27"/>
+      <c r="AJR48" s="27"/>
+      <c r="AJS48" s="27"/>
+      <c r="AJT48" s="27"/>
+      <c r="AJU48" s="27"/>
+      <c r="AJV48" s="27"/>
+      <c r="AJW48" s="27"/>
+      <c r="AJX48" s="27"/>
+      <c r="AJY48" s="27"/>
+      <c r="AJZ48" s="27"/>
+      <c r="AKA48" s="27"/>
+      <c r="AKB48" s="27"/>
+      <c r="AKC48" s="27"/>
+      <c r="AKD48" s="27"/>
+      <c r="AKE48" s="27"/>
+      <c r="AKF48" s="27"/>
+      <c r="AKG48" s="27"/>
+      <c r="AKH48" s="27"/>
+      <c r="AKI48" s="27"/>
+      <c r="AKJ48" s="27"/>
+      <c r="AKK48" s="27"/>
+      <c r="AKL48" s="27"/>
+      <c r="AKM48" s="27"/>
+      <c r="AKN48" s="27"/>
+      <c r="AKO48" s="27"/>
+      <c r="AKP48" s="27"/>
+      <c r="AKQ48" s="27"/>
+      <c r="AKR48" s="27"/>
+      <c r="AKS48" s="27"/>
+      <c r="AKT48" s="27"/>
+      <c r="AKU48" s="27"/>
+      <c r="AKV48" s="27"/>
+      <c r="AKW48" s="27"/>
+      <c r="AKX48" s="27"/>
+      <c r="AKY48" s="27"/>
+      <c r="AKZ48" s="27"/>
+      <c r="ALA48" s="27"/>
+      <c r="ALB48" s="27"/>
+      <c r="ALC48" s="27"/>
+      <c r="ALD48" s="27"/>
+      <c r="ALE48" s="27"/>
+      <c r="ALF48" s="27"/>
+      <c r="ALG48" s="27"/>
+      <c r="ALH48" s="27"/>
+      <c r="ALI48" s="27"/>
+      <c r="ALJ48" s="27"/>
+      <c r="ALK48" s="27"/>
+      <c r="ALL48" s="27"/>
+      <c r="ALM48" s="27"/>
+      <c r="ALN48" s="27"/>
+      <c r="ALO48" s="27"/>
+      <c r="ALP48" s="27"/>
+      <c r="ALQ48" s="27"/>
+      <c r="ALR48" s="27"/>
+      <c r="ALS48" s="27"/>
+      <c r="ALT48" s="27"/>
+      <c r="ALU48" s="27"/>
+      <c r="ALV48" s="27"/>
+      <c r="ALW48" s="27"/>
+      <c r="ALX48" s="27"/>
+      <c r="ALY48" s="27"/>
+      <c r="ALZ48" s="27"/>
+      <c r="AMA48" s="27"/>
+      <c r="AMB48" s="27"/>
+      <c r="AMC48" s="27"/>
+      <c r="AMD48" s="27"/>
+      <c r="AME48" s="27"/>
+      <c r="AMF48" s="27"/>
+      <c r="AMG48" s="27"/>
+      <c r="AMH48" s="27"/>
+      <c r="AMI48" s="27"/>
+      <c r="AMJ48" s="27"/>
+      <c r="AMK48" s="27"/>
+    </row>
+    <row r="49" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="5" t="s">
-        <v>279</v>
+        <v>210</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
-        <v>164</v>
+        <v>59</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5" t="s">
@@ -5056,17 +6078,14 @@
       <c r="K49" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L49" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="L49" s="5"/>
       <c r="M49" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="N49" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O49" s="5"/>
+        <v>213</v>
+      </c>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5" t="s">
+        <v>212</v>
+      </c>
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
@@ -5074,15 +6093,17 @@
         <v>83</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+      <c r="U49" s="23"/>
+    </row>
+    <row r="50" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="23"/>
       <c r="B50" s="5" t="s">
-        <v>214</v>
+        <v>279</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>58</v>
@@ -5109,8 +6130,8 @@
         <v>240</v>
       </c>
       <c r="N50" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
@@ -5120,15 +6141,15 @@
         <v>83</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>58</v>
@@ -5166,15 +6187,15 @@
         <v>83</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>58</v>
@@ -5198,11 +6219,11 @@
         <v>58</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="N52" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
@@ -5212,30 +6233,28 @@
         <v>83</v>
       </c>
       <c r="T52" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="B53" s="5" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>237</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="F53" s="5"/>
       <c r="G53" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
@@ -5243,15 +6262,16 @@
         <v>58</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5" t="s">
-        <v>238</v>
-      </c>
+      <c r="N53" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O53" s="5"/>
       <c r="P53" s="5"/>
       <c r="Q53" s="5"/>
       <c r="R53" s="5"/>
@@ -5259,1120 +6279,1167 @@
         <v>83</v>
       </c>
       <c r="T53" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+      <c r="B54" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="T54" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B57" s="5" t="s">
+    <row r="56" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B58" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5" t="s">
+      <c r="D58" s="5"/>
+      <c r="E58" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H57" s="5" t="s">
+      <c r="F58" s="5"/>
+      <c r="G58" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H58" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5" t="s">
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
-      <c r="P57" s="5"/>
-      <c r="Q57" s="5"/>
-      <c r="R57" s="5"/>
-      <c r="S57" s="5" t="s">
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="T57" s="5" t="s">
+      <c r="T58" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="34" t="s">
+    <row r="60" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="C61" s="34"/>
-    </row>
-    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="31" t="s">
+      <c r="C62" s="35"/>
+    </row>
+    <row r="63" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="C62" s="31"/>
-    </row>
-    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="31" t="s">
+      <c r="C63" s="32"/>
+    </row>
+    <row r="64" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="31"/>
-    </row>
-    <row r="64" spans="1:20" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="32" t="s">
+      <c r="C64" s="32"/>
+    </row>
+    <row r="65" spans="1:1025" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="C64" s="32"/>
-    </row>
-    <row r="65" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="B65" s="32" t="s">
+      <c r="C65" s="33"/>
+    </row>
+    <row r="66" spans="1:1025" x14ac:dyDescent="0.35">
+      <c r="B66" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C65" s="32"/>
-    </row>
-    <row r="66" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="A66" s="26"/>
-      <c r="B66" s="32" t="s">
+      <c r="C66" s="33"/>
+    </row>
+    <row r="67" spans="1:1025" x14ac:dyDescent="0.35">
+      <c r="A67" s="26"/>
+      <c r="B67" s="33" t="s">
         <v>259</v>
       </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="26"/>
-      <c r="J66" s="26"/>
-      <c r="K66" s="26"/>
-      <c r="L66" s="26"/>
-      <c r="M66" s="26"/>
-      <c r="N66" s="26"/>
-      <c r="O66" s="26"/>
-      <c r="P66" s="26"/>
-      <c r="Q66" s="26"/>
-      <c r="R66" s="26"/>
-      <c r="S66" s="26"/>
-      <c r="T66" s="26"/>
-      <c r="U66" s="26"/>
-      <c r="V66" s="26"/>
-      <c r="W66" s="26"/>
-      <c r="X66" s="26"/>
-      <c r="Y66" s="26"/>
-      <c r="Z66" s="26"/>
-      <c r="AA66" s="26"/>
-      <c r="AB66" s="26"/>
-      <c r="AC66" s="26"/>
-      <c r="AD66" s="26"/>
-      <c r="AE66" s="26"/>
-      <c r="AF66" s="26"/>
-      <c r="AG66" s="26"/>
-      <c r="AH66" s="26"/>
-      <c r="AI66" s="26"/>
-      <c r="AJ66" s="26"/>
-      <c r="AK66" s="26"/>
-      <c r="AL66" s="26"/>
-      <c r="AM66" s="26"/>
-      <c r="AN66" s="26"/>
-      <c r="AO66" s="26"/>
-      <c r="AP66" s="26"/>
-      <c r="AQ66" s="26"/>
-      <c r="AR66" s="26"/>
-      <c r="AS66" s="26"/>
-      <c r="AT66" s="26"/>
-      <c r="AU66" s="26"/>
-      <c r="AV66" s="26"/>
-      <c r="AW66" s="26"/>
-      <c r="AX66" s="26"/>
-      <c r="AY66" s="26"/>
-      <c r="AZ66" s="26"/>
-      <c r="BA66" s="26"/>
-      <c r="BB66" s="26"/>
-      <c r="BC66" s="26"/>
-      <c r="BD66" s="26"/>
-      <c r="BE66" s="26"/>
-      <c r="BF66" s="26"/>
-      <c r="BG66" s="26"/>
-      <c r="BH66" s="26"/>
-      <c r="BI66" s="26"/>
-      <c r="BJ66" s="26"/>
-      <c r="BK66" s="26"/>
-      <c r="BL66" s="26"/>
-      <c r="BM66" s="26"/>
-      <c r="BN66" s="26"/>
-      <c r="BO66" s="26"/>
-      <c r="BP66" s="26"/>
-      <c r="BQ66" s="26"/>
-      <c r="BR66" s="26"/>
-      <c r="BS66" s="26"/>
-      <c r="BT66" s="26"/>
-      <c r="BU66" s="26"/>
-      <c r="BV66" s="26"/>
-      <c r="BW66" s="26"/>
-      <c r="BX66" s="26"/>
-      <c r="BY66" s="26"/>
-      <c r="BZ66" s="26"/>
-      <c r="CA66" s="26"/>
-      <c r="CB66" s="26"/>
-      <c r="CC66" s="26"/>
-      <c r="CD66" s="26"/>
-      <c r="CE66" s="26"/>
-      <c r="CF66" s="26"/>
-      <c r="CG66" s="26"/>
-      <c r="CH66" s="26"/>
-      <c r="CI66" s="26"/>
-      <c r="CJ66" s="26"/>
-      <c r="CK66" s="26"/>
-      <c r="CL66" s="26"/>
-      <c r="CM66" s="26"/>
-      <c r="CN66" s="26"/>
-      <c r="CO66" s="26"/>
-      <c r="CP66" s="26"/>
-      <c r="CQ66" s="26"/>
-      <c r="CR66" s="26"/>
-      <c r="CS66" s="26"/>
-      <c r="CT66" s="26"/>
-      <c r="CU66" s="26"/>
-      <c r="CV66" s="26"/>
-      <c r="CW66" s="26"/>
-      <c r="CX66" s="26"/>
-      <c r="CY66" s="26"/>
-      <c r="CZ66" s="26"/>
-      <c r="DA66" s="26"/>
-      <c r="DB66" s="26"/>
-      <c r="DC66" s="26"/>
-      <c r="DD66" s="26"/>
-      <c r="DE66" s="26"/>
-      <c r="DF66" s="26"/>
-      <c r="DG66" s="26"/>
-      <c r="DH66" s="26"/>
-      <c r="DI66" s="26"/>
-      <c r="DJ66" s="26"/>
-      <c r="DK66" s="26"/>
-      <c r="DL66" s="26"/>
-      <c r="DM66" s="26"/>
-      <c r="DN66" s="26"/>
-      <c r="DO66" s="26"/>
-      <c r="DP66" s="26"/>
-      <c r="DQ66" s="26"/>
-      <c r="DR66" s="26"/>
-      <c r="DS66" s="26"/>
-      <c r="DT66" s="26"/>
-      <c r="DU66" s="26"/>
-      <c r="DV66" s="26"/>
-      <c r="DW66" s="26"/>
-      <c r="DX66" s="26"/>
-      <c r="DY66" s="26"/>
-      <c r="DZ66" s="26"/>
-      <c r="EA66" s="26"/>
-      <c r="EB66" s="26"/>
-      <c r="EC66" s="26"/>
-      <c r="ED66" s="26"/>
-      <c r="EE66" s="26"/>
-      <c r="EF66" s="26"/>
-      <c r="EG66" s="26"/>
-      <c r="EH66" s="26"/>
-      <c r="EI66" s="26"/>
-      <c r="EJ66" s="26"/>
-      <c r="EK66" s="26"/>
-      <c r="EL66" s="26"/>
-      <c r="EM66" s="26"/>
-      <c r="EN66" s="26"/>
-      <c r="EO66" s="26"/>
-      <c r="EP66" s="26"/>
-      <c r="EQ66" s="26"/>
-      <c r="ER66" s="26"/>
-      <c r="ES66" s="26"/>
-      <c r="ET66" s="26"/>
-      <c r="EU66" s="26"/>
-      <c r="EV66" s="26"/>
-      <c r="EW66" s="26"/>
-      <c r="EX66" s="26"/>
-      <c r="EY66" s="26"/>
-      <c r="EZ66" s="26"/>
-      <c r="FA66" s="26"/>
-      <c r="FB66" s="26"/>
-      <c r="FC66" s="26"/>
-      <c r="FD66" s="26"/>
-      <c r="FE66" s="26"/>
-      <c r="FF66" s="26"/>
-      <c r="FG66" s="26"/>
-      <c r="FH66" s="26"/>
-      <c r="FI66" s="26"/>
-      <c r="FJ66" s="26"/>
-      <c r="FK66" s="26"/>
-      <c r="FL66" s="26"/>
-      <c r="FM66" s="26"/>
-      <c r="FN66" s="26"/>
-      <c r="FO66" s="26"/>
-      <c r="FP66" s="26"/>
-      <c r="FQ66" s="26"/>
-      <c r="FR66" s="26"/>
-      <c r="FS66" s="26"/>
-      <c r="FT66" s="26"/>
-      <c r="FU66" s="26"/>
-      <c r="FV66" s="26"/>
-      <c r="FW66" s="26"/>
-      <c r="FX66" s="26"/>
-      <c r="FY66" s="26"/>
-      <c r="FZ66" s="26"/>
-      <c r="GA66" s="26"/>
-      <c r="GB66" s="26"/>
-      <c r="GC66" s="26"/>
-      <c r="GD66" s="26"/>
-      <c r="GE66" s="26"/>
-      <c r="GF66" s="26"/>
-      <c r="GG66" s="26"/>
-      <c r="GH66" s="26"/>
-      <c r="GI66" s="26"/>
-      <c r="GJ66" s="26"/>
-      <c r="GK66" s="26"/>
-      <c r="GL66" s="26"/>
-      <c r="GM66" s="26"/>
-      <c r="GN66" s="26"/>
-      <c r="GO66" s="26"/>
-      <c r="GP66" s="26"/>
-      <c r="GQ66" s="26"/>
-      <c r="GR66" s="26"/>
-      <c r="GS66" s="26"/>
-      <c r="GT66" s="26"/>
-      <c r="GU66" s="26"/>
-      <c r="GV66" s="26"/>
-      <c r="GW66" s="26"/>
-      <c r="GX66" s="26"/>
-      <c r="GY66" s="26"/>
-      <c r="GZ66" s="26"/>
-      <c r="HA66" s="26"/>
-      <c r="HB66" s="26"/>
-      <c r="HC66" s="26"/>
-      <c r="HD66" s="26"/>
-      <c r="HE66" s="26"/>
-      <c r="HF66" s="26"/>
-      <c r="HG66" s="26"/>
-      <c r="HH66" s="26"/>
-      <c r="HI66" s="26"/>
-      <c r="HJ66" s="26"/>
-      <c r="HK66" s="26"/>
-      <c r="HL66" s="26"/>
-      <c r="HM66" s="26"/>
-      <c r="HN66" s="26"/>
-      <c r="HO66" s="26"/>
-      <c r="HP66" s="26"/>
-      <c r="HQ66" s="26"/>
-      <c r="HR66" s="26"/>
-      <c r="HS66" s="26"/>
-      <c r="HT66" s="26"/>
-      <c r="HU66" s="26"/>
-      <c r="HV66" s="26"/>
-      <c r="HW66" s="26"/>
-      <c r="HX66" s="26"/>
-      <c r="HY66" s="26"/>
-      <c r="HZ66" s="26"/>
-      <c r="IA66" s="26"/>
-      <c r="IB66" s="26"/>
-      <c r="IC66" s="26"/>
-      <c r="ID66" s="26"/>
-      <c r="IE66" s="26"/>
-      <c r="IF66" s="26"/>
-      <c r="IG66" s="26"/>
-      <c r="IH66" s="26"/>
-      <c r="II66" s="26"/>
-      <c r="IJ66" s="26"/>
-      <c r="IK66" s="26"/>
-      <c r="IL66" s="26"/>
-      <c r="IM66" s="26"/>
-      <c r="IN66" s="26"/>
-      <c r="IO66" s="26"/>
-      <c r="IP66" s="26"/>
-      <c r="IQ66" s="26"/>
-      <c r="IR66" s="26"/>
-      <c r="IS66" s="26"/>
-      <c r="IT66" s="26"/>
-      <c r="IU66" s="26"/>
-      <c r="IV66" s="26"/>
-      <c r="IW66" s="26"/>
-      <c r="IX66" s="26"/>
-      <c r="IY66" s="26"/>
-      <c r="IZ66" s="26"/>
-      <c r="JA66" s="26"/>
-      <c r="JB66" s="26"/>
-      <c r="JC66" s="26"/>
-      <c r="JD66" s="26"/>
-      <c r="JE66" s="26"/>
-      <c r="JF66" s="26"/>
-      <c r="JG66" s="26"/>
-      <c r="JH66" s="26"/>
-      <c r="JI66" s="26"/>
-      <c r="JJ66" s="26"/>
-      <c r="JK66" s="26"/>
-      <c r="JL66" s="26"/>
-      <c r="JM66" s="26"/>
-      <c r="JN66" s="26"/>
-      <c r="JO66" s="26"/>
-      <c r="JP66" s="26"/>
-      <c r="JQ66" s="26"/>
-      <c r="JR66" s="26"/>
-      <c r="JS66" s="26"/>
-      <c r="JT66" s="26"/>
-      <c r="JU66" s="26"/>
-      <c r="JV66" s="26"/>
-      <c r="JW66" s="26"/>
-      <c r="JX66" s="26"/>
-      <c r="JY66" s="26"/>
-      <c r="JZ66" s="26"/>
-      <c r="KA66" s="26"/>
-      <c r="KB66" s="26"/>
-      <c r="KC66" s="26"/>
-      <c r="KD66" s="26"/>
-      <c r="KE66" s="26"/>
-      <c r="KF66" s="26"/>
-      <c r="KG66" s="26"/>
-      <c r="KH66" s="26"/>
-      <c r="KI66" s="26"/>
-      <c r="KJ66" s="26"/>
-      <c r="KK66" s="26"/>
-      <c r="KL66" s="26"/>
-      <c r="KM66" s="26"/>
-      <c r="KN66" s="26"/>
-      <c r="KO66" s="26"/>
-      <c r="KP66" s="26"/>
-      <c r="KQ66" s="26"/>
-      <c r="KR66" s="26"/>
-      <c r="KS66" s="26"/>
-      <c r="KT66" s="26"/>
-      <c r="KU66" s="26"/>
-      <c r="KV66" s="26"/>
-      <c r="KW66" s="26"/>
-      <c r="KX66" s="26"/>
-      <c r="KY66" s="26"/>
-      <c r="KZ66" s="26"/>
-      <c r="LA66" s="26"/>
-      <c r="LB66" s="26"/>
-      <c r="LC66" s="26"/>
-      <c r="LD66" s="26"/>
-      <c r="LE66" s="26"/>
-      <c r="LF66" s="26"/>
-      <c r="LG66" s="26"/>
-      <c r="LH66" s="26"/>
-      <c r="LI66" s="26"/>
-      <c r="LJ66" s="26"/>
-      <c r="LK66" s="26"/>
-      <c r="LL66" s="26"/>
-      <c r="LM66" s="26"/>
-      <c r="LN66" s="26"/>
-      <c r="LO66" s="26"/>
-      <c r="LP66" s="26"/>
-      <c r="LQ66" s="26"/>
-      <c r="LR66" s="26"/>
-      <c r="LS66" s="26"/>
-      <c r="LT66" s="26"/>
-      <c r="LU66" s="26"/>
-      <c r="LV66" s="26"/>
-      <c r="LW66" s="26"/>
-      <c r="LX66" s="26"/>
-      <c r="LY66" s="26"/>
-      <c r="LZ66" s="26"/>
-      <c r="MA66" s="26"/>
-      <c r="MB66" s="26"/>
-      <c r="MC66" s="26"/>
-      <c r="MD66" s="26"/>
-      <c r="ME66" s="26"/>
-      <c r="MF66" s="26"/>
-      <c r="MG66" s="26"/>
-      <c r="MH66" s="26"/>
-      <c r="MI66" s="26"/>
-      <c r="MJ66" s="26"/>
-      <c r="MK66" s="26"/>
-      <c r="ML66" s="26"/>
-      <c r="MM66" s="26"/>
-      <c r="MN66" s="26"/>
-      <c r="MO66" s="26"/>
-      <c r="MP66" s="26"/>
-      <c r="MQ66" s="26"/>
-      <c r="MR66" s="26"/>
-      <c r="MS66" s="26"/>
-      <c r="MT66" s="26"/>
-      <c r="MU66" s="26"/>
-      <c r="MV66" s="26"/>
-      <c r="MW66" s="26"/>
-      <c r="MX66" s="26"/>
-      <c r="MY66" s="26"/>
-      <c r="MZ66" s="26"/>
-      <c r="NA66" s="26"/>
-      <c r="NB66" s="26"/>
-      <c r="NC66" s="26"/>
-      <c r="ND66" s="26"/>
-      <c r="NE66" s="26"/>
-      <c r="NF66" s="26"/>
-      <c r="NG66" s="26"/>
-      <c r="NH66" s="26"/>
-      <c r="NI66" s="26"/>
-      <c r="NJ66" s="26"/>
-      <c r="NK66" s="26"/>
-      <c r="NL66" s="26"/>
-      <c r="NM66" s="26"/>
-      <c r="NN66" s="26"/>
-      <c r="NO66" s="26"/>
-      <c r="NP66" s="26"/>
-      <c r="NQ66" s="26"/>
-      <c r="NR66" s="26"/>
-      <c r="NS66" s="26"/>
-      <c r="NT66" s="26"/>
-      <c r="NU66" s="26"/>
-      <c r="NV66" s="26"/>
-      <c r="NW66" s="26"/>
-      <c r="NX66" s="26"/>
-      <c r="NY66" s="26"/>
-      <c r="NZ66" s="26"/>
-      <c r="OA66" s="26"/>
-      <c r="OB66" s="26"/>
-      <c r="OC66" s="26"/>
-      <c r="OD66" s="26"/>
-      <c r="OE66" s="26"/>
-      <c r="OF66" s="26"/>
-      <c r="OG66" s="26"/>
-      <c r="OH66" s="26"/>
-      <c r="OI66" s="26"/>
-      <c r="OJ66" s="26"/>
-      <c r="OK66" s="26"/>
-      <c r="OL66" s="26"/>
-      <c r="OM66" s="26"/>
-      <c r="ON66" s="26"/>
-      <c r="OO66" s="26"/>
-      <c r="OP66" s="26"/>
-      <c r="OQ66" s="26"/>
-      <c r="OR66" s="26"/>
-      <c r="OS66" s="26"/>
-      <c r="OT66" s="26"/>
-      <c r="OU66" s="26"/>
-      <c r="OV66" s="26"/>
-      <c r="OW66" s="26"/>
-      <c r="OX66" s="26"/>
-      <c r="OY66" s="26"/>
-      <c r="OZ66" s="26"/>
-      <c r="PA66" s="26"/>
-      <c r="PB66" s="26"/>
-      <c r="PC66" s="26"/>
-      <c r="PD66" s="26"/>
-      <c r="PE66" s="26"/>
-      <c r="PF66" s="26"/>
-      <c r="PG66" s="26"/>
-      <c r="PH66" s="26"/>
-      <c r="PI66" s="26"/>
-      <c r="PJ66" s="26"/>
-      <c r="PK66" s="26"/>
-      <c r="PL66" s="26"/>
-      <c r="PM66" s="26"/>
-      <c r="PN66" s="26"/>
-      <c r="PO66" s="26"/>
-      <c r="PP66" s="26"/>
-      <c r="PQ66" s="26"/>
-      <c r="PR66" s="26"/>
-      <c r="PS66" s="26"/>
-      <c r="PT66" s="26"/>
-      <c r="PU66" s="26"/>
-      <c r="PV66" s="26"/>
-      <c r="PW66" s="26"/>
-      <c r="PX66" s="26"/>
-      <c r="PY66" s="26"/>
-      <c r="PZ66" s="26"/>
-      <c r="QA66" s="26"/>
-      <c r="QB66" s="26"/>
-      <c r="QC66" s="26"/>
-      <c r="QD66" s="26"/>
-      <c r="QE66" s="26"/>
-      <c r="QF66" s="26"/>
-      <c r="QG66" s="26"/>
-      <c r="QH66" s="26"/>
-      <c r="QI66" s="26"/>
-      <c r="QJ66" s="26"/>
-      <c r="QK66" s="26"/>
-      <c r="QL66" s="26"/>
-      <c r="QM66" s="26"/>
-      <c r="QN66" s="26"/>
-      <c r="QO66" s="26"/>
-      <c r="QP66" s="26"/>
-      <c r="QQ66" s="26"/>
-      <c r="QR66" s="26"/>
-      <c r="QS66" s="26"/>
-      <c r="QT66" s="26"/>
-      <c r="QU66" s="26"/>
-      <c r="QV66" s="26"/>
-      <c r="QW66" s="26"/>
-      <c r="QX66" s="26"/>
-      <c r="QY66" s="26"/>
-      <c r="QZ66" s="26"/>
-      <c r="RA66" s="26"/>
-      <c r="RB66" s="26"/>
-      <c r="RC66" s="26"/>
-      <c r="RD66" s="26"/>
-      <c r="RE66" s="26"/>
-      <c r="RF66" s="26"/>
-      <c r="RG66" s="26"/>
-      <c r="RH66" s="26"/>
-      <c r="RI66" s="26"/>
-      <c r="RJ66" s="26"/>
-      <c r="RK66" s="26"/>
-      <c r="RL66" s="26"/>
-      <c r="RM66" s="26"/>
-      <c r="RN66" s="26"/>
-      <c r="RO66" s="26"/>
-      <c r="RP66" s="26"/>
-      <c r="RQ66" s="26"/>
-      <c r="RR66" s="26"/>
-      <c r="RS66" s="26"/>
-      <c r="RT66" s="26"/>
-      <c r="RU66" s="26"/>
-      <c r="RV66" s="26"/>
-      <c r="RW66" s="26"/>
-      <c r="RX66" s="26"/>
-      <c r="RY66" s="26"/>
-      <c r="RZ66" s="26"/>
-      <c r="SA66" s="26"/>
-      <c r="SB66" s="26"/>
-      <c r="SC66" s="26"/>
-      <c r="SD66" s="26"/>
-      <c r="SE66" s="26"/>
-      <c r="SF66" s="26"/>
-      <c r="SG66" s="26"/>
-      <c r="SH66" s="26"/>
-      <c r="SI66" s="26"/>
-      <c r="SJ66" s="26"/>
-      <c r="SK66" s="26"/>
-      <c r="SL66" s="26"/>
-      <c r="SM66" s="26"/>
-      <c r="SN66" s="26"/>
-      <c r="SO66" s="26"/>
-      <c r="SP66" s="26"/>
-      <c r="SQ66" s="26"/>
-      <c r="SR66" s="26"/>
-      <c r="SS66" s="26"/>
-      <c r="ST66" s="26"/>
-      <c r="SU66" s="26"/>
-      <c r="SV66" s="26"/>
-      <c r="SW66" s="26"/>
-      <c r="SX66" s="26"/>
-      <c r="SY66" s="26"/>
-      <c r="SZ66" s="26"/>
-      <c r="TA66" s="26"/>
-      <c r="TB66" s="26"/>
-      <c r="TC66" s="26"/>
-      <c r="TD66" s="26"/>
-      <c r="TE66" s="26"/>
-      <c r="TF66" s="26"/>
-      <c r="TG66" s="26"/>
-      <c r="TH66" s="26"/>
-      <c r="TI66" s="26"/>
-      <c r="TJ66" s="26"/>
-      <c r="TK66" s="26"/>
-      <c r="TL66" s="26"/>
-      <c r="TM66" s="26"/>
-      <c r="TN66" s="26"/>
-      <c r="TO66" s="26"/>
-      <c r="TP66" s="26"/>
-      <c r="TQ66" s="26"/>
-      <c r="TR66" s="26"/>
-      <c r="TS66" s="26"/>
-      <c r="TT66" s="26"/>
-      <c r="TU66" s="26"/>
-      <c r="TV66" s="26"/>
-      <c r="TW66" s="26"/>
-      <c r="TX66" s="26"/>
-      <c r="TY66" s="26"/>
-      <c r="TZ66" s="26"/>
-      <c r="UA66" s="26"/>
-      <c r="UB66" s="26"/>
-      <c r="UC66" s="26"/>
-      <c r="UD66" s="26"/>
-      <c r="UE66" s="26"/>
-      <c r="UF66" s="26"/>
-      <c r="UG66" s="26"/>
-      <c r="UH66" s="26"/>
-      <c r="UI66" s="26"/>
-      <c r="UJ66" s="26"/>
-      <c r="UK66" s="26"/>
-      <c r="UL66" s="26"/>
-      <c r="UM66" s="26"/>
-      <c r="UN66" s="26"/>
-      <c r="UO66" s="26"/>
-      <c r="UP66" s="26"/>
-      <c r="UQ66" s="26"/>
-      <c r="UR66" s="26"/>
-      <c r="US66" s="26"/>
-      <c r="UT66" s="26"/>
-      <c r="UU66" s="26"/>
-      <c r="UV66" s="26"/>
-      <c r="UW66" s="26"/>
-      <c r="UX66" s="26"/>
-      <c r="UY66" s="26"/>
-      <c r="UZ66" s="26"/>
-      <c r="VA66" s="26"/>
-      <c r="VB66" s="26"/>
-      <c r="VC66" s="26"/>
-      <c r="VD66" s="26"/>
-      <c r="VE66" s="26"/>
-      <c r="VF66" s="26"/>
-      <c r="VG66" s="26"/>
-      <c r="VH66" s="26"/>
-      <c r="VI66" s="26"/>
-      <c r="VJ66" s="26"/>
-      <c r="VK66" s="26"/>
-      <c r="VL66" s="26"/>
-      <c r="VM66" s="26"/>
-      <c r="VN66" s="26"/>
-      <c r="VO66" s="26"/>
-      <c r="VP66" s="26"/>
-      <c r="VQ66" s="26"/>
-      <c r="VR66" s="26"/>
-      <c r="VS66" s="26"/>
-      <c r="VT66" s="26"/>
-      <c r="VU66" s="26"/>
-      <c r="VV66" s="26"/>
-      <c r="VW66" s="26"/>
-      <c r="VX66" s="26"/>
-      <c r="VY66" s="26"/>
-      <c r="VZ66" s="26"/>
-      <c r="WA66" s="26"/>
-      <c r="WB66" s="26"/>
-      <c r="WC66" s="26"/>
-      <c r="WD66" s="26"/>
-      <c r="WE66" s="26"/>
-      <c r="WF66" s="26"/>
-      <c r="WG66" s="26"/>
-      <c r="WH66" s="26"/>
-      <c r="WI66" s="26"/>
-      <c r="WJ66" s="26"/>
-      <c r="WK66" s="26"/>
-      <c r="WL66" s="26"/>
-      <c r="WM66" s="26"/>
-      <c r="WN66" s="26"/>
-      <c r="WO66" s="26"/>
-      <c r="WP66" s="26"/>
-      <c r="WQ66" s="26"/>
-      <c r="WR66" s="26"/>
-      <c r="WS66" s="26"/>
-      <c r="WT66" s="26"/>
-      <c r="WU66" s="26"/>
-      <c r="WV66" s="26"/>
-      <c r="WW66" s="26"/>
-      <c r="WX66" s="26"/>
-      <c r="WY66" s="26"/>
-      <c r="WZ66" s="26"/>
-      <c r="XA66" s="26"/>
-      <c r="XB66" s="26"/>
-      <c r="XC66" s="26"/>
-      <c r="XD66" s="26"/>
-      <c r="XE66" s="26"/>
-      <c r="XF66" s="26"/>
-      <c r="XG66" s="26"/>
-      <c r="XH66" s="26"/>
-      <c r="XI66" s="26"/>
-      <c r="XJ66" s="26"/>
-      <c r="XK66" s="26"/>
-      <c r="XL66" s="26"/>
-      <c r="XM66" s="26"/>
-      <c r="XN66" s="26"/>
-      <c r="XO66" s="26"/>
-      <c r="XP66" s="26"/>
-      <c r="XQ66" s="26"/>
-      <c r="XR66" s="26"/>
-      <c r="XS66" s="26"/>
-      <c r="XT66" s="26"/>
-      <c r="XU66" s="26"/>
-      <c r="XV66" s="26"/>
-      <c r="XW66" s="26"/>
-      <c r="XX66" s="26"/>
-      <c r="XY66" s="26"/>
-      <c r="XZ66" s="26"/>
-      <c r="YA66" s="26"/>
-      <c r="YB66" s="26"/>
-      <c r="YC66" s="26"/>
-      <c r="YD66" s="26"/>
-      <c r="YE66" s="26"/>
-      <c r="YF66" s="26"/>
-      <c r="YG66" s="26"/>
-      <c r="YH66" s="26"/>
-      <c r="YI66" s="26"/>
-      <c r="YJ66" s="26"/>
-      <c r="YK66" s="26"/>
-      <c r="YL66" s="26"/>
-      <c r="YM66" s="26"/>
-      <c r="YN66" s="26"/>
-      <c r="YO66" s="26"/>
-      <c r="YP66" s="26"/>
-      <c r="YQ66" s="26"/>
-      <c r="YR66" s="26"/>
-      <c r="YS66" s="26"/>
-      <c r="YT66" s="26"/>
-      <c r="YU66" s="26"/>
-      <c r="YV66" s="26"/>
-      <c r="YW66" s="26"/>
-      <c r="YX66" s="26"/>
-      <c r="YY66" s="26"/>
-      <c r="YZ66" s="26"/>
-      <c r="ZA66" s="26"/>
-      <c r="ZB66" s="26"/>
-      <c r="ZC66" s="26"/>
-      <c r="ZD66" s="26"/>
-      <c r="ZE66" s="26"/>
-      <c r="ZF66" s="26"/>
-      <c r="ZG66" s="26"/>
-      <c r="ZH66" s="26"/>
-      <c r="ZI66" s="26"/>
-      <c r="ZJ66" s="26"/>
-      <c r="ZK66" s="26"/>
-      <c r="ZL66" s="26"/>
-      <c r="ZM66" s="26"/>
-      <c r="ZN66" s="26"/>
-      <c r="ZO66" s="26"/>
-      <c r="ZP66" s="26"/>
-      <c r="ZQ66" s="26"/>
-      <c r="ZR66" s="26"/>
-      <c r="ZS66" s="26"/>
-      <c r="ZT66" s="26"/>
-      <c r="ZU66" s="26"/>
-      <c r="ZV66" s="26"/>
-      <c r="ZW66" s="26"/>
-      <c r="ZX66" s="26"/>
-      <c r="ZY66" s="26"/>
-      <c r="ZZ66" s="26"/>
-      <c r="AAA66" s="26"/>
-      <c r="AAB66" s="26"/>
-      <c r="AAC66" s="26"/>
-      <c r="AAD66" s="26"/>
-      <c r="AAE66" s="26"/>
-      <c r="AAF66" s="26"/>
-      <c r="AAG66" s="26"/>
-      <c r="AAH66" s="26"/>
-      <c r="AAI66" s="26"/>
-      <c r="AAJ66" s="26"/>
-      <c r="AAK66" s="26"/>
-      <c r="AAL66" s="26"/>
-      <c r="AAM66" s="26"/>
-      <c r="AAN66" s="26"/>
-      <c r="AAO66" s="26"/>
-      <c r="AAP66" s="26"/>
-      <c r="AAQ66" s="26"/>
-      <c r="AAR66" s="26"/>
-      <c r="AAS66" s="26"/>
-      <c r="AAT66" s="26"/>
-      <c r="AAU66" s="26"/>
-      <c r="AAV66" s="26"/>
-      <c r="AAW66" s="26"/>
-      <c r="AAX66" s="26"/>
-      <c r="AAY66" s="26"/>
-      <c r="AAZ66" s="26"/>
-      <c r="ABA66" s="26"/>
-      <c r="ABB66" s="26"/>
-      <c r="ABC66" s="26"/>
-      <c r="ABD66" s="26"/>
-      <c r="ABE66" s="26"/>
-      <c r="ABF66" s="26"/>
-      <c r="ABG66" s="26"/>
-      <c r="ABH66" s="26"/>
-      <c r="ABI66" s="26"/>
-      <c r="ABJ66" s="26"/>
-      <c r="ABK66" s="26"/>
-      <c r="ABL66" s="26"/>
-      <c r="ABM66" s="26"/>
-      <c r="ABN66" s="26"/>
-      <c r="ABO66" s="26"/>
-      <c r="ABP66" s="26"/>
-      <c r="ABQ66" s="26"/>
-      <c r="ABR66" s="26"/>
-      <c r="ABS66" s="26"/>
-      <c r="ABT66" s="26"/>
-      <c r="ABU66" s="26"/>
-      <c r="ABV66" s="26"/>
-      <c r="ABW66" s="26"/>
-      <c r="ABX66" s="26"/>
-      <c r="ABY66" s="26"/>
-      <c r="ABZ66" s="26"/>
-      <c r="ACA66" s="26"/>
-      <c r="ACB66" s="26"/>
-      <c r="ACC66" s="26"/>
-      <c r="ACD66" s="26"/>
-      <c r="ACE66" s="26"/>
-      <c r="ACF66" s="26"/>
-      <c r="ACG66" s="26"/>
-      <c r="ACH66" s="26"/>
-      <c r="ACI66" s="26"/>
-      <c r="ACJ66" s="26"/>
-      <c r="ACK66" s="26"/>
-      <c r="ACL66" s="26"/>
-      <c r="ACM66" s="26"/>
-      <c r="ACN66" s="26"/>
-      <c r="ACO66" s="26"/>
-      <c r="ACP66" s="26"/>
-      <c r="ACQ66" s="26"/>
-      <c r="ACR66" s="26"/>
-      <c r="ACS66" s="26"/>
-      <c r="ACT66" s="26"/>
-      <c r="ACU66" s="26"/>
-      <c r="ACV66" s="26"/>
-      <c r="ACW66" s="26"/>
-      <c r="ACX66" s="26"/>
-      <c r="ACY66" s="26"/>
-      <c r="ACZ66" s="26"/>
-      <c r="ADA66" s="26"/>
-      <c r="ADB66" s="26"/>
-      <c r="ADC66" s="26"/>
-      <c r="ADD66" s="26"/>
-      <c r="ADE66" s="26"/>
-      <c r="ADF66" s="26"/>
-      <c r="ADG66" s="26"/>
-      <c r="ADH66" s="26"/>
-      <c r="ADI66" s="26"/>
-      <c r="ADJ66" s="26"/>
-      <c r="ADK66" s="26"/>
-      <c r="ADL66" s="26"/>
-      <c r="ADM66" s="26"/>
-      <c r="ADN66" s="26"/>
-      <c r="ADO66" s="26"/>
-      <c r="ADP66" s="26"/>
-      <c r="ADQ66" s="26"/>
-      <c r="ADR66" s="26"/>
-      <c r="ADS66" s="26"/>
-      <c r="ADT66" s="26"/>
-      <c r="ADU66" s="26"/>
-      <c r="ADV66" s="26"/>
-      <c r="ADW66" s="26"/>
-      <c r="ADX66" s="26"/>
-      <c r="ADY66" s="26"/>
-      <c r="ADZ66" s="26"/>
-      <c r="AEA66" s="26"/>
-      <c r="AEB66" s="26"/>
-      <c r="AEC66" s="26"/>
-      <c r="AED66" s="26"/>
-      <c r="AEE66" s="26"/>
-      <c r="AEF66" s="26"/>
-      <c r="AEG66" s="26"/>
-      <c r="AEH66" s="26"/>
-      <c r="AEI66" s="26"/>
-      <c r="AEJ66" s="26"/>
-      <c r="AEK66" s="26"/>
-      <c r="AEL66" s="26"/>
-      <c r="AEM66" s="26"/>
-      <c r="AEN66" s="26"/>
-      <c r="AEO66" s="26"/>
-      <c r="AEP66" s="26"/>
-      <c r="AEQ66" s="26"/>
-      <c r="AER66" s="26"/>
-      <c r="AES66" s="26"/>
-      <c r="AET66" s="26"/>
-      <c r="AEU66" s="26"/>
-      <c r="AEV66" s="26"/>
-      <c r="AEW66" s="26"/>
-      <c r="AEX66" s="26"/>
-      <c r="AEY66" s="26"/>
-      <c r="AEZ66" s="26"/>
-      <c r="AFA66" s="26"/>
-      <c r="AFB66" s="26"/>
-      <c r="AFC66" s="26"/>
-      <c r="AFD66" s="26"/>
-      <c r="AFE66" s="26"/>
-      <c r="AFF66" s="26"/>
-      <c r="AFG66" s="26"/>
-      <c r="AFH66" s="26"/>
-      <c r="AFI66" s="26"/>
-      <c r="AFJ66" s="26"/>
-      <c r="AFK66" s="26"/>
-      <c r="AFL66" s="26"/>
-      <c r="AFM66" s="26"/>
-      <c r="AFN66" s="26"/>
-      <c r="AFO66" s="26"/>
-      <c r="AFP66" s="26"/>
-      <c r="AFQ66" s="26"/>
-      <c r="AFR66" s="26"/>
-      <c r="AFS66" s="26"/>
-      <c r="AFT66" s="26"/>
-      <c r="AFU66" s="26"/>
-      <c r="AFV66" s="26"/>
-      <c r="AFW66" s="26"/>
-      <c r="AFX66" s="26"/>
-      <c r="AFY66" s="26"/>
-      <c r="AFZ66" s="26"/>
-      <c r="AGA66" s="26"/>
-      <c r="AGB66" s="26"/>
-      <c r="AGC66" s="26"/>
-      <c r="AGD66" s="26"/>
-      <c r="AGE66" s="26"/>
-      <c r="AGF66" s="26"/>
-      <c r="AGG66" s="26"/>
-      <c r="AGH66" s="26"/>
-      <c r="AGI66" s="26"/>
-      <c r="AGJ66" s="26"/>
-      <c r="AGK66" s="26"/>
-      <c r="AGL66" s="26"/>
-      <c r="AGM66" s="26"/>
-      <c r="AGN66" s="26"/>
-      <c r="AGO66" s="26"/>
-      <c r="AGP66" s="26"/>
-      <c r="AGQ66" s="26"/>
-      <c r="AGR66" s="26"/>
-      <c r="AGS66" s="26"/>
-      <c r="AGT66" s="26"/>
-      <c r="AGU66" s="26"/>
-      <c r="AGV66" s="26"/>
-      <c r="AGW66" s="26"/>
-      <c r="AGX66" s="26"/>
-      <c r="AGY66" s="26"/>
-      <c r="AGZ66" s="26"/>
-      <c r="AHA66" s="26"/>
-      <c r="AHB66" s="26"/>
-      <c r="AHC66" s="26"/>
-      <c r="AHD66" s="26"/>
-      <c r="AHE66" s="26"/>
-      <c r="AHF66" s="26"/>
-      <c r="AHG66" s="26"/>
-      <c r="AHH66" s="26"/>
-      <c r="AHI66" s="26"/>
-      <c r="AHJ66" s="26"/>
-      <c r="AHK66" s="26"/>
-      <c r="AHL66" s="26"/>
-      <c r="AHM66" s="26"/>
-      <c r="AHN66" s="26"/>
-      <c r="AHO66" s="26"/>
-      <c r="AHP66" s="26"/>
-      <c r="AHQ66" s="26"/>
-      <c r="AHR66" s="26"/>
-      <c r="AHS66" s="26"/>
-      <c r="AHT66" s="26"/>
-      <c r="AHU66" s="26"/>
-      <c r="AHV66" s="26"/>
-      <c r="AHW66" s="26"/>
-      <c r="AHX66" s="26"/>
-      <c r="AHY66" s="26"/>
-      <c r="AHZ66" s="26"/>
-      <c r="AIA66" s="26"/>
-      <c r="AIB66" s="26"/>
-      <c r="AIC66" s="26"/>
-      <c r="AID66" s="26"/>
-      <c r="AIE66" s="26"/>
-      <c r="AIF66" s="26"/>
-      <c r="AIG66" s="26"/>
-      <c r="AIH66" s="26"/>
-      <c r="AII66" s="26"/>
-      <c r="AIJ66" s="26"/>
-      <c r="AIK66" s="26"/>
-      <c r="AIL66" s="26"/>
-      <c r="AIM66" s="26"/>
-      <c r="AIN66" s="26"/>
-      <c r="AIO66" s="26"/>
-      <c r="AIP66" s="26"/>
-      <c r="AIQ66" s="26"/>
-      <c r="AIR66" s="26"/>
-      <c r="AIS66" s="26"/>
-      <c r="AIT66" s="26"/>
-      <c r="AIU66" s="26"/>
-      <c r="AIV66" s="26"/>
-      <c r="AIW66" s="26"/>
-      <c r="AIX66" s="26"/>
-      <c r="AIY66" s="26"/>
-      <c r="AIZ66" s="26"/>
-      <c r="AJA66" s="26"/>
-      <c r="AJB66" s="26"/>
-      <c r="AJC66" s="26"/>
-      <c r="AJD66" s="26"/>
-      <c r="AJE66" s="26"/>
-      <c r="AJF66" s="26"/>
-      <c r="AJG66" s="26"/>
-      <c r="AJH66" s="26"/>
-      <c r="AJI66" s="26"/>
-      <c r="AJJ66" s="26"/>
-      <c r="AJK66" s="26"/>
-      <c r="AJL66" s="26"/>
-      <c r="AJM66" s="26"/>
-      <c r="AJN66" s="26"/>
-      <c r="AJO66" s="26"/>
-      <c r="AJP66" s="26"/>
-      <c r="AJQ66" s="26"/>
-      <c r="AJR66" s="26"/>
-      <c r="AJS66" s="26"/>
-      <c r="AJT66" s="26"/>
-      <c r="AJU66" s="26"/>
-      <c r="AJV66" s="26"/>
-      <c r="AJW66" s="26"/>
-      <c r="AJX66" s="26"/>
-      <c r="AJY66" s="26"/>
-      <c r="AJZ66" s="26"/>
-      <c r="AKA66" s="26"/>
-      <c r="AKB66" s="26"/>
-      <c r="AKC66" s="26"/>
-      <c r="AKD66" s="26"/>
-      <c r="AKE66" s="26"/>
-      <c r="AKF66" s="26"/>
-      <c r="AKG66" s="26"/>
-      <c r="AKH66" s="26"/>
-      <c r="AKI66" s="26"/>
-      <c r="AKJ66" s="26"/>
-      <c r="AKK66" s="26"/>
-      <c r="AKL66" s="26"/>
-      <c r="AKM66" s="26"/>
-      <c r="AKN66" s="26"/>
-      <c r="AKO66" s="26"/>
-      <c r="AKP66" s="26"/>
-      <c r="AKQ66" s="26"/>
-      <c r="AKR66" s="26"/>
-      <c r="AKS66" s="26"/>
-      <c r="AKT66" s="26"/>
-      <c r="AKU66" s="26"/>
-      <c r="AKV66" s="26"/>
-      <c r="AKW66" s="26"/>
-      <c r="AKX66" s="26"/>
-      <c r="AKY66" s="26"/>
-      <c r="AKZ66" s="26"/>
-      <c r="ALA66" s="26"/>
-      <c r="ALB66" s="26"/>
-      <c r="ALC66" s="26"/>
-      <c r="ALD66" s="26"/>
-      <c r="ALE66" s="26"/>
-      <c r="ALF66" s="26"/>
-      <c r="ALG66" s="26"/>
-      <c r="ALH66" s="26"/>
-      <c r="ALI66" s="26"/>
-      <c r="ALJ66" s="26"/>
-      <c r="ALK66" s="26"/>
-      <c r="ALL66" s="26"/>
-      <c r="ALM66" s="26"/>
-      <c r="ALN66" s="26"/>
-      <c r="ALO66" s="26"/>
-      <c r="ALP66" s="26"/>
-      <c r="ALQ66" s="26"/>
-      <c r="ALR66" s="26"/>
-      <c r="ALS66" s="26"/>
-      <c r="ALT66" s="26"/>
-      <c r="ALU66" s="26"/>
-      <c r="ALV66" s="26"/>
-      <c r="ALW66" s="26"/>
-      <c r="ALX66" s="26"/>
-      <c r="ALY66" s="26"/>
-      <c r="ALZ66" s="26"/>
-      <c r="AMA66" s="26"/>
-      <c r="AMB66" s="26"/>
-      <c r="AMC66" s="26"/>
-      <c r="AMD66" s="26"/>
-      <c r="AME66" s="26"/>
-      <c r="AMF66" s="26"/>
-      <c r="AMG66" s="26"/>
-      <c r="AMH66" s="26"/>
-      <c r="AMI66" s="26"/>
-      <c r="AMJ66" s="26"/>
-      <c r="AMK66" s="26"/>
-    </row>
-    <row r="67" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="B67" s="33" t="s">
+      <c r="C67" s="33"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
+      <c r="H67" s="26"/>
+      <c r="I67" s="26"/>
+      <c r="J67" s="26"/>
+      <c r="K67" s="26"/>
+      <c r="L67" s="26"/>
+      <c r="M67" s="26"/>
+      <c r="N67" s="26"/>
+      <c r="O67" s="26"/>
+      <c r="P67" s="26"/>
+      <c r="Q67" s="26"/>
+      <c r="R67" s="26"/>
+      <c r="S67" s="26"/>
+      <c r="T67" s="26"/>
+      <c r="U67" s="26"/>
+      <c r="V67" s="26"/>
+      <c r="W67" s="26"/>
+      <c r="X67" s="26"/>
+      <c r="Y67" s="26"/>
+      <c r="Z67" s="26"/>
+      <c r="AA67" s="26"/>
+      <c r="AB67" s="26"/>
+      <c r="AC67" s="26"/>
+      <c r="AD67" s="26"/>
+      <c r="AE67" s="26"/>
+      <c r="AF67" s="26"/>
+      <c r="AG67" s="26"/>
+      <c r="AH67" s="26"/>
+      <c r="AI67" s="26"/>
+      <c r="AJ67" s="26"/>
+      <c r="AK67" s="26"/>
+      <c r="AL67" s="26"/>
+      <c r="AM67" s="26"/>
+      <c r="AN67" s="26"/>
+      <c r="AO67" s="26"/>
+      <c r="AP67" s="26"/>
+      <c r="AQ67" s="26"/>
+      <c r="AR67" s="26"/>
+      <c r="AS67" s="26"/>
+      <c r="AT67" s="26"/>
+      <c r="AU67" s="26"/>
+      <c r="AV67" s="26"/>
+      <c r="AW67" s="26"/>
+      <c r="AX67" s="26"/>
+      <c r="AY67" s="26"/>
+      <c r="AZ67" s="26"/>
+      <c r="BA67" s="26"/>
+      <c r="BB67" s="26"/>
+      <c r="BC67" s="26"/>
+      <c r="BD67" s="26"/>
+      <c r="BE67" s="26"/>
+      <c r="BF67" s="26"/>
+      <c r="BG67" s="26"/>
+      <c r="BH67" s="26"/>
+      <c r="BI67" s="26"/>
+      <c r="BJ67" s="26"/>
+      <c r="BK67" s="26"/>
+      <c r="BL67" s="26"/>
+      <c r="BM67" s="26"/>
+      <c r="BN67" s="26"/>
+      <c r="BO67" s="26"/>
+      <c r="BP67" s="26"/>
+      <c r="BQ67" s="26"/>
+      <c r="BR67" s="26"/>
+      <c r="BS67" s="26"/>
+      <c r="BT67" s="26"/>
+      <c r="BU67" s="26"/>
+      <c r="BV67" s="26"/>
+      <c r="BW67" s="26"/>
+      <c r="BX67" s="26"/>
+      <c r="BY67" s="26"/>
+      <c r="BZ67" s="26"/>
+      <c r="CA67" s="26"/>
+      <c r="CB67" s="26"/>
+      <c r="CC67" s="26"/>
+      <c r="CD67" s="26"/>
+      <c r="CE67" s="26"/>
+      <c r="CF67" s="26"/>
+      <c r="CG67" s="26"/>
+      <c r="CH67" s="26"/>
+      <c r="CI67" s="26"/>
+      <c r="CJ67" s="26"/>
+      <c r="CK67" s="26"/>
+      <c r="CL67" s="26"/>
+      <c r="CM67" s="26"/>
+      <c r="CN67" s="26"/>
+      <c r="CO67" s="26"/>
+      <c r="CP67" s="26"/>
+      <c r="CQ67" s="26"/>
+      <c r="CR67" s="26"/>
+      <c r="CS67" s="26"/>
+      <c r="CT67" s="26"/>
+      <c r="CU67" s="26"/>
+      <c r="CV67" s="26"/>
+      <c r="CW67" s="26"/>
+      <c r="CX67" s="26"/>
+      <c r="CY67" s="26"/>
+      <c r="CZ67" s="26"/>
+      <c r="DA67" s="26"/>
+      <c r="DB67" s="26"/>
+      <c r="DC67" s="26"/>
+      <c r="DD67" s="26"/>
+      <c r="DE67" s="26"/>
+      <c r="DF67" s="26"/>
+      <c r="DG67" s="26"/>
+      <c r="DH67" s="26"/>
+      <c r="DI67" s="26"/>
+      <c r="DJ67" s="26"/>
+      <c r="DK67" s="26"/>
+      <c r="DL67" s="26"/>
+      <c r="DM67" s="26"/>
+      <c r="DN67" s="26"/>
+      <c r="DO67" s="26"/>
+      <c r="DP67" s="26"/>
+      <c r="DQ67" s="26"/>
+      <c r="DR67" s="26"/>
+      <c r="DS67" s="26"/>
+      <c r="DT67" s="26"/>
+      <c r="DU67" s="26"/>
+      <c r="DV67" s="26"/>
+      <c r="DW67" s="26"/>
+      <c r="DX67" s="26"/>
+      <c r="DY67" s="26"/>
+      <c r="DZ67" s="26"/>
+      <c r="EA67" s="26"/>
+      <c r="EB67" s="26"/>
+      <c r="EC67" s="26"/>
+      <c r="ED67" s="26"/>
+      <c r="EE67" s="26"/>
+      <c r="EF67" s="26"/>
+      <c r="EG67" s="26"/>
+      <c r="EH67" s="26"/>
+      <c r="EI67" s="26"/>
+      <c r="EJ67" s="26"/>
+      <c r="EK67" s="26"/>
+      <c r="EL67" s="26"/>
+      <c r="EM67" s="26"/>
+      <c r="EN67" s="26"/>
+      <c r="EO67" s="26"/>
+      <c r="EP67" s="26"/>
+      <c r="EQ67" s="26"/>
+      <c r="ER67" s="26"/>
+      <c r="ES67" s="26"/>
+      <c r="ET67" s="26"/>
+      <c r="EU67" s="26"/>
+      <c r="EV67" s="26"/>
+      <c r="EW67" s="26"/>
+      <c r="EX67" s="26"/>
+      <c r="EY67" s="26"/>
+      <c r="EZ67" s="26"/>
+      <c r="FA67" s="26"/>
+      <c r="FB67" s="26"/>
+      <c r="FC67" s="26"/>
+      <c r="FD67" s="26"/>
+      <c r="FE67" s="26"/>
+      <c r="FF67" s="26"/>
+      <c r="FG67" s="26"/>
+      <c r="FH67" s="26"/>
+      <c r="FI67" s="26"/>
+      <c r="FJ67" s="26"/>
+      <c r="FK67" s="26"/>
+      <c r="FL67" s="26"/>
+      <c r="FM67" s="26"/>
+      <c r="FN67" s="26"/>
+      <c r="FO67" s="26"/>
+      <c r="FP67" s="26"/>
+      <c r="FQ67" s="26"/>
+      <c r="FR67" s="26"/>
+      <c r="FS67" s="26"/>
+      <c r="FT67" s="26"/>
+      <c r="FU67" s="26"/>
+      <c r="FV67" s="26"/>
+      <c r="FW67" s="26"/>
+      <c r="FX67" s="26"/>
+      <c r="FY67" s="26"/>
+      <c r="FZ67" s="26"/>
+      <c r="GA67" s="26"/>
+      <c r="GB67" s="26"/>
+      <c r="GC67" s="26"/>
+      <c r="GD67" s="26"/>
+      <c r="GE67" s="26"/>
+      <c r="GF67" s="26"/>
+      <c r="GG67" s="26"/>
+      <c r="GH67" s="26"/>
+      <c r="GI67" s="26"/>
+      <c r="GJ67" s="26"/>
+      <c r="GK67" s="26"/>
+      <c r="GL67" s="26"/>
+      <c r="GM67" s="26"/>
+      <c r="GN67" s="26"/>
+      <c r="GO67" s="26"/>
+      <c r="GP67" s="26"/>
+      <c r="GQ67" s="26"/>
+      <c r="GR67" s="26"/>
+      <c r="GS67" s="26"/>
+      <c r="GT67" s="26"/>
+      <c r="GU67" s="26"/>
+      <c r="GV67" s="26"/>
+      <c r="GW67" s="26"/>
+      <c r="GX67" s="26"/>
+      <c r="GY67" s="26"/>
+      <c r="GZ67" s="26"/>
+      <c r="HA67" s="26"/>
+      <c r="HB67" s="26"/>
+      <c r="HC67" s="26"/>
+      <c r="HD67" s="26"/>
+      <c r="HE67" s="26"/>
+      <c r="HF67" s="26"/>
+      <c r="HG67" s="26"/>
+      <c r="HH67" s="26"/>
+      <c r="HI67" s="26"/>
+      <c r="HJ67" s="26"/>
+      <c r="HK67" s="26"/>
+      <c r="HL67" s="26"/>
+      <c r="HM67" s="26"/>
+      <c r="HN67" s="26"/>
+      <c r="HO67" s="26"/>
+      <c r="HP67" s="26"/>
+      <c r="HQ67" s="26"/>
+      <c r="HR67" s="26"/>
+      <c r="HS67" s="26"/>
+      <c r="HT67" s="26"/>
+      <c r="HU67" s="26"/>
+      <c r="HV67" s="26"/>
+      <c r="HW67" s="26"/>
+      <c r="HX67" s="26"/>
+      <c r="HY67" s="26"/>
+      <c r="HZ67" s="26"/>
+      <c r="IA67" s="26"/>
+      <c r="IB67" s="26"/>
+      <c r="IC67" s="26"/>
+      <c r="ID67" s="26"/>
+      <c r="IE67" s="26"/>
+      <c r="IF67" s="26"/>
+      <c r="IG67" s="26"/>
+      <c r="IH67" s="26"/>
+      <c r="II67" s="26"/>
+      <c r="IJ67" s="26"/>
+      <c r="IK67" s="26"/>
+      <c r="IL67" s="26"/>
+      <c r="IM67" s="26"/>
+      <c r="IN67" s="26"/>
+      <c r="IO67" s="26"/>
+      <c r="IP67" s="26"/>
+      <c r="IQ67" s="26"/>
+      <c r="IR67" s="26"/>
+      <c r="IS67" s="26"/>
+      <c r="IT67" s="26"/>
+      <c r="IU67" s="26"/>
+      <c r="IV67" s="26"/>
+      <c r="IW67" s="26"/>
+      <c r="IX67" s="26"/>
+      <c r="IY67" s="26"/>
+      <c r="IZ67" s="26"/>
+      <c r="JA67" s="26"/>
+      <c r="JB67" s="26"/>
+      <c r="JC67" s="26"/>
+      <c r="JD67" s="26"/>
+      <c r="JE67" s="26"/>
+      <c r="JF67" s="26"/>
+      <c r="JG67" s="26"/>
+      <c r="JH67" s="26"/>
+      <c r="JI67" s="26"/>
+      <c r="JJ67" s="26"/>
+      <c r="JK67" s="26"/>
+      <c r="JL67" s="26"/>
+      <c r="JM67" s="26"/>
+      <c r="JN67" s="26"/>
+      <c r="JO67" s="26"/>
+      <c r="JP67" s="26"/>
+      <c r="JQ67" s="26"/>
+      <c r="JR67" s="26"/>
+      <c r="JS67" s="26"/>
+      <c r="JT67" s="26"/>
+      <c r="JU67" s="26"/>
+      <c r="JV67" s="26"/>
+      <c r="JW67" s="26"/>
+      <c r="JX67" s="26"/>
+      <c r="JY67" s="26"/>
+      <c r="JZ67" s="26"/>
+      <c r="KA67" s="26"/>
+      <c r="KB67" s="26"/>
+      <c r="KC67" s="26"/>
+      <c r="KD67" s="26"/>
+      <c r="KE67" s="26"/>
+      <c r="KF67" s="26"/>
+      <c r="KG67" s="26"/>
+      <c r="KH67" s="26"/>
+      <c r="KI67" s="26"/>
+      <c r="KJ67" s="26"/>
+      <c r="KK67" s="26"/>
+      <c r="KL67" s="26"/>
+      <c r="KM67" s="26"/>
+      <c r="KN67" s="26"/>
+      <c r="KO67" s="26"/>
+      <c r="KP67" s="26"/>
+      <c r="KQ67" s="26"/>
+      <c r="KR67" s="26"/>
+      <c r="KS67" s="26"/>
+      <c r="KT67" s="26"/>
+      <c r="KU67" s="26"/>
+      <c r="KV67" s="26"/>
+      <c r="KW67" s="26"/>
+      <c r="KX67" s="26"/>
+      <c r="KY67" s="26"/>
+      <c r="KZ67" s="26"/>
+      <c r="LA67" s="26"/>
+      <c r="LB67" s="26"/>
+      <c r="LC67" s="26"/>
+      <c r="LD67" s="26"/>
+      <c r="LE67" s="26"/>
+      <c r="LF67" s="26"/>
+      <c r="LG67" s="26"/>
+      <c r="LH67" s="26"/>
+      <c r="LI67" s="26"/>
+      <c r="LJ67" s="26"/>
+      <c r="LK67" s="26"/>
+      <c r="LL67" s="26"/>
+      <c r="LM67" s="26"/>
+      <c r="LN67" s="26"/>
+      <c r="LO67" s="26"/>
+      <c r="LP67" s="26"/>
+      <c r="LQ67" s="26"/>
+      <c r="LR67" s="26"/>
+      <c r="LS67" s="26"/>
+      <c r="LT67" s="26"/>
+      <c r="LU67" s="26"/>
+      <c r="LV67" s="26"/>
+      <c r="LW67" s="26"/>
+      <c r="LX67" s="26"/>
+      <c r="LY67" s="26"/>
+      <c r="LZ67" s="26"/>
+      <c r="MA67" s="26"/>
+      <c r="MB67" s="26"/>
+      <c r="MC67" s="26"/>
+      <c r="MD67" s="26"/>
+      <c r="ME67" s="26"/>
+      <c r="MF67" s="26"/>
+      <c r="MG67" s="26"/>
+      <c r="MH67" s="26"/>
+      <c r="MI67" s="26"/>
+      <c r="MJ67" s="26"/>
+      <c r="MK67" s="26"/>
+      <c r="ML67" s="26"/>
+      <c r="MM67" s="26"/>
+      <c r="MN67" s="26"/>
+      <c r="MO67" s="26"/>
+      <c r="MP67" s="26"/>
+      <c r="MQ67" s="26"/>
+      <c r="MR67" s="26"/>
+      <c r="MS67" s="26"/>
+      <c r="MT67" s="26"/>
+      <c r="MU67" s="26"/>
+      <c r="MV67" s="26"/>
+      <c r="MW67" s="26"/>
+      <c r="MX67" s="26"/>
+      <c r="MY67" s="26"/>
+      <c r="MZ67" s="26"/>
+      <c r="NA67" s="26"/>
+      <c r="NB67" s="26"/>
+      <c r="NC67" s="26"/>
+      <c r="ND67" s="26"/>
+      <c r="NE67" s="26"/>
+      <c r="NF67" s="26"/>
+      <c r="NG67" s="26"/>
+      <c r="NH67" s="26"/>
+      <c r="NI67" s="26"/>
+      <c r="NJ67" s="26"/>
+      <c r="NK67" s="26"/>
+      <c r="NL67" s="26"/>
+      <c r="NM67" s="26"/>
+      <c r="NN67" s="26"/>
+      <c r="NO67" s="26"/>
+      <c r="NP67" s="26"/>
+      <c r="NQ67" s="26"/>
+      <c r="NR67" s="26"/>
+      <c r="NS67" s="26"/>
+      <c r="NT67" s="26"/>
+      <c r="NU67" s="26"/>
+      <c r="NV67" s="26"/>
+      <c r="NW67" s="26"/>
+      <c r="NX67" s="26"/>
+      <c r="NY67" s="26"/>
+      <c r="NZ67" s="26"/>
+      <c r="OA67" s="26"/>
+      <c r="OB67" s="26"/>
+      <c r="OC67" s="26"/>
+      <c r="OD67" s="26"/>
+      <c r="OE67" s="26"/>
+      <c r="OF67" s="26"/>
+      <c r="OG67" s="26"/>
+      <c r="OH67" s="26"/>
+      <c r="OI67" s="26"/>
+      <c r="OJ67" s="26"/>
+      <c r="OK67" s="26"/>
+      <c r="OL67" s="26"/>
+      <c r="OM67" s="26"/>
+      <c r="ON67" s="26"/>
+      <c r="OO67" s="26"/>
+      <c r="OP67" s="26"/>
+      <c r="OQ67" s="26"/>
+      <c r="OR67" s="26"/>
+      <c r="OS67" s="26"/>
+      <c r="OT67" s="26"/>
+      <c r="OU67" s="26"/>
+      <c r="OV67" s="26"/>
+      <c r="OW67" s="26"/>
+      <c r="OX67" s="26"/>
+      <c r="OY67" s="26"/>
+      <c r="OZ67" s="26"/>
+      <c r="PA67" s="26"/>
+      <c r="PB67" s="26"/>
+      <c r="PC67" s="26"/>
+      <c r="PD67" s="26"/>
+      <c r="PE67" s="26"/>
+      <c r="PF67" s="26"/>
+      <c r="PG67" s="26"/>
+      <c r="PH67" s="26"/>
+      <c r="PI67" s="26"/>
+      <c r="PJ67" s="26"/>
+      <c r="PK67" s="26"/>
+      <c r="PL67" s="26"/>
+      <c r="PM67" s="26"/>
+      <c r="PN67" s="26"/>
+      <c r="PO67" s="26"/>
+      <c r="PP67" s="26"/>
+      <c r="PQ67" s="26"/>
+      <c r="PR67" s="26"/>
+      <c r="PS67" s="26"/>
+      <c r="PT67" s="26"/>
+      <c r="PU67" s="26"/>
+      <c r="PV67" s="26"/>
+      <c r="PW67" s="26"/>
+      <c r="PX67" s="26"/>
+      <c r="PY67" s="26"/>
+      <c r="PZ67" s="26"/>
+      <c r="QA67" s="26"/>
+      <c r="QB67" s="26"/>
+      <c r="QC67" s="26"/>
+      <c r="QD67" s="26"/>
+      <c r="QE67" s="26"/>
+      <c r="QF67" s="26"/>
+      <c r="QG67" s="26"/>
+      <c r="QH67" s="26"/>
+      <c r="QI67" s="26"/>
+      <c r="QJ67" s="26"/>
+      <c r="QK67" s="26"/>
+      <c r="QL67" s="26"/>
+      <c r="QM67" s="26"/>
+      <c r="QN67" s="26"/>
+      <c r="QO67" s="26"/>
+      <c r="QP67" s="26"/>
+      <c r="QQ67" s="26"/>
+      <c r="QR67" s="26"/>
+      <c r="QS67" s="26"/>
+      <c r="QT67" s="26"/>
+      <c r="QU67" s="26"/>
+      <c r="QV67" s="26"/>
+      <c r="QW67" s="26"/>
+      <c r="QX67" s="26"/>
+      <c r="QY67" s="26"/>
+      <c r="QZ67" s="26"/>
+      <c r="RA67" s="26"/>
+      <c r="RB67" s="26"/>
+      <c r="RC67" s="26"/>
+      <c r="RD67" s="26"/>
+      <c r="RE67" s="26"/>
+      <c r="RF67" s="26"/>
+      <c r="RG67" s="26"/>
+      <c r="RH67" s="26"/>
+      <c r="RI67" s="26"/>
+      <c r="RJ67" s="26"/>
+      <c r="RK67" s="26"/>
+      <c r="RL67" s="26"/>
+      <c r="RM67" s="26"/>
+      <c r="RN67" s="26"/>
+      <c r="RO67" s="26"/>
+      <c r="RP67" s="26"/>
+      <c r="RQ67" s="26"/>
+      <c r="RR67" s="26"/>
+      <c r="RS67" s="26"/>
+      <c r="RT67" s="26"/>
+      <c r="RU67" s="26"/>
+      <c r="RV67" s="26"/>
+      <c r="RW67" s="26"/>
+      <c r="RX67" s="26"/>
+      <c r="RY67" s="26"/>
+      <c r="RZ67" s="26"/>
+      <c r="SA67" s="26"/>
+      <c r="SB67" s="26"/>
+      <c r="SC67" s="26"/>
+      <c r="SD67" s="26"/>
+      <c r="SE67" s="26"/>
+      <c r="SF67" s="26"/>
+      <c r="SG67" s="26"/>
+      <c r="SH67" s="26"/>
+      <c r="SI67" s="26"/>
+      <c r="SJ67" s="26"/>
+      <c r="SK67" s="26"/>
+      <c r="SL67" s="26"/>
+      <c r="SM67" s="26"/>
+      <c r="SN67" s="26"/>
+      <c r="SO67" s="26"/>
+      <c r="SP67" s="26"/>
+      <c r="SQ67" s="26"/>
+      <c r="SR67" s="26"/>
+      <c r="SS67" s="26"/>
+      <c r="ST67" s="26"/>
+      <c r="SU67" s="26"/>
+      <c r="SV67" s="26"/>
+      <c r="SW67" s="26"/>
+      <c r="SX67" s="26"/>
+      <c r="SY67" s="26"/>
+      <c r="SZ67" s="26"/>
+      <c r="TA67" s="26"/>
+      <c r="TB67" s="26"/>
+      <c r="TC67" s="26"/>
+      <c r="TD67" s="26"/>
+      <c r="TE67" s="26"/>
+      <c r="TF67" s="26"/>
+      <c r="TG67" s="26"/>
+      <c r="TH67" s="26"/>
+      <c r="TI67" s="26"/>
+      <c r="TJ67" s="26"/>
+      <c r="TK67" s="26"/>
+      <c r="TL67" s="26"/>
+      <c r="TM67" s="26"/>
+      <c r="TN67" s="26"/>
+      <c r="TO67" s="26"/>
+      <c r="TP67" s="26"/>
+      <c r="TQ67" s="26"/>
+      <c r="TR67" s="26"/>
+      <c r="TS67" s="26"/>
+      <c r="TT67" s="26"/>
+      <c r="TU67" s="26"/>
+      <c r="TV67" s="26"/>
+      <c r="TW67" s="26"/>
+      <c r="TX67" s="26"/>
+      <c r="TY67" s="26"/>
+      <c r="TZ67" s="26"/>
+      <c r="UA67" s="26"/>
+      <c r="UB67" s="26"/>
+      <c r="UC67" s="26"/>
+      <c r="UD67" s="26"/>
+      <c r="UE67" s="26"/>
+      <c r="UF67" s="26"/>
+      <c r="UG67" s="26"/>
+      <c r="UH67" s="26"/>
+      <c r="UI67" s="26"/>
+      <c r="UJ67" s="26"/>
+      <c r="UK67" s="26"/>
+      <c r="UL67" s="26"/>
+      <c r="UM67" s="26"/>
+      <c r="UN67" s="26"/>
+      <c r="UO67" s="26"/>
+      <c r="UP67" s="26"/>
+      <c r="UQ67" s="26"/>
+      <c r="UR67" s="26"/>
+      <c r="US67" s="26"/>
+      <c r="UT67" s="26"/>
+      <c r="UU67" s="26"/>
+      <c r="UV67" s="26"/>
+      <c r="UW67" s="26"/>
+      <c r="UX67" s="26"/>
+      <c r="UY67" s="26"/>
+      <c r="UZ67" s="26"/>
+      <c r="VA67" s="26"/>
+      <c r="VB67" s="26"/>
+      <c r="VC67" s="26"/>
+      <c r="VD67" s="26"/>
+      <c r="VE67" s="26"/>
+      <c r="VF67" s="26"/>
+      <c r="VG67" s="26"/>
+      <c r="VH67" s="26"/>
+      <c r="VI67" s="26"/>
+      <c r="VJ67" s="26"/>
+      <c r="VK67" s="26"/>
+      <c r="VL67" s="26"/>
+      <c r="VM67" s="26"/>
+      <c r="VN67" s="26"/>
+      <c r="VO67" s="26"/>
+      <c r="VP67" s="26"/>
+      <c r="VQ67" s="26"/>
+      <c r="VR67" s="26"/>
+      <c r="VS67" s="26"/>
+      <c r="VT67" s="26"/>
+      <c r="VU67" s="26"/>
+      <c r="VV67" s="26"/>
+      <c r="VW67" s="26"/>
+      <c r="VX67" s="26"/>
+      <c r="VY67" s="26"/>
+      <c r="VZ67" s="26"/>
+      <c r="WA67" s="26"/>
+      <c r="WB67" s="26"/>
+      <c r="WC67" s="26"/>
+      <c r="WD67" s="26"/>
+      <c r="WE67" s="26"/>
+      <c r="WF67" s="26"/>
+      <c r="WG67" s="26"/>
+      <c r="WH67" s="26"/>
+      <c r="WI67" s="26"/>
+      <c r="WJ67" s="26"/>
+      <c r="WK67" s="26"/>
+      <c r="WL67" s="26"/>
+      <c r="WM67" s="26"/>
+      <c r="WN67" s="26"/>
+      <c r="WO67" s="26"/>
+      <c r="WP67" s="26"/>
+      <c r="WQ67" s="26"/>
+      <c r="WR67" s="26"/>
+      <c r="WS67" s="26"/>
+      <c r="WT67" s="26"/>
+      <c r="WU67" s="26"/>
+      <c r="WV67" s="26"/>
+      <c r="WW67" s="26"/>
+      <c r="WX67" s="26"/>
+      <c r="WY67" s="26"/>
+      <c r="WZ67" s="26"/>
+      <c r="XA67" s="26"/>
+      <c r="XB67" s="26"/>
+      <c r="XC67" s="26"/>
+      <c r="XD67" s="26"/>
+      <c r="XE67" s="26"/>
+      <c r="XF67" s="26"/>
+      <c r="XG67" s="26"/>
+      <c r="XH67" s="26"/>
+      <c r="XI67" s="26"/>
+      <c r="XJ67" s="26"/>
+      <c r="XK67" s="26"/>
+      <c r="XL67" s="26"/>
+      <c r="XM67" s="26"/>
+      <c r="XN67" s="26"/>
+      <c r="XO67" s="26"/>
+      <c r="XP67" s="26"/>
+      <c r="XQ67" s="26"/>
+      <c r="XR67" s="26"/>
+      <c r="XS67" s="26"/>
+      <c r="XT67" s="26"/>
+      <c r="XU67" s="26"/>
+      <c r="XV67" s="26"/>
+      <c r="XW67" s="26"/>
+      <c r="XX67" s="26"/>
+      <c r="XY67" s="26"/>
+      <c r="XZ67" s="26"/>
+      <c r="YA67" s="26"/>
+      <c r="YB67" s="26"/>
+      <c r="YC67" s="26"/>
+      <c r="YD67" s="26"/>
+      <c r="YE67" s="26"/>
+      <c r="YF67" s="26"/>
+      <c r="YG67" s="26"/>
+      <c r="YH67" s="26"/>
+      <c r="YI67" s="26"/>
+      <c r="YJ67" s="26"/>
+      <c r="YK67" s="26"/>
+      <c r="YL67" s="26"/>
+      <c r="YM67" s="26"/>
+      <c r="YN67" s="26"/>
+      <c r="YO67" s="26"/>
+      <c r="YP67" s="26"/>
+      <c r="YQ67" s="26"/>
+      <c r="YR67" s="26"/>
+      <c r="YS67" s="26"/>
+      <c r="YT67" s="26"/>
+      <c r="YU67" s="26"/>
+      <c r="YV67" s="26"/>
+      <c r="YW67" s="26"/>
+      <c r="YX67" s="26"/>
+      <c r="YY67" s="26"/>
+      <c r="YZ67" s="26"/>
+      <c r="ZA67" s="26"/>
+      <c r="ZB67" s="26"/>
+      <c r="ZC67" s="26"/>
+      <c r="ZD67" s="26"/>
+      <c r="ZE67" s="26"/>
+      <c r="ZF67" s="26"/>
+      <c r="ZG67" s="26"/>
+      <c r="ZH67" s="26"/>
+      <c r="ZI67" s="26"/>
+      <c r="ZJ67" s="26"/>
+      <c r="ZK67" s="26"/>
+      <c r="ZL67" s="26"/>
+      <c r="ZM67" s="26"/>
+      <c r="ZN67" s="26"/>
+      <c r="ZO67" s="26"/>
+      <c r="ZP67" s="26"/>
+      <c r="ZQ67" s="26"/>
+      <c r="ZR67" s="26"/>
+      <c r="ZS67" s="26"/>
+      <c r="ZT67" s="26"/>
+      <c r="ZU67" s="26"/>
+      <c r="ZV67" s="26"/>
+      <c r="ZW67" s="26"/>
+      <c r="ZX67" s="26"/>
+      <c r="ZY67" s="26"/>
+      <c r="ZZ67" s="26"/>
+      <c r="AAA67" s="26"/>
+      <c r="AAB67" s="26"/>
+      <c r="AAC67" s="26"/>
+      <c r="AAD67" s="26"/>
+      <c r="AAE67" s="26"/>
+      <c r="AAF67" s="26"/>
+      <c r="AAG67" s="26"/>
+      <c r="AAH67" s="26"/>
+      <c r="AAI67" s="26"/>
+      <c r="AAJ67" s="26"/>
+      <c r="AAK67" s="26"/>
+      <c r="AAL67" s="26"/>
+      <c r="AAM67" s="26"/>
+      <c r="AAN67" s="26"/>
+      <c r="AAO67" s="26"/>
+      <c r="AAP67" s="26"/>
+      <c r="AAQ67" s="26"/>
+      <c r="AAR67" s="26"/>
+      <c r="AAS67" s="26"/>
+      <c r="AAT67" s="26"/>
+      <c r="AAU67" s="26"/>
+      <c r="AAV67" s="26"/>
+      <c r="AAW67" s="26"/>
+      <c r="AAX67" s="26"/>
+      <c r="AAY67" s="26"/>
+      <c r="AAZ67" s="26"/>
+      <c r="ABA67" s="26"/>
+      <c r="ABB67" s="26"/>
+      <c r="ABC67" s="26"/>
+      <c r="ABD67" s="26"/>
+      <c r="ABE67" s="26"/>
+      <c r="ABF67" s="26"/>
+      <c r="ABG67" s="26"/>
+      <c r="ABH67" s="26"/>
+      <c r="ABI67" s="26"/>
+      <c r="ABJ67" s="26"/>
+      <c r="ABK67" s="26"/>
+      <c r="ABL67" s="26"/>
+      <c r="ABM67" s="26"/>
+      <c r="ABN67" s="26"/>
+      <c r="ABO67" s="26"/>
+      <c r="ABP67" s="26"/>
+      <c r="ABQ67" s="26"/>
+      <c r="ABR67" s="26"/>
+      <c r="ABS67" s="26"/>
+      <c r="ABT67" s="26"/>
+      <c r="ABU67" s="26"/>
+      <c r="ABV67" s="26"/>
+      <c r="ABW67" s="26"/>
+      <c r="ABX67" s="26"/>
+      <c r="ABY67" s="26"/>
+      <c r="ABZ67" s="26"/>
+      <c r="ACA67" s="26"/>
+      <c r="ACB67" s="26"/>
+      <c r="ACC67" s="26"/>
+      <c r="ACD67" s="26"/>
+      <c r="ACE67" s="26"/>
+      <c r="ACF67" s="26"/>
+      <c r="ACG67" s="26"/>
+      <c r="ACH67" s="26"/>
+      <c r="ACI67" s="26"/>
+      <c r="ACJ67" s="26"/>
+      <c r="ACK67" s="26"/>
+      <c r="ACL67" s="26"/>
+      <c r="ACM67" s="26"/>
+      <c r="ACN67" s="26"/>
+      <c r="ACO67" s="26"/>
+      <c r="ACP67" s="26"/>
+      <c r="ACQ67" s="26"/>
+      <c r="ACR67" s="26"/>
+      <c r="ACS67" s="26"/>
+      <c r="ACT67" s="26"/>
+      <c r="ACU67" s="26"/>
+      <c r="ACV67" s="26"/>
+      <c r="ACW67" s="26"/>
+      <c r="ACX67" s="26"/>
+      <c r="ACY67" s="26"/>
+      <c r="ACZ67" s="26"/>
+      <c r="ADA67" s="26"/>
+      <c r="ADB67" s="26"/>
+      <c r="ADC67" s="26"/>
+      <c r="ADD67" s="26"/>
+      <c r="ADE67" s="26"/>
+      <c r="ADF67" s="26"/>
+      <c r="ADG67" s="26"/>
+      <c r="ADH67" s="26"/>
+      <c r="ADI67" s="26"/>
+      <c r="ADJ67" s="26"/>
+      <c r="ADK67" s="26"/>
+      <c r="ADL67" s="26"/>
+      <c r="ADM67" s="26"/>
+      <c r="ADN67" s="26"/>
+      <c r="ADO67" s="26"/>
+      <c r="ADP67" s="26"/>
+      <c r="ADQ67" s="26"/>
+      <c r="ADR67" s="26"/>
+      <c r="ADS67" s="26"/>
+      <c r="ADT67" s="26"/>
+      <c r="ADU67" s="26"/>
+      <c r="ADV67" s="26"/>
+      <c r="ADW67" s="26"/>
+      <c r="ADX67" s="26"/>
+      <c r="ADY67" s="26"/>
+      <c r="ADZ67" s="26"/>
+      <c r="AEA67" s="26"/>
+      <c r="AEB67" s="26"/>
+      <c r="AEC67" s="26"/>
+      <c r="AED67" s="26"/>
+      <c r="AEE67" s="26"/>
+      <c r="AEF67" s="26"/>
+      <c r="AEG67" s="26"/>
+      <c r="AEH67" s="26"/>
+      <c r="AEI67" s="26"/>
+      <c r="AEJ67" s="26"/>
+      <c r="AEK67" s="26"/>
+      <c r="AEL67" s="26"/>
+      <c r="AEM67" s="26"/>
+      <c r="AEN67" s="26"/>
+      <c r="AEO67" s="26"/>
+      <c r="AEP67" s="26"/>
+      <c r="AEQ67" s="26"/>
+      <c r="AER67" s="26"/>
+      <c r="AES67" s="26"/>
+      <c r="AET67" s="26"/>
+      <c r="AEU67" s="26"/>
+      <c r="AEV67" s="26"/>
+      <c r="AEW67" s="26"/>
+      <c r="AEX67" s="26"/>
+      <c r="AEY67" s="26"/>
+      <c r="AEZ67" s="26"/>
+      <c r="AFA67" s="26"/>
+      <c r="AFB67" s="26"/>
+      <c r="AFC67" s="26"/>
+      <c r="AFD67" s="26"/>
+      <c r="AFE67" s="26"/>
+      <c r="AFF67" s="26"/>
+      <c r="AFG67" s="26"/>
+      <c r="AFH67" s="26"/>
+      <c r="AFI67" s="26"/>
+      <c r="AFJ67" s="26"/>
+      <c r="AFK67" s="26"/>
+      <c r="AFL67" s="26"/>
+      <c r="AFM67" s="26"/>
+      <c r="AFN67" s="26"/>
+      <c r="AFO67" s="26"/>
+      <c r="AFP67" s="26"/>
+      <c r="AFQ67" s="26"/>
+      <c r="AFR67" s="26"/>
+      <c r="AFS67" s="26"/>
+      <c r="AFT67" s="26"/>
+      <c r="AFU67" s="26"/>
+      <c r="AFV67" s="26"/>
+      <c r="AFW67" s="26"/>
+      <c r="AFX67" s="26"/>
+      <c r="AFY67" s="26"/>
+      <c r="AFZ67" s="26"/>
+      <c r="AGA67" s="26"/>
+      <c r="AGB67" s="26"/>
+      <c r="AGC67" s="26"/>
+      <c r="AGD67" s="26"/>
+      <c r="AGE67" s="26"/>
+      <c r="AGF67" s="26"/>
+      <c r="AGG67" s="26"/>
+      <c r="AGH67" s="26"/>
+      <c r="AGI67" s="26"/>
+      <c r="AGJ67" s="26"/>
+      <c r="AGK67" s="26"/>
+      <c r="AGL67" s="26"/>
+      <c r="AGM67" s="26"/>
+      <c r="AGN67" s="26"/>
+      <c r="AGO67" s="26"/>
+      <c r="AGP67" s="26"/>
+      <c r="AGQ67" s="26"/>
+      <c r="AGR67" s="26"/>
+      <c r="AGS67" s="26"/>
+      <c r="AGT67" s="26"/>
+      <c r="AGU67" s="26"/>
+      <c r="AGV67" s="26"/>
+      <c r="AGW67" s="26"/>
+      <c r="AGX67" s="26"/>
+      <c r="AGY67" s="26"/>
+      <c r="AGZ67" s="26"/>
+      <c r="AHA67" s="26"/>
+      <c r="AHB67" s="26"/>
+      <c r="AHC67" s="26"/>
+      <c r="AHD67" s="26"/>
+      <c r="AHE67" s="26"/>
+      <c r="AHF67" s="26"/>
+      <c r="AHG67" s="26"/>
+      <c r="AHH67" s="26"/>
+      <c r="AHI67" s="26"/>
+      <c r="AHJ67" s="26"/>
+      <c r="AHK67" s="26"/>
+      <c r="AHL67" s="26"/>
+      <c r="AHM67" s="26"/>
+      <c r="AHN67" s="26"/>
+      <c r="AHO67" s="26"/>
+      <c r="AHP67" s="26"/>
+      <c r="AHQ67" s="26"/>
+      <c r="AHR67" s="26"/>
+      <c r="AHS67" s="26"/>
+      <c r="AHT67" s="26"/>
+      <c r="AHU67" s="26"/>
+      <c r="AHV67" s="26"/>
+      <c r="AHW67" s="26"/>
+      <c r="AHX67" s="26"/>
+      <c r="AHY67" s="26"/>
+      <c r="AHZ67" s="26"/>
+      <c r="AIA67" s="26"/>
+      <c r="AIB67" s="26"/>
+      <c r="AIC67" s="26"/>
+      <c r="AID67" s="26"/>
+      <c r="AIE67" s="26"/>
+      <c r="AIF67" s="26"/>
+      <c r="AIG67" s="26"/>
+      <c r="AIH67" s="26"/>
+      <c r="AII67" s="26"/>
+      <c r="AIJ67" s="26"/>
+      <c r="AIK67" s="26"/>
+      <c r="AIL67" s="26"/>
+      <c r="AIM67" s="26"/>
+      <c r="AIN67" s="26"/>
+      <c r="AIO67" s="26"/>
+      <c r="AIP67" s="26"/>
+      <c r="AIQ67" s="26"/>
+      <c r="AIR67" s="26"/>
+      <c r="AIS67" s="26"/>
+      <c r="AIT67" s="26"/>
+      <c r="AIU67" s="26"/>
+      <c r="AIV67" s="26"/>
+      <c r="AIW67" s="26"/>
+      <c r="AIX67" s="26"/>
+      <c r="AIY67" s="26"/>
+      <c r="AIZ67" s="26"/>
+      <c r="AJA67" s="26"/>
+      <c r="AJB67" s="26"/>
+      <c r="AJC67" s="26"/>
+      <c r="AJD67" s="26"/>
+      <c r="AJE67" s="26"/>
+      <c r="AJF67" s="26"/>
+      <c r="AJG67" s="26"/>
+      <c r="AJH67" s="26"/>
+      <c r="AJI67" s="26"/>
+      <c r="AJJ67" s="26"/>
+      <c r="AJK67" s="26"/>
+      <c r="AJL67" s="26"/>
+      <c r="AJM67" s="26"/>
+      <c r="AJN67" s="26"/>
+      <c r="AJO67" s="26"/>
+      <c r="AJP67" s="26"/>
+      <c r="AJQ67" s="26"/>
+      <c r="AJR67" s="26"/>
+      <c r="AJS67" s="26"/>
+      <c r="AJT67" s="26"/>
+      <c r="AJU67" s="26"/>
+      <c r="AJV67" s="26"/>
+      <c r="AJW67" s="26"/>
+      <c r="AJX67" s="26"/>
+      <c r="AJY67" s="26"/>
+      <c r="AJZ67" s="26"/>
+      <c r="AKA67" s="26"/>
+      <c r="AKB67" s="26"/>
+      <c r="AKC67" s="26"/>
+      <c r="AKD67" s="26"/>
+      <c r="AKE67" s="26"/>
+      <c r="AKF67" s="26"/>
+      <c r="AKG67" s="26"/>
+      <c r="AKH67" s="26"/>
+      <c r="AKI67" s="26"/>
+      <c r="AKJ67" s="26"/>
+      <c r="AKK67" s="26"/>
+      <c r="AKL67" s="26"/>
+      <c r="AKM67" s="26"/>
+      <c r="AKN67" s="26"/>
+      <c r="AKO67" s="26"/>
+      <c r="AKP67" s="26"/>
+      <c r="AKQ67" s="26"/>
+      <c r="AKR67" s="26"/>
+      <c r="AKS67" s="26"/>
+      <c r="AKT67" s="26"/>
+      <c r="AKU67" s="26"/>
+      <c r="AKV67" s="26"/>
+      <c r="AKW67" s="26"/>
+      <c r="AKX67" s="26"/>
+      <c r="AKY67" s="26"/>
+      <c r="AKZ67" s="26"/>
+      <c r="ALA67" s="26"/>
+      <c r="ALB67" s="26"/>
+      <c r="ALC67" s="26"/>
+      <c r="ALD67" s="26"/>
+      <c r="ALE67" s="26"/>
+      <c r="ALF67" s="26"/>
+      <c r="ALG67" s="26"/>
+      <c r="ALH67" s="26"/>
+      <c r="ALI67" s="26"/>
+      <c r="ALJ67" s="26"/>
+      <c r="ALK67" s="26"/>
+      <c r="ALL67" s="26"/>
+      <c r="ALM67" s="26"/>
+      <c r="ALN67" s="26"/>
+      <c r="ALO67" s="26"/>
+      <c r="ALP67" s="26"/>
+      <c r="ALQ67" s="26"/>
+      <c r="ALR67" s="26"/>
+      <c r="ALS67" s="26"/>
+      <c r="ALT67" s="26"/>
+      <c r="ALU67" s="26"/>
+      <c r="ALV67" s="26"/>
+      <c r="ALW67" s="26"/>
+      <c r="ALX67" s="26"/>
+      <c r="ALY67" s="26"/>
+      <c r="ALZ67" s="26"/>
+      <c r="AMA67" s="26"/>
+      <c r="AMB67" s="26"/>
+      <c r="AMC67" s="26"/>
+      <c r="AMD67" s="26"/>
+      <c r="AME67" s="26"/>
+      <c r="AMF67" s="26"/>
+      <c r="AMG67" s="26"/>
+      <c r="AMH67" s="26"/>
+      <c r="AMI67" s="26"/>
+      <c r="AMJ67" s="26"/>
+      <c r="AMK67" s="26"/>
+    </row>
+    <row r="68" spans="1:1025" x14ac:dyDescent="0.35">
+      <c r="B68" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="C67" s="33"/>
+      <c r="C68" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B61:C61"/>
     <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
     <mergeCell ref="C6:L6"/>
     <mergeCell ref="C7:L7"/>
     <mergeCell ref="C8:L8"/>
@@ -6383,11 +7450,11 @@
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="C5:L5"/>
-    <mergeCell ref="B63:C63"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -6410,16 +7477,16 @@
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>196</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -6430,7 +7497,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="36"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="8" t="s">
         <v>198</v>
       </c>
@@ -6439,7 +7506,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="36"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="8" t="s">
         <v>199</v>
       </c>
@@ -6448,7 +7515,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="36"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="8" t="s">
         <v>200</v>
       </c>
@@ -6457,13 +7524,13 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="36"/>
-      <c r="C10" s="37" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6498,11 +7565,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">

</xml_diff>

<commit_message>
EPBDS-7066 Add new dev property to control a possibility of returning empty result. Refactoring.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F001C1F-B47F-41A1-B5B2-4936384EDFD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CB911D-2DF2-483A-BA35-C096A2FDB231}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -901,19 +901,19 @@
     <t>Controls generation additional properties with table structure details in an output model</t>
   </si>
   <si>
-    <t>Calculation Mode</t>
-  </si>
-  <si>
     <t>The way of calculation of the DT table</t>
   </si>
   <si>
-    <t>DTCalculationModeEnum</t>
-  </si>
-  <si>
-    <t>calculationMode</t>
-  </si>
-  <si>
-    <t>AVOID_EMPTY_RESULT</t>
+    <t>resultCalculationMode</t>
+  </si>
+  <si>
+    <t>DTResultCalculationModeEnum</t>
+  </si>
+  <si>
+    <t>Result Calculation Mode</t>
+  </si>
+  <si>
+    <t>AVOID_EMPTY</t>
   </si>
 </sst>
 </file>
@@ -1414,14 +1414,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1430,9 +1433,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1936,16 +1936,16 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
@@ -1981,31 +1981,31 @@
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
@@ -2059,13 +2059,13 @@
       <c r="C12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7" t="s">
@@ -2074,13 +2074,13 @@
       <c r="C13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
@@ -2089,34 +2089,29 @@
       <c r="C14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -2126,6 +2121,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2142,7 +2142,7 @@
   <dimension ref="A1:AMK68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2208,18 +2208,18 @@
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
@@ -2259,35 +2259,35 @@
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
@@ -2333,27 +2333,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
@@ -5009,10 +5009,10 @@
     <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="27"/>
       <c r="B48" s="5" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>58</v>
@@ -5047,7 +5047,7 @@
         <v>83</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="U48" s="27"/>
       <c r="V48" s="27"/>
@@ -6372,41 +6372,41 @@
     <row r="60" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="62" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="35" t="s">
+      <c r="B62" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="C62" s="35"/>
+      <c r="C62" s="32"/>
     </row>
     <row r="63" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="32" t="s">
+      <c r="B63" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="C63" s="32"/>
+      <c r="C63" s="33"/>
     </row>
     <row r="64" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="32" t="s">
+      <c r="B64" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="C64" s="32"/>
+      <c r="C64" s="33"/>
     </row>
     <row r="65" spans="1:1025" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="33" t="s">
+      <c r="B65" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="C65" s="33"/>
+      <c r="C65" s="34"/>
     </row>
     <row r="66" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="B66" s="33" t="s">
+      <c r="B66" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="C66" s="33"/>
+      <c r="C66" s="34"/>
     </row>
     <row r="67" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A67" s="26"/>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="C67" s="33"/>
+      <c r="C67" s="34"/>
       <c r="D67" s="26"/>
       <c r="E67" s="26"/>
       <c r="F67" s="26"/>
@@ -7431,13 +7431,23 @@
       <c r="AMK67" s="26"/>
     </row>
     <row r="68" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="B68" s="34" t="s">
+      <c r="B68" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="C68" s="34"/>
+      <c r="C68" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:L5"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="C6:L6"/>
@@ -7445,16 +7455,6 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-7066 Add new dev property to control a possibility of returning empty result. Renaming.
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21604B0B-4562-46E3-83C6-FA27A1D69CFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24A4423-FFC0-45AF-B939-CCD3DC9A9BB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -898,22 +898,22 @@
     <t>CaProvincesEnum</t>
   </si>
   <si>
-    <t>The way of calculation of the DT table</t>
-  </si>
-  <si>
-    <t>Result Calculation Mode</t>
-  </si>
-  <si>
-    <t>resultCalculationMode</t>
-  </si>
-  <si>
-    <t>DTResultCalculationModeEnum</t>
-  </si>
-  <si>
-    <t>AVOID_EMPTY</t>
-  </si>
-  <si>
     <t>Detailed Plain Model</t>
+  </si>
+  <si>
+    <t>Empty Result Processing</t>
+  </si>
+  <si>
+    <t>emptyResultProcessing</t>
+  </si>
+  <si>
+    <t>DTEmptyResultProcessingEnum</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>The way of calculation result of the DT table</t>
   </si>
 </sst>
 </file>
@@ -1414,17 +1414,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1433,6 +1430,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1936,16 +1936,16 @@
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
@@ -1981,31 +1981,31 @@
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
@@ -2059,13 +2059,13 @@
       <c r="C12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7" t="s">
@@ -2074,13 +2074,13 @@
       <c r="C13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
@@ -2089,29 +2089,34 @@
       <c r="C14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -2121,11 +2126,6 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2141,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="T49" sqref="T49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2208,18 +2208,18 @@
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
@@ -2259,35 +2259,35 @@
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
@@ -2333,27 +2333,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
@@ -5047,7 +5047,7 @@
         <v>83</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="U48" s="27"/>
       <c r="V48" s="27"/>
@@ -6100,7 +6100,7 @@
     <row r="50" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="23"/>
       <c r="B50" s="5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>248</v>
@@ -6372,41 +6372,41 @@
     <row r="60" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="62" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="32" t="s">
+      <c r="B62" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="C62" s="32"/>
+      <c r="C62" s="35"/>
     </row>
     <row r="63" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="C63" s="33"/>
+      <c r="C63" s="32"/>
     </row>
     <row r="64" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="33" t="s">
+      <c r="B64" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C64" s="33"/>
+      <c r="C64" s="32"/>
     </row>
     <row r="65" spans="1:1025" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="34" t="s">
+      <c r="B65" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="C65" s="34"/>
+      <c r="C65" s="33"/>
     </row>
     <row r="66" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="B66" s="34" t="s">
+      <c r="B66" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C66" s="34"/>
+      <c r="C66" s="33"/>
     </row>
     <row r="67" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A67" s="26"/>
-      <c r="B67" s="34" t="s">
+      <c r="B67" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="C67" s="34"/>
+      <c r="C67" s="33"/>
       <c r="D67" s="26"/>
       <c r="E67" s="26"/>
       <c r="F67" s="26"/>
@@ -7431,23 +7431,13 @@
       <c r="AMK67" s="26"/>
     </row>
     <row r="68" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="C68" s="35"/>
+      <c r="C68" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C5:L5"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="C6:L6"/>
@@ -7455,6 +7445,16 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-12727 Implemented virtual function msg(String, Object...) for getting localized messages from i18n bundles
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpikus/Sources/OpenL/openl-tablets/DEV/org.openl.rules/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819AF603-E0A5-4190-9C4B-B7281ABA459B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF493FE-5ED0-F647-A4AE-EFCAEDF33AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34940" windowHeight="21360" tabRatio="783" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,16 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="290">
   <si>
     <t>Display Name</t>
   </si>
@@ -914,6 +924,15 @@
   </si>
   <si>
     <t>The way of processing result calculation of the DT table</t>
+  </si>
+  <si>
+    <t>locale</t>
+  </si>
+  <si>
+    <t>Locale</t>
+  </si>
+  <si>
+    <t>A Locale object represents a specific geographical, political, or cultural region.</t>
   </si>
 </sst>
 </file>
@@ -1414,14 +1433,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1430,9 +1452,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1455,39 +1474,39 @@
     </xf>
   </cellXfs>
   <cellStyles count="33">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1571,9 +1590,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1611,7 +1630,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1717,7 +1736,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1897,12 +1916,12 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.81640625" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1917,7 +1936,7 @@
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
     </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1932,22 +1951,22 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1962,7 +1981,7 @@
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1977,37 +1996,37 @@
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
     </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-    </row>
-    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+    </row>
+    <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-    </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
@@ -2022,7 +2041,7 @@
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
     </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
@@ -2037,7 +2056,7 @@
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
     </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
@@ -2052,71 +2071,66 @@
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-    </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-    </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+    </row>
+    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="30" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
@@ -2126,6 +2140,11 @@
     <mergeCell ref="C9:J9"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2141,36 +2160,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1"/>
-    <col min="2" max="2" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="49.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="73.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="1025" width="8.81640625" style="1"/>
+    <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="73.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2187,7 +2206,7 @@
       <c r="K1" s="28"/>
       <c r="L1" s="28"/>
     </row>
-    <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -2204,24 +2223,24 @@
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
     </row>
-    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-    </row>
-    <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+    </row>
+    <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -2238,7 +2257,7 @@
       <c r="K4" s="28"/>
       <c r="L4" s="28"/>
     </row>
-    <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2255,41 +2274,41 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-    </row>
-    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+    </row>
+    <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-    </row>
-    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+    </row>
+    <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
@@ -2306,7 +2325,7 @@
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
     </row>
-    <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
@@ -2323,7 +2342,7 @@
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
     </row>
-    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2332,30 +2351,30 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="35" t="s">
+    <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-    </row>
-    <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+    </row>
+    <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
@@ -2414,7 +2433,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
@@ -2473,7 +2492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
@@ -2520,7 +2539,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>66</v>
       </c>
@@ -2563,7 +2582,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>100</v>
       </c>
@@ -2610,7 +2629,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>105</v>
       </c>
@@ -2659,7 +2678,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>109</v>
       </c>
@@ -2706,7 +2725,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>113</v>
       </c>
@@ -2755,7 +2774,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
@@ -2798,7 +2817,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>72</v>
       </c>
@@ -2841,7 +2860,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>76</v>
       </c>
@@ -2890,7 +2909,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>85</v>
       </c>
@@ -2939,7 +2958,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>90</v>
       </c>
@@ -2988,7 +3007,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>95</v>
       </c>
@@ -3037,7 +3056,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>229</v>
       </c>
@@ -3082,7 +3101,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>222</v>
       </c>
@@ -3127,7 +3146,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>138</v>
       </c>
@@ -3172,7 +3191,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>154</v>
       </c>
@@ -3217,7 +3236,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>142</v>
       </c>
@@ -3262,7 +3281,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>146</v>
       </c>
@@ -3307,7 +3326,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>130</v>
       </c>
@@ -3354,7 +3373,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>216</v>
       </c>
@@ -3397,7 +3416,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>134</v>
       </c>
@@ -3442,7 +3461,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>150</v>
       </c>
@@ -3487,7 +3506,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>158</v>
       </c>
@@ -3528,7 +3547,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>162</v>
       </c>
@@ -3572,7 +3591,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>116</v>
       </c>
@@ -3619,7 +3638,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>123</v>
       </c>
@@ -3662,7 +3681,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
         <v>127</v>
       </c>
@@ -3705,7 +3724,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>167</v>
       </c>
@@ -3747,7 +3766,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>170</v>
       </c>
@@ -3788,7 +3807,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="25"/>
       <c r="B43" s="5" t="s">
         <v>254</v>
@@ -3832,7 +3851,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1025" ht="32" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>175</v>
       </c>
@@ -3876,7 +3895,7 @@
       </c>
       <c r="U44" s="24"/>
     </row>
-    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="24"/>
       <c r="B45" s="5" t="s">
         <v>248</v>
@@ -3920,7 +3939,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="5" t="s">
         <v>181</v>
       </c>
@@ -3961,7 +3980,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="s">
         <v>183</v>
       </c>
@@ -5006,7 +5025,7 @@
       <c r="AMJ47" s="23"/>
       <c r="AMK47" s="23"/>
     </row>
-    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="27"/>
       <c r="B48" s="5" t="s">
         <v>282</v>
@@ -6055,7 +6074,7 @@
       <c r="AMJ48" s="27"/>
       <c r="AMK48" s="27"/>
     </row>
-    <row r="49" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
         <v>210</v>
       </c>
@@ -6097,7 +6116,7 @@
       </c>
       <c r="U49" s="23"/>
     </row>
-    <row r="50" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="23"/>
       <c r="B50" s="5" t="s">
         <v>279</v>
@@ -6144,7 +6163,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="5" t="s">
         <v>214</v>
       </c>
@@ -6190,7 +6209,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="5" t="s">
         <v>245</v>
       </c>
@@ -6236,7 +6255,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" ht="32" x14ac:dyDescent="0.2">
       <c r="B53" s="5" t="s">
         <v>242</v>
       </c>
@@ -6282,7 +6301,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" ht="32" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="s">
         <v>235</v>
       </c>
@@ -6329,8 +6348,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="s">
         <v>186</v>
       </c>
@@ -6369,44 +6388,44 @@
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="35" t="s">
+    <row r="60" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="C62" s="35"/>
-    </row>
-    <row r="63" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="32" t="s">
+      <c r="C62" s="32"/>
+    </row>
+    <row r="63" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="C63" s="32"/>
-    </row>
-    <row r="64" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="32" t="s">
+      <c r="C63" s="33"/>
+    </row>
+    <row r="64" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="C64" s="32"/>
-    </row>
-    <row r="65" spans="1:1025" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="33" t="s">
+      <c r="C64" s="33"/>
+    </row>
+    <row r="65" spans="1:1025" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="C65" s="33"/>
-    </row>
-    <row r="66" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="B66" s="33" t="s">
+      <c r="C65" s="34"/>
+    </row>
+    <row r="66" spans="1:1025" x14ac:dyDescent="0.2">
+      <c r="B66" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="C66" s="33"/>
-    </row>
-    <row r="67" spans="1:1025" x14ac:dyDescent="0.35">
+      <c r="C66" s="34"/>
+    </row>
+    <row r="67" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A67" s="26"/>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="C67" s="33"/>
+      <c r="C67" s="34"/>
       <c r="D67" s="26"/>
       <c r="E67" s="26"/>
       <c r="F67" s="26"/>
@@ -7430,14 +7449,24 @@
       <c r="AMJ67" s="26"/>
       <c r="AMK67" s="26"/>
     </row>
-    <row r="68" spans="1:1025" x14ac:dyDescent="0.35">
-      <c r="B68" s="34" t="s">
+    <row r="68" spans="1:1025" x14ac:dyDescent="0.2">
+      <c r="B68" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="C68" s="34"/>
+      <c r="C68" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:L5"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="C6:L6"/>
@@ -7445,16 +7474,6 @@
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="B11:T11"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -7474,9 +7493,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="36" t="s">
         <v>195</v>
       </c>
@@ -7485,7 +7504,7 @@
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
     </row>
-    <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="37" t="s">
         <v>196</v>
       </c>
@@ -7496,7 +7515,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="37"/>
       <c r="C7" s="8" t="s">
         <v>198</v>
@@ -7505,7 +7524,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="37"/>
       <c r="C8" s="8" t="s">
         <v>199</v>
@@ -7514,7 +7533,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="37"/>
       <c r="C9" s="8" t="s">
         <v>200</v>
@@ -7523,7 +7542,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="37"/>
       <c r="C10" s="38" t="s">
         <v>201</v>
@@ -7550,28 +7569,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="39" t="s">
         <v>202</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="41"/>
     </row>
-    <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
@@ -7582,7 +7601,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
@@ -7593,7 +7612,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
         <v>107</v>
       </c>
@@ -7604,7 +7623,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
         <v>203</v>
       </c>
@@ -7615,7 +7634,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="18" t="s">
         <v>131</v>
       </c>
@@ -7626,7 +7645,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
         <v>236</v>
       </c>
@@ -7637,7 +7656,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="18" t="s">
         <v>204</v>
       </c>
@@ -7648,7 +7667,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="18" t="s">
         <v>139</v>
       </c>
@@ -7659,7 +7678,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="18" t="s">
         <v>207</v>
       </c>
@@ -7670,7 +7689,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
         <v>143</v>
       </c>
@@ -7681,7 +7700,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>147</v>
       </c>
@@ -7692,7 +7711,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>155</v>
       </c>
@@ -7703,7 +7722,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>221</v>
       </c>
@@ -7714,15 +7733,26 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="20" t="s">
+    <row r="16" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="19" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B17" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -7730,7 +7760,7 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
EPBDS-14241 Origin: rename deviation, add origin to the runtime context
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpikus/Sources/OpenL/openl-tablets/DEV/org.openl.rules/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF493FE-5ED0-F647-A4AE-EFCAEDF33AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAE68B1-530B-5C4D-A1AB-EE45332B9FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="34940" windowHeight="21360" tabRatio="783" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="291">
   <si>
     <t>Display Name</t>
   </si>
@@ -933,6 +933,9 @@
   </si>
   <si>
     <t>A Locale object represents a specific geographical, political, or cultural region.</t>
+  </si>
+  <si>
+    <t>eq(origin)</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1035,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1311,6 +1314,45 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1349,7 +1391,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1415,19 +1457,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1590,9 +1626,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1630,9 +1666,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1665,26 +1701,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1717,26 +1736,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1925,207 +1927,207 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
@@ -2160,8 +2162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK68"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="I29" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2193,154 +2195,154 @@
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
@@ -2352,27 +2354,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
@@ -3373,7 +3375,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>216</v>
       </c>
@@ -3386,7 +3388,9 @@
       <c r="E33" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G33" s="5" t="s">
         <v>78</v>
       </c>
@@ -3416,7 +3420,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>134</v>
       </c>
@@ -3461,7 +3465,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>150</v>
       </c>
@@ -3506,7 +3510,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>158</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>162</v>
       </c>
@@ -3591,7 +3595,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>116</v>
       </c>
@@ -3638,7 +3642,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>123</v>
       </c>
@@ -3681,7 +3685,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
         <v>127</v>
       </c>
@@ -3724,7 +3728,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>167</v>
       </c>
@@ -3766,7 +3770,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>170</v>
       </c>
@@ -3807,8 +3811,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25"/>
+    <row r="43" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
         <v>254</v>
       </c>
@@ -3851,7 +3854,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:20" ht="32" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>175</v>
       </c>
@@ -3893,10 +3896,8 @@
       <c r="T44" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="U44" s="24"/>
-    </row>
-    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
+    </row>
+    <row r="45" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="5" t="s">
         <v>248</v>
       </c>
@@ -3939,7 +3940,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="5" t="s">
         <v>181</v>
       </c>
@@ -3980,7 +3981,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="s">
         <v>183</v>
       </c>
@@ -4020,1013 +4021,8 @@
       <c r="T47" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="V47" s="23"/>
-      <c r="W47" s="23"/>
-      <c r="X47" s="23"/>
-      <c r="Y47" s="23"/>
-      <c r="Z47" s="23"/>
-      <c r="AA47" s="23"/>
-      <c r="AB47" s="23"/>
-      <c r="AC47" s="23"/>
-      <c r="AD47" s="23"/>
-      <c r="AE47" s="23"/>
-      <c r="AF47" s="23"/>
-      <c r="AG47" s="23"/>
-      <c r="AH47" s="23"/>
-      <c r="AI47" s="23"/>
-      <c r="AJ47" s="23"/>
-      <c r="AK47" s="23"/>
-      <c r="AL47" s="23"/>
-      <c r="AM47" s="23"/>
-      <c r="AN47" s="23"/>
-      <c r="AO47" s="23"/>
-      <c r="AP47" s="23"/>
-      <c r="AQ47" s="23"/>
-      <c r="AR47" s="23"/>
-      <c r="AS47" s="23"/>
-      <c r="AT47" s="23"/>
-      <c r="AU47" s="23"/>
-      <c r="AV47" s="23"/>
-      <c r="AW47" s="23"/>
-      <c r="AX47" s="23"/>
-      <c r="AY47" s="23"/>
-      <c r="AZ47" s="23"/>
-      <c r="BA47" s="23"/>
-      <c r="BB47" s="23"/>
-      <c r="BC47" s="23"/>
-      <c r="BD47" s="23"/>
-      <c r="BE47" s="23"/>
-      <c r="BF47" s="23"/>
-      <c r="BG47" s="23"/>
-      <c r="BH47" s="23"/>
-      <c r="BI47" s="23"/>
-      <c r="BJ47" s="23"/>
-      <c r="BK47" s="23"/>
-      <c r="BL47" s="23"/>
-      <c r="BM47" s="23"/>
-      <c r="BN47" s="23"/>
-      <c r="BO47" s="23"/>
-      <c r="BP47" s="23"/>
-      <c r="BQ47" s="23"/>
-      <c r="BR47" s="23"/>
-      <c r="BS47" s="23"/>
-      <c r="BT47" s="23"/>
-      <c r="BU47" s="23"/>
-      <c r="BV47" s="23"/>
-      <c r="BW47" s="23"/>
-      <c r="BX47" s="23"/>
-      <c r="BY47" s="23"/>
-      <c r="BZ47" s="23"/>
-      <c r="CA47" s="23"/>
-      <c r="CB47" s="23"/>
-      <c r="CC47" s="23"/>
-      <c r="CD47" s="23"/>
-      <c r="CE47" s="23"/>
-      <c r="CF47" s="23"/>
-      <c r="CG47" s="23"/>
-      <c r="CH47" s="23"/>
-      <c r="CI47" s="23"/>
-      <c r="CJ47" s="23"/>
-      <c r="CK47" s="23"/>
-      <c r="CL47" s="23"/>
-      <c r="CM47" s="23"/>
-      <c r="CN47" s="23"/>
-      <c r="CO47" s="23"/>
-      <c r="CP47" s="23"/>
-      <c r="CQ47" s="23"/>
-      <c r="CR47" s="23"/>
-      <c r="CS47" s="23"/>
-      <c r="CT47" s="23"/>
-      <c r="CU47" s="23"/>
-      <c r="CV47" s="23"/>
-      <c r="CW47" s="23"/>
-      <c r="CX47" s="23"/>
-      <c r="CY47" s="23"/>
-      <c r="CZ47" s="23"/>
-      <c r="DA47" s="23"/>
-      <c r="DB47" s="23"/>
-      <c r="DC47" s="23"/>
-      <c r="DD47" s="23"/>
-      <c r="DE47" s="23"/>
-      <c r="DF47" s="23"/>
-      <c r="DG47" s="23"/>
-      <c r="DH47" s="23"/>
-      <c r="DI47" s="23"/>
-      <c r="DJ47" s="23"/>
-      <c r="DK47" s="23"/>
-      <c r="DL47" s="23"/>
-      <c r="DM47" s="23"/>
-      <c r="DN47" s="23"/>
-      <c r="DO47" s="23"/>
-      <c r="DP47" s="23"/>
-      <c r="DQ47" s="23"/>
-      <c r="DR47" s="23"/>
-      <c r="DS47" s="23"/>
-      <c r="DT47" s="23"/>
-      <c r="DU47" s="23"/>
-      <c r="DV47" s="23"/>
-      <c r="DW47" s="23"/>
-      <c r="DX47" s="23"/>
-      <c r="DY47" s="23"/>
-      <c r="DZ47" s="23"/>
-      <c r="EA47" s="23"/>
-      <c r="EB47" s="23"/>
-      <c r="EC47" s="23"/>
-      <c r="ED47" s="23"/>
-      <c r="EE47" s="23"/>
-      <c r="EF47" s="23"/>
-      <c r="EG47" s="23"/>
-      <c r="EH47" s="23"/>
-      <c r="EI47" s="23"/>
-      <c r="EJ47" s="23"/>
-      <c r="EK47" s="23"/>
-      <c r="EL47" s="23"/>
-      <c r="EM47" s="23"/>
-      <c r="EN47" s="23"/>
-      <c r="EO47" s="23"/>
-      <c r="EP47" s="23"/>
-      <c r="EQ47" s="23"/>
-      <c r="ER47" s="23"/>
-      <c r="ES47" s="23"/>
-      <c r="ET47" s="23"/>
-      <c r="EU47" s="23"/>
-      <c r="EV47" s="23"/>
-      <c r="EW47" s="23"/>
-      <c r="EX47" s="23"/>
-      <c r="EY47" s="23"/>
-      <c r="EZ47" s="23"/>
-      <c r="FA47" s="23"/>
-      <c r="FB47" s="23"/>
-      <c r="FC47" s="23"/>
-      <c r="FD47" s="23"/>
-      <c r="FE47" s="23"/>
-      <c r="FF47" s="23"/>
-      <c r="FG47" s="23"/>
-      <c r="FH47" s="23"/>
-      <c r="FI47" s="23"/>
-      <c r="FJ47" s="23"/>
-      <c r="FK47" s="23"/>
-      <c r="FL47" s="23"/>
-      <c r="FM47" s="23"/>
-      <c r="FN47" s="23"/>
-      <c r="FO47" s="23"/>
-      <c r="FP47" s="23"/>
-      <c r="FQ47" s="23"/>
-      <c r="FR47" s="23"/>
-      <c r="FS47" s="23"/>
-      <c r="FT47" s="23"/>
-      <c r="FU47" s="23"/>
-      <c r="FV47" s="23"/>
-      <c r="FW47" s="23"/>
-      <c r="FX47" s="23"/>
-      <c r="FY47" s="23"/>
-      <c r="FZ47" s="23"/>
-      <c r="GA47" s="23"/>
-      <c r="GB47" s="23"/>
-      <c r="GC47" s="23"/>
-      <c r="GD47" s="23"/>
-      <c r="GE47" s="23"/>
-      <c r="GF47" s="23"/>
-      <c r="GG47" s="23"/>
-      <c r="GH47" s="23"/>
-      <c r="GI47" s="23"/>
-      <c r="GJ47" s="23"/>
-      <c r="GK47" s="23"/>
-      <c r="GL47" s="23"/>
-      <c r="GM47" s="23"/>
-      <c r="GN47" s="23"/>
-      <c r="GO47" s="23"/>
-      <c r="GP47" s="23"/>
-      <c r="GQ47" s="23"/>
-      <c r="GR47" s="23"/>
-      <c r="GS47" s="23"/>
-      <c r="GT47" s="23"/>
-      <c r="GU47" s="23"/>
-      <c r="GV47" s="23"/>
-      <c r="GW47" s="23"/>
-      <c r="GX47" s="23"/>
-      <c r="GY47" s="23"/>
-      <c r="GZ47" s="23"/>
-      <c r="HA47" s="23"/>
-      <c r="HB47" s="23"/>
-      <c r="HC47" s="23"/>
-      <c r="HD47" s="23"/>
-      <c r="HE47" s="23"/>
-      <c r="HF47" s="23"/>
-      <c r="HG47" s="23"/>
-      <c r="HH47" s="23"/>
-      <c r="HI47" s="23"/>
-      <c r="HJ47" s="23"/>
-      <c r="HK47" s="23"/>
-      <c r="HL47" s="23"/>
-      <c r="HM47" s="23"/>
-      <c r="HN47" s="23"/>
-      <c r="HO47" s="23"/>
-      <c r="HP47" s="23"/>
-      <c r="HQ47" s="23"/>
-      <c r="HR47" s="23"/>
-      <c r="HS47" s="23"/>
-      <c r="HT47" s="23"/>
-      <c r="HU47" s="23"/>
-      <c r="HV47" s="23"/>
-      <c r="HW47" s="23"/>
-      <c r="HX47" s="23"/>
-      <c r="HY47" s="23"/>
-      <c r="HZ47" s="23"/>
-      <c r="IA47" s="23"/>
-      <c r="IB47" s="23"/>
-      <c r="IC47" s="23"/>
-      <c r="ID47" s="23"/>
-      <c r="IE47" s="23"/>
-      <c r="IF47" s="23"/>
-      <c r="IG47" s="23"/>
-      <c r="IH47" s="23"/>
-      <c r="II47" s="23"/>
-      <c r="IJ47" s="23"/>
-      <c r="IK47" s="23"/>
-      <c r="IL47" s="23"/>
-      <c r="IM47" s="23"/>
-      <c r="IN47" s="23"/>
-      <c r="IO47" s="23"/>
-      <c r="IP47" s="23"/>
-      <c r="IQ47" s="23"/>
-      <c r="IR47" s="23"/>
-      <c r="IS47" s="23"/>
-      <c r="IT47" s="23"/>
-      <c r="IU47" s="23"/>
-      <c r="IV47" s="23"/>
-      <c r="IW47" s="23"/>
-      <c r="IX47" s="23"/>
-      <c r="IY47" s="23"/>
-      <c r="IZ47" s="23"/>
-      <c r="JA47" s="23"/>
-      <c r="JB47" s="23"/>
-      <c r="JC47" s="23"/>
-      <c r="JD47" s="23"/>
-      <c r="JE47" s="23"/>
-      <c r="JF47" s="23"/>
-      <c r="JG47" s="23"/>
-      <c r="JH47" s="23"/>
-      <c r="JI47" s="23"/>
-      <c r="JJ47" s="23"/>
-      <c r="JK47" s="23"/>
-      <c r="JL47" s="23"/>
-      <c r="JM47" s="23"/>
-      <c r="JN47" s="23"/>
-      <c r="JO47" s="23"/>
-      <c r="JP47" s="23"/>
-      <c r="JQ47" s="23"/>
-      <c r="JR47" s="23"/>
-      <c r="JS47" s="23"/>
-      <c r="JT47" s="23"/>
-      <c r="JU47" s="23"/>
-      <c r="JV47" s="23"/>
-      <c r="JW47" s="23"/>
-      <c r="JX47" s="23"/>
-      <c r="JY47" s="23"/>
-      <c r="JZ47" s="23"/>
-      <c r="KA47" s="23"/>
-      <c r="KB47" s="23"/>
-      <c r="KC47" s="23"/>
-      <c r="KD47" s="23"/>
-      <c r="KE47" s="23"/>
-      <c r="KF47" s="23"/>
-      <c r="KG47" s="23"/>
-      <c r="KH47" s="23"/>
-      <c r="KI47" s="23"/>
-      <c r="KJ47" s="23"/>
-      <c r="KK47" s="23"/>
-      <c r="KL47" s="23"/>
-      <c r="KM47" s="23"/>
-      <c r="KN47" s="23"/>
-      <c r="KO47" s="23"/>
-      <c r="KP47" s="23"/>
-      <c r="KQ47" s="23"/>
-      <c r="KR47" s="23"/>
-      <c r="KS47" s="23"/>
-      <c r="KT47" s="23"/>
-      <c r="KU47" s="23"/>
-      <c r="KV47" s="23"/>
-      <c r="KW47" s="23"/>
-      <c r="KX47" s="23"/>
-      <c r="KY47" s="23"/>
-      <c r="KZ47" s="23"/>
-      <c r="LA47" s="23"/>
-      <c r="LB47" s="23"/>
-      <c r="LC47" s="23"/>
-      <c r="LD47" s="23"/>
-      <c r="LE47" s="23"/>
-      <c r="LF47" s="23"/>
-      <c r="LG47" s="23"/>
-      <c r="LH47" s="23"/>
-      <c r="LI47" s="23"/>
-      <c r="LJ47" s="23"/>
-      <c r="LK47" s="23"/>
-      <c r="LL47" s="23"/>
-      <c r="LM47" s="23"/>
-      <c r="LN47" s="23"/>
-      <c r="LO47" s="23"/>
-      <c r="LP47" s="23"/>
-      <c r="LQ47" s="23"/>
-      <c r="LR47" s="23"/>
-      <c r="LS47" s="23"/>
-      <c r="LT47" s="23"/>
-      <c r="LU47" s="23"/>
-      <c r="LV47" s="23"/>
-      <c r="LW47" s="23"/>
-      <c r="LX47" s="23"/>
-      <c r="LY47" s="23"/>
-      <c r="LZ47" s="23"/>
-      <c r="MA47" s="23"/>
-      <c r="MB47" s="23"/>
-      <c r="MC47" s="23"/>
-      <c r="MD47" s="23"/>
-      <c r="ME47" s="23"/>
-      <c r="MF47" s="23"/>
-      <c r="MG47" s="23"/>
-      <c r="MH47" s="23"/>
-      <c r="MI47" s="23"/>
-      <c r="MJ47" s="23"/>
-      <c r="MK47" s="23"/>
-      <c r="ML47" s="23"/>
-      <c r="MM47" s="23"/>
-      <c r="MN47" s="23"/>
-      <c r="MO47" s="23"/>
-      <c r="MP47" s="23"/>
-      <c r="MQ47" s="23"/>
-      <c r="MR47" s="23"/>
-      <c r="MS47" s="23"/>
-      <c r="MT47" s="23"/>
-      <c r="MU47" s="23"/>
-      <c r="MV47" s="23"/>
-      <c r="MW47" s="23"/>
-      <c r="MX47" s="23"/>
-      <c r="MY47" s="23"/>
-      <c r="MZ47" s="23"/>
-      <c r="NA47" s="23"/>
-      <c r="NB47" s="23"/>
-      <c r="NC47" s="23"/>
-      <c r="ND47" s="23"/>
-      <c r="NE47" s="23"/>
-      <c r="NF47" s="23"/>
-      <c r="NG47" s="23"/>
-      <c r="NH47" s="23"/>
-      <c r="NI47" s="23"/>
-      <c r="NJ47" s="23"/>
-      <c r="NK47" s="23"/>
-      <c r="NL47" s="23"/>
-      <c r="NM47" s="23"/>
-      <c r="NN47" s="23"/>
-      <c r="NO47" s="23"/>
-      <c r="NP47" s="23"/>
-      <c r="NQ47" s="23"/>
-      <c r="NR47" s="23"/>
-      <c r="NS47" s="23"/>
-      <c r="NT47" s="23"/>
-      <c r="NU47" s="23"/>
-      <c r="NV47" s="23"/>
-      <c r="NW47" s="23"/>
-      <c r="NX47" s="23"/>
-      <c r="NY47" s="23"/>
-      <c r="NZ47" s="23"/>
-      <c r="OA47" s="23"/>
-      <c r="OB47" s="23"/>
-      <c r="OC47" s="23"/>
-      <c r="OD47" s="23"/>
-      <c r="OE47" s="23"/>
-      <c r="OF47" s="23"/>
-      <c r="OG47" s="23"/>
-      <c r="OH47" s="23"/>
-      <c r="OI47" s="23"/>
-      <c r="OJ47" s="23"/>
-      <c r="OK47" s="23"/>
-      <c r="OL47" s="23"/>
-      <c r="OM47" s="23"/>
-      <c r="ON47" s="23"/>
-      <c r="OO47" s="23"/>
-      <c r="OP47" s="23"/>
-      <c r="OQ47" s="23"/>
-      <c r="OR47" s="23"/>
-      <c r="OS47" s="23"/>
-      <c r="OT47" s="23"/>
-      <c r="OU47" s="23"/>
-      <c r="OV47" s="23"/>
-      <c r="OW47" s="23"/>
-      <c r="OX47" s="23"/>
-      <c r="OY47" s="23"/>
-      <c r="OZ47" s="23"/>
-      <c r="PA47" s="23"/>
-      <c r="PB47" s="23"/>
-      <c r="PC47" s="23"/>
-      <c r="PD47" s="23"/>
-      <c r="PE47" s="23"/>
-      <c r="PF47" s="23"/>
-      <c r="PG47" s="23"/>
-      <c r="PH47" s="23"/>
-      <c r="PI47" s="23"/>
-      <c r="PJ47" s="23"/>
-      <c r="PK47" s="23"/>
-      <c r="PL47" s="23"/>
-      <c r="PM47" s="23"/>
-      <c r="PN47" s="23"/>
-      <c r="PO47" s="23"/>
-      <c r="PP47" s="23"/>
-      <c r="PQ47" s="23"/>
-      <c r="PR47" s="23"/>
-      <c r="PS47" s="23"/>
-      <c r="PT47" s="23"/>
-      <c r="PU47" s="23"/>
-      <c r="PV47" s="23"/>
-      <c r="PW47" s="23"/>
-      <c r="PX47" s="23"/>
-      <c r="PY47" s="23"/>
-      <c r="PZ47" s="23"/>
-      <c r="QA47" s="23"/>
-      <c r="QB47" s="23"/>
-      <c r="QC47" s="23"/>
-      <c r="QD47" s="23"/>
-      <c r="QE47" s="23"/>
-      <c r="QF47" s="23"/>
-      <c r="QG47" s="23"/>
-      <c r="QH47" s="23"/>
-      <c r="QI47" s="23"/>
-      <c r="QJ47" s="23"/>
-      <c r="QK47" s="23"/>
-      <c r="QL47" s="23"/>
-      <c r="QM47" s="23"/>
-      <c r="QN47" s="23"/>
-      <c r="QO47" s="23"/>
-      <c r="QP47" s="23"/>
-      <c r="QQ47" s="23"/>
-      <c r="QR47" s="23"/>
-      <c r="QS47" s="23"/>
-      <c r="QT47" s="23"/>
-      <c r="QU47" s="23"/>
-      <c r="QV47" s="23"/>
-      <c r="QW47" s="23"/>
-      <c r="QX47" s="23"/>
-      <c r="QY47" s="23"/>
-      <c r="QZ47" s="23"/>
-      <c r="RA47" s="23"/>
-      <c r="RB47" s="23"/>
-      <c r="RC47" s="23"/>
-      <c r="RD47" s="23"/>
-      <c r="RE47" s="23"/>
-      <c r="RF47" s="23"/>
-      <c r="RG47" s="23"/>
-      <c r="RH47" s="23"/>
-      <c r="RI47" s="23"/>
-      <c r="RJ47" s="23"/>
-      <c r="RK47" s="23"/>
-      <c r="RL47" s="23"/>
-      <c r="RM47" s="23"/>
-      <c r="RN47" s="23"/>
-      <c r="RO47" s="23"/>
-      <c r="RP47" s="23"/>
-      <c r="RQ47" s="23"/>
-      <c r="RR47" s="23"/>
-      <c r="RS47" s="23"/>
-      <c r="RT47" s="23"/>
-      <c r="RU47" s="23"/>
-      <c r="RV47" s="23"/>
-      <c r="RW47" s="23"/>
-      <c r="RX47" s="23"/>
-      <c r="RY47" s="23"/>
-      <c r="RZ47" s="23"/>
-      <c r="SA47" s="23"/>
-      <c r="SB47" s="23"/>
-      <c r="SC47" s="23"/>
-      <c r="SD47" s="23"/>
-      <c r="SE47" s="23"/>
-      <c r="SF47" s="23"/>
-      <c r="SG47" s="23"/>
-      <c r="SH47" s="23"/>
-      <c r="SI47" s="23"/>
-      <c r="SJ47" s="23"/>
-      <c r="SK47" s="23"/>
-      <c r="SL47" s="23"/>
-      <c r="SM47" s="23"/>
-      <c r="SN47" s="23"/>
-      <c r="SO47" s="23"/>
-      <c r="SP47" s="23"/>
-      <c r="SQ47" s="23"/>
-      <c r="SR47" s="23"/>
-      <c r="SS47" s="23"/>
-      <c r="ST47" s="23"/>
-      <c r="SU47" s="23"/>
-      <c r="SV47" s="23"/>
-      <c r="SW47" s="23"/>
-      <c r="SX47" s="23"/>
-      <c r="SY47" s="23"/>
-      <c r="SZ47" s="23"/>
-      <c r="TA47" s="23"/>
-      <c r="TB47" s="23"/>
-      <c r="TC47" s="23"/>
-      <c r="TD47" s="23"/>
-      <c r="TE47" s="23"/>
-      <c r="TF47" s="23"/>
-      <c r="TG47" s="23"/>
-      <c r="TH47" s="23"/>
-      <c r="TI47" s="23"/>
-      <c r="TJ47" s="23"/>
-      <c r="TK47" s="23"/>
-      <c r="TL47" s="23"/>
-      <c r="TM47" s="23"/>
-      <c r="TN47" s="23"/>
-      <c r="TO47" s="23"/>
-      <c r="TP47" s="23"/>
-      <c r="TQ47" s="23"/>
-      <c r="TR47" s="23"/>
-      <c r="TS47" s="23"/>
-      <c r="TT47" s="23"/>
-      <c r="TU47" s="23"/>
-      <c r="TV47" s="23"/>
-      <c r="TW47" s="23"/>
-      <c r="TX47" s="23"/>
-      <c r="TY47" s="23"/>
-      <c r="TZ47" s="23"/>
-      <c r="UA47" s="23"/>
-      <c r="UB47" s="23"/>
-      <c r="UC47" s="23"/>
-      <c r="UD47" s="23"/>
-      <c r="UE47" s="23"/>
-      <c r="UF47" s="23"/>
-      <c r="UG47" s="23"/>
-      <c r="UH47" s="23"/>
-      <c r="UI47" s="23"/>
-      <c r="UJ47" s="23"/>
-      <c r="UK47" s="23"/>
-      <c r="UL47" s="23"/>
-      <c r="UM47" s="23"/>
-      <c r="UN47" s="23"/>
-      <c r="UO47" s="23"/>
-      <c r="UP47" s="23"/>
-      <c r="UQ47" s="23"/>
-      <c r="UR47" s="23"/>
-      <c r="US47" s="23"/>
-      <c r="UT47" s="23"/>
-      <c r="UU47" s="23"/>
-      <c r="UV47" s="23"/>
-      <c r="UW47" s="23"/>
-      <c r="UX47" s="23"/>
-      <c r="UY47" s="23"/>
-      <c r="UZ47" s="23"/>
-      <c r="VA47" s="23"/>
-      <c r="VB47" s="23"/>
-      <c r="VC47" s="23"/>
-      <c r="VD47" s="23"/>
-      <c r="VE47" s="23"/>
-      <c r="VF47" s="23"/>
-      <c r="VG47" s="23"/>
-      <c r="VH47" s="23"/>
-      <c r="VI47" s="23"/>
-      <c r="VJ47" s="23"/>
-      <c r="VK47" s="23"/>
-      <c r="VL47" s="23"/>
-      <c r="VM47" s="23"/>
-      <c r="VN47" s="23"/>
-      <c r="VO47" s="23"/>
-      <c r="VP47" s="23"/>
-      <c r="VQ47" s="23"/>
-      <c r="VR47" s="23"/>
-      <c r="VS47" s="23"/>
-      <c r="VT47" s="23"/>
-      <c r="VU47" s="23"/>
-      <c r="VV47" s="23"/>
-      <c r="VW47" s="23"/>
-      <c r="VX47" s="23"/>
-      <c r="VY47" s="23"/>
-      <c r="VZ47" s="23"/>
-      <c r="WA47" s="23"/>
-      <c r="WB47" s="23"/>
-      <c r="WC47" s="23"/>
-      <c r="WD47" s="23"/>
-      <c r="WE47" s="23"/>
-      <c r="WF47" s="23"/>
-      <c r="WG47" s="23"/>
-      <c r="WH47" s="23"/>
-      <c r="WI47" s="23"/>
-      <c r="WJ47" s="23"/>
-      <c r="WK47" s="23"/>
-      <c r="WL47" s="23"/>
-      <c r="WM47" s="23"/>
-      <c r="WN47" s="23"/>
-      <c r="WO47" s="23"/>
-      <c r="WP47" s="23"/>
-      <c r="WQ47" s="23"/>
-      <c r="WR47" s="23"/>
-      <c r="WS47" s="23"/>
-      <c r="WT47" s="23"/>
-      <c r="WU47" s="23"/>
-      <c r="WV47" s="23"/>
-      <c r="WW47" s="23"/>
-      <c r="WX47" s="23"/>
-      <c r="WY47" s="23"/>
-      <c r="WZ47" s="23"/>
-      <c r="XA47" s="23"/>
-      <c r="XB47" s="23"/>
-      <c r="XC47" s="23"/>
-      <c r="XD47" s="23"/>
-      <c r="XE47" s="23"/>
-      <c r="XF47" s="23"/>
-      <c r="XG47" s="23"/>
-      <c r="XH47" s="23"/>
-      <c r="XI47" s="23"/>
-      <c r="XJ47" s="23"/>
-      <c r="XK47" s="23"/>
-      <c r="XL47" s="23"/>
-      <c r="XM47" s="23"/>
-      <c r="XN47" s="23"/>
-      <c r="XO47" s="23"/>
-      <c r="XP47" s="23"/>
-      <c r="XQ47" s="23"/>
-      <c r="XR47" s="23"/>
-      <c r="XS47" s="23"/>
-      <c r="XT47" s="23"/>
-      <c r="XU47" s="23"/>
-      <c r="XV47" s="23"/>
-      <c r="XW47" s="23"/>
-      <c r="XX47" s="23"/>
-      <c r="XY47" s="23"/>
-      <c r="XZ47" s="23"/>
-      <c r="YA47" s="23"/>
-      <c r="YB47" s="23"/>
-      <c r="YC47" s="23"/>
-      <c r="YD47" s="23"/>
-      <c r="YE47" s="23"/>
-      <c r="YF47" s="23"/>
-      <c r="YG47" s="23"/>
-      <c r="YH47" s="23"/>
-      <c r="YI47" s="23"/>
-      <c r="YJ47" s="23"/>
-      <c r="YK47" s="23"/>
-      <c r="YL47" s="23"/>
-      <c r="YM47" s="23"/>
-      <c r="YN47" s="23"/>
-      <c r="YO47" s="23"/>
-      <c r="YP47" s="23"/>
-      <c r="YQ47" s="23"/>
-      <c r="YR47" s="23"/>
-      <c r="YS47" s="23"/>
-      <c r="YT47" s="23"/>
-      <c r="YU47" s="23"/>
-      <c r="YV47" s="23"/>
-      <c r="YW47" s="23"/>
-      <c r="YX47" s="23"/>
-      <c r="YY47" s="23"/>
-      <c r="YZ47" s="23"/>
-      <c r="ZA47" s="23"/>
-      <c r="ZB47" s="23"/>
-      <c r="ZC47" s="23"/>
-      <c r="ZD47" s="23"/>
-      <c r="ZE47" s="23"/>
-      <c r="ZF47" s="23"/>
-      <c r="ZG47" s="23"/>
-      <c r="ZH47" s="23"/>
-      <c r="ZI47" s="23"/>
-      <c r="ZJ47" s="23"/>
-      <c r="ZK47" s="23"/>
-      <c r="ZL47" s="23"/>
-      <c r="ZM47" s="23"/>
-      <c r="ZN47" s="23"/>
-      <c r="ZO47" s="23"/>
-      <c r="ZP47" s="23"/>
-      <c r="ZQ47" s="23"/>
-      <c r="ZR47" s="23"/>
-      <c r="ZS47" s="23"/>
-      <c r="ZT47" s="23"/>
-      <c r="ZU47" s="23"/>
-      <c r="ZV47" s="23"/>
-      <c r="ZW47" s="23"/>
-      <c r="ZX47" s="23"/>
-      <c r="ZY47" s="23"/>
-      <c r="ZZ47" s="23"/>
-      <c r="AAA47" s="23"/>
-      <c r="AAB47" s="23"/>
-      <c r="AAC47" s="23"/>
-      <c r="AAD47" s="23"/>
-      <c r="AAE47" s="23"/>
-      <c r="AAF47" s="23"/>
-      <c r="AAG47" s="23"/>
-      <c r="AAH47" s="23"/>
-      <c r="AAI47" s="23"/>
-      <c r="AAJ47" s="23"/>
-      <c r="AAK47" s="23"/>
-      <c r="AAL47" s="23"/>
-      <c r="AAM47" s="23"/>
-      <c r="AAN47" s="23"/>
-      <c r="AAO47" s="23"/>
-      <c r="AAP47" s="23"/>
-      <c r="AAQ47" s="23"/>
-      <c r="AAR47" s="23"/>
-      <c r="AAS47" s="23"/>
-      <c r="AAT47" s="23"/>
-      <c r="AAU47" s="23"/>
-      <c r="AAV47" s="23"/>
-      <c r="AAW47" s="23"/>
-      <c r="AAX47" s="23"/>
-      <c r="AAY47" s="23"/>
-      <c r="AAZ47" s="23"/>
-      <c r="ABA47" s="23"/>
-      <c r="ABB47" s="23"/>
-      <c r="ABC47" s="23"/>
-      <c r="ABD47" s="23"/>
-      <c r="ABE47" s="23"/>
-      <c r="ABF47" s="23"/>
-      <c r="ABG47" s="23"/>
-      <c r="ABH47" s="23"/>
-      <c r="ABI47" s="23"/>
-      <c r="ABJ47" s="23"/>
-      <c r="ABK47" s="23"/>
-      <c r="ABL47" s="23"/>
-      <c r="ABM47" s="23"/>
-      <c r="ABN47" s="23"/>
-      <c r="ABO47" s="23"/>
-      <c r="ABP47" s="23"/>
-      <c r="ABQ47" s="23"/>
-      <c r="ABR47" s="23"/>
-      <c r="ABS47" s="23"/>
-      <c r="ABT47" s="23"/>
-      <c r="ABU47" s="23"/>
-      <c r="ABV47" s="23"/>
-      <c r="ABW47" s="23"/>
-      <c r="ABX47" s="23"/>
-      <c r="ABY47" s="23"/>
-      <c r="ABZ47" s="23"/>
-      <c r="ACA47" s="23"/>
-      <c r="ACB47" s="23"/>
-      <c r="ACC47" s="23"/>
-      <c r="ACD47" s="23"/>
-      <c r="ACE47" s="23"/>
-      <c r="ACF47" s="23"/>
-      <c r="ACG47" s="23"/>
-      <c r="ACH47" s="23"/>
-      <c r="ACI47" s="23"/>
-      <c r="ACJ47" s="23"/>
-      <c r="ACK47" s="23"/>
-      <c r="ACL47" s="23"/>
-      <c r="ACM47" s="23"/>
-      <c r="ACN47" s="23"/>
-      <c r="ACO47" s="23"/>
-      <c r="ACP47" s="23"/>
-      <c r="ACQ47" s="23"/>
-      <c r="ACR47" s="23"/>
-      <c r="ACS47" s="23"/>
-      <c r="ACT47" s="23"/>
-      <c r="ACU47" s="23"/>
-      <c r="ACV47" s="23"/>
-      <c r="ACW47" s="23"/>
-      <c r="ACX47" s="23"/>
-      <c r="ACY47" s="23"/>
-      <c r="ACZ47" s="23"/>
-      <c r="ADA47" s="23"/>
-      <c r="ADB47" s="23"/>
-      <c r="ADC47" s="23"/>
-      <c r="ADD47" s="23"/>
-      <c r="ADE47" s="23"/>
-      <c r="ADF47" s="23"/>
-      <c r="ADG47" s="23"/>
-      <c r="ADH47" s="23"/>
-      <c r="ADI47" s="23"/>
-      <c r="ADJ47" s="23"/>
-      <c r="ADK47" s="23"/>
-      <c r="ADL47" s="23"/>
-      <c r="ADM47" s="23"/>
-      <c r="ADN47" s="23"/>
-      <c r="ADO47" s="23"/>
-      <c r="ADP47" s="23"/>
-      <c r="ADQ47" s="23"/>
-      <c r="ADR47" s="23"/>
-      <c r="ADS47" s="23"/>
-      <c r="ADT47" s="23"/>
-      <c r="ADU47" s="23"/>
-      <c r="ADV47" s="23"/>
-      <c r="ADW47" s="23"/>
-      <c r="ADX47" s="23"/>
-      <c r="ADY47" s="23"/>
-      <c r="ADZ47" s="23"/>
-      <c r="AEA47" s="23"/>
-      <c r="AEB47" s="23"/>
-      <c r="AEC47" s="23"/>
-      <c r="AED47" s="23"/>
-      <c r="AEE47" s="23"/>
-      <c r="AEF47" s="23"/>
-      <c r="AEG47" s="23"/>
-      <c r="AEH47" s="23"/>
-      <c r="AEI47" s="23"/>
-      <c r="AEJ47" s="23"/>
-      <c r="AEK47" s="23"/>
-      <c r="AEL47" s="23"/>
-      <c r="AEM47" s="23"/>
-      <c r="AEN47" s="23"/>
-      <c r="AEO47" s="23"/>
-      <c r="AEP47" s="23"/>
-      <c r="AEQ47" s="23"/>
-      <c r="AER47" s="23"/>
-      <c r="AES47" s="23"/>
-      <c r="AET47" s="23"/>
-      <c r="AEU47" s="23"/>
-      <c r="AEV47" s="23"/>
-      <c r="AEW47" s="23"/>
-      <c r="AEX47" s="23"/>
-      <c r="AEY47" s="23"/>
-      <c r="AEZ47" s="23"/>
-      <c r="AFA47" s="23"/>
-      <c r="AFB47" s="23"/>
-      <c r="AFC47" s="23"/>
-      <c r="AFD47" s="23"/>
-      <c r="AFE47" s="23"/>
-      <c r="AFF47" s="23"/>
-      <c r="AFG47" s="23"/>
-      <c r="AFH47" s="23"/>
-      <c r="AFI47" s="23"/>
-      <c r="AFJ47" s="23"/>
-      <c r="AFK47" s="23"/>
-      <c r="AFL47" s="23"/>
-      <c r="AFM47" s="23"/>
-      <c r="AFN47" s="23"/>
-      <c r="AFO47" s="23"/>
-      <c r="AFP47" s="23"/>
-      <c r="AFQ47" s="23"/>
-      <c r="AFR47" s="23"/>
-      <c r="AFS47" s="23"/>
-      <c r="AFT47" s="23"/>
-      <c r="AFU47" s="23"/>
-      <c r="AFV47" s="23"/>
-      <c r="AFW47" s="23"/>
-      <c r="AFX47" s="23"/>
-      <c r="AFY47" s="23"/>
-      <c r="AFZ47" s="23"/>
-      <c r="AGA47" s="23"/>
-      <c r="AGB47" s="23"/>
-      <c r="AGC47" s="23"/>
-      <c r="AGD47" s="23"/>
-      <c r="AGE47" s="23"/>
-      <c r="AGF47" s="23"/>
-      <c r="AGG47" s="23"/>
-      <c r="AGH47" s="23"/>
-      <c r="AGI47" s="23"/>
-      <c r="AGJ47" s="23"/>
-      <c r="AGK47" s="23"/>
-      <c r="AGL47" s="23"/>
-      <c r="AGM47" s="23"/>
-      <c r="AGN47" s="23"/>
-      <c r="AGO47" s="23"/>
-      <c r="AGP47" s="23"/>
-      <c r="AGQ47" s="23"/>
-      <c r="AGR47" s="23"/>
-      <c r="AGS47" s="23"/>
-      <c r="AGT47" s="23"/>
-      <c r="AGU47" s="23"/>
-      <c r="AGV47" s="23"/>
-      <c r="AGW47" s="23"/>
-      <c r="AGX47" s="23"/>
-      <c r="AGY47" s="23"/>
-      <c r="AGZ47" s="23"/>
-      <c r="AHA47" s="23"/>
-      <c r="AHB47" s="23"/>
-      <c r="AHC47" s="23"/>
-      <c r="AHD47" s="23"/>
-      <c r="AHE47" s="23"/>
-      <c r="AHF47" s="23"/>
-      <c r="AHG47" s="23"/>
-      <c r="AHH47" s="23"/>
-      <c r="AHI47" s="23"/>
-      <c r="AHJ47" s="23"/>
-      <c r="AHK47" s="23"/>
-      <c r="AHL47" s="23"/>
-      <c r="AHM47" s="23"/>
-      <c r="AHN47" s="23"/>
-      <c r="AHO47" s="23"/>
-      <c r="AHP47" s="23"/>
-      <c r="AHQ47" s="23"/>
-      <c r="AHR47" s="23"/>
-      <c r="AHS47" s="23"/>
-      <c r="AHT47" s="23"/>
-      <c r="AHU47" s="23"/>
-      <c r="AHV47" s="23"/>
-      <c r="AHW47" s="23"/>
-      <c r="AHX47" s="23"/>
-      <c r="AHY47" s="23"/>
-      <c r="AHZ47" s="23"/>
-      <c r="AIA47" s="23"/>
-      <c r="AIB47" s="23"/>
-      <c r="AIC47" s="23"/>
-      <c r="AID47" s="23"/>
-      <c r="AIE47" s="23"/>
-      <c r="AIF47" s="23"/>
-      <c r="AIG47" s="23"/>
-      <c r="AIH47" s="23"/>
-      <c r="AII47" s="23"/>
-      <c r="AIJ47" s="23"/>
-      <c r="AIK47" s="23"/>
-      <c r="AIL47" s="23"/>
-      <c r="AIM47" s="23"/>
-      <c r="AIN47" s="23"/>
-      <c r="AIO47" s="23"/>
-      <c r="AIP47" s="23"/>
-      <c r="AIQ47" s="23"/>
-      <c r="AIR47" s="23"/>
-      <c r="AIS47" s="23"/>
-      <c r="AIT47" s="23"/>
-      <c r="AIU47" s="23"/>
-      <c r="AIV47" s="23"/>
-      <c r="AIW47" s="23"/>
-      <c r="AIX47" s="23"/>
-      <c r="AIY47" s="23"/>
-      <c r="AIZ47" s="23"/>
-      <c r="AJA47" s="23"/>
-      <c r="AJB47" s="23"/>
-      <c r="AJC47" s="23"/>
-      <c r="AJD47" s="23"/>
-      <c r="AJE47" s="23"/>
-      <c r="AJF47" s="23"/>
-      <c r="AJG47" s="23"/>
-      <c r="AJH47" s="23"/>
-      <c r="AJI47" s="23"/>
-      <c r="AJJ47" s="23"/>
-      <c r="AJK47" s="23"/>
-      <c r="AJL47" s="23"/>
-      <c r="AJM47" s="23"/>
-      <c r="AJN47" s="23"/>
-      <c r="AJO47" s="23"/>
-      <c r="AJP47" s="23"/>
-      <c r="AJQ47" s="23"/>
-      <c r="AJR47" s="23"/>
-      <c r="AJS47" s="23"/>
-      <c r="AJT47" s="23"/>
-      <c r="AJU47" s="23"/>
-      <c r="AJV47" s="23"/>
-      <c r="AJW47" s="23"/>
-      <c r="AJX47" s="23"/>
-      <c r="AJY47" s="23"/>
-      <c r="AJZ47" s="23"/>
-      <c r="AKA47" s="23"/>
-      <c r="AKB47" s="23"/>
-      <c r="AKC47" s="23"/>
-      <c r="AKD47" s="23"/>
-      <c r="AKE47" s="23"/>
-      <c r="AKF47" s="23"/>
-      <c r="AKG47" s="23"/>
-      <c r="AKH47" s="23"/>
-      <c r="AKI47" s="23"/>
-      <c r="AKJ47" s="23"/>
-      <c r="AKK47" s="23"/>
-      <c r="AKL47" s="23"/>
-      <c r="AKM47" s="23"/>
-      <c r="AKN47" s="23"/>
-      <c r="AKO47" s="23"/>
-      <c r="AKP47" s="23"/>
-      <c r="AKQ47" s="23"/>
-      <c r="AKR47" s="23"/>
-      <c r="AKS47" s="23"/>
-      <c r="AKT47" s="23"/>
-      <c r="AKU47" s="23"/>
-      <c r="AKV47" s="23"/>
-      <c r="AKW47" s="23"/>
-      <c r="AKX47" s="23"/>
-      <c r="AKY47" s="23"/>
-      <c r="AKZ47" s="23"/>
-      <c r="ALA47" s="23"/>
-      <c r="ALB47" s="23"/>
-      <c r="ALC47" s="23"/>
-      <c r="ALD47" s="23"/>
-      <c r="ALE47" s="23"/>
-      <c r="ALF47" s="23"/>
-      <c r="ALG47" s="23"/>
-      <c r="ALH47" s="23"/>
-      <c r="ALI47" s="23"/>
-      <c r="ALJ47" s="23"/>
-      <c r="ALK47" s="23"/>
-      <c r="ALL47" s="23"/>
-      <c r="ALM47" s="23"/>
-      <c r="ALN47" s="23"/>
-      <c r="ALO47" s="23"/>
-      <c r="ALP47" s="23"/>
-      <c r="ALQ47" s="23"/>
-      <c r="ALR47" s="23"/>
-      <c r="ALS47" s="23"/>
-      <c r="ALT47" s="23"/>
-      <c r="ALU47" s="23"/>
-      <c r="ALV47" s="23"/>
-      <c r="ALW47" s="23"/>
-      <c r="ALX47" s="23"/>
-      <c r="ALY47" s="23"/>
-      <c r="ALZ47" s="23"/>
-      <c r="AMA47" s="23"/>
-      <c r="AMB47" s="23"/>
-      <c r="AMC47" s="23"/>
-      <c r="AMD47" s="23"/>
-      <c r="AME47" s="23"/>
-      <c r="AMF47" s="23"/>
-      <c r="AMG47" s="23"/>
-      <c r="AMH47" s="23"/>
-      <c r="AMI47" s="23"/>
-      <c r="AMJ47" s="23"/>
-      <c r="AMK47" s="23"/>
-    </row>
-    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="27"/>
+    </row>
+    <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="5" t="s">
         <v>282</v>
       </c>
@@ -5068,1013 +4064,8 @@
       <c r="T48" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="U48" s="27"/>
-      <c r="V48" s="27"/>
-      <c r="W48" s="27"/>
-      <c r="X48" s="27"/>
-      <c r="Y48" s="27"/>
-      <c r="Z48" s="27"/>
-      <c r="AA48" s="27"/>
-      <c r="AB48" s="27"/>
-      <c r="AC48" s="27"/>
-      <c r="AD48" s="27"/>
-      <c r="AE48" s="27"/>
-      <c r="AF48" s="27"/>
-      <c r="AG48" s="27"/>
-      <c r="AH48" s="27"/>
-      <c r="AI48" s="27"/>
-      <c r="AJ48" s="27"/>
-      <c r="AK48" s="27"/>
-      <c r="AL48" s="27"/>
-      <c r="AM48" s="27"/>
-      <c r="AN48" s="27"/>
-      <c r="AO48" s="27"/>
-      <c r="AP48" s="27"/>
-      <c r="AQ48" s="27"/>
-      <c r="AR48" s="27"/>
-      <c r="AS48" s="27"/>
-      <c r="AT48" s="27"/>
-      <c r="AU48" s="27"/>
-      <c r="AV48" s="27"/>
-      <c r="AW48" s="27"/>
-      <c r="AX48" s="27"/>
-      <c r="AY48" s="27"/>
-      <c r="AZ48" s="27"/>
-      <c r="BA48" s="27"/>
-      <c r="BB48" s="27"/>
-      <c r="BC48" s="27"/>
-      <c r="BD48" s="27"/>
-      <c r="BE48" s="27"/>
-      <c r="BF48" s="27"/>
-      <c r="BG48" s="27"/>
-      <c r="BH48" s="27"/>
-      <c r="BI48" s="27"/>
-      <c r="BJ48" s="27"/>
-      <c r="BK48" s="27"/>
-      <c r="BL48" s="27"/>
-      <c r="BM48" s="27"/>
-      <c r="BN48" s="27"/>
-      <c r="BO48" s="27"/>
-      <c r="BP48" s="27"/>
-      <c r="BQ48" s="27"/>
-      <c r="BR48" s="27"/>
-      <c r="BS48" s="27"/>
-      <c r="BT48" s="27"/>
-      <c r="BU48" s="27"/>
-      <c r="BV48" s="27"/>
-      <c r="BW48" s="27"/>
-      <c r="BX48" s="27"/>
-      <c r="BY48" s="27"/>
-      <c r="BZ48" s="27"/>
-      <c r="CA48" s="27"/>
-      <c r="CB48" s="27"/>
-      <c r="CC48" s="27"/>
-      <c r="CD48" s="27"/>
-      <c r="CE48" s="27"/>
-      <c r="CF48" s="27"/>
-      <c r="CG48" s="27"/>
-      <c r="CH48" s="27"/>
-      <c r="CI48" s="27"/>
-      <c r="CJ48" s="27"/>
-      <c r="CK48" s="27"/>
-      <c r="CL48" s="27"/>
-      <c r="CM48" s="27"/>
-      <c r="CN48" s="27"/>
-      <c r="CO48" s="27"/>
-      <c r="CP48" s="27"/>
-      <c r="CQ48" s="27"/>
-      <c r="CR48" s="27"/>
-      <c r="CS48" s="27"/>
-      <c r="CT48" s="27"/>
-      <c r="CU48" s="27"/>
-      <c r="CV48" s="27"/>
-      <c r="CW48" s="27"/>
-      <c r="CX48" s="27"/>
-      <c r="CY48" s="27"/>
-      <c r="CZ48" s="27"/>
-      <c r="DA48" s="27"/>
-      <c r="DB48" s="27"/>
-      <c r="DC48" s="27"/>
-      <c r="DD48" s="27"/>
-      <c r="DE48" s="27"/>
-      <c r="DF48" s="27"/>
-      <c r="DG48" s="27"/>
-      <c r="DH48" s="27"/>
-      <c r="DI48" s="27"/>
-      <c r="DJ48" s="27"/>
-      <c r="DK48" s="27"/>
-      <c r="DL48" s="27"/>
-      <c r="DM48" s="27"/>
-      <c r="DN48" s="27"/>
-      <c r="DO48" s="27"/>
-      <c r="DP48" s="27"/>
-      <c r="DQ48" s="27"/>
-      <c r="DR48" s="27"/>
-      <c r="DS48" s="27"/>
-      <c r="DT48" s="27"/>
-      <c r="DU48" s="27"/>
-      <c r="DV48" s="27"/>
-      <c r="DW48" s="27"/>
-      <c r="DX48" s="27"/>
-      <c r="DY48" s="27"/>
-      <c r="DZ48" s="27"/>
-      <c r="EA48" s="27"/>
-      <c r="EB48" s="27"/>
-      <c r="EC48" s="27"/>
-      <c r="ED48" s="27"/>
-      <c r="EE48" s="27"/>
-      <c r="EF48" s="27"/>
-      <c r="EG48" s="27"/>
-      <c r="EH48" s="27"/>
-      <c r="EI48" s="27"/>
-      <c r="EJ48" s="27"/>
-      <c r="EK48" s="27"/>
-      <c r="EL48" s="27"/>
-      <c r="EM48" s="27"/>
-      <c r="EN48" s="27"/>
-      <c r="EO48" s="27"/>
-      <c r="EP48" s="27"/>
-      <c r="EQ48" s="27"/>
-      <c r="ER48" s="27"/>
-      <c r="ES48" s="27"/>
-      <c r="ET48" s="27"/>
-      <c r="EU48" s="27"/>
-      <c r="EV48" s="27"/>
-      <c r="EW48" s="27"/>
-      <c r="EX48" s="27"/>
-      <c r="EY48" s="27"/>
-      <c r="EZ48" s="27"/>
-      <c r="FA48" s="27"/>
-      <c r="FB48" s="27"/>
-      <c r="FC48" s="27"/>
-      <c r="FD48" s="27"/>
-      <c r="FE48" s="27"/>
-      <c r="FF48" s="27"/>
-      <c r="FG48" s="27"/>
-      <c r="FH48" s="27"/>
-      <c r="FI48" s="27"/>
-      <c r="FJ48" s="27"/>
-      <c r="FK48" s="27"/>
-      <c r="FL48" s="27"/>
-      <c r="FM48" s="27"/>
-      <c r="FN48" s="27"/>
-      <c r="FO48" s="27"/>
-      <c r="FP48" s="27"/>
-      <c r="FQ48" s="27"/>
-      <c r="FR48" s="27"/>
-      <c r="FS48" s="27"/>
-      <c r="FT48" s="27"/>
-      <c r="FU48" s="27"/>
-      <c r="FV48" s="27"/>
-      <c r="FW48" s="27"/>
-      <c r="FX48" s="27"/>
-      <c r="FY48" s="27"/>
-      <c r="FZ48" s="27"/>
-      <c r="GA48" s="27"/>
-      <c r="GB48" s="27"/>
-      <c r="GC48" s="27"/>
-      <c r="GD48" s="27"/>
-      <c r="GE48" s="27"/>
-      <c r="GF48" s="27"/>
-      <c r="GG48" s="27"/>
-      <c r="GH48" s="27"/>
-      <c r="GI48" s="27"/>
-      <c r="GJ48" s="27"/>
-      <c r="GK48" s="27"/>
-      <c r="GL48" s="27"/>
-      <c r="GM48" s="27"/>
-      <c r="GN48" s="27"/>
-      <c r="GO48" s="27"/>
-      <c r="GP48" s="27"/>
-      <c r="GQ48" s="27"/>
-      <c r="GR48" s="27"/>
-      <c r="GS48" s="27"/>
-      <c r="GT48" s="27"/>
-      <c r="GU48" s="27"/>
-      <c r="GV48" s="27"/>
-      <c r="GW48" s="27"/>
-      <c r="GX48" s="27"/>
-      <c r="GY48" s="27"/>
-      <c r="GZ48" s="27"/>
-      <c r="HA48" s="27"/>
-      <c r="HB48" s="27"/>
-      <c r="HC48" s="27"/>
-      <c r="HD48" s="27"/>
-      <c r="HE48" s="27"/>
-      <c r="HF48" s="27"/>
-      <c r="HG48" s="27"/>
-      <c r="HH48" s="27"/>
-      <c r="HI48" s="27"/>
-      <c r="HJ48" s="27"/>
-      <c r="HK48" s="27"/>
-      <c r="HL48" s="27"/>
-      <c r="HM48" s="27"/>
-      <c r="HN48" s="27"/>
-      <c r="HO48" s="27"/>
-      <c r="HP48" s="27"/>
-      <c r="HQ48" s="27"/>
-      <c r="HR48" s="27"/>
-      <c r="HS48" s="27"/>
-      <c r="HT48" s="27"/>
-      <c r="HU48" s="27"/>
-      <c r="HV48" s="27"/>
-      <c r="HW48" s="27"/>
-      <c r="HX48" s="27"/>
-      <c r="HY48" s="27"/>
-      <c r="HZ48" s="27"/>
-      <c r="IA48" s="27"/>
-      <c r="IB48" s="27"/>
-      <c r="IC48" s="27"/>
-      <c r="ID48" s="27"/>
-      <c r="IE48" s="27"/>
-      <c r="IF48" s="27"/>
-      <c r="IG48" s="27"/>
-      <c r="IH48" s="27"/>
-      <c r="II48" s="27"/>
-      <c r="IJ48" s="27"/>
-      <c r="IK48" s="27"/>
-      <c r="IL48" s="27"/>
-      <c r="IM48" s="27"/>
-      <c r="IN48" s="27"/>
-      <c r="IO48" s="27"/>
-      <c r="IP48" s="27"/>
-      <c r="IQ48" s="27"/>
-      <c r="IR48" s="27"/>
-      <c r="IS48" s="27"/>
-      <c r="IT48" s="27"/>
-      <c r="IU48" s="27"/>
-      <c r="IV48" s="27"/>
-      <c r="IW48" s="27"/>
-      <c r="IX48" s="27"/>
-      <c r="IY48" s="27"/>
-      <c r="IZ48" s="27"/>
-      <c r="JA48" s="27"/>
-      <c r="JB48" s="27"/>
-      <c r="JC48" s="27"/>
-      <c r="JD48" s="27"/>
-      <c r="JE48" s="27"/>
-      <c r="JF48" s="27"/>
-      <c r="JG48" s="27"/>
-      <c r="JH48" s="27"/>
-      <c r="JI48" s="27"/>
-      <c r="JJ48" s="27"/>
-      <c r="JK48" s="27"/>
-      <c r="JL48" s="27"/>
-      <c r="JM48" s="27"/>
-      <c r="JN48" s="27"/>
-      <c r="JO48" s="27"/>
-      <c r="JP48" s="27"/>
-      <c r="JQ48" s="27"/>
-      <c r="JR48" s="27"/>
-      <c r="JS48" s="27"/>
-      <c r="JT48" s="27"/>
-      <c r="JU48" s="27"/>
-      <c r="JV48" s="27"/>
-      <c r="JW48" s="27"/>
-      <c r="JX48" s="27"/>
-      <c r="JY48" s="27"/>
-      <c r="JZ48" s="27"/>
-      <c r="KA48" s="27"/>
-      <c r="KB48" s="27"/>
-      <c r="KC48" s="27"/>
-      <c r="KD48" s="27"/>
-      <c r="KE48" s="27"/>
-      <c r="KF48" s="27"/>
-      <c r="KG48" s="27"/>
-      <c r="KH48" s="27"/>
-      <c r="KI48" s="27"/>
-      <c r="KJ48" s="27"/>
-      <c r="KK48" s="27"/>
-      <c r="KL48" s="27"/>
-      <c r="KM48" s="27"/>
-      <c r="KN48" s="27"/>
-      <c r="KO48" s="27"/>
-      <c r="KP48" s="27"/>
-      <c r="KQ48" s="27"/>
-      <c r="KR48" s="27"/>
-      <c r="KS48" s="27"/>
-      <c r="KT48" s="27"/>
-      <c r="KU48" s="27"/>
-      <c r="KV48" s="27"/>
-      <c r="KW48" s="27"/>
-      <c r="KX48" s="27"/>
-      <c r="KY48" s="27"/>
-      <c r="KZ48" s="27"/>
-      <c r="LA48" s="27"/>
-      <c r="LB48" s="27"/>
-      <c r="LC48" s="27"/>
-      <c r="LD48" s="27"/>
-      <c r="LE48" s="27"/>
-      <c r="LF48" s="27"/>
-      <c r="LG48" s="27"/>
-      <c r="LH48" s="27"/>
-      <c r="LI48" s="27"/>
-      <c r="LJ48" s="27"/>
-      <c r="LK48" s="27"/>
-      <c r="LL48" s="27"/>
-      <c r="LM48" s="27"/>
-      <c r="LN48" s="27"/>
-      <c r="LO48" s="27"/>
-      <c r="LP48" s="27"/>
-      <c r="LQ48" s="27"/>
-      <c r="LR48" s="27"/>
-      <c r="LS48" s="27"/>
-      <c r="LT48" s="27"/>
-      <c r="LU48" s="27"/>
-      <c r="LV48" s="27"/>
-      <c r="LW48" s="27"/>
-      <c r="LX48" s="27"/>
-      <c r="LY48" s="27"/>
-      <c r="LZ48" s="27"/>
-      <c r="MA48" s="27"/>
-      <c r="MB48" s="27"/>
-      <c r="MC48" s="27"/>
-      <c r="MD48" s="27"/>
-      <c r="ME48" s="27"/>
-      <c r="MF48" s="27"/>
-      <c r="MG48" s="27"/>
-      <c r="MH48" s="27"/>
-      <c r="MI48" s="27"/>
-      <c r="MJ48" s="27"/>
-      <c r="MK48" s="27"/>
-      <c r="ML48" s="27"/>
-      <c r="MM48" s="27"/>
-      <c r="MN48" s="27"/>
-      <c r="MO48" s="27"/>
-      <c r="MP48" s="27"/>
-      <c r="MQ48" s="27"/>
-      <c r="MR48" s="27"/>
-      <c r="MS48" s="27"/>
-      <c r="MT48" s="27"/>
-      <c r="MU48" s="27"/>
-      <c r="MV48" s="27"/>
-      <c r="MW48" s="27"/>
-      <c r="MX48" s="27"/>
-      <c r="MY48" s="27"/>
-      <c r="MZ48" s="27"/>
-      <c r="NA48" s="27"/>
-      <c r="NB48" s="27"/>
-      <c r="NC48" s="27"/>
-      <c r="ND48" s="27"/>
-      <c r="NE48" s="27"/>
-      <c r="NF48" s="27"/>
-      <c r="NG48" s="27"/>
-      <c r="NH48" s="27"/>
-      <c r="NI48" s="27"/>
-      <c r="NJ48" s="27"/>
-      <c r="NK48" s="27"/>
-      <c r="NL48" s="27"/>
-      <c r="NM48" s="27"/>
-      <c r="NN48" s="27"/>
-      <c r="NO48" s="27"/>
-      <c r="NP48" s="27"/>
-      <c r="NQ48" s="27"/>
-      <c r="NR48" s="27"/>
-      <c r="NS48" s="27"/>
-      <c r="NT48" s="27"/>
-      <c r="NU48" s="27"/>
-      <c r="NV48" s="27"/>
-      <c r="NW48" s="27"/>
-      <c r="NX48" s="27"/>
-      <c r="NY48" s="27"/>
-      <c r="NZ48" s="27"/>
-      <c r="OA48" s="27"/>
-      <c r="OB48" s="27"/>
-      <c r="OC48" s="27"/>
-      <c r="OD48" s="27"/>
-      <c r="OE48" s="27"/>
-      <c r="OF48" s="27"/>
-      <c r="OG48" s="27"/>
-      <c r="OH48" s="27"/>
-      <c r="OI48" s="27"/>
-      <c r="OJ48" s="27"/>
-      <c r="OK48" s="27"/>
-      <c r="OL48" s="27"/>
-      <c r="OM48" s="27"/>
-      <c r="ON48" s="27"/>
-      <c r="OO48" s="27"/>
-      <c r="OP48" s="27"/>
-      <c r="OQ48" s="27"/>
-      <c r="OR48" s="27"/>
-      <c r="OS48" s="27"/>
-      <c r="OT48" s="27"/>
-      <c r="OU48" s="27"/>
-      <c r="OV48" s="27"/>
-      <c r="OW48" s="27"/>
-      <c r="OX48" s="27"/>
-      <c r="OY48" s="27"/>
-      <c r="OZ48" s="27"/>
-      <c r="PA48" s="27"/>
-      <c r="PB48" s="27"/>
-      <c r="PC48" s="27"/>
-      <c r="PD48" s="27"/>
-      <c r="PE48" s="27"/>
-      <c r="PF48" s="27"/>
-      <c r="PG48" s="27"/>
-      <c r="PH48" s="27"/>
-      <c r="PI48" s="27"/>
-      <c r="PJ48" s="27"/>
-      <c r="PK48" s="27"/>
-      <c r="PL48" s="27"/>
-      <c r="PM48" s="27"/>
-      <c r="PN48" s="27"/>
-      <c r="PO48" s="27"/>
-      <c r="PP48" s="27"/>
-      <c r="PQ48" s="27"/>
-      <c r="PR48" s="27"/>
-      <c r="PS48" s="27"/>
-      <c r="PT48" s="27"/>
-      <c r="PU48" s="27"/>
-      <c r="PV48" s="27"/>
-      <c r="PW48" s="27"/>
-      <c r="PX48" s="27"/>
-      <c r="PY48" s="27"/>
-      <c r="PZ48" s="27"/>
-      <c r="QA48" s="27"/>
-      <c r="QB48" s="27"/>
-      <c r="QC48" s="27"/>
-      <c r="QD48" s="27"/>
-      <c r="QE48" s="27"/>
-      <c r="QF48" s="27"/>
-      <c r="QG48" s="27"/>
-      <c r="QH48" s="27"/>
-      <c r="QI48" s="27"/>
-      <c r="QJ48" s="27"/>
-      <c r="QK48" s="27"/>
-      <c r="QL48" s="27"/>
-      <c r="QM48" s="27"/>
-      <c r="QN48" s="27"/>
-      <c r="QO48" s="27"/>
-      <c r="QP48" s="27"/>
-      <c r="QQ48" s="27"/>
-      <c r="QR48" s="27"/>
-      <c r="QS48" s="27"/>
-      <c r="QT48" s="27"/>
-      <c r="QU48" s="27"/>
-      <c r="QV48" s="27"/>
-      <c r="QW48" s="27"/>
-      <c r="QX48" s="27"/>
-      <c r="QY48" s="27"/>
-      <c r="QZ48" s="27"/>
-      <c r="RA48" s="27"/>
-      <c r="RB48" s="27"/>
-      <c r="RC48" s="27"/>
-      <c r="RD48" s="27"/>
-      <c r="RE48" s="27"/>
-      <c r="RF48" s="27"/>
-      <c r="RG48" s="27"/>
-      <c r="RH48" s="27"/>
-      <c r="RI48" s="27"/>
-      <c r="RJ48" s="27"/>
-      <c r="RK48" s="27"/>
-      <c r="RL48" s="27"/>
-      <c r="RM48" s="27"/>
-      <c r="RN48" s="27"/>
-      <c r="RO48" s="27"/>
-      <c r="RP48" s="27"/>
-      <c r="RQ48" s="27"/>
-      <c r="RR48" s="27"/>
-      <c r="RS48" s="27"/>
-      <c r="RT48" s="27"/>
-      <c r="RU48" s="27"/>
-      <c r="RV48" s="27"/>
-      <c r="RW48" s="27"/>
-      <c r="RX48" s="27"/>
-      <c r="RY48" s="27"/>
-      <c r="RZ48" s="27"/>
-      <c r="SA48" s="27"/>
-      <c r="SB48" s="27"/>
-      <c r="SC48" s="27"/>
-      <c r="SD48" s="27"/>
-      <c r="SE48" s="27"/>
-      <c r="SF48" s="27"/>
-      <c r="SG48" s="27"/>
-      <c r="SH48" s="27"/>
-      <c r="SI48" s="27"/>
-      <c r="SJ48" s="27"/>
-      <c r="SK48" s="27"/>
-      <c r="SL48" s="27"/>
-      <c r="SM48" s="27"/>
-      <c r="SN48" s="27"/>
-      <c r="SO48" s="27"/>
-      <c r="SP48" s="27"/>
-      <c r="SQ48" s="27"/>
-      <c r="SR48" s="27"/>
-      <c r="SS48" s="27"/>
-      <c r="ST48" s="27"/>
-      <c r="SU48" s="27"/>
-      <c r="SV48" s="27"/>
-      <c r="SW48" s="27"/>
-      <c r="SX48" s="27"/>
-      <c r="SY48" s="27"/>
-      <c r="SZ48" s="27"/>
-      <c r="TA48" s="27"/>
-      <c r="TB48" s="27"/>
-      <c r="TC48" s="27"/>
-      <c r="TD48" s="27"/>
-      <c r="TE48" s="27"/>
-      <c r="TF48" s="27"/>
-      <c r="TG48" s="27"/>
-      <c r="TH48" s="27"/>
-      <c r="TI48" s="27"/>
-      <c r="TJ48" s="27"/>
-      <c r="TK48" s="27"/>
-      <c r="TL48" s="27"/>
-      <c r="TM48" s="27"/>
-      <c r="TN48" s="27"/>
-      <c r="TO48" s="27"/>
-      <c r="TP48" s="27"/>
-      <c r="TQ48" s="27"/>
-      <c r="TR48" s="27"/>
-      <c r="TS48" s="27"/>
-      <c r="TT48" s="27"/>
-      <c r="TU48" s="27"/>
-      <c r="TV48" s="27"/>
-      <c r="TW48" s="27"/>
-      <c r="TX48" s="27"/>
-      <c r="TY48" s="27"/>
-      <c r="TZ48" s="27"/>
-      <c r="UA48" s="27"/>
-      <c r="UB48" s="27"/>
-      <c r="UC48" s="27"/>
-      <c r="UD48" s="27"/>
-      <c r="UE48" s="27"/>
-      <c r="UF48" s="27"/>
-      <c r="UG48" s="27"/>
-      <c r="UH48" s="27"/>
-      <c r="UI48" s="27"/>
-      <c r="UJ48" s="27"/>
-      <c r="UK48" s="27"/>
-      <c r="UL48" s="27"/>
-      <c r="UM48" s="27"/>
-      <c r="UN48" s="27"/>
-      <c r="UO48" s="27"/>
-      <c r="UP48" s="27"/>
-      <c r="UQ48" s="27"/>
-      <c r="UR48" s="27"/>
-      <c r="US48" s="27"/>
-      <c r="UT48" s="27"/>
-      <c r="UU48" s="27"/>
-      <c r="UV48" s="27"/>
-      <c r="UW48" s="27"/>
-      <c r="UX48" s="27"/>
-      <c r="UY48" s="27"/>
-      <c r="UZ48" s="27"/>
-      <c r="VA48" s="27"/>
-      <c r="VB48" s="27"/>
-      <c r="VC48" s="27"/>
-      <c r="VD48" s="27"/>
-      <c r="VE48" s="27"/>
-      <c r="VF48" s="27"/>
-      <c r="VG48" s="27"/>
-      <c r="VH48" s="27"/>
-      <c r="VI48" s="27"/>
-      <c r="VJ48" s="27"/>
-      <c r="VK48" s="27"/>
-      <c r="VL48" s="27"/>
-      <c r="VM48" s="27"/>
-      <c r="VN48" s="27"/>
-      <c r="VO48" s="27"/>
-      <c r="VP48" s="27"/>
-      <c r="VQ48" s="27"/>
-      <c r="VR48" s="27"/>
-      <c r="VS48" s="27"/>
-      <c r="VT48" s="27"/>
-      <c r="VU48" s="27"/>
-      <c r="VV48" s="27"/>
-      <c r="VW48" s="27"/>
-      <c r="VX48" s="27"/>
-      <c r="VY48" s="27"/>
-      <c r="VZ48" s="27"/>
-      <c r="WA48" s="27"/>
-      <c r="WB48" s="27"/>
-      <c r="WC48" s="27"/>
-      <c r="WD48" s="27"/>
-      <c r="WE48" s="27"/>
-      <c r="WF48" s="27"/>
-      <c r="WG48" s="27"/>
-      <c r="WH48" s="27"/>
-      <c r="WI48" s="27"/>
-      <c r="WJ48" s="27"/>
-      <c r="WK48" s="27"/>
-      <c r="WL48" s="27"/>
-      <c r="WM48" s="27"/>
-      <c r="WN48" s="27"/>
-      <c r="WO48" s="27"/>
-      <c r="WP48" s="27"/>
-      <c r="WQ48" s="27"/>
-      <c r="WR48" s="27"/>
-      <c r="WS48" s="27"/>
-      <c r="WT48" s="27"/>
-      <c r="WU48" s="27"/>
-      <c r="WV48" s="27"/>
-      <c r="WW48" s="27"/>
-      <c r="WX48" s="27"/>
-      <c r="WY48" s="27"/>
-      <c r="WZ48" s="27"/>
-      <c r="XA48" s="27"/>
-      <c r="XB48" s="27"/>
-      <c r="XC48" s="27"/>
-      <c r="XD48" s="27"/>
-      <c r="XE48" s="27"/>
-      <c r="XF48" s="27"/>
-      <c r="XG48" s="27"/>
-      <c r="XH48" s="27"/>
-      <c r="XI48" s="27"/>
-      <c r="XJ48" s="27"/>
-      <c r="XK48" s="27"/>
-      <c r="XL48" s="27"/>
-      <c r="XM48" s="27"/>
-      <c r="XN48" s="27"/>
-      <c r="XO48" s="27"/>
-      <c r="XP48" s="27"/>
-      <c r="XQ48" s="27"/>
-      <c r="XR48" s="27"/>
-      <c r="XS48" s="27"/>
-      <c r="XT48" s="27"/>
-      <c r="XU48" s="27"/>
-      <c r="XV48" s="27"/>
-      <c r="XW48" s="27"/>
-      <c r="XX48" s="27"/>
-      <c r="XY48" s="27"/>
-      <c r="XZ48" s="27"/>
-      <c r="YA48" s="27"/>
-      <c r="YB48" s="27"/>
-      <c r="YC48" s="27"/>
-      <c r="YD48" s="27"/>
-      <c r="YE48" s="27"/>
-      <c r="YF48" s="27"/>
-      <c r="YG48" s="27"/>
-      <c r="YH48" s="27"/>
-      <c r="YI48" s="27"/>
-      <c r="YJ48" s="27"/>
-      <c r="YK48" s="27"/>
-      <c r="YL48" s="27"/>
-      <c r="YM48" s="27"/>
-      <c r="YN48" s="27"/>
-      <c r="YO48" s="27"/>
-      <c r="YP48" s="27"/>
-      <c r="YQ48" s="27"/>
-      <c r="YR48" s="27"/>
-      <c r="YS48" s="27"/>
-      <c r="YT48" s="27"/>
-      <c r="YU48" s="27"/>
-      <c r="YV48" s="27"/>
-      <c r="YW48" s="27"/>
-      <c r="YX48" s="27"/>
-      <c r="YY48" s="27"/>
-      <c r="YZ48" s="27"/>
-      <c r="ZA48" s="27"/>
-      <c r="ZB48" s="27"/>
-      <c r="ZC48" s="27"/>
-      <c r="ZD48" s="27"/>
-      <c r="ZE48" s="27"/>
-      <c r="ZF48" s="27"/>
-      <c r="ZG48" s="27"/>
-      <c r="ZH48" s="27"/>
-      <c r="ZI48" s="27"/>
-      <c r="ZJ48" s="27"/>
-      <c r="ZK48" s="27"/>
-      <c r="ZL48" s="27"/>
-      <c r="ZM48" s="27"/>
-      <c r="ZN48" s="27"/>
-      <c r="ZO48" s="27"/>
-      <c r="ZP48" s="27"/>
-      <c r="ZQ48" s="27"/>
-      <c r="ZR48" s="27"/>
-      <c r="ZS48" s="27"/>
-      <c r="ZT48" s="27"/>
-      <c r="ZU48" s="27"/>
-      <c r="ZV48" s="27"/>
-      <c r="ZW48" s="27"/>
-      <c r="ZX48" s="27"/>
-      <c r="ZY48" s="27"/>
-      <c r="ZZ48" s="27"/>
-      <c r="AAA48" s="27"/>
-      <c r="AAB48" s="27"/>
-      <c r="AAC48" s="27"/>
-      <c r="AAD48" s="27"/>
-      <c r="AAE48" s="27"/>
-      <c r="AAF48" s="27"/>
-      <c r="AAG48" s="27"/>
-      <c r="AAH48" s="27"/>
-      <c r="AAI48" s="27"/>
-      <c r="AAJ48" s="27"/>
-      <c r="AAK48" s="27"/>
-      <c r="AAL48" s="27"/>
-      <c r="AAM48" s="27"/>
-      <c r="AAN48" s="27"/>
-      <c r="AAO48" s="27"/>
-      <c r="AAP48" s="27"/>
-      <c r="AAQ48" s="27"/>
-      <c r="AAR48" s="27"/>
-      <c r="AAS48" s="27"/>
-      <c r="AAT48" s="27"/>
-      <c r="AAU48" s="27"/>
-      <c r="AAV48" s="27"/>
-      <c r="AAW48" s="27"/>
-      <c r="AAX48" s="27"/>
-      <c r="AAY48" s="27"/>
-      <c r="AAZ48" s="27"/>
-      <c r="ABA48" s="27"/>
-      <c r="ABB48" s="27"/>
-      <c r="ABC48" s="27"/>
-      <c r="ABD48" s="27"/>
-      <c r="ABE48" s="27"/>
-      <c r="ABF48" s="27"/>
-      <c r="ABG48" s="27"/>
-      <c r="ABH48" s="27"/>
-      <c r="ABI48" s="27"/>
-      <c r="ABJ48" s="27"/>
-      <c r="ABK48" s="27"/>
-      <c r="ABL48" s="27"/>
-      <c r="ABM48" s="27"/>
-      <c r="ABN48" s="27"/>
-      <c r="ABO48" s="27"/>
-      <c r="ABP48" s="27"/>
-      <c r="ABQ48" s="27"/>
-      <c r="ABR48" s="27"/>
-      <c r="ABS48" s="27"/>
-      <c r="ABT48" s="27"/>
-      <c r="ABU48" s="27"/>
-      <c r="ABV48" s="27"/>
-      <c r="ABW48" s="27"/>
-      <c r="ABX48" s="27"/>
-      <c r="ABY48" s="27"/>
-      <c r="ABZ48" s="27"/>
-      <c r="ACA48" s="27"/>
-      <c r="ACB48" s="27"/>
-      <c r="ACC48" s="27"/>
-      <c r="ACD48" s="27"/>
-      <c r="ACE48" s="27"/>
-      <c r="ACF48" s="27"/>
-      <c r="ACG48" s="27"/>
-      <c r="ACH48" s="27"/>
-      <c r="ACI48" s="27"/>
-      <c r="ACJ48" s="27"/>
-      <c r="ACK48" s="27"/>
-      <c r="ACL48" s="27"/>
-      <c r="ACM48" s="27"/>
-      <c r="ACN48" s="27"/>
-      <c r="ACO48" s="27"/>
-      <c r="ACP48" s="27"/>
-      <c r="ACQ48" s="27"/>
-      <c r="ACR48" s="27"/>
-      <c r="ACS48" s="27"/>
-      <c r="ACT48" s="27"/>
-      <c r="ACU48" s="27"/>
-      <c r="ACV48" s="27"/>
-      <c r="ACW48" s="27"/>
-      <c r="ACX48" s="27"/>
-      <c r="ACY48" s="27"/>
-      <c r="ACZ48" s="27"/>
-      <c r="ADA48" s="27"/>
-      <c r="ADB48" s="27"/>
-      <c r="ADC48" s="27"/>
-      <c r="ADD48" s="27"/>
-      <c r="ADE48" s="27"/>
-      <c r="ADF48" s="27"/>
-      <c r="ADG48" s="27"/>
-      <c r="ADH48" s="27"/>
-      <c r="ADI48" s="27"/>
-      <c r="ADJ48" s="27"/>
-      <c r="ADK48" s="27"/>
-      <c r="ADL48" s="27"/>
-      <c r="ADM48" s="27"/>
-      <c r="ADN48" s="27"/>
-      <c r="ADO48" s="27"/>
-      <c r="ADP48" s="27"/>
-      <c r="ADQ48" s="27"/>
-      <c r="ADR48" s="27"/>
-      <c r="ADS48" s="27"/>
-      <c r="ADT48" s="27"/>
-      <c r="ADU48" s="27"/>
-      <c r="ADV48" s="27"/>
-      <c r="ADW48" s="27"/>
-      <c r="ADX48" s="27"/>
-      <c r="ADY48" s="27"/>
-      <c r="ADZ48" s="27"/>
-      <c r="AEA48" s="27"/>
-      <c r="AEB48" s="27"/>
-      <c r="AEC48" s="27"/>
-      <c r="AED48" s="27"/>
-      <c r="AEE48" s="27"/>
-      <c r="AEF48" s="27"/>
-      <c r="AEG48" s="27"/>
-      <c r="AEH48" s="27"/>
-      <c r="AEI48" s="27"/>
-      <c r="AEJ48" s="27"/>
-      <c r="AEK48" s="27"/>
-      <c r="AEL48" s="27"/>
-      <c r="AEM48" s="27"/>
-      <c r="AEN48" s="27"/>
-      <c r="AEO48" s="27"/>
-      <c r="AEP48" s="27"/>
-      <c r="AEQ48" s="27"/>
-      <c r="AER48" s="27"/>
-      <c r="AES48" s="27"/>
-      <c r="AET48" s="27"/>
-      <c r="AEU48" s="27"/>
-      <c r="AEV48" s="27"/>
-      <c r="AEW48" s="27"/>
-      <c r="AEX48" s="27"/>
-      <c r="AEY48" s="27"/>
-      <c r="AEZ48" s="27"/>
-      <c r="AFA48" s="27"/>
-      <c r="AFB48" s="27"/>
-      <c r="AFC48" s="27"/>
-      <c r="AFD48" s="27"/>
-      <c r="AFE48" s="27"/>
-      <c r="AFF48" s="27"/>
-      <c r="AFG48" s="27"/>
-      <c r="AFH48" s="27"/>
-      <c r="AFI48" s="27"/>
-      <c r="AFJ48" s="27"/>
-      <c r="AFK48" s="27"/>
-      <c r="AFL48" s="27"/>
-      <c r="AFM48" s="27"/>
-      <c r="AFN48" s="27"/>
-      <c r="AFO48" s="27"/>
-      <c r="AFP48" s="27"/>
-      <c r="AFQ48" s="27"/>
-      <c r="AFR48" s="27"/>
-      <c r="AFS48" s="27"/>
-      <c r="AFT48" s="27"/>
-      <c r="AFU48" s="27"/>
-      <c r="AFV48" s="27"/>
-      <c r="AFW48" s="27"/>
-      <c r="AFX48" s="27"/>
-      <c r="AFY48" s="27"/>
-      <c r="AFZ48" s="27"/>
-      <c r="AGA48" s="27"/>
-      <c r="AGB48" s="27"/>
-      <c r="AGC48" s="27"/>
-      <c r="AGD48" s="27"/>
-      <c r="AGE48" s="27"/>
-      <c r="AGF48" s="27"/>
-      <c r="AGG48" s="27"/>
-      <c r="AGH48" s="27"/>
-      <c r="AGI48" s="27"/>
-      <c r="AGJ48" s="27"/>
-      <c r="AGK48" s="27"/>
-      <c r="AGL48" s="27"/>
-      <c r="AGM48" s="27"/>
-      <c r="AGN48" s="27"/>
-      <c r="AGO48" s="27"/>
-      <c r="AGP48" s="27"/>
-      <c r="AGQ48" s="27"/>
-      <c r="AGR48" s="27"/>
-      <c r="AGS48" s="27"/>
-      <c r="AGT48" s="27"/>
-      <c r="AGU48" s="27"/>
-      <c r="AGV48" s="27"/>
-      <c r="AGW48" s="27"/>
-      <c r="AGX48" s="27"/>
-      <c r="AGY48" s="27"/>
-      <c r="AGZ48" s="27"/>
-      <c r="AHA48" s="27"/>
-      <c r="AHB48" s="27"/>
-      <c r="AHC48" s="27"/>
-      <c r="AHD48" s="27"/>
-      <c r="AHE48" s="27"/>
-      <c r="AHF48" s="27"/>
-      <c r="AHG48" s="27"/>
-      <c r="AHH48" s="27"/>
-      <c r="AHI48" s="27"/>
-      <c r="AHJ48" s="27"/>
-      <c r="AHK48" s="27"/>
-      <c r="AHL48" s="27"/>
-      <c r="AHM48" s="27"/>
-      <c r="AHN48" s="27"/>
-      <c r="AHO48" s="27"/>
-      <c r="AHP48" s="27"/>
-      <c r="AHQ48" s="27"/>
-      <c r="AHR48" s="27"/>
-      <c r="AHS48" s="27"/>
-      <c r="AHT48" s="27"/>
-      <c r="AHU48" s="27"/>
-      <c r="AHV48" s="27"/>
-      <c r="AHW48" s="27"/>
-      <c r="AHX48" s="27"/>
-      <c r="AHY48" s="27"/>
-      <c r="AHZ48" s="27"/>
-      <c r="AIA48" s="27"/>
-      <c r="AIB48" s="27"/>
-      <c r="AIC48" s="27"/>
-      <c r="AID48" s="27"/>
-      <c r="AIE48" s="27"/>
-      <c r="AIF48" s="27"/>
-      <c r="AIG48" s="27"/>
-      <c r="AIH48" s="27"/>
-      <c r="AII48" s="27"/>
-      <c r="AIJ48" s="27"/>
-      <c r="AIK48" s="27"/>
-      <c r="AIL48" s="27"/>
-      <c r="AIM48" s="27"/>
-      <c r="AIN48" s="27"/>
-      <c r="AIO48" s="27"/>
-      <c r="AIP48" s="27"/>
-      <c r="AIQ48" s="27"/>
-      <c r="AIR48" s="27"/>
-      <c r="AIS48" s="27"/>
-      <c r="AIT48" s="27"/>
-      <c r="AIU48" s="27"/>
-      <c r="AIV48" s="27"/>
-      <c r="AIW48" s="27"/>
-      <c r="AIX48" s="27"/>
-      <c r="AIY48" s="27"/>
-      <c r="AIZ48" s="27"/>
-      <c r="AJA48" s="27"/>
-      <c r="AJB48" s="27"/>
-      <c r="AJC48" s="27"/>
-      <c r="AJD48" s="27"/>
-      <c r="AJE48" s="27"/>
-      <c r="AJF48" s="27"/>
-      <c r="AJG48" s="27"/>
-      <c r="AJH48" s="27"/>
-      <c r="AJI48" s="27"/>
-      <c r="AJJ48" s="27"/>
-      <c r="AJK48" s="27"/>
-      <c r="AJL48" s="27"/>
-      <c r="AJM48" s="27"/>
-      <c r="AJN48" s="27"/>
-      <c r="AJO48" s="27"/>
-      <c r="AJP48" s="27"/>
-      <c r="AJQ48" s="27"/>
-      <c r="AJR48" s="27"/>
-      <c r="AJS48" s="27"/>
-      <c r="AJT48" s="27"/>
-      <c r="AJU48" s="27"/>
-      <c r="AJV48" s="27"/>
-      <c r="AJW48" s="27"/>
-      <c r="AJX48" s="27"/>
-      <c r="AJY48" s="27"/>
-      <c r="AJZ48" s="27"/>
-      <c r="AKA48" s="27"/>
-      <c r="AKB48" s="27"/>
-      <c r="AKC48" s="27"/>
-      <c r="AKD48" s="27"/>
-      <c r="AKE48" s="27"/>
-      <c r="AKF48" s="27"/>
-      <c r="AKG48" s="27"/>
-      <c r="AKH48" s="27"/>
-      <c r="AKI48" s="27"/>
-      <c r="AKJ48" s="27"/>
-      <c r="AKK48" s="27"/>
-      <c r="AKL48" s="27"/>
-      <c r="AKM48" s="27"/>
-      <c r="AKN48" s="27"/>
-      <c r="AKO48" s="27"/>
-      <c r="AKP48" s="27"/>
-      <c r="AKQ48" s="27"/>
-      <c r="AKR48" s="27"/>
-      <c r="AKS48" s="27"/>
-      <c r="AKT48" s="27"/>
-      <c r="AKU48" s="27"/>
-      <c r="AKV48" s="27"/>
-      <c r="AKW48" s="27"/>
-      <c r="AKX48" s="27"/>
-      <c r="AKY48" s="27"/>
-      <c r="AKZ48" s="27"/>
-      <c r="ALA48" s="27"/>
-      <c r="ALB48" s="27"/>
-      <c r="ALC48" s="27"/>
-      <c r="ALD48" s="27"/>
-      <c r="ALE48" s="27"/>
-      <c r="ALF48" s="27"/>
-      <c r="ALG48" s="27"/>
-      <c r="ALH48" s="27"/>
-      <c r="ALI48" s="27"/>
-      <c r="ALJ48" s="27"/>
-      <c r="ALK48" s="27"/>
-      <c r="ALL48" s="27"/>
-      <c r="ALM48" s="27"/>
-      <c r="ALN48" s="27"/>
-      <c r="ALO48" s="27"/>
-      <c r="ALP48" s="27"/>
-      <c r="ALQ48" s="27"/>
-      <c r="ALR48" s="27"/>
-      <c r="ALS48" s="27"/>
-      <c r="ALT48" s="27"/>
-      <c r="ALU48" s="27"/>
-      <c r="ALV48" s="27"/>
-      <c r="ALW48" s="27"/>
-      <c r="ALX48" s="27"/>
-      <c r="ALY48" s="27"/>
-      <c r="ALZ48" s="27"/>
-      <c r="AMA48" s="27"/>
-      <c r="AMB48" s="27"/>
-      <c r="AMC48" s="27"/>
-      <c r="AMD48" s="27"/>
-      <c r="AME48" s="27"/>
-      <c r="AMF48" s="27"/>
-      <c r="AMG48" s="27"/>
-      <c r="AMH48" s="27"/>
-      <c r="AMI48" s="27"/>
-      <c r="AMJ48" s="27"/>
-      <c r="AMK48" s="27"/>
-    </row>
-    <row r="49" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
         <v>210</v>
       </c>
@@ -6114,10 +4105,8 @@
       <c r="T49" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="U49" s="23"/>
-    </row>
-    <row r="50" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="23"/>
+    </row>
+    <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="5" t="s">
         <v>279</v>
       </c>
@@ -6163,7 +4152,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="5" t="s">
         <v>214</v>
       </c>
@@ -6209,7 +4198,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="5" t="s">
         <v>245</v>
       </c>
@@ -6255,7 +4244,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:20" ht="32" x14ac:dyDescent="0.2">
       <c r="B53" s="5" t="s">
         <v>242</v>
       </c>
@@ -6301,7 +4290,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:20" ht="32" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="s">
         <v>235</v>
       </c>
@@ -6348,8 +4337,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="2:20" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="s">
         <v>186</v>
       </c>
@@ -6388,1072 +4377,49 @@
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="32" t="s">
+    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="C62" s="32"/>
-    </row>
-    <row r="63" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="33" t="s">
+      <c r="C62" s="30"/>
+    </row>
+    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="C63" s="33"/>
-    </row>
-    <row r="64" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="33" t="s">
+      <c r="C63" s="31"/>
+    </row>
+    <row r="64" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="C64" s="33"/>
-    </row>
-    <row r="65" spans="1:1025" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="34" t="s">
+      <c r="C64" s="31"/>
+    </row>
+    <row r="65" spans="2:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="C65" s="34"/>
-    </row>
-    <row r="66" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="B66" s="34" t="s">
+      <c r="C65" s="32"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B66" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="C66" s="34"/>
-    </row>
-    <row r="67" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A67" s="26"/>
-      <c r="B67" s="34" t="s">
+      <c r="C66" s="32"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B67" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="C67" s="34"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="26"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="26"/>
-      <c r="K67" s="26"/>
-      <c r="L67" s="26"/>
-      <c r="M67" s="26"/>
-      <c r="N67" s="26"/>
-      <c r="O67" s="26"/>
-      <c r="P67" s="26"/>
-      <c r="Q67" s="26"/>
-      <c r="R67" s="26"/>
-      <c r="S67" s="26"/>
-      <c r="T67" s="26"/>
-      <c r="U67" s="26"/>
-      <c r="V67" s="26"/>
-      <c r="W67" s="26"/>
-      <c r="X67" s="26"/>
-      <c r="Y67" s="26"/>
-      <c r="Z67" s="26"/>
-      <c r="AA67" s="26"/>
-      <c r="AB67" s="26"/>
-      <c r="AC67" s="26"/>
-      <c r="AD67" s="26"/>
-      <c r="AE67" s="26"/>
-      <c r="AF67" s="26"/>
-      <c r="AG67" s="26"/>
-      <c r="AH67" s="26"/>
-      <c r="AI67" s="26"/>
-      <c r="AJ67" s="26"/>
-      <c r="AK67" s="26"/>
-      <c r="AL67" s="26"/>
-      <c r="AM67" s="26"/>
-      <c r="AN67" s="26"/>
-      <c r="AO67" s="26"/>
-      <c r="AP67" s="26"/>
-      <c r="AQ67" s="26"/>
-      <c r="AR67" s="26"/>
-      <c r="AS67" s="26"/>
-      <c r="AT67" s="26"/>
-      <c r="AU67" s="26"/>
-      <c r="AV67" s="26"/>
-      <c r="AW67" s="26"/>
-      <c r="AX67" s="26"/>
-      <c r="AY67" s="26"/>
-      <c r="AZ67" s="26"/>
-      <c r="BA67" s="26"/>
-      <c r="BB67" s="26"/>
-      <c r="BC67" s="26"/>
-      <c r="BD67" s="26"/>
-      <c r="BE67" s="26"/>
-      <c r="BF67" s="26"/>
-      <c r="BG67" s="26"/>
-      <c r="BH67" s="26"/>
-      <c r="BI67" s="26"/>
-      <c r="BJ67" s="26"/>
-      <c r="BK67" s="26"/>
-      <c r="BL67" s="26"/>
-      <c r="BM67" s="26"/>
-      <c r="BN67" s="26"/>
-      <c r="BO67" s="26"/>
-      <c r="BP67" s="26"/>
-      <c r="BQ67" s="26"/>
-      <c r="BR67" s="26"/>
-      <c r="BS67" s="26"/>
-      <c r="BT67" s="26"/>
-      <c r="BU67" s="26"/>
-      <c r="BV67" s="26"/>
-      <c r="BW67" s="26"/>
-      <c r="BX67" s="26"/>
-      <c r="BY67" s="26"/>
-      <c r="BZ67" s="26"/>
-      <c r="CA67" s="26"/>
-      <c r="CB67" s="26"/>
-      <c r="CC67" s="26"/>
-      <c r="CD67" s="26"/>
-      <c r="CE67" s="26"/>
-      <c r="CF67" s="26"/>
-      <c r="CG67" s="26"/>
-      <c r="CH67" s="26"/>
-      <c r="CI67" s="26"/>
-      <c r="CJ67" s="26"/>
-      <c r="CK67" s="26"/>
-      <c r="CL67" s="26"/>
-      <c r="CM67" s="26"/>
-      <c r="CN67" s="26"/>
-      <c r="CO67" s="26"/>
-      <c r="CP67" s="26"/>
-      <c r="CQ67" s="26"/>
-      <c r="CR67" s="26"/>
-      <c r="CS67" s="26"/>
-      <c r="CT67" s="26"/>
-      <c r="CU67" s="26"/>
-      <c r="CV67" s="26"/>
-      <c r="CW67" s="26"/>
-      <c r="CX67" s="26"/>
-      <c r="CY67" s="26"/>
-      <c r="CZ67" s="26"/>
-      <c r="DA67" s="26"/>
-      <c r="DB67" s="26"/>
-      <c r="DC67" s="26"/>
-      <c r="DD67" s="26"/>
-      <c r="DE67" s="26"/>
-      <c r="DF67" s="26"/>
-      <c r="DG67" s="26"/>
-      <c r="DH67" s="26"/>
-      <c r="DI67" s="26"/>
-      <c r="DJ67" s="26"/>
-      <c r="DK67" s="26"/>
-      <c r="DL67" s="26"/>
-      <c r="DM67" s="26"/>
-      <c r="DN67" s="26"/>
-      <c r="DO67" s="26"/>
-      <c r="DP67" s="26"/>
-      <c r="DQ67" s="26"/>
-      <c r="DR67" s="26"/>
-      <c r="DS67" s="26"/>
-      <c r="DT67" s="26"/>
-      <c r="DU67" s="26"/>
-      <c r="DV67" s="26"/>
-      <c r="DW67" s="26"/>
-      <c r="DX67" s="26"/>
-      <c r="DY67" s="26"/>
-      <c r="DZ67" s="26"/>
-      <c r="EA67" s="26"/>
-      <c r="EB67" s="26"/>
-      <c r="EC67" s="26"/>
-      <c r="ED67" s="26"/>
-      <c r="EE67" s="26"/>
-      <c r="EF67" s="26"/>
-      <c r="EG67" s="26"/>
-      <c r="EH67" s="26"/>
-      <c r="EI67" s="26"/>
-      <c r="EJ67" s="26"/>
-      <c r="EK67" s="26"/>
-      <c r="EL67" s="26"/>
-      <c r="EM67" s="26"/>
-      <c r="EN67" s="26"/>
-      <c r="EO67" s="26"/>
-      <c r="EP67" s="26"/>
-      <c r="EQ67" s="26"/>
-      <c r="ER67" s="26"/>
-      <c r="ES67" s="26"/>
-      <c r="ET67" s="26"/>
-      <c r="EU67" s="26"/>
-      <c r="EV67" s="26"/>
-      <c r="EW67" s="26"/>
-      <c r="EX67" s="26"/>
-      <c r="EY67" s="26"/>
-      <c r="EZ67" s="26"/>
-      <c r="FA67" s="26"/>
-      <c r="FB67" s="26"/>
-      <c r="FC67" s="26"/>
-      <c r="FD67" s="26"/>
-      <c r="FE67" s="26"/>
-      <c r="FF67" s="26"/>
-      <c r="FG67" s="26"/>
-      <c r="FH67" s="26"/>
-      <c r="FI67" s="26"/>
-      <c r="FJ67" s="26"/>
-      <c r="FK67" s="26"/>
-      <c r="FL67" s="26"/>
-      <c r="FM67" s="26"/>
-      <c r="FN67" s="26"/>
-      <c r="FO67" s="26"/>
-      <c r="FP67" s="26"/>
-      <c r="FQ67" s="26"/>
-      <c r="FR67" s="26"/>
-      <c r="FS67" s="26"/>
-      <c r="FT67" s="26"/>
-      <c r="FU67" s="26"/>
-      <c r="FV67" s="26"/>
-      <c r="FW67" s="26"/>
-      <c r="FX67" s="26"/>
-      <c r="FY67" s="26"/>
-      <c r="FZ67" s="26"/>
-      <c r="GA67" s="26"/>
-      <c r="GB67" s="26"/>
-      <c r="GC67" s="26"/>
-      <c r="GD67" s="26"/>
-      <c r="GE67" s="26"/>
-      <c r="GF67" s="26"/>
-      <c r="GG67" s="26"/>
-      <c r="GH67" s="26"/>
-      <c r="GI67" s="26"/>
-      <c r="GJ67" s="26"/>
-      <c r="GK67" s="26"/>
-      <c r="GL67" s="26"/>
-      <c r="GM67" s="26"/>
-      <c r="GN67" s="26"/>
-      <c r="GO67" s="26"/>
-      <c r="GP67" s="26"/>
-      <c r="GQ67" s="26"/>
-      <c r="GR67" s="26"/>
-      <c r="GS67" s="26"/>
-      <c r="GT67" s="26"/>
-      <c r="GU67" s="26"/>
-      <c r="GV67" s="26"/>
-      <c r="GW67" s="26"/>
-      <c r="GX67" s="26"/>
-      <c r="GY67" s="26"/>
-      <c r="GZ67" s="26"/>
-      <c r="HA67" s="26"/>
-      <c r="HB67" s="26"/>
-      <c r="HC67" s="26"/>
-      <c r="HD67" s="26"/>
-      <c r="HE67" s="26"/>
-      <c r="HF67" s="26"/>
-      <c r="HG67" s="26"/>
-      <c r="HH67" s="26"/>
-      <c r="HI67" s="26"/>
-      <c r="HJ67" s="26"/>
-      <c r="HK67" s="26"/>
-      <c r="HL67" s="26"/>
-      <c r="HM67" s="26"/>
-      <c r="HN67" s="26"/>
-      <c r="HO67" s="26"/>
-      <c r="HP67" s="26"/>
-      <c r="HQ67" s="26"/>
-      <c r="HR67" s="26"/>
-      <c r="HS67" s="26"/>
-      <c r="HT67" s="26"/>
-      <c r="HU67" s="26"/>
-      <c r="HV67" s="26"/>
-      <c r="HW67" s="26"/>
-      <c r="HX67" s="26"/>
-      <c r="HY67" s="26"/>
-      <c r="HZ67" s="26"/>
-      <c r="IA67" s="26"/>
-      <c r="IB67" s="26"/>
-      <c r="IC67" s="26"/>
-      <c r="ID67" s="26"/>
-      <c r="IE67" s="26"/>
-      <c r="IF67" s="26"/>
-      <c r="IG67" s="26"/>
-      <c r="IH67" s="26"/>
-      <c r="II67" s="26"/>
-      <c r="IJ67" s="26"/>
-      <c r="IK67" s="26"/>
-      <c r="IL67" s="26"/>
-      <c r="IM67" s="26"/>
-      <c r="IN67" s="26"/>
-      <c r="IO67" s="26"/>
-      <c r="IP67" s="26"/>
-      <c r="IQ67" s="26"/>
-      <c r="IR67" s="26"/>
-      <c r="IS67" s="26"/>
-      <c r="IT67" s="26"/>
-      <c r="IU67" s="26"/>
-      <c r="IV67" s="26"/>
-      <c r="IW67" s="26"/>
-      <c r="IX67" s="26"/>
-      <c r="IY67" s="26"/>
-      <c r="IZ67" s="26"/>
-      <c r="JA67" s="26"/>
-      <c r="JB67" s="26"/>
-      <c r="JC67" s="26"/>
-      <c r="JD67" s="26"/>
-      <c r="JE67" s="26"/>
-      <c r="JF67" s="26"/>
-      <c r="JG67" s="26"/>
-      <c r="JH67" s="26"/>
-      <c r="JI67" s="26"/>
-      <c r="JJ67" s="26"/>
-      <c r="JK67" s="26"/>
-      <c r="JL67" s="26"/>
-      <c r="JM67" s="26"/>
-      <c r="JN67" s="26"/>
-      <c r="JO67" s="26"/>
-      <c r="JP67" s="26"/>
-      <c r="JQ67" s="26"/>
-      <c r="JR67" s="26"/>
-      <c r="JS67" s="26"/>
-      <c r="JT67" s="26"/>
-      <c r="JU67" s="26"/>
-      <c r="JV67" s="26"/>
-      <c r="JW67" s="26"/>
-      <c r="JX67" s="26"/>
-      <c r="JY67" s="26"/>
-      <c r="JZ67" s="26"/>
-      <c r="KA67" s="26"/>
-      <c r="KB67" s="26"/>
-      <c r="KC67" s="26"/>
-      <c r="KD67" s="26"/>
-      <c r="KE67" s="26"/>
-      <c r="KF67" s="26"/>
-      <c r="KG67" s="26"/>
-      <c r="KH67" s="26"/>
-      <c r="KI67" s="26"/>
-      <c r="KJ67" s="26"/>
-      <c r="KK67" s="26"/>
-      <c r="KL67" s="26"/>
-      <c r="KM67" s="26"/>
-      <c r="KN67" s="26"/>
-      <c r="KO67" s="26"/>
-      <c r="KP67" s="26"/>
-      <c r="KQ67" s="26"/>
-      <c r="KR67" s="26"/>
-      <c r="KS67" s="26"/>
-      <c r="KT67" s="26"/>
-      <c r="KU67" s="26"/>
-      <c r="KV67" s="26"/>
-      <c r="KW67" s="26"/>
-      <c r="KX67" s="26"/>
-      <c r="KY67" s="26"/>
-      <c r="KZ67" s="26"/>
-      <c r="LA67" s="26"/>
-      <c r="LB67" s="26"/>
-      <c r="LC67" s="26"/>
-      <c r="LD67" s="26"/>
-      <c r="LE67" s="26"/>
-      <c r="LF67" s="26"/>
-      <c r="LG67" s="26"/>
-      <c r="LH67" s="26"/>
-      <c r="LI67" s="26"/>
-      <c r="LJ67" s="26"/>
-      <c r="LK67" s="26"/>
-      <c r="LL67" s="26"/>
-      <c r="LM67" s="26"/>
-      <c r="LN67" s="26"/>
-      <c r="LO67" s="26"/>
-      <c r="LP67" s="26"/>
-      <c r="LQ67" s="26"/>
-      <c r="LR67" s="26"/>
-      <c r="LS67" s="26"/>
-      <c r="LT67" s="26"/>
-      <c r="LU67" s="26"/>
-      <c r="LV67" s="26"/>
-      <c r="LW67" s="26"/>
-      <c r="LX67" s="26"/>
-      <c r="LY67" s="26"/>
-      <c r="LZ67" s="26"/>
-      <c r="MA67" s="26"/>
-      <c r="MB67" s="26"/>
-      <c r="MC67" s="26"/>
-      <c r="MD67" s="26"/>
-      <c r="ME67" s="26"/>
-      <c r="MF67" s="26"/>
-      <c r="MG67" s="26"/>
-      <c r="MH67" s="26"/>
-      <c r="MI67" s="26"/>
-      <c r="MJ67" s="26"/>
-      <c r="MK67" s="26"/>
-      <c r="ML67" s="26"/>
-      <c r="MM67" s="26"/>
-      <c r="MN67" s="26"/>
-      <c r="MO67" s="26"/>
-      <c r="MP67" s="26"/>
-      <c r="MQ67" s="26"/>
-      <c r="MR67" s="26"/>
-      <c r="MS67" s="26"/>
-      <c r="MT67" s="26"/>
-      <c r="MU67" s="26"/>
-      <c r="MV67" s="26"/>
-      <c r="MW67" s="26"/>
-      <c r="MX67" s="26"/>
-      <c r="MY67" s="26"/>
-      <c r="MZ67" s="26"/>
-      <c r="NA67" s="26"/>
-      <c r="NB67" s="26"/>
-      <c r="NC67" s="26"/>
-      <c r="ND67" s="26"/>
-      <c r="NE67" s="26"/>
-      <c r="NF67" s="26"/>
-      <c r="NG67" s="26"/>
-      <c r="NH67" s="26"/>
-      <c r="NI67" s="26"/>
-      <c r="NJ67" s="26"/>
-      <c r="NK67" s="26"/>
-      <c r="NL67" s="26"/>
-      <c r="NM67" s="26"/>
-      <c r="NN67" s="26"/>
-      <c r="NO67" s="26"/>
-      <c r="NP67" s="26"/>
-      <c r="NQ67" s="26"/>
-      <c r="NR67" s="26"/>
-      <c r="NS67" s="26"/>
-      <c r="NT67" s="26"/>
-      <c r="NU67" s="26"/>
-      <c r="NV67" s="26"/>
-      <c r="NW67" s="26"/>
-      <c r="NX67" s="26"/>
-      <c r="NY67" s="26"/>
-      <c r="NZ67" s="26"/>
-      <c r="OA67" s="26"/>
-      <c r="OB67" s="26"/>
-      <c r="OC67" s="26"/>
-      <c r="OD67" s="26"/>
-      <c r="OE67" s="26"/>
-      <c r="OF67" s="26"/>
-      <c r="OG67" s="26"/>
-      <c r="OH67" s="26"/>
-      <c r="OI67" s="26"/>
-      <c r="OJ67" s="26"/>
-      <c r="OK67" s="26"/>
-      <c r="OL67" s="26"/>
-      <c r="OM67" s="26"/>
-      <c r="ON67" s="26"/>
-      <c r="OO67" s="26"/>
-      <c r="OP67" s="26"/>
-      <c r="OQ67" s="26"/>
-      <c r="OR67" s="26"/>
-      <c r="OS67" s="26"/>
-      <c r="OT67" s="26"/>
-      <c r="OU67" s="26"/>
-      <c r="OV67" s="26"/>
-      <c r="OW67" s="26"/>
-      <c r="OX67" s="26"/>
-      <c r="OY67" s="26"/>
-      <c r="OZ67" s="26"/>
-      <c r="PA67" s="26"/>
-      <c r="PB67" s="26"/>
-      <c r="PC67" s="26"/>
-      <c r="PD67" s="26"/>
-      <c r="PE67" s="26"/>
-      <c r="PF67" s="26"/>
-      <c r="PG67" s="26"/>
-      <c r="PH67" s="26"/>
-      <c r="PI67" s="26"/>
-      <c r="PJ67" s="26"/>
-      <c r="PK67" s="26"/>
-      <c r="PL67" s="26"/>
-      <c r="PM67" s="26"/>
-      <c r="PN67" s="26"/>
-      <c r="PO67" s="26"/>
-      <c r="PP67" s="26"/>
-      <c r="PQ67" s="26"/>
-      <c r="PR67" s="26"/>
-      <c r="PS67" s="26"/>
-      <c r="PT67" s="26"/>
-      <c r="PU67" s="26"/>
-      <c r="PV67" s="26"/>
-      <c r="PW67" s="26"/>
-      <c r="PX67" s="26"/>
-      <c r="PY67" s="26"/>
-      <c r="PZ67" s="26"/>
-      <c r="QA67" s="26"/>
-      <c r="QB67" s="26"/>
-      <c r="QC67" s="26"/>
-      <c r="QD67" s="26"/>
-      <c r="QE67" s="26"/>
-      <c r="QF67" s="26"/>
-      <c r="QG67" s="26"/>
-      <c r="QH67" s="26"/>
-      <c r="QI67" s="26"/>
-      <c r="QJ67" s="26"/>
-      <c r="QK67" s="26"/>
-      <c r="QL67" s="26"/>
-      <c r="QM67" s="26"/>
-      <c r="QN67" s="26"/>
-      <c r="QO67" s="26"/>
-      <c r="QP67" s="26"/>
-      <c r="QQ67" s="26"/>
-      <c r="QR67" s="26"/>
-      <c r="QS67" s="26"/>
-      <c r="QT67" s="26"/>
-      <c r="QU67" s="26"/>
-      <c r="QV67" s="26"/>
-      <c r="QW67" s="26"/>
-      <c r="QX67" s="26"/>
-      <c r="QY67" s="26"/>
-      <c r="QZ67" s="26"/>
-      <c r="RA67" s="26"/>
-      <c r="RB67" s="26"/>
-      <c r="RC67" s="26"/>
-      <c r="RD67" s="26"/>
-      <c r="RE67" s="26"/>
-      <c r="RF67" s="26"/>
-      <c r="RG67" s="26"/>
-      <c r="RH67" s="26"/>
-      <c r="RI67" s="26"/>
-      <c r="RJ67" s="26"/>
-      <c r="RK67" s="26"/>
-      <c r="RL67" s="26"/>
-      <c r="RM67" s="26"/>
-      <c r="RN67" s="26"/>
-      <c r="RO67" s="26"/>
-      <c r="RP67" s="26"/>
-      <c r="RQ67" s="26"/>
-      <c r="RR67" s="26"/>
-      <c r="RS67" s="26"/>
-      <c r="RT67" s="26"/>
-      <c r="RU67" s="26"/>
-      <c r="RV67" s="26"/>
-      <c r="RW67" s="26"/>
-      <c r="RX67" s="26"/>
-      <c r="RY67" s="26"/>
-      <c r="RZ67" s="26"/>
-      <c r="SA67" s="26"/>
-      <c r="SB67" s="26"/>
-      <c r="SC67" s="26"/>
-      <c r="SD67" s="26"/>
-      <c r="SE67" s="26"/>
-      <c r="SF67" s="26"/>
-      <c r="SG67" s="26"/>
-      <c r="SH67" s="26"/>
-      <c r="SI67" s="26"/>
-      <c r="SJ67" s="26"/>
-      <c r="SK67" s="26"/>
-      <c r="SL67" s="26"/>
-      <c r="SM67" s="26"/>
-      <c r="SN67" s="26"/>
-      <c r="SO67" s="26"/>
-      <c r="SP67" s="26"/>
-      <c r="SQ67" s="26"/>
-      <c r="SR67" s="26"/>
-      <c r="SS67" s="26"/>
-      <c r="ST67" s="26"/>
-      <c r="SU67" s="26"/>
-      <c r="SV67" s="26"/>
-      <c r="SW67" s="26"/>
-      <c r="SX67" s="26"/>
-      <c r="SY67" s="26"/>
-      <c r="SZ67" s="26"/>
-      <c r="TA67" s="26"/>
-      <c r="TB67" s="26"/>
-      <c r="TC67" s="26"/>
-      <c r="TD67" s="26"/>
-      <c r="TE67" s="26"/>
-      <c r="TF67" s="26"/>
-      <c r="TG67" s="26"/>
-      <c r="TH67" s="26"/>
-      <c r="TI67" s="26"/>
-      <c r="TJ67" s="26"/>
-      <c r="TK67" s="26"/>
-      <c r="TL67" s="26"/>
-      <c r="TM67" s="26"/>
-      <c r="TN67" s="26"/>
-      <c r="TO67" s="26"/>
-      <c r="TP67" s="26"/>
-      <c r="TQ67" s="26"/>
-      <c r="TR67" s="26"/>
-      <c r="TS67" s="26"/>
-      <c r="TT67" s="26"/>
-      <c r="TU67" s="26"/>
-      <c r="TV67" s="26"/>
-      <c r="TW67" s="26"/>
-      <c r="TX67" s="26"/>
-      <c r="TY67" s="26"/>
-      <c r="TZ67" s="26"/>
-      <c r="UA67" s="26"/>
-      <c r="UB67" s="26"/>
-      <c r="UC67" s="26"/>
-      <c r="UD67" s="26"/>
-      <c r="UE67" s="26"/>
-      <c r="UF67" s="26"/>
-      <c r="UG67" s="26"/>
-      <c r="UH67" s="26"/>
-      <c r="UI67" s="26"/>
-      <c r="UJ67" s="26"/>
-      <c r="UK67" s="26"/>
-      <c r="UL67" s="26"/>
-      <c r="UM67" s="26"/>
-      <c r="UN67" s="26"/>
-      <c r="UO67" s="26"/>
-      <c r="UP67" s="26"/>
-      <c r="UQ67" s="26"/>
-      <c r="UR67" s="26"/>
-      <c r="US67" s="26"/>
-      <c r="UT67" s="26"/>
-      <c r="UU67" s="26"/>
-      <c r="UV67" s="26"/>
-      <c r="UW67" s="26"/>
-      <c r="UX67" s="26"/>
-      <c r="UY67" s="26"/>
-      <c r="UZ67" s="26"/>
-      <c r="VA67" s="26"/>
-      <c r="VB67" s="26"/>
-      <c r="VC67" s="26"/>
-      <c r="VD67" s="26"/>
-      <c r="VE67" s="26"/>
-      <c r="VF67" s="26"/>
-      <c r="VG67" s="26"/>
-      <c r="VH67" s="26"/>
-      <c r="VI67" s="26"/>
-      <c r="VJ67" s="26"/>
-      <c r="VK67" s="26"/>
-      <c r="VL67" s="26"/>
-      <c r="VM67" s="26"/>
-      <c r="VN67" s="26"/>
-      <c r="VO67" s="26"/>
-      <c r="VP67" s="26"/>
-      <c r="VQ67" s="26"/>
-      <c r="VR67" s="26"/>
-      <c r="VS67" s="26"/>
-      <c r="VT67" s="26"/>
-      <c r="VU67" s="26"/>
-      <c r="VV67" s="26"/>
-      <c r="VW67" s="26"/>
-      <c r="VX67" s="26"/>
-      <c r="VY67" s="26"/>
-      <c r="VZ67" s="26"/>
-      <c r="WA67" s="26"/>
-      <c r="WB67" s="26"/>
-      <c r="WC67" s="26"/>
-      <c r="WD67" s="26"/>
-      <c r="WE67" s="26"/>
-      <c r="WF67" s="26"/>
-      <c r="WG67" s="26"/>
-      <c r="WH67" s="26"/>
-      <c r="WI67" s="26"/>
-      <c r="WJ67" s="26"/>
-      <c r="WK67" s="26"/>
-      <c r="WL67" s="26"/>
-      <c r="WM67" s="26"/>
-      <c r="WN67" s="26"/>
-      <c r="WO67" s="26"/>
-      <c r="WP67" s="26"/>
-      <c r="WQ67" s="26"/>
-      <c r="WR67" s="26"/>
-      <c r="WS67" s="26"/>
-      <c r="WT67" s="26"/>
-      <c r="WU67" s="26"/>
-      <c r="WV67" s="26"/>
-      <c r="WW67" s="26"/>
-      <c r="WX67" s="26"/>
-      <c r="WY67" s="26"/>
-      <c r="WZ67" s="26"/>
-      <c r="XA67" s="26"/>
-      <c r="XB67" s="26"/>
-      <c r="XC67" s="26"/>
-      <c r="XD67" s="26"/>
-      <c r="XE67" s="26"/>
-      <c r="XF67" s="26"/>
-      <c r="XG67" s="26"/>
-      <c r="XH67" s="26"/>
-      <c r="XI67" s="26"/>
-      <c r="XJ67" s="26"/>
-      <c r="XK67" s="26"/>
-      <c r="XL67" s="26"/>
-      <c r="XM67" s="26"/>
-      <c r="XN67" s="26"/>
-      <c r="XO67" s="26"/>
-      <c r="XP67" s="26"/>
-      <c r="XQ67" s="26"/>
-      <c r="XR67" s="26"/>
-      <c r="XS67" s="26"/>
-      <c r="XT67" s="26"/>
-      <c r="XU67" s="26"/>
-      <c r="XV67" s="26"/>
-      <c r="XW67" s="26"/>
-      <c r="XX67" s="26"/>
-      <c r="XY67" s="26"/>
-      <c r="XZ67" s="26"/>
-      <c r="YA67" s="26"/>
-      <c r="YB67" s="26"/>
-      <c r="YC67" s="26"/>
-      <c r="YD67" s="26"/>
-      <c r="YE67" s="26"/>
-      <c r="YF67" s="26"/>
-      <c r="YG67" s="26"/>
-      <c r="YH67" s="26"/>
-      <c r="YI67" s="26"/>
-      <c r="YJ67" s="26"/>
-      <c r="YK67" s="26"/>
-      <c r="YL67" s="26"/>
-      <c r="YM67" s="26"/>
-      <c r="YN67" s="26"/>
-      <c r="YO67" s="26"/>
-      <c r="YP67" s="26"/>
-      <c r="YQ67" s="26"/>
-      <c r="YR67" s="26"/>
-      <c r="YS67" s="26"/>
-      <c r="YT67" s="26"/>
-      <c r="YU67" s="26"/>
-      <c r="YV67" s="26"/>
-      <c r="YW67" s="26"/>
-      <c r="YX67" s="26"/>
-      <c r="YY67" s="26"/>
-      <c r="YZ67" s="26"/>
-      <c r="ZA67" s="26"/>
-      <c r="ZB67" s="26"/>
-      <c r="ZC67" s="26"/>
-      <c r="ZD67" s="26"/>
-      <c r="ZE67" s="26"/>
-      <c r="ZF67" s="26"/>
-      <c r="ZG67" s="26"/>
-      <c r="ZH67" s="26"/>
-      <c r="ZI67" s="26"/>
-      <c r="ZJ67" s="26"/>
-      <c r="ZK67" s="26"/>
-      <c r="ZL67" s="26"/>
-      <c r="ZM67" s="26"/>
-      <c r="ZN67" s="26"/>
-      <c r="ZO67" s="26"/>
-      <c r="ZP67" s="26"/>
-      <c r="ZQ67" s="26"/>
-      <c r="ZR67" s="26"/>
-      <c r="ZS67" s="26"/>
-      <c r="ZT67" s="26"/>
-      <c r="ZU67" s="26"/>
-      <c r="ZV67" s="26"/>
-      <c r="ZW67" s="26"/>
-      <c r="ZX67" s="26"/>
-      <c r="ZY67" s="26"/>
-      <c r="ZZ67" s="26"/>
-      <c r="AAA67" s="26"/>
-      <c r="AAB67" s="26"/>
-      <c r="AAC67" s="26"/>
-      <c r="AAD67" s="26"/>
-      <c r="AAE67" s="26"/>
-      <c r="AAF67" s="26"/>
-      <c r="AAG67" s="26"/>
-      <c r="AAH67" s="26"/>
-      <c r="AAI67" s="26"/>
-      <c r="AAJ67" s="26"/>
-      <c r="AAK67" s="26"/>
-      <c r="AAL67" s="26"/>
-      <c r="AAM67" s="26"/>
-      <c r="AAN67" s="26"/>
-      <c r="AAO67" s="26"/>
-      <c r="AAP67" s="26"/>
-      <c r="AAQ67" s="26"/>
-      <c r="AAR67" s="26"/>
-      <c r="AAS67" s="26"/>
-      <c r="AAT67" s="26"/>
-      <c r="AAU67" s="26"/>
-      <c r="AAV67" s="26"/>
-      <c r="AAW67" s="26"/>
-      <c r="AAX67" s="26"/>
-      <c r="AAY67" s="26"/>
-      <c r="AAZ67" s="26"/>
-      <c r="ABA67" s="26"/>
-      <c r="ABB67" s="26"/>
-      <c r="ABC67" s="26"/>
-      <c r="ABD67" s="26"/>
-      <c r="ABE67" s="26"/>
-      <c r="ABF67" s="26"/>
-      <c r="ABG67" s="26"/>
-      <c r="ABH67" s="26"/>
-      <c r="ABI67" s="26"/>
-      <c r="ABJ67" s="26"/>
-      <c r="ABK67" s="26"/>
-      <c r="ABL67" s="26"/>
-      <c r="ABM67" s="26"/>
-      <c r="ABN67" s="26"/>
-      <c r="ABO67" s="26"/>
-      <c r="ABP67" s="26"/>
-      <c r="ABQ67" s="26"/>
-      <c r="ABR67" s="26"/>
-      <c r="ABS67" s="26"/>
-      <c r="ABT67" s="26"/>
-      <c r="ABU67" s="26"/>
-      <c r="ABV67" s="26"/>
-      <c r="ABW67" s="26"/>
-      <c r="ABX67" s="26"/>
-      <c r="ABY67" s="26"/>
-      <c r="ABZ67" s="26"/>
-      <c r="ACA67" s="26"/>
-      <c r="ACB67" s="26"/>
-      <c r="ACC67" s="26"/>
-      <c r="ACD67" s="26"/>
-      <c r="ACE67" s="26"/>
-      <c r="ACF67" s="26"/>
-      <c r="ACG67" s="26"/>
-      <c r="ACH67" s="26"/>
-      <c r="ACI67" s="26"/>
-      <c r="ACJ67" s="26"/>
-      <c r="ACK67" s="26"/>
-      <c r="ACL67" s="26"/>
-      <c r="ACM67" s="26"/>
-      <c r="ACN67" s="26"/>
-      <c r="ACO67" s="26"/>
-      <c r="ACP67" s="26"/>
-      <c r="ACQ67" s="26"/>
-      <c r="ACR67" s="26"/>
-      <c r="ACS67" s="26"/>
-      <c r="ACT67" s="26"/>
-      <c r="ACU67" s="26"/>
-      <c r="ACV67" s="26"/>
-      <c r="ACW67" s="26"/>
-      <c r="ACX67" s="26"/>
-      <c r="ACY67" s="26"/>
-      <c r="ACZ67" s="26"/>
-      <c r="ADA67" s="26"/>
-      <c r="ADB67" s="26"/>
-      <c r="ADC67" s="26"/>
-      <c r="ADD67" s="26"/>
-      <c r="ADE67" s="26"/>
-      <c r="ADF67" s="26"/>
-      <c r="ADG67" s="26"/>
-      <c r="ADH67" s="26"/>
-      <c r="ADI67" s="26"/>
-      <c r="ADJ67" s="26"/>
-      <c r="ADK67" s="26"/>
-      <c r="ADL67" s="26"/>
-      <c r="ADM67" s="26"/>
-      <c r="ADN67" s="26"/>
-      <c r="ADO67" s="26"/>
-      <c r="ADP67" s="26"/>
-      <c r="ADQ67" s="26"/>
-      <c r="ADR67" s="26"/>
-      <c r="ADS67" s="26"/>
-      <c r="ADT67" s="26"/>
-      <c r="ADU67" s="26"/>
-      <c r="ADV67" s="26"/>
-      <c r="ADW67" s="26"/>
-      <c r="ADX67" s="26"/>
-      <c r="ADY67" s="26"/>
-      <c r="ADZ67" s="26"/>
-      <c r="AEA67" s="26"/>
-      <c r="AEB67" s="26"/>
-      <c r="AEC67" s="26"/>
-      <c r="AED67" s="26"/>
-      <c r="AEE67" s="26"/>
-      <c r="AEF67" s="26"/>
-      <c r="AEG67" s="26"/>
-      <c r="AEH67" s="26"/>
-      <c r="AEI67" s="26"/>
-      <c r="AEJ67" s="26"/>
-      <c r="AEK67" s="26"/>
-      <c r="AEL67" s="26"/>
-      <c r="AEM67" s="26"/>
-      <c r="AEN67" s="26"/>
-      <c r="AEO67" s="26"/>
-      <c r="AEP67" s="26"/>
-      <c r="AEQ67" s="26"/>
-      <c r="AER67" s="26"/>
-      <c r="AES67" s="26"/>
-      <c r="AET67" s="26"/>
-      <c r="AEU67" s="26"/>
-      <c r="AEV67" s="26"/>
-      <c r="AEW67" s="26"/>
-      <c r="AEX67" s="26"/>
-      <c r="AEY67" s="26"/>
-      <c r="AEZ67" s="26"/>
-      <c r="AFA67" s="26"/>
-      <c r="AFB67" s="26"/>
-      <c r="AFC67" s="26"/>
-      <c r="AFD67" s="26"/>
-      <c r="AFE67" s="26"/>
-      <c r="AFF67" s="26"/>
-      <c r="AFG67" s="26"/>
-      <c r="AFH67" s="26"/>
-      <c r="AFI67" s="26"/>
-      <c r="AFJ67" s="26"/>
-      <c r="AFK67" s="26"/>
-      <c r="AFL67" s="26"/>
-      <c r="AFM67" s="26"/>
-      <c r="AFN67" s="26"/>
-      <c r="AFO67" s="26"/>
-      <c r="AFP67" s="26"/>
-      <c r="AFQ67" s="26"/>
-      <c r="AFR67" s="26"/>
-      <c r="AFS67" s="26"/>
-      <c r="AFT67" s="26"/>
-      <c r="AFU67" s="26"/>
-      <c r="AFV67" s="26"/>
-      <c r="AFW67" s="26"/>
-      <c r="AFX67" s="26"/>
-      <c r="AFY67" s="26"/>
-      <c r="AFZ67" s="26"/>
-      <c r="AGA67" s="26"/>
-      <c r="AGB67" s="26"/>
-      <c r="AGC67" s="26"/>
-      <c r="AGD67" s="26"/>
-      <c r="AGE67" s="26"/>
-      <c r="AGF67" s="26"/>
-      <c r="AGG67" s="26"/>
-      <c r="AGH67" s="26"/>
-      <c r="AGI67" s="26"/>
-      <c r="AGJ67" s="26"/>
-      <c r="AGK67" s="26"/>
-      <c r="AGL67" s="26"/>
-      <c r="AGM67" s="26"/>
-      <c r="AGN67" s="26"/>
-      <c r="AGO67" s="26"/>
-      <c r="AGP67" s="26"/>
-      <c r="AGQ67" s="26"/>
-      <c r="AGR67" s="26"/>
-      <c r="AGS67" s="26"/>
-      <c r="AGT67" s="26"/>
-      <c r="AGU67" s="26"/>
-      <c r="AGV67" s="26"/>
-      <c r="AGW67" s="26"/>
-      <c r="AGX67" s="26"/>
-      <c r="AGY67" s="26"/>
-      <c r="AGZ67" s="26"/>
-      <c r="AHA67" s="26"/>
-      <c r="AHB67" s="26"/>
-      <c r="AHC67" s="26"/>
-      <c r="AHD67" s="26"/>
-      <c r="AHE67" s="26"/>
-      <c r="AHF67" s="26"/>
-      <c r="AHG67" s="26"/>
-      <c r="AHH67" s="26"/>
-      <c r="AHI67" s="26"/>
-      <c r="AHJ67" s="26"/>
-      <c r="AHK67" s="26"/>
-      <c r="AHL67" s="26"/>
-      <c r="AHM67" s="26"/>
-      <c r="AHN67" s="26"/>
-      <c r="AHO67" s="26"/>
-      <c r="AHP67" s="26"/>
-      <c r="AHQ67" s="26"/>
-      <c r="AHR67" s="26"/>
-      <c r="AHS67" s="26"/>
-      <c r="AHT67" s="26"/>
-      <c r="AHU67" s="26"/>
-      <c r="AHV67" s="26"/>
-      <c r="AHW67" s="26"/>
-      <c r="AHX67" s="26"/>
-      <c r="AHY67" s="26"/>
-      <c r="AHZ67" s="26"/>
-      <c r="AIA67" s="26"/>
-      <c r="AIB67" s="26"/>
-      <c r="AIC67" s="26"/>
-      <c r="AID67" s="26"/>
-      <c r="AIE67" s="26"/>
-      <c r="AIF67" s="26"/>
-      <c r="AIG67" s="26"/>
-      <c r="AIH67" s="26"/>
-      <c r="AII67" s="26"/>
-      <c r="AIJ67" s="26"/>
-      <c r="AIK67" s="26"/>
-      <c r="AIL67" s="26"/>
-      <c r="AIM67" s="26"/>
-      <c r="AIN67" s="26"/>
-      <c r="AIO67" s="26"/>
-      <c r="AIP67" s="26"/>
-      <c r="AIQ67" s="26"/>
-      <c r="AIR67" s="26"/>
-      <c r="AIS67" s="26"/>
-      <c r="AIT67" s="26"/>
-      <c r="AIU67" s="26"/>
-      <c r="AIV67" s="26"/>
-      <c r="AIW67" s="26"/>
-      <c r="AIX67" s="26"/>
-      <c r="AIY67" s="26"/>
-      <c r="AIZ67" s="26"/>
-      <c r="AJA67" s="26"/>
-      <c r="AJB67" s="26"/>
-      <c r="AJC67" s="26"/>
-      <c r="AJD67" s="26"/>
-      <c r="AJE67" s="26"/>
-      <c r="AJF67" s="26"/>
-      <c r="AJG67" s="26"/>
-      <c r="AJH67" s="26"/>
-      <c r="AJI67" s="26"/>
-      <c r="AJJ67" s="26"/>
-      <c r="AJK67" s="26"/>
-      <c r="AJL67" s="26"/>
-      <c r="AJM67" s="26"/>
-      <c r="AJN67" s="26"/>
-      <c r="AJO67" s="26"/>
-      <c r="AJP67" s="26"/>
-      <c r="AJQ67" s="26"/>
-      <c r="AJR67" s="26"/>
-      <c r="AJS67" s="26"/>
-      <c r="AJT67" s="26"/>
-      <c r="AJU67" s="26"/>
-      <c r="AJV67" s="26"/>
-      <c r="AJW67" s="26"/>
-      <c r="AJX67" s="26"/>
-      <c r="AJY67" s="26"/>
-      <c r="AJZ67" s="26"/>
-      <c r="AKA67" s="26"/>
-      <c r="AKB67" s="26"/>
-      <c r="AKC67" s="26"/>
-      <c r="AKD67" s="26"/>
-      <c r="AKE67" s="26"/>
-      <c r="AKF67" s="26"/>
-      <c r="AKG67" s="26"/>
-      <c r="AKH67" s="26"/>
-      <c r="AKI67" s="26"/>
-      <c r="AKJ67" s="26"/>
-      <c r="AKK67" s="26"/>
-      <c r="AKL67" s="26"/>
-      <c r="AKM67" s="26"/>
-      <c r="AKN67" s="26"/>
-      <c r="AKO67" s="26"/>
-      <c r="AKP67" s="26"/>
-      <c r="AKQ67" s="26"/>
-      <c r="AKR67" s="26"/>
-      <c r="AKS67" s="26"/>
-      <c r="AKT67" s="26"/>
-      <c r="AKU67" s="26"/>
-      <c r="AKV67" s="26"/>
-      <c r="AKW67" s="26"/>
-      <c r="AKX67" s="26"/>
-      <c r="AKY67" s="26"/>
-      <c r="AKZ67" s="26"/>
-      <c r="ALA67" s="26"/>
-      <c r="ALB67" s="26"/>
-      <c r="ALC67" s="26"/>
-      <c r="ALD67" s="26"/>
-      <c r="ALE67" s="26"/>
-      <c r="ALF67" s="26"/>
-      <c r="ALG67" s="26"/>
-      <c r="ALH67" s="26"/>
-      <c r="ALI67" s="26"/>
-      <c r="ALJ67" s="26"/>
-      <c r="ALK67" s="26"/>
-      <c r="ALL67" s="26"/>
-      <c r="ALM67" s="26"/>
-      <c r="ALN67" s="26"/>
-      <c r="ALO67" s="26"/>
-      <c r="ALP67" s="26"/>
-      <c r="ALQ67" s="26"/>
-      <c r="ALR67" s="26"/>
-      <c r="ALS67" s="26"/>
-      <c r="ALT67" s="26"/>
-      <c r="ALU67" s="26"/>
-      <c r="ALV67" s="26"/>
-      <c r="ALW67" s="26"/>
-      <c r="ALX67" s="26"/>
-      <c r="ALY67" s="26"/>
-      <c r="ALZ67" s="26"/>
-      <c r="AMA67" s="26"/>
-      <c r="AMB67" s="26"/>
-      <c r="AMC67" s="26"/>
-      <c r="AMD67" s="26"/>
-      <c r="AME67" s="26"/>
-      <c r="AMF67" s="26"/>
-      <c r="AMG67" s="26"/>
-      <c r="AMH67" s="26"/>
-      <c r="AMI67" s="26"/>
-      <c r="AMJ67" s="26"/>
-      <c r="AMK67" s="26"/>
-    </row>
-    <row r="68" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="B68" s="35" t="s">
+      <c r="C67" s="32"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B68" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="C68" s="35"/>
+      <c r="C68" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -7496,16 +4462,16 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>196</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -7516,7 +4482,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="37"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="8" t="s">
         <v>198</v>
       </c>
@@ -7525,7 +4491,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="37"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="8" t="s">
         <v>199</v>
       </c>
@@ -7534,7 +4500,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="37"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="8" t="s">
         <v>200</v>
       </c>
@@ -7543,13 +4509,13 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7569,10 +4535,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:D17"/>
+  <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="95" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7584,11 +4550,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
@@ -7744,14 +4710,25 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B17" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B18" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C18" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D18" s="22" t="s">
         <v>289</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-13811 Fix trace for `origin` and `active` properties
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
+++ b/DEV/org.openl.rules/doc/TablePropertyDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpikus/Sources/OpenL/openl-tablets/DEV/org.openl.rules/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF493FE-5ED0-F647-A4AE-EFCAEDF33AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE44650-3659-7344-ADC1-43A93E2F1070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="34940" windowHeight="21360" tabRatio="783" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34940" windowHeight="21360" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="291">
   <si>
     <t>Display Name</t>
   </si>
@@ -933,6 +933,9 @@
   </si>
   <si>
     <t>A Locale object represents a specific geographical, political, or cultural region.</t>
+  </si>
+  <si>
+    <t>eq(origin)</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1035,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1311,6 +1314,45 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1349,7 +1391,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1415,19 +1457,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1590,9 +1626,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1630,9 +1666,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1665,26 +1701,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1717,26 +1736,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1925,207 +1927,207 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="2:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
@@ -2160,8 +2162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK68"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2193,154 +2195,154 @@
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="2:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="2:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="2:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="2:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
     </row>
     <row r="8" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="2:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
@@ -2352,27 +2354,27 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
     </row>
     <row r="12" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
@@ -3373,7 +3375,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>216</v>
       </c>
@@ -3386,7 +3388,9 @@
       <c r="E33" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G33" s="5" t="s">
         <v>78</v>
       </c>
@@ -3416,7 +3420,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>134</v>
       </c>
@@ -3461,7 +3465,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>150</v>
       </c>
@@ -3506,7 +3510,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>158</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>162</v>
       </c>
@@ -3591,7 +3595,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>116</v>
       </c>
@@ -3638,7 +3642,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>123</v>
       </c>
@@ -3681,7 +3685,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
         <v>127</v>
       </c>
@@ -3724,7 +3728,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>167</v>
       </c>
@@ -3766,7 +3770,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>170</v>
       </c>
@@ -3807,8 +3811,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25"/>
+    <row r="43" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
         <v>254</v>
       </c>
@@ -3851,7 +3854,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="44" spans="1:1025" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:20" ht="32" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>175</v>
       </c>
@@ -3893,10 +3896,8 @@
       <c r="T44" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="U44" s="24"/>
-    </row>
-    <row r="45" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
+    </row>
+    <row r="45" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="5" t="s">
         <v>248</v>
       </c>
@@ -3939,7 +3940,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="5" t="s">
         <v>181</v>
       </c>
@@ -3980,7 +3981,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="s">
         <v>183</v>
       </c>
@@ -4020,1013 +4021,8 @@
       <c r="T47" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="V47" s="23"/>
-      <c r="W47" s="23"/>
-      <c r="X47" s="23"/>
-      <c r="Y47" s="23"/>
-      <c r="Z47" s="23"/>
-      <c r="AA47" s="23"/>
-      <c r="AB47" s="23"/>
-      <c r="AC47" s="23"/>
-      <c r="AD47" s="23"/>
-      <c r="AE47" s="23"/>
-      <c r="AF47" s="23"/>
-      <c r="AG47" s="23"/>
-      <c r="AH47" s="23"/>
-      <c r="AI47" s="23"/>
-      <c r="AJ47" s="23"/>
-      <c r="AK47" s="23"/>
-      <c r="AL47" s="23"/>
-      <c r="AM47" s="23"/>
-      <c r="AN47" s="23"/>
-      <c r="AO47" s="23"/>
-      <c r="AP47" s="23"/>
-      <c r="AQ47" s="23"/>
-      <c r="AR47" s="23"/>
-      <c r="AS47" s="23"/>
-      <c r="AT47" s="23"/>
-      <c r="AU47" s="23"/>
-      <c r="AV47" s="23"/>
-      <c r="AW47" s="23"/>
-      <c r="AX47" s="23"/>
-      <c r="AY47" s="23"/>
-      <c r="AZ47" s="23"/>
-      <c r="BA47" s="23"/>
-      <c r="BB47" s="23"/>
-      <c r="BC47" s="23"/>
-      <c r="BD47" s="23"/>
-      <c r="BE47" s="23"/>
-      <c r="BF47" s="23"/>
-      <c r="BG47" s="23"/>
-      <c r="BH47" s="23"/>
-      <c r="BI47" s="23"/>
-      <c r="BJ47" s="23"/>
-      <c r="BK47" s="23"/>
-      <c r="BL47" s="23"/>
-      <c r="BM47" s="23"/>
-      <c r="BN47" s="23"/>
-      <c r="BO47" s="23"/>
-      <c r="BP47" s="23"/>
-      <c r="BQ47" s="23"/>
-      <c r="BR47" s="23"/>
-      <c r="BS47" s="23"/>
-      <c r="BT47" s="23"/>
-      <c r="BU47" s="23"/>
-      <c r="BV47" s="23"/>
-      <c r="BW47" s="23"/>
-      <c r="BX47" s="23"/>
-      <c r="BY47" s="23"/>
-      <c r="BZ47" s="23"/>
-      <c r="CA47" s="23"/>
-      <c r="CB47" s="23"/>
-      <c r="CC47" s="23"/>
-      <c r="CD47" s="23"/>
-      <c r="CE47" s="23"/>
-      <c r="CF47" s="23"/>
-      <c r="CG47" s="23"/>
-      <c r="CH47" s="23"/>
-      <c r="CI47" s="23"/>
-      <c r="CJ47" s="23"/>
-      <c r="CK47" s="23"/>
-      <c r="CL47" s="23"/>
-      <c r="CM47" s="23"/>
-      <c r="CN47" s="23"/>
-      <c r="CO47" s="23"/>
-      <c r="CP47" s="23"/>
-      <c r="CQ47" s="23"/>
-      <c r="CR47" s="23"/>
-      <c r="CS47" s="23"/>
-      <c r="CT47" s="23"/>
-      <c r="CU47" s="23"/>
-      <c r="CV47" s="23"/>
-      <c r="CW47" s="23"/>
-      <c r="CX47" s="23"/>
-      <c r="CY47" s="23"/>
-      <c r="CZ47" s="23"/>
-      <c r="DA47" s="23"/>
-      <c r="DB47" s="23"/>
-      <c r="DC47" s="23"/>
-      <c r="DD47" s="23"/>
-      <c r="DE47" s="23"/>
-      <c r="DF47" s="23"/>
-      <c r="DG47" s="23"/>
-      <c r="DH47" s="23"/>
-      <c r="DI47" s="23"/>
-      <c r="DJ47" s="23"/>
-      <c r="DK47" s="23"/>
-      <c r="DL47" s="23"/>
-      <c r="DM47" s="23"/>
-      <c r="DN47" s="23"/>
-      <c r="DO47" s="23"/>
-      <c r="DP47" s="23"/>
-      <c r="DQ47" s="23"/>
-      <c r="DR47" s="23"/>
-      <c r="DS47" s="23"/>
-      <c r="DT47" s="23"/>
-      <c r="DU47" s="23"/>
-      <c r="DV47" s="23"/>
-      <c r="DW47" s="23"/>
-      <c r="DX47" s="23"/>
-      <c r="DY47" s="23"/>
-      <c r="DZ47" s="23"/>
-      <c r="EA47" s="23"/>
-      <c r="EB47" s="23"/>
-      <c r="EC47" s="23"/>
-      <c r="ED47" s="23"/>
-      <c r="EE47" s="23"/>
-      <c r="EF47" s="23"/>
-      <c r="EG47" s="23"/>
-      <c r="EH47" s="23"/>
-      <c r="EI47" s="23"/>
-      <c r="EJ47" s="23"/>
-      <c r="EK47" s="23"/>
-      <c r="EL47" s="23"/>
-      <c r="EM47" s="23"/>
-      <c r="EN47" s="23"/>
-      <c r="EO47" s="23"/>
-      <c r="EP47" s="23"/>
-      <c r="EQ47" s="23"/>
-      <c r="ER47" s="23"/>
-      <c r="ES47" s="23"/>
-      <c r="ET47" s="23"/>
-      <c r="EU47" s="23"/>
-      <c r="EV47" s="23"/>
-      <c r="EW47" s="23"/>
-      <c r="EX47" s="23"/>
-      <c r="EY47" s="23"/>
-      <c r="EZ47" s="23"/>
-      <c r="FA47" s="23"/>
-      <c r="FB47" s="23"/>
-      <c r="FC47" s="23"/>
-      <c r="FD47" s="23"/>
-      <c r="FE47" s="23"/>
-      <c r="FF47" s="23"/>
-      <c r="FG47" s="23"/>
-      <c r="FH47" s="23"/>
-      <c r="FI47" s="23"/>
-      <c r="FJ47" s="23"/>
-      <c r="FK47" s="23"/>
-      <c r="FL47" s="23"/>
-      <c r="FM47" s="23"/>
-      <c r="FN47" s="23"/>
-      <c r="FO47" s="23"/>
-      <c r="FP47" s="23"/>
-      <c r="FQ47" s="23"/>
-      <c r="FR47" s="23"/>
-      <c r="FS47" s="23"/>
-      <c r="FT47" s="23"/>
-      <c r="FU47" s="23"/>
-      <c r="FV47" s="23"/>
-      <c r="FW47" s="23"/>
-      <c r="FX47" s="23"/>
-      <c r="FY47" s="23"/>
-      <c r="FZ47" s="23"/>
-      <c r="GA47" s="23"/>
-      <c r="GB47" s="23"/>
-      <c r="GC47" s="23"/>
-      <c r="GD47" s="23"/>
-      <c r="GE47" s="23"/>
-      <c r="GF47" s="23"/>
-      <c r="GG47" s="23"/>
-      <c r="GH47" s="23"/>
-      <c r="GI47" s="23"/>
-      <c r="GJ47" s="23"/>
-      <c r="GK47" s="23"/>
-      <c r="GL47" s="23"/>
-      <c r="GM47" s="23"/>
-      <c r="GN47" s="23"/>
-      <c r="GO47" s="23"/>
-      <c r="GP47" s="23"/>
-      <c r="GQ47" s="23"/>
-      <c r="GR47" s="23"/>
-      <c r="GS47" s="23"/>
-      <c r="GT47" s="23"/>
-      <c r="GU47" s="23"/>
-      <c r="GV47" s="23"/>
-      <c r="GW47" s="23"/>
-      <c r="GX47" s="23"/>
-      <c r="GY47" s="23"/>
-      <c r="GZ47" s="23"/>
-      <c r="HA47" s="23"/>
-      <c r="HB47" s="23"/>
-      <c r="HC47" s="23"/>
-      <c r="HD47" s="23"/>
-      <c r="HE47" s="23"/>
-      <c r="HF47" s="23"/>
-      <c r="HG47" s="23"/>
-      <c r="HH47" s="23"/>
-      <c r="HI47" s="23"/>
-      <c r="HJ47" s="23"/>
-      <c r="HK47" s="23"/>
-      <c r="HL47" s="23"/>
-      <c r="HM47" s="23"/>
-      <c r="HN47" s="23"/>
-      <c r="HO47" s="23"/>
-      <c r="HP47" s="23"/>
-      <c r="HQ47" s="23"/>
-      <c r="HR47" s="23"/>
-      <c r="HS47" s="23"/>
-      <c r="HT47" s="23"/>
-      <c r="HU47" s="23"/>
-      <c r="HV47" s="23"/>
-      <c r="HW47" s="23"/>
-      <c r="HX47" s="23"/>
-      <c r="HY47" s="23"/>
-      <c r="HZ47" s="23"/>
-      <c r="IA47" s="23"/>
-      <c r="IB47" s="23"/>
-      <c r="IC47" s="23"/>
-      <c r="ID47" s="23"/>
-      <c r="IE47" s="23"/>
-      <c r="IF47" s="23"/>
-      <c r="IG47" s="23"/>
-      <c r="IH47" s="23"/>
-      <c r="II47" s="23"/>
-      <c r="IJ47" s="23"/>
-      <c r="IK47" s="23"/>
-      <c r="IL47" s="23"/>
-      <c r="IM47" s="23"/>
-      <c r="IN47" s="23"/>
-      <c r="IO47" s="23"/>
-      <c r="IP47" s="23"/>
-      <c r="IQ47" s="23"/>
-      <c r="IR47" s="23"/>
-      <c r="IS47" s="23"/>
-      <c r="IT47" s="23"/>
-      <c r="IU47" s="23"/>
-      <c r="IV47" s="23"/>
-      <c r="IW47" s="23"/>
-      <c r="IX47" s="23"/>
-      <c r="IY47" s="23"/>
-      <c r="IZ47" s="23"/>
-      <c r="JA47" s="23"/>
-      <c r="JB47" s="23"/>
-      <c r="JC47" s="23"/>
-      <c r="JD47" s="23"/>
-      <c r="JE47" s="23"/>
-      <c r="JF47" s="23"/>
-      <c r="JG47" s="23"/>
-      <c r="JH47" s="23"/>
-      <c r="JI47" s="23"/>
-      <c r="JJ47" s="23"/>
-      <c r="JK47" s="23"/>
-      <c r="JL47" s="23"/>
-      <c r="JM47" s="23"/>
-      <c r="JN47" s="23"/>
-      <c r="JO47" s="23"/>
-      <c r="JP47" s="23"/>
-      <c r="JQ47" s="23"/>
-      <c r="JR47" s="23"/>
-      <c r="JS47" s="23"/>
-      <c r="JT47" s="23"/>
-      <c r="JU47" s="23"/>
-      <c r="JV47" s="23"/>
-      <c r="JW47" s="23"/>
-      <c r="JX47" s="23"/>
-      <c r="JY47" s="23"/>
-      <c r="JZ47" s="23"/>
-      <c r="KA47" s="23"/>
-      <c r="KB47" s="23"/>
-      <c r="KC47" s="23"/>
-      <c r="KD47" s="23"/>
-      <c r="KE47" s="23"/>
-      <c r="KF47" s="23"/>
-      <c r="KG47" s="23"/>
-      <c r="KH47" s="23"/>
-      <c r="KI47" s="23"/>
-      <c r="KJ47" s="23"/>
-      <c r="KK47" s="23"/>
-      <c r="KL47" s="23"/>
-      <c r="KM47" s="23"/>
-      <c r="KN47" s="23"/>
-      <c r="KO47" s="23"/>
-      <c r="KP47" s="23"/>
-      <c r="KQ47" s="23"/>
-      <c r="KR47" s="23"/>
-      <c r="KS47" s="23"/>
-      <c r="KT47" s="23"/>
-      <c r="KU47" s="23"/>
-      <c r="KV47" s="23"/>
-      <c r="KW47" s="23"/>
-      <c r="KX47" s="23"/>
-      <c r="KY47" s="23"/>
-      <c r="KZ47" s="23"/>
-      <c r="LA47" s="23"/>
-      <c r="LB47" s="23"/>
-      <c r="LC47" s="23"/>
-      <c r="LD47" s="23"/>
-      <c r="LE47" s="23"/>
-      <c r="LF47" s="23"/>
-      <c r="LG47" s="23"/>
-      <c r="LH47" s="23"/>
-      <c r="LI47" s="23"/>
-      <c r="LJ47" s="23"/>
-      <c r="LK47" s="23"/>
-      <c r="LL47" s="23"/>
-      <c r="LM47" s="23"/>
-      <c r="LN47" s="23"/>
-      <c r="LO47" s="23"/>
-      <c r="LP47" s="23"/>
-      <c r="LQ47" s="23"/>
-      <c r="LR47" s="23"/>
-      <c r="LS47" s="23"/>
-      <c r="LT47" s="23"/>
-      <c r="LU47" s="23"/>
-      <c r="LV47" s="23"/>
-      <c r="LW47" s="23"/>
-      <c r="LX47" s="23"/>
-      <c r="LY47" s="23"/>
-      <c r="LZ47" s="23"/>
-      <c r="MA47" s="23"/>
-      <c r="MB47" s="23"/>
-      <c r="MC47" s="23"/>
-      <c r="MD47" s="23"/>
-      <c r="ME47" s="23"/>
-      <c r="MF47" s="23"/>
-      <c r="MG47" s="23"/>
-      <c r="MH47" s="23"/>
-      <c r="MI47" s="23"/>
-      <c r="MJ47" s="23"/>
-      <c r="MK47" s="23"/>
-      <c r="ML47" s="23"/>
-      <c r="MM47" s="23"/>
-      <c r="MN47" s="23"/>
-      <c r="MO47" s="23"/>
-      <c r="MP47" s="23"/>
-      <c r="MQ47" s="23"/>
-      <c r="MR47" s="23"/>
-      <c r="MS47" s="23"/>
-      <c r="MT47" s="23"/>
-      <c r="MU47" s="23"/>
-      <c r="MV47" s="23"/>
-      <c r="MW47" s="23"/>
-      <c r="MX47" s="23"/>
-      <c r="MY47" s="23"/>
-      <c r="MZ47" s="23"/>
-      <c r="NA47" s="23"/>
-      <c r="NB47" s="23"/>
-      <c r="NC47" s="23"/>
-      <c r="ND47" s="23"/>
-      <c r="NE47" s="23"/>
-      <c r="NF47" s="23"/>
-      <c r="NG47" s="23"/>
-      <c r="NH47" s="23"/>
-      <c r="NI47" s="23"/>
-      <c r="NJ47" s="23"/>
-      <c r="NK47" s="23"/>
-      <c r="NL47" s="23"/>
-      <c r="NM47" s="23"/>
-      <c r="NN47" s="23"/>
-      <c r="NO47" s="23"/>
-      <c r="NP47" s="23"/>
-      <c r="NQ47" s="23"/>
-      <c r="NR47" s="23"/>
-      <c r="NS47" s="23"/>
-      <c r="NT47" s="23"/>
-      <c r="NU47" s="23"/>
-      <c r="NV47" s="23"/>
-      <c r="NW47" s="23"/>
-      <c r="NX47" s="23"/>
-      <c r="NY47" s="23"/>
-      <c r="NZ47" s="23"/>
-      <c r="OA47" s="23"/>
-      <c r="OB47" s="23"/>
-      <c r="OC47" s="23"/>
-      <c r="OD47" s="23"/>
-      <c r="OE47" s="23"/>
-      <c r="OF47" s="23"/>
-      <c r="OG47" s="23"/>
-      <c r="OH47" s="23"/>
-      <c r="OI47" s="23"/>
-      <c r="OJ47" s="23"/>
-      <c r="OK47" s="23"/>
-      <c r="OL47" s="23"/>
-      <c r="OM47" s="23"/>
-      <c r="ON47" s="23"/>
-      <c r="OO47" s="23"/>
-      <c r="OP47" s="23"/>
-      <c r="OQ47" s="23"/>
-      <c r="OR47" s="23"/>
-      <c r="OS47" s="23"/>
-      <c r="OT47" s="23"/>
-      <c r="OU47" s="23"/>
-      <c r="OV47" s="23"/>
-      <c r="OW47" s="23"/>
-      <c r="OX47" s="23"/>
-      <c r="OY47" s="23"/>
-      <c r="OZ47" s="23"/>
-      <c r="PA47" s="23"/>
-      <c r="PB47" s="23"/>
-      <c r="PC47" s="23"/>
-      <c r="PD47" s="23"/>
-      <c r="PE47" s="23"/>
-      <c r="PF47" s="23"/>
-      <c r="PG47" s="23"/>
-      <c r="PH47" s="23"/>
-      <c r="PI47" s="23"/>
-      <c r="PJ47" s="23"/>
-      <c r="PK47" s="23"/>
-      <c r="PL47" s="23"/>
-      <c r="PM47" s="23"/>
-      <c r="PN47" s="23"/>
-      <c r="PO47" s="23"/>
-      <c r="PP47" s="23"/>
-      <c r="PQ47" s="23"/>
-      <c r="PR47" s="23"/>
-      <c r="PS47" s="23"/>
-      <c r="PT47" s="23"/>
-      <c r="PU47" s="23"/>
-      <c r="PV47" s="23"/>
-      <c r="PW47" s="23"/>
-      <c r="PX47" s="23"/>
-      <c r="PY47" s="23"/>
-      <c r="PZ47" s="23"/>
-      <c r="QA47" s="23"/>
-      <c r="QB47" s="23"/>
-      <c r="QC47" s="23"/>
-      <c r="QD47" s="23"/>
-      <c r="QE47" s="23"/>
-      <c r="QF47" s="23"/>
-      <c r="QG47" s="23"/>
-      <c r="QH47" s="23"/>
-      <c r="QI47" s="23"/>
-      <c r="QJ47" s="23"/>
-      <c r="QK47" s="23"/>
-      <c r="QL47" s="23"/>
-      <c r="QM47" s="23"/>
-      <c r="QN47" s="23"/>
-      <c r="QO47" s="23"/>
-      <c r="QP47" s="23"/>
-      <c r="QQ47" s="23"/>
-      <c r="QR47" s="23"/>
-      <c r="QS47" s="23"/>
-      <c r="QT47" s="23"/>
-      <c r="QU47" s="23"/>
-      <c r="QV47" s="23"/>
-      <c r="QW47" s="23"/>
-      <c r="QX47" s="23"/>
-      <c r="QY47" s="23"/>
-      <c r="QZ47" s="23"/>
-      <c r="RA47" s="23"/>
-      <c r="RB47" s="23"/>
-      <c r="RC47" s="23"/>
-      <c r="RD47" s="23"/>
-      <c r="RE47" s="23"/>
-      <c r="RF47" s="23"/>
-      <c r="RG47" s="23"/>
-      <c r="RH47" s="23"/>
-      <c r="RI47" s="23"/>
-      <c r="RJ47" s="23"/>
-      <c r="RK47" s="23"/>
-      <c r="RL47" s="23"/>
-      <c r="RM47" s="23"/>
-      <c r="RN47" s="23"/>
-      <c r="RO47" s="23"/>
-      <c r="RP47" s="23"/>
-      <c r="RQ47" s="23"/>
-      <c r="RR47" s="23"/>
-      <c r="RS47" s="23"/>
-      <c r="RT47" s="23"/>
-      <c r="RU47" s="23"/>
-      <c r="RV47" s="23"/>
-      <c r="RW47" s="23"/>
-      <c r="RX47" s="23"/>
-      <c r="RY47" s="23"/>
-      <c r="RZ47" s="23"/>
-      <c r="SA47" s="23"/>
-      <c r="SB47" s="23"/>
-      <c r="SC47" s="23"/>
-      <c r="SD47" s="23"/>
-      <c r="SE47" s="23"/>
-      <c r="SF47" s="23"/>
-      <c r="SG47" s="23"/>
-      <c r="SH47" s="23"/>
-      <c r="SI47" s="23"/>
-      <c r="SJ47" s="23"/>
-      <c r="SK47" s="23"/>
-      <c r="SL47" s="23"/>
-      <c r="SM47" s="23"/>
-      <c r="SN47" s="23"/>
-      <c r="SO47" s="23"/>
-      <c r="SP47" s="23"/>
-      <c r="SQ47" s="23"/>
-      <c r="SR47" s="23"/>
-      <c r="SS47" s="23"/>
-      <c r="ST47" s="23"/>
-      <c r="SU47" s="23"/>
-      <c r="SV47" s="23"/>
-      <c r="SW47" s="23"/>
-      <c r="SX47" s="23"/>
-      <c r="SY47" s="23"/>
-      <c r="SZ47" s="23"/>
-      <c r="TA47" s="23"/>
-      <c r="TB47" s="23"/>
-      <c r="TC47" s="23"/>
-      <c r="TD47" s="23"/>
-      <c r="TE47" s="23"/>
-      <c r="TF47" s="23"/>
-      <c r="TG47" s="23"/>
-      <c r="TH47" s="23"/>
-      <c r="TI47" s="23"/>
-      <c r="TJ47" s="23"/>
-      <c r="TK47" s="23"/>
-      <c r="TL47" s="23"/>
-      <c r="TM47" s="23"/>
-      <c r="TN47" s="23"/>
-      <c r="TO47" s="23"/>
-      <c r="TP47" s="23"/>
-      <c r="TQ47" s="23"/>
-      <c r="TR47" s="23"/>
-      <c r="TS47" s="23"/>
-      <c r="TT47" s="23"/>
-      <c r="TU47" s="23"/>
-      <c r="TV47" s="23"/>
-      <c r="TW47" s="23"/>
-      <c r="TX47" s="23"/>
-      <c r="TY47" s="23"/>
-      <c r="TZ47" s="23"/>
-      <c r="UA47" s="23"/>
-      <c r="UB47" s="23"/>
-      <c r="UC47" s="23"/>
-      <c r="UD47" s="23"/>
-      <c r="UE47" s="23"/>
-      <c r="UF47" s="23"/>
-      <c r="UG47" s="23"/>
-      <c r="UH47" s="23"/>
-      <c r="UI47" s="23"/>
-      <c r="UJ47" s="23"/>
-      <c r="UK47" s="23"/>
-      <c r="UL47" s="23"/>
-      <c r="UM47" s="23"/>
-      <c r="UN47" s="23"/>
-      <c r="UO47" s="23"/>
-      <c r="UP47" s="23"/>
-      <c r="UQ47" s="23"/>
-      <c r="UR47" s="23"/>
-      <c r="US47" s="23"/>
-      <c r="UT47" s="23"/>
-      <c r="UU47" s="23"/>
-      <c r="UV47" s="23"/>
-      <c r="UW47" s="23"/>
-      <c r="UX47" s="23"/>
-      <c r="UY47" s="23"/>
-      <c r="UZ47" s="23"/>
-      <c r="VA47" s="23"/>
-      <c r="VB47" s="23"/>
-      <c r="VC47" s="23"/>
-      <c r="VD47" s="23"/>
-      <c r="VE47" s="23"/>
-      <c r="VF47" s="23"/>
-      <c r="VG47" s="23"/>
-      <c r="VH47" s="23"/>
-      <c r="VI47" s="23"/>
-      <c r="VJ47" s="23"/>
-      <c r="VK47" s="23"/>
-      <c r="VL47" s="23"/>
-      <c r="VM47" s="23"/>
-      <c r="VN47" s="23"/>
-      <c r="VO47" s="23"/>
-      <c r="VP47" s="23"/>
-      <c r="VQ47" s="23"/>
-      <c r="VR47" s="23"/>
-      <c r="VS47" s="23"/>
-      <c r="VT47" s="23"/>
-      <c r="VU47" s="23"/>
-      <c r="VV47" s="23"/>
-      <c r="VW47" s="23"/>
-      <c r="VX47" s="23"/>
-      <c r="VY47" s="23"/>
-      <c r="VZ47" s="23"/>
-      <c r="WA47" s="23"/>
-      <c r="WB47" s="23"/>
-      <c r="WC47" s="23"/>
-      <c r="WD47" s="23"/>
-      <c r="WE47" s="23"/>
-      <c r="WF47" s="23"/>
-      <c r="WG47" s="23"/>
-      <c r="WH47" s="23"/>
-      <c r="WI47" s="23"/>
-      <c r="WJ47" s="23"/>
-      <c r="WK47" s="23"/>
-      <c r="WL47" s="23"/>
-      <c r="WM47" s="23"/>
-      <c r="WN47" s="23"/>
-      <c r="WO47" s="23"/>
-      <c r="WP47" s="23"/>
-      <c r="WQ47" s="23"/>
-      <c r="WR47" s="23"/>
-      <c r="WS47" s="23"/>
-      <c r="WT47" s="23"/>
-      <c r="WU47" s="23"/>
-      <c r="WV47" s="23"/>
-      <c r="WW47" s="23"/>
-      <c r="WX47" s="23"/>
-      <c r="WY47" s="23"/>
-      <c r="WZ47" s="23"/>
-      <c r="XA47" s="23"/>
-      <c r="XB47" s="23"/>
-      <c r="XC47" s="23"/>
-      <c r="XD47" s="23"/>
-      <c r="XE47" s="23"/>
-      <c r="XF47" s="23"/>
-      <c r="XG47" s="23"/>
-      <c r="XH47" s="23"/>
-      <c r="XI47" s="23"/>
-      <c r="XJ47" s="23"/>
-      <c r="XK47" s="23"/>
-      <c r="XL47" s="23"/>
-      <c r="XM47" s="23"/>
-      <c r="XN47" s="23"/>
-      <c r="XO47" s="23"/>
-      <c r="XP47" s="23"/>
-      <c r="XQ47" s="23"/>
-      <c r="XR47" s="23"/>
-      <c r="XS47" s="23"/>
-      <c r="XT47" s="23"/>
-      <c r="XU47" s="23"/>
-      <c r="XV47" s="23"/>
-      <c r="XW47" s="23"/>
-      <c r="XX47" s="23"/>
-      <c r="XY47" s="23"/>
-      <c r="XZ47" s="23"/>
-      <c r="YA47" s="23"/>
-      <c r="YB47" s="23"/>
-      <c r="YC47" s="23"/>
-      <c r="YD47" s="23"/>
-      <c r="YE47" s="23"/>
-      <c r="YF47" s="23"/>
-      <c r="YG47" s="23"/>
-      <c r="YH47" s="23"/>
-      <c r="YI47" s="23"/>
-      <c r="YJ47" s="23"/>
-      <c r="YK47" s="23"/>
-      <c r="YL47" s="23"/>
-      <c r="YM47" s="23"/>
-      <c r="YN47" s="23"/>
-      <c r="YO47" s="23"/>
-      <c r="YP47" s="23"/>
-      <c r="YQ47" s="23"/>
-      <c r="YR47" s="23"/>
-      <c r="YS47" s="23"/>
-      <c r="YT47" s="23"/>
-      <c r="YU47" s="23"/>
-      <c r="YV47" s="23"/>
-      <c r="YW47" s="23"/>
-      <c r="YX47" s="23"/>
-      <c r="YY47" s="23"/>
-      <c r="YZ47" s="23"/>
-      <c r="ZA47" s="23"/>
-      <c r="ZB47" s="23"/>
-      <c r="ZC47" s="23"/>
-      <c r="ZD47" s="23"/>
-      <c r="ZE47" s="23"/>
-      <c r="ZF47" s="23"/>
-      <c r="ZG47" s="23"/>
-      <c r="ZH47" s="23"/>
-      <c r="ZI47" s="23"/>
-      <c r="ZJ47" s="23"/>
-      <c r="ZK47" s="23"/>
-      <c r="ZL47" s="23"/>
-      <c r="ZM47" s="23"/>
-      <c r="ZN47" s="23"/>
-      <c r="ZO47" s="23"/>
-      <c r="ZP47" s="23"/>
-      <c r="ZQ47" s="23"/>
-      <c r="ZR47" s="23"/>
-      <c r="ZS47" s="23"/>
-      <c r="ZT47" s="23"/>
-      <c r="ZU47" s="23"/>
-      <c r="ZV47" s="23"/>
-      <c r="ZW47" s="23"/>
-      <c r="ZX47" s="23"/>
-      <c r="ZY47" s="23"/>
-      <c r="ZZ47" s="23"/>
-      <c r="AAA47" s="23"/>
-      <c r="AAB47" s="23"/>
-      <c r="AAC47" s="23"/>
-      <c r="AAD47" s="23"/>
-      <c r="AAE47" s="23"/>
-      <c r="AAF47" s="23"/>
-      <c r="AAG47" s="23"/>
-      <c r="AAH47" s="23"/>
-      <c r="AAI47" s="23"/>
-      <c r="AAJ47" s="23"/>
-      <c r="AAK47" s="23"/>
-      <c r="AAL47" s="23"/>
-      <c r="AAM47" s="23"/>
-      <c r="AAN47" s="23"/>
-      <c r="AAO47" s="23"/>
-      <c r="AAP47" s="23"/>
-      <c r="AAQ47" s="23"/>
-      <c r="AAR47" s="23"/>
-      <c r="AAS47" s="23"/>
-      <c r="AAT47" s="23"/>
-      <c r="AAU47" s="23"/>
-      <c r="AAV47" s="23"/>
-      <c r="AAW47" s="23"/>
-      <c r="AAX47" s="23"/>
-      <c r="AAY47" s="23"/>
-      <c r="AAZ47" s="23"/>
-      <c r="ABA47" s="23"/>
-      <c r="ABB47" s="23"/>
-      <c r="ABC47" s="23"/>
-      <c r="ABD47" s="23"/>
-      <c r="ABE47" s="23"/>
-      <c r="ABF47" s="23"/>
-      <c r="ABG47" s="23"/>
-      <c r="ABH47" s="23"/>
-      <c r="ABI47" s="23"/>
-      <c r="ABJ47" s="23"/>
-      <c r="ABK47" s="23"/>
-      <c r="ABL47" s="23"/>
-      <c r="ABM47" s="23"/>
-      <c r="ABN47" s="23"/>
-      <c r="ABO47" s="23"/>
-      <c r="ABP47" s="23"/>
-      <c r="ABQ47" s="23"/>
-      <c r="ABR47" s="23"/>
-      <c r="ABS47" s="23"/>
-      <c r="ABT47" s="23"/>
-      <c r="ABU47" s="23"/>
-      <c r="ABV47" s="23"/>
-      <c r="ABW47" s="23"/>
-      <c r="ABX47" s="23"/>
-      <c r="ABY47" s="23"/>
-      <c r="ABZ47" s="23"/>
-      <c r="ACA47" s="23"/>
-      <c r="ACB47" s="23"/>
-      <c r="ACC47" s="23"/>
-      <c r="ACD47" s="23"/>
-      <c r="ACE47" s="23"/>
-      <c r="ACF47" s="23"/>
-      <c r="ACG47" s="23"/>
-      <c r="ACH47" s="23"/>
-      <c r="ACI47" s="23"/>
-      <c r="ACJ47" s="23"/>
-      <c r="ACK47" s="23"/>
-      <c r="ACL47" s="23"/>
-      <c r="ACM47" s="23"/>
-      <c r="ACN47" s="23"/>
-      <c r="ACO47" s="23"/>
-      <c r="ACP47" s="23"/>
-      <c r="ACQ47" s="23"/>
-      <c r="ACR47" s="23"/>
-      <c r="ACS47" s="23"/>
-      <c r="ACT47" s="23"/>
-      <c r="ACU47" s="23"/>
-      <c r="ACV47" s="23"/>
-      <c r="ACW47" s="23"/>
-      <c r="ACX47" s="23"/>
-      <c r="ACY47" s="23"/>
-      <c r="ACZ47" s="23"/>
-      <c r="ADA47" s="23"/>
-      <c r="ADB47" s="23"/>
-      <c r="ADC47" s="23"/>
-      <c r="ADD47" s="23"/>
-      <c r="ADE47" s="23"/>
-      <c r="ADF47" s="23"/>
-      <c r="ADG47" s="23"/>
-      <c r="ADH47" s="23"/>
-      <c r="ADI47" s="23"/>
-      <c r="ADJ47" s="23"/>
-      <c r="ADK47" s="23"/>
-      <c r="ADL47" s="23"/>
-      <c r="ADM47" s="23"/>
-      <c r="ADN47" s="23"/>
-      <c r="ADO47" s="23"/>
-      <c r="ADP47" s="23"/>
-      <c r="ADQ47" s="23"/>
-      <c r="ADR47" s="23"/>
-      <c r="ADS47" s="23"/>
-      <c r="ADT47" s="23"/>
-      <c r="ADU47" s="23"/>
-      <c r="ADV47" s="23"/>
-      <c r="ADW47" s="23"/>
-      <c r="ADX47" s="23"/>
-      <c r="ADY47" s="23"/>
-      <c r="ADZ47" s="23"/>
-      <c r="AEA47" s="23"/>
-      <c r="AEB47" s="23"/>
-      <c r="AEC47" s="23"/>
-      <c r="AED47" s="23"/>
-      <c r="AEE47" s="23"/>
-      <c r="AEF47" s="23"/>
-      <c r="AEG47" s="23"/>
-      <c r="AEH47" s="23"/>
-      <c r="AEI47" s="23"/>
-      <c r="AEJ47" s="23"/>
-      <c r="AEK47" s="23"/>
-      <c r="AEL47" s="23"/>
-      <c r="AEM47" s="23"/>
-      <c r="AEN47" s="23"/>
-      <c r="AEO47" s="23"/>
-      <c r="AEP47" s="23"/>
-      <c r="AEQ47" s="23"/>
-      <c r="AER47" s="23"/>
-      <c r="AES47" s="23"/>
-      <c r="AET47" s="23"/>
-      <c r="AEU47" s="23"/>
-      <c r="AEV47" s="23"/>
-      <c r="AEW47" s="23"/>
-      <c r="AEX47" s="23"/>
-      <c r="AEY47" s="23"/>
-      <c r="AEZ47" s="23"/>
-      <c r="AFA47" s="23"/>
-      <c r="AFB47" s="23"/>
-      <c r="AFC47" s="23"/>
-      <c r="AFD47" s="23"/>
-      <c r="AFE47" s="23"/>
-      <c r="AFF47" s="23"/>
-      <c r="AFG47" s="23"/>
-      <c r="AFH47" s="23"/>
-      <c r="AFI47" s="23"/>
-      <c r="AFJ47" s="23"/>
-      <c r="AFK47" s="23"/>
-      <c r="AFL47" s="23"/>
-      <c r="AFM47" s="23"/>
-      <c r="AFN47" s="23"/>
-      <c r="AFO47" s="23"/>
-      <c r="AFP47" s="23"/>
-      <c r="AFQ47" s="23"/>
-      <c r="AFR47" s="23"/>
-      <c r="AFS47" s="23"/>
-      <c r="AFT47" s="23"/>
-      <c r="AFU47" s="23"/>
-      <c r="AFV47" s="23"/>
-      <c r="AFW47" s="23"/>
-      <c r="AFX47" s="23"/>
-      <c r="AFY47" s="23"/>
-      <c r="AFZ47" s="23"/>
-      <c r="AGA47" s="23"/>
-      <c r="AGB47" s="23"/>
-      <c r="AGC47" s="23"/>
-      <c r="AGD47" s="23"/>
-      <c r="AGE47" s="23"/>
-      <c r="AGF47" s="23"/>
-      <c r="AGG47" s="23"/>
-      <c r="AGH47" s="23"/>
-      <c r="AGI47" s="23"/>
-      <c r="AGJ47" s="23"/>
-      <c r="AGK47" s="23"/>
-      <c r="AGL47" s="23"/>
-      <c r="AGM47" s="23"/>
-      <c r="AGN47" s="23"/>
-      <c r="AGO47" s="23"/>
-      <c r="AGP47" s="23"/>
-      <c r="AGQ47" s="23"/>
-      <c r="AGR47" s="23"/>
-      <c r="AGS47" s="23"/>
-      <c r="AGT47" s="23"/>
-      <c r="AGU47" s="23"/>
-      <c r="AGV47" s="23"/>
-      <c r="AGW47" s="23"/>
-      <c r="AGX47" s="23"/>
-      <c r="AGY47" s="23"/>
-      <c r="AGZ47" s="23"/>
-      <c r="AHA47" s="23"/>
-      <c r="AHB47" s="23"/>
-      <c r="AHC47" s="23"/>
-      <c r="AHD47" s="23"/>
-      <c r="AHE47" s="23"/>
-      <c r="AHF47" s="23"/>
-      <c r="AHG47" s="23"/>
-      <c r="AHH47" s="23"/>
-      <c r="AHI47" s="23"/>
-      <c r="AHJ47" s="23"/>
-      <c r="AHK47" s="23"/>
-      <c r="AHL47" s="23"/>
-      <c r="AHM47" s="23"/>
-      <c r="AHN47" s="23"/>
-      <c r="AHO47" s="23"/>
-      <c r="AHP47" s="23"/>
-      <c r="AHQ47" s="23"/>
-      <c r="AHR47" s="23"/>
-      <c r="AHS47" s="23"/>
-      <c r="AHT47" s="23"/>
-      <c r="AHU47" s="23"/>
-      <c r="AHV47" s="23"/>
-      <c r="AHW47" s="23"/>
-      <c r="AHX47" s="23"/>
-      <c r="AHY47" s="23"/>
-      <c r="AHZ47" s="23"/>
-      <c r="AIA47" s="23"/>
-      <c r="AIB47" s="23"/>
-      <c r="AIC47" s="23"/>
-      <c r="AID47" s="23"/>
-      <c r="AIE47" s="23"/>
-      <c r="AIF47" s="23"/>
-      <c r="AIG47" s="23"/>
-      <c r="AIH47" s="23"/>
-      <c r="AII47" s="23"/>
-      <c r="AIJ47" s="23"/>
-      <c r="AIK47" s="23"/>
-      <c r="AIL47" s="23"/>
-      <c r="AIM47" s="23"/>
-      <c r="AIN47" s="23"/>
-      <c r="AIO47" s="23"/>
-      <c r="AIP47" s="23"/>
-      <c r="AIQ47" s="23"/>
-      <c r="AIR47" s="23"/>
-      <c r="AIS47" s="23"/>
-      <c r="AIT47" s="23"/>
-      <c r="AIU47" s="23"/>
-      <c r="AIV47" s="23"/>
-      <c r="AIW47" s="23"/>
-      <c r="AIX47" s="23"/>
-      <c r="AIY47" s="23"/>
-      <c r="AIZ47" s="23"/>
-      <c r="AJA47" s="23"/>
-      <c r="AJB47" s="23"/>
-      <c r="AJC47" s="23"/>
-      <c r="AJD47" s="23"/>
-      <c r="AJE47" s="23"/>
-      <c r="AJF47" s="23"/>
-      <c r="AJG47" s="23"/>
-      <c r="AJH47" s="23"/>
-      <c r="AJI47" s="23"/>
-      <c r="AJJ47" s="23"/>
-      <c r="AJK47" s="23"/>
-      <c r="AJL47" s="23"/>
-      <c r="AJM47" s="23"/>
-      <c r="AJN47" s="23"/>
-      <c r="AJO47" s="23"/>
-      <c r="AJP47" s="23"/>
-      <c r="AJQ47" s="23"/>
-      <c r="AJR47" s="23"/>
-      <c r="AJS47" s="23"/>
-      <c r="AJT47" s="23"/>
-      <c r="AJU47" s="23"/>
-      <c r="AJV47" s="23"/>
-      <c r="AJW47" s="23"/>
-      <c r="AJX47" s="23"/>
-      <c r="AJY47" s="23"/>
-      <c r="AJZ47" s="23"/>
-      <c r="AKA47" s="23"/>
-      <c r="AKB47" s="23"/>
-      <c r="AKC47" s="23"/>
-      <c r="AKD47" s="23"/>
-      <c r="AKE47" s="23"/>
-      <c r="AKF47" s="23"/>
-      <c r="AKG47" s="23"/>
-      <c r="AKH47" s="23"/>
-      <c r="AKI47" s="23"/>
-      <c r="AKJ47" s="23"/>
-      <c r="AKK47" s="23"/>
-      <c r="AKL47" s="23"/>
-      <c r="AKM47" s="23"/>
-      <c r="AKN47" s="23"/>
-      <c r="AKO47" s="23"/>
-      <c r="AKP47" s="23"/>
-      <c r="AKQ47" s="23"/>
-      <c r="AKR47" s="23"/>
-      <c r="AKS47" s="23"/>
-      <c r="AKT47" s="23"/>
-      <c r="AKU47" s="23"/>
-      <c r="AKV47" s="23"/>
-      <c r="AKW47" s="23"/>
-      <c r="AKX47" s="23"/>
-      <c r="AKY47" s="23"/>
-      <c r="AKZ47" s="23"/>
-      <c r="ALA47" s="23"/>
-      <c r="ALB47" s="23"/>
-      <c r="ALC47" s="23"/>
-      <c r="ALD47" s="23"/>
-      <c r="ALE47" s="23"/>
-      <c r="ALF47" s="23"/>
-      <c r="ALG47" s="23"/>
-      <c r="ALH47" s="23"/>
-      <c r="ALI47" s="23"/>
-      <c r="ALJ47" s="23"/>
-      <c r="ALK47" s="23"/>
-      <c r="ALL47" s="23"/>
-      <c r="ALM47" s="23"/>
-      <c r="ALN47" s="23"/>
-      <c r="ALO47" s="23"/>
-      <c r="ALP47" s="23"/>
-      <c r="ALQ47" s="23"/>
-      <c r="ALR47" s="23"/>
-      <c r="ALS47" s="23"/>
-      <c r="ALT47" s="23"/>
-      <c r="ALU47" s="23"/>
-      <c r="ALV47" s="23"/>
-      <c r="ALW47" s="23"/>
-      <c r="ALX47" s="23"/>
-      <c r="ALY47" s="23"/>
-      <c r="ALZ47" s="23"/>
-      <c r="AMA47" s="23"/>
-      <c r="AMB47" s="23"/>
-      <c r="AMC47" s="23"/>
-      <c r="AMD47" s="23"/>
-      <c r="AME47" s="23"/>
-      <c r="AMF47" s="23"/>
-      <c r="AMG47" s="23"/>
-      <c r="AMH47" s="23"/>
-      <c r="AMI47" s="23"/>
-      <c r="AMJ47" s="23"/>
-      <c r="AMK47" s="23"/>
-    </row>
-    <row r="48" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="27"/>
+    </row>
+    <row r="48" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="5" t="s">
         <v>282</v>
       </c>
@@ -5068,1013 +4064,8 @@
       <c r="T48" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="U48" s="27"/>
-      <c r="V48" s="27"/>
-      <c r="W48" s="27"/>
-      <c r="X48" s="27"/>
-      <c r="Y48" s="27"/>
-      <c r="Z48" s="27"/>
-      <c r="AA48" s="27"/>
-      <c r="AB48" s="27"/>
-      <c r="AC48" s="27"/>
-      <c r="AD48" s="27"/>
-      <c r="AE48" s="27"/>
-      <c r="AF48" s="27"/>
-      <c r="AG48" s="27"/>
-      <c r="AH48" s="27"/>
-      <c r="AI48" s="27"/>
-      <c r="AJ48" s="27"/>
-      <c r="AK48" s="27"/>
-      <c r="AL48" s="27"/>
-      <c r="AM48" s="27"/>
-      <c r="AN48" s="27"/>
-      <c r="AO48" s="27"/>
-      <c r="AP48" s="27"/>
-      <c r="AQ48" s="27"/>
-      <c r="AR48" s="27"/>
-      <c r="AS48" s="27"/>
-      <c r="AT48" s="27"/>
-      <c r="AU48" s="27"/>
-      <c r="AV48" s="27"/>
-      <c r="AW48" s="27"/>
-      <c r="AX48" s="27"/>
-      <c r="AY48" s="27"/>
-      <c r="AZ48" s="27"/>
-      <c r="BA48" s="27"/>
-      <c r="BB48" s="27"/>
-      <c r="BC48" s="27"/>
-      <c r="BD48" s="27"/>
-      <c r="BE48" s="27"/>
-      <c r="BF48" s="27"/>
-      <c r="BG48" s="27"/>
-      <c r="BH48" s="27"/>
-      <c r="BI48" s="27"/>
-      <c r="BJ48" s="27"/>
-      <c r="BK48" s="27"/>
-      <c r="BL48" s="27"/>
-      <c r="BM48" s="27"/>
-      <c r="BN48" s="27"/>
-      <c r="BO48" s="27"/>
-      <c r="BP48" s="27"/>
-      <c r="BQ48" s="27"/>
-      <c r="BR48" s="27"/>
-      <c r="BS48" s="27"/>
-      <c r="BT48" s="27"/>
-      <c r="BU48" s="27"/>
-      <c r="BV48" s="27"/>
-      <c r="BW48" s="27"/>
-      <c r="BX48" s="27"/>
-      <c r="BY48" s="27"/>
-      <c r="BZ48" s="27"/>
-      <c r="CA48" s="27"/>
-      <c r="CB48" s="27"/>
-      <c r="CC48" s="27"/>
-      <c r="CD48" s="27"/>
-      <c r="CE48" s="27"/>
-      <c r="CF48" s="27"/>
-      <c r="CG48" s="27"/>
-      <c r="CH48" s="27"/>
-      <c r="CI48" s="27"/>
-      <c r="CJ48" s="27"/>
-      <c r="CK48" s="27"/>
-      <c r="CL48" s="27"/>
-      <c r="CM48" s="27"/>
-      <c r="CN48" s="27"/>
-      <c r="CO48" s="27"/>
-      <c r="CP48" s="27"/>
-      <c r="CQ48" s="27"/>
-      <c r="CR48" s="27"/>
-      <c r="CS48" s="27"/>
-      <c r="CT48" s="27"/>
-      <c r="CU48" s="27"/>
-      <c r="CV48" s="27"/>
-      <c r="CW48" s="27"/>
-      <c r="CX48" s="27"/>
-      <c r="CY48" s="27"/>
-      <c r="CZ48" s="27"/>
-      <c r="DA48" s="27"/>
-      <c r="DB48" s="27"/>
-      <c r="DC48" s="27"/>
-      <c r="DD48" s="27"/>
-      <c r="DE48" s="27"/>
-      <c r="DF48" s="27"/>
-      <c r="DG48" s="27"/>
-      <c r="DH48" s="27"/>
-      <c r="DI48" s="27"/>
-      <c r="DJ48" s="27"/>
-      <c r="DK48" s="27"/>
-      <c r="DL48" s="27"/>
-      <c r="DM48" s="27"/>
-      <c r="DN48" s="27"/>
-      <c r="DO48" s="27"/>
-      <c r="DP48" s="27"/>
-      <c r="DQ48" s="27"/>
-      <c r="DR48" s="27"/>
-      <c r="DS48" s="27"/>
-      <c r="DT48" s="27"/>
-      <c r="DU48" s="27"/>
-      <c r="DV48" s="27"/>
-      <c r="DW48" s="27"/>
-      <c r="DX48" s="27"/>
-      <c r="DY48" s="27"/>
-      <c r="DZ48" s="27"/>
-      <c r="EA48" s="27"/>
-      <c r="EB48" s="27"/>
-      <c r="EC48" s="27"/>
-      <c r="ED48" s="27"/>
-      <c r="EE48" s="27"/>
-      <c r="EF48" s="27"/>
-      <c r="EG48" s="27"/>
-      <c r="EH48" s="27"/>
-      <c r="EI48" s="27"/>
-      <c r="EJ48" s="27"/>
-      <c r="EK48" s="27"/>
-      <c r="EL48" s="27"/>
-      <c r="EM48" s="27"/>
-      <c r="EN48" s="27"/>
-      <c r="EO48" s="27"/>
-      <c r="EP48" s="27"/>
-      <c r="EQ48" s="27"/>
-      <c r="ER48" s="27"/>
-      <c r="ES48" s="27"/>
-      <c r="ET48" s="27"/>
-      <c r="EU48" s="27"/>
-      <c r="EV48" s="27"/>
-      <c r="EW48" s="27"/>
-      <c r="EX48" s="27"/>
-      <c r="EY48" s="27"/>
-      <c r="EZ48" s="27"/>
-      <c r="FA48" s="27"/>
-      <c r="FB48" s="27"/>
-      <c r="FC48" s="27"/>
-      <c r="FD48" s="27"/>
-      <c r="FE48" s="27"/>
-      <c r="FF48" s="27"/>
-      <c r="FG48" s="27"/>
-      <c r="FH48" s="27"/>
-      <c r="FI48" s="27"/>
-      <c r="FJ48" s="27"/>
-      <c r="FK48" s="27"/>
-      <c r="FL48" s="27"/>
-      <c r="FM48" s="27"/>
-      <c r="FN48" s="27"/>
-      <c r="FO48" s="27"/>
-      <c r="FP48" s="27"/>
-      <c r="FQ48" s="27"/>
-      <c r="FR48" s="27"/>
-      <c r="FS48" s="27"/>
-      <c r="FT48" s="27"/>
-      <c r="FU48" s="27"/>
-      <c r="FV48" s="27"/>
-      <c r="FW48" s="27"/>
-      <c r="FX48" s="27"/>
-      <c r="FY48" s="27"/>
-      <c r="FZ48" s="27"/>
-      <c r="GA48" s="27"/>
-      <c r="GB48" s="27"/>
-      <c r="GC48" s="27"/>
-      <c r="GD48" s="27"/>
-      <c r="GE48" s="27"/>
-      <c r="GF48" s="27"/>
-      <c r="GG48" s="27"/>
-      <c r="GH48" s="27"/>
-      <c r="GI48" s="27"/>
-      <c r="GJ48" s="27"/>
-      <c r="GK48" s="27"/>
-      <c r="GL48" s="27"/>
-      <c r="GM48" s="27"/>
-      <c r="GN48" s="27"/>
-      <c r="GO48" s="27"/>
-      <c r="GP48" s="27"/>
-      <c r="GQ48" s="27"/>
-      <c r="GR48" s="27"/>
-      <c r="GS48" s="27"/>
-      <c r="GT48" s="27"/>
-      <c r="GU48" s="27"/>
-      <c r="GV48" s="27"/>
-      <c r="GW48" s="27"/>
-      <c r="GX48" s="27"/>
-      <c r="GY48" s="27"/>
-      <c r="GZ48" s="27"/>
-      <c r="HA48" s="27"/>
-      <c r="HB48" s="27"/>
-      <c r="HC48" s="27"/>
-      <c r="HD48" s="27"/>
-      <c r="HE48" s="27"/>
-      <c r="HF48" s="27"/>
-      <c r="HG48" s="27"/>
-      <c r="HH48" s="27"/>
-      <c r="HI48" s="27"/>
-      <c r="HJ48" s="27"/>
-      <c r="HK48" s="27"/>
-      <c r="HL48" s="27"/>
-      <c r="HM48" s="27"/>
-      <c r="HN48" s="27"/>
-      <c r="HO48" s="27"/>
-      <c r="HP48" s="27"/>
-      <c r="HQ48" s="27"/>
-      <c r="HR48" s="27"/>
-      <c r="HS48" s="27"/>
-      <c r="HT48" s="27"/>
-      <c r="HU48" s="27"/>
-      <c r="HV48" s="27"/>
-      <c r="HW48" s="27"/>
-      <c r="HX48" s="27"/>
-      <c r="HY48" s="27"/>
-      <c r="HZ48" s="27"/>
-      <c r="IA48" s="27"/>
-      <c r="IB48" s="27"/>
-      <c r="IC48" s="27"/>
-      <c r="ID48" s="27"/>
-      <c r="IE48" s="27"/>
-      <c r="IF48" s="27"/>
-      <c r="IG48" s="27"/>
-      <c r="IH48" s="27"/>
-      <c r="II48" s="27"/>
-      <c r="IJ48" s="27"/>
-      <c r="IK48" s="27"/>
-      <c r="IL48" s="27"/>
-      <c r="IM48" s="27"/>
-      <c r="IN48" s="27"/>
-      <c r="IO48" s="27"/>
-      <c r="IP48" s="27"/>
-      <c r="IQ48" s="27"/>
-      <c r="IR48" s="27"/>
-      <c r="IS48" s="27"/>
-      <c r="IT48" s="27"/>
-      <c r="IU48" s="27"/>
-      <c r="IV48" s="27"/>
-      <c r="IW48" s="27"/>
-      <c r="IX48" s="27"/>
-      <c r="IY48" s="27"/>
-      <c r="IZ48" s="27"/>
-      <c r="JA48" s="27"/>
-      <c r="JB48" s="27"/>
-      <c r="JC48" s="27"/>
-      <c r="JD48" s="27"/>
-      <c r="JE48" s="27"/>
-      <c r="JF48" s="27"/>
-      <c r="JG48" s="27"/>
-      <c r="JH48" s="27"/>
-      <c r="JI48" s="27"/>
-      <c r="JJ48" s="27"/>
-      <c r="JK48" s="27"/>
-      <c r="JL48" s="27"/>
-      <c r="JM48" s="27"/>
-      <c r="JN48" s="27"/>
-      <c r="JO48" s="27"/>
-      <c r="JP48" s="27"/>
-      <c r="JQ48" s="27"/>
-      <c r="JR48" s="27"/>
-      <c r="JS48" s="27"/>
-      <c r="JT48" s="27"/>
-      <c r="JU48" s="27"/>
-      <c r="JV48" s="27"/>
-      <c r="JW48" s="27"/>
-      <c r="JX48" s="27"/>
-      <c r="JY48" s="27"/>
-      <c r="JZ48" s="27"/>
-      <c r="KA48" s="27"/>
-      <c r="KB48" s="27"/>
-      <c r="KC48" s="27"/>
-      <c r="KD48" s="27"/>
-      <c r="KE48" s="27"/>
-      <c r="KF48" s="27"/>
-      <c r="KG48" s="27"/>
-      <c r="KH48" s="27"/>
-      <c r="KI48" s="27"/>
-      <c r="KJ48" s="27"/>
-      <c r="KK48" s="27"/>
-      <c r="KL48" s="27"/>
-      <c r="KM48" s="27"/>
-      <c r="KN48" s="27"/>
-      <c r="KO48" s="27"/>
-      <c r="KP48" s="27"/>
-      <c r="KQ48" s="27"/>
-      <c r="KR48" s="27"/>
-      <c r="KS48" s="27"/>
-      <c r="KT48" s="27"/>
-      <c r="KU48" s="27"/>
-      <c r="KV48" s="27"/>
-      <c r="KW48" s="27"/>
-      <c r="KX48" s="27"/>
-      <c r="KY48" s="27"/>
-      <c r="KZ48" s="27"/>
-      <c r="LA48" s="27"/>
-      <c r="LB48" s="27"/>
-      <c r="LC48" s="27"/>
-      <c r="LD48" s="27"/>
-      <c r="LE48" s="27"/>
-      <c r="LF48" s="27"/>
-      <c r="LG48" s="27"/>
-      <c r="LH48" s="27"/>
-      <c r="LI48" s="27"/>
-      <c r="LJ48" s="27"/>
-      <c r="LK48" s="27"/>
-      <c r="LL48" s="27"/>
-      <c r="LM48" s="27"/>
-      <c r="LN48" s="27"/>
-      <c r="LO48" s="27"/>
-      <c r="LP48" s="27"/>
-      <c r="LQ48" s="27"/>
-      <c r="LR48" s="27"/>
-      <c r="LS48" s="27"/>
-      <c r="LT48" s="27"/>
-      <c r="LU48" s="27"/>
-      <c r="LV48" s="27"/>
-      <c r="LW48" s="27"/>
-      <c r="LX48" s="27"/>
-      <c r="LY48" s="27"/>
-      <c r="LZ48" s="27"/>
-      <c r="MA48" s="27"/>
-      <c r="MB48" s="27"/>
-      <c r="MC48" s="27"/>
-      <c r="MD48" s="27"/>
-      <c r="ME48" s="27"/>
-      <c r="MF48" s="27"/>
-      <c r="MG48" s="27"/>
-      <c r="MH48" s="27"/>
-      <c r="MI48" s="27"/>
-      <c r="MJ48" s="27"/>
-      <c r="MK48" s="27"/>
-      <c r="ML48" s="27"/>
-      <c r="MM48" s="27"/>
-      <c r="MN48" s="27"/>
-      <c r="MO48" s="27"/>
-      <c r="MP48" s="27"/>
-      <c r="MQ48" s="27"/>
-      <c r="MR48" s="27"/>
-      <c r="MS48" s="27"/>
-      <c r="MT48" s="27"/>
-      <c r="MU48" s="27"/>
-      <c r="MV48" s="27"/>
-      <c r="MW48" s="27"/>
-      <c r="MX48" s="27"/>
-      <c r="MY48" s="27"/>
-      <c r="MZ48" s="27"/>
-      <c r="NA48" s="27"/>
-      <c r="NB48" s="27"/>
-      <c r="NC48" s="27"/>
-      <c r="ND48" s="27"/>
-      <c r="NE48" s="27"/>
-      <c r="NF48" s="27"/>
-      <c r="NG48" s="27"/>
-      <c r="NH48" s="27"/>
-      <c r="NI48" s="27"/>
-      <c r="NJ48" s="27"/>
-      <c r="NK48" s="27"/>
-      <c r="NL48" s="27"/>
-      <c r="NM48" s="27"/>
-      <c r="NN48" s="27"/>
-      <c r="NO48" s="27"/>
-      <c r="NP48" s="27"/>
-      <c r="NQ48" s="27"/>
-      <c r="NR48" s="27"/>
-      <c r="NS48" s="27"/>
-      <c r="NT48" s="27"/>
-      <c r="NU48" s="27"/>
-      <c r="NV48" s="27"/>
-      <c r="NW48" s="27"/>
-      <c r="NX48" s="27"/>
-      <c r="NY48" s="27"/>
-      <c r="NZ48" s="27"/>
-      <c r="OA48" s="27"/>
-      <c r="OB48" s="27"/>
-      <c r="OC48" s="27"/>
-      <c r="OD48" s="27"/>
-      <c r="OE48" s="27"/>
-      <c r="OF48" s="27"/>
-      <c r="OG48" s="27"/>
-      <c r="OH48" s="27"/>
-      <c r="OI48" s="27"/>
-      <c r="OJ48" s="27"/>
-      <c r="OK48" s="27"/>
-      <c r="OL48" s="27"/>
-      <c r="OM48" s="27"/>
-      <c r="ON48" s="27"/>
-      <c r="OO48" s="27"/>
-      <c r="OP48" s="27"/>
-      <c r="OQ48" s="27"/>
-      <c r="OR48" s="27"/>
-      <c r="OS48" s="27"/>
-      <c r="OT48" s="27"/>
-      <c r="OU48" s="27"/>
-      <c r="OV48" s="27"/>
-      <c r="OW48" s="27"/>
-      <c r="OX48" s="27"/>
-      <c r="OY48" s="27"/>
-      <c r="OZ48" s="27"/>
-      <c r="PA48" s="27"/>
-      <c r="PB48" s="27"/>
-      <c r="PC48" s="27"/>
-      <c r="PD48" s="27"/>
-      <c r="PE48" s="27"/>
-      <c r="PF48" s="27"/>
-      <c r="PG48" s="27"/>
-      <c r="PH48" s="27"/>
-      <c r="PI48" s="27"/>
-      <c r="PJ48" s="27"/>
-      <c r="PK48" s="27"/>
-      <c r="PL48" s="27"/>
-      <c r="PM48" s="27"/>
-      <c r="PN48" s="27"/>
-      <c r="PO48" s="27"/>
-      <c r="PP48" s="27"/>
-      <c r="PQ48" s="27"/>
-      <c r="PR48" s="27"/>
-      <c r="PS48" s="27"/>
-      <c r="PT48" s="27"/>
-      <c r="PU48" s="27"/>
-      <c r="PV48" s="27"/>
-      <c r="PW48" s="27"/>
-      <c r="PX48" s="27"/>
-      <c r="PY48" s="27"/>
-      <c r="PZ48" s="27"/>
-      <c r="QA48" s="27"/>
-      <c r="QB48" s="27"/>
-      <c r="QC48" s="27"/>
-      <c r="QD48" s="27"/>
-      <c r="QE48" s="27"/>
-      <c r="QF48" s="27"/>
-      <c r="QG48" s="27"/>
-      <c r="QH48" s="27"/>
-      <c r="QI48" s="27"/>
-      <c r="QJ48" s="27"/>
-      <c r="QK48" s="27"/>
-      <c r="QL48" s="27"/>
-      <c r="QM48" s="27"/>
-      <c r="QN48" s="27"/>
-      <c r="QO48" s="27"/>
-      <c r="QP48" s="27"/>
-      <c r="QQ48" s="27"/>
-      <c r="QR48" s="27"/>
-      <c r="QS48" s="27"/>
-      <c r="QT48" s="27"/>
-      <c r="QU48" s="27"/>
-      <c r="QV48" s="27"/>
-      <c r="QW48" s="27"/>
-      <c r="QX48" s="27"/>
-      <c r="QY48" s="27"/>
-      <c r="QZ48" s="27"/>
-      <c r="RA48" s="27"/>
-      <c r="RB48" s="27"/>
-      <c r="RC48" s="27"/>
-      <c r="RD48" s="27"/>
-      <c r="RE48" s="27"/>
-      <c r="RF48" s="27"/>
-      <c r="RG48" s="27"/>
-      <c r="RH48" s="27"/>
-      <c r="RI48" s="27"/>
-      <c r="RJ48" s="27"/>
-      <c r="RK48" s="27"/>
-      <c r="RL48" s="27"/>
-      <c r="RM48" s="27"/>
-      <c r="RN48" s="27"/>
-      <c r="RO48" s="27"/>
-      <c r="RP48" s="27"/>
-      <c r="RQ48" s="27"/>
-      <c r="RR48" s="27"/>
-      <c r="RS48" s="27"/>
-      <c r="RT48" s="27"/>
-      <c r="RU48" s="27"/>
-      <c r="RV48" s="27"/>
-      <c r="RW48" s="27"/>
-      <c r="RX48" s="27"/>
-      <c r="RY48" s="27"/>
-      <c r="RZ48" s="27"/>
-      <c r="SA48" s="27"/>
-      <c r="SB48" s="27"/>
-      <c r="SC48" s="27"/>
-      <c r="SD48" s="27"/>
-      <c r="SE48" s="27"/>
-      <c r="SF48" s="27"/>
-      <c r="SG48" s="27"/>
-      <c r="SH48" s="27"/>
-      <c r="SI48" s="27"/>
-      <c r="SJ48" s="27"/>
-      <c r="SK48" s="27"/>
-      <c r="SL48" s="27"/>
-      <c r="SM48" s="27"/>
-      <c r="SN48" s="27"/>
-      <c r="SO48" s="27"/>
-      <c r="SP48" s="27"/>
-      <c r="SQ48" s="27"/>
-      <c r="SR48" s="27"/>
-      <c r="SS48" s="27"/>
-      <c r="ST48" s="27"/>
-      <c r="SU48" s="27"/>
-      <c r="SV48" s="27"/>
-      <c r="SW48" s="27"/>
-      <c r="SX48" s="27"/>
-      <c r="SY48" s="27"/>
-      <c r="SZ48" s="27"/>
-      <c r="TA48" s="27"/>
-      <c r="TB48" s="27"/>
-      <c r="TC48" s="27"/>
-      <c r="TD48" s="27"/>
-      <c r="TE48" s="27"/>
-      <c r="TF48" s="27"/>
-      <c r="TG48" s="27"/>
-      <c r="TH48" s="27"/>
-      <c r="TI48" s="27"/>
-      <c r="TJ48" s="27"/>
-      <c r="TK48" s="27"/>
-      <c r="TL48" s="27"/>
-      <c r="TM48" s="27"/>
-      <c r="TN48" s="27"/>
-      <c r="TO48" s="27"/>
-      <c r="TP48" s="27"/>
-      <c r="TQ48" s="27"/>
-      <c r="TR48" s="27"/>
-      <c r="TS48" s="27"/>
-      <c r="TT48" s="27"/>
-      <c r="TU48" s="27"/>
-      <c r="TV48" s="27"/>
-      <c r="TW48" s="27"/>
-      <c r="TX48" s="27"/>
-      <c r="TY48" s="27"/>
-      <c r="TZ48" s="27"/>
-      <c r="UA48" s="27"/>
-      <c r="UB48" s="27"/>
-      <c r="UC48" s="27"/>
-      <c r="UD48" s="27"/>
-      <c r="UE48" s="27"/>
-      <c r="UF48" s="27"/>
-      <c r="UG48" s="27"/>
-      <c r="UH48" s="27"/>
-      <c r="UI48" s="27"/>
-      <c r="UJ48" s="27"/>
-      <c r="UK48" s="27"/>
-      <c r="UL48" s="27"/>
-      <c r="UM48" s="27"/>
-      <c r="UN48" s="27"/>
-      <c r="UO48" s="27"/>
-      <c r="UP48" s="27"/>
-      <c r="UQ48" s="27"/>
-      <c r="UR48" s="27"/>
-      <c r="US48" s="27"/>
-      <c r="UT48" s="27"/>
-      <c r="UU48" s="27"/>
-      <c r="UV48" s="27"/>
-      <c r="UW48" s="27"/>
-      <c r="UX48" s="27"/>
-      <c r="UY48" s="27"/>
-      <c r="UZ48" s="27"/>
-      <c r="VA48" s="27"/>
-      <c r="VB48" s="27"/>
-      <c r="VC48" s="27"/>
-      <c r="VD48" s="27"/>
-      <c r="VE48" s="27"/>
-      <c r="VF48" s="27"/>
-      <c r="VG48" s="27"/>
-      <c r="VH48" s="27"/>
-      <c r="VI48" s="27"/>
-      <c r="VJ48" s="27"/>
-      <c r="VK48" s="27"/>
-      <c r="VL48" s="27"/>
-      <c r="VM48" s="27"/>
-      <c r="VN48" s="27"/>
-      <c r="VO48" s="27"/>
-      <c r="VP48" s="27"/>
-      <c r="VQ48" s="27"/>
-      <c r="VR48" s="27"/>
-      <c r="VS48" s="27"/>
-      <c r="VT48" s="27"/>
-      <c r="VU48" s="27"/>
-      <c r="VV48" s="27"/>
-      <c r="VW48" s="27"/>
-      <c r="VX48" s="27"/>
-      <c r="VY48" s="27"/>
-      <c r="VZ48" s="27"/>
-      <c r="WA48" s="27"/>
-      <c r="WB48" s="27"/>
-      <c r="WC48" s="27"/>
-      <c r="WD48" s="27"/>
-      <c r="WE48" s="27"/>
-      <c r="WF48" s="27"/>
-      <c r="WG48" s="27"/>
-      <c r="WH48" s="27"/>
-      <c r="WI48" s="27"/>
-      <c r="WJ48" s="27"/>
-      <c r="WK48" s="27"/>
-      <c r="WL48" s="27"/>
-      <c r="WM48" s="27"/>
-      <c r="WN48" s="27"/>
-      <c r="WO48" s="27"/>
-      <c r="WP48" s="27"/>
-      <c r="WQ48" s="27"/>
-      <c r="WR48" s="27"/>
-      <c r="WS48" s="27"/>
-      <c r="WT48" s="27"/>
-      <c r="WU48" s="27"/>
-      <c r="WV48" s="27"/>
-      <c r="WW48" s="27"/>
-      <c r="WX48" s="27"/>
-      <c r="WY48" s="27"/>
-      <c r="WZ48" s="27"/>
-      <c r="XA48" s="27"/>
-      <c r="XB48" s="27"/>
-      <c r="XC48" s="27"/>
-      <c r="XD48" s="27"/>
-      <c r="XE48" s="27"/>
-      <c r="XF48" s="27"/>
-      <c r="XG48" s="27"/>
-      <c r="XH48" s="27"/>
-      <c r="XI48" s="27"/>
-      <c r="XJ48" s="27"/>
-      <c r="XK48" s="27"/>
-      <c r="XL48" s="27"/>
-      <c r="XM48" s="27"/>
-      <c r="XN48" s="27"/>
-      <c r="XO48" s="27"/>
-      <c r="XP48" s="27"/>
-      <c r="XQ48" s="27"/>
-      <c r="XR48" s="27"/>
-      <c r="XS48" s="27"/>
-      <c r="XT48" s="27"/>
-      <c r="XU48" s="27"/>
-      <c r="XV48" s="27"/>
-      <c r="XW48" s="27"/>
-      <c r="XX48" s="27"/>
-      <c r="XY48" s="27"/>
-      <c r="XZ48" s="27"/>
-      <c r="YA48" s="27"/>
-      <c r="YB48" s="27"/>
-      <c r="YC48" s="27"/>
-      <c r="YD48" s="27"/>
-      <c r="YE48" s="27"/>
-      <c r="YF48" s="27"/>
-      <c r="YG48" s="27"/>
-      <c r="YH48" s="27"/>
-      <c r="YI48" s="27"/>
-      <c r="YJ48" s="27"/>
-      <c r="YK48" s="27"/>
-      <c r="YL48" s="27"/>
-      <c r="YM48" s="27"/>
-      <c r="YN48" s="27"/>
-      <c r="YO48" s="27"/>
-      <c r="YP48" s="27"/>
-      <c r="YQ48" s="27"/>
-      <c r="YR48" s="27"/>
-      <c r="YS48" s="27"/>
-      <c r="YT48" s="27"/>
-      <c r="YU48" s="27"/>
-      <c r="YV48" s="27"/>
-      <c r="YW48" s="27"/>
-      <c r="YX48" s="27"/>
-      <c r="YY48" s="27"/>
-      <c r="YZ48" s="27"/>
-      <c r="ZA48" s="27"/>
-      <c r="ZB48" s="27"/>
-      <c r="ZC48" s="27"/>
-      <c r="ZD48" s="27"/>
-      <c r="ZE48" s="27"/>
-      <c r="ZF48" s="27"/>
-      <c r="ZG48" s="27"/>
-      <c r="ZH48" s="27"/>
-      <c r="ZI48" s="27"/>
-      <c r="ZJ48" s="27"/>
-      <c r="ZK48" s="27"/>
-      <c r="ZL48" s="27"/>
-      <c r="ZM48" s="27"/>
-      <c r="ZN48" s="27"/>
-      <c r="ZO48" s="27"/>
-      <c r="ZP48" s="27"/>
-      <c r="ZQ48" s="27"/>
-      <c r="ZR48" s="27"/>
-      <c r="ZS48" s="27"/>
-      <c r="ZT48" s="27"/>
-      <c r="ZU48" s="27"/>
-      <c r="ZV48" s="27"/>
-      <c r="ZW48" s="27"/>
-      <c r="ZX48" s="27"/>
-      <c r="ZY48" s="27"/>
-      <c r="ZZ48" s="27"/>
-      <c r="AAA48" s="27"/>
-      <c r="AAB48" s="27"/>
-      <c r="AAC48" s="27"/>
-      <c r="AAD48" s="27"/>
-      <c r="AAE48" s="27"/>
-      <c r="AAF48" s="27"/>
-      <c r="AAG48" s="27"/>
-      <c r="AAH48" s="27"/>
-      <c r="AAI48" s="27"/>
-      <c r="AAJ48" s="27"/>
-      <c r="AAK48" s="27"/>
-      <c r="AAL48" s="27"/>
-      <c r="AAM48" s="27"/>
-      <c r="AAN48" s="27"/>
-      <c r="AAO48" s="27"/>
-      <c r="AAP48" s="27"/>
-      <c r="AAQ48" s="27"/>
-      <c r="AAR48" s="27"/>
-      <c r="AAS48" s="27"/>
-      <c r="AAT48" s="27"/>
-      <c r="AAU48" s="27"/>
-      <c r="AAV48" s="27"/>
-      <c r="AAW48" s="27"/>
-      <c r="AAX48" s="27"/>
-      <c r="AAY48" s="27"/>
-      <c r="AAZ48" s="27"/>
-      <c r="ABA48" s="27"/>
-      <c r="ABB48" s="27"/>
-      <c r="ABC48" s="27"/>
-      <c r="ABD48" s="27"/>
-      <c r="ABE48" s="27"/>
-      <c r="ABF48" s="27"/>
-      <c r="ABG48" s="27"/>
-      <c r="ABH48" s="27"/>
-      <c r="ABI48" s="27"/>
-      <c r="ABJ48" s="27"/>
-      <c r="ABK48" s="27"/>
-      <c r="ABL48" s="27"/>
-      <c r="ABM48" s="27"/>
-      <c r="ABN48" s="27"/>
-      <c r="ABO48" s="27"/>
-      <c r="ABP48" s="27"/>
-      <c r="ABQ48" s="27"/>
-      <c r="ABR48" s="27"/>
-      <c r="ABS48" s="27"/>
-      <c r="ABT48" s="27"/>
-      <c r="ABU48" s="27"/>
-      <c r="ABV48" s="27"/>
-      <c r="ABW48" s="27"/>
-      <c r="ABX48" s="27"/>
-      <c r="ABY48" s="27"/>
-      <c r="ABZ48" s="27"/>
-      <c r="ACA48" s="27"/>
-      <c r="ACB48" s="27"/>
-      <c r="ACC48" s="27"/>
-      <c r="ACD48" s="27"/>
-      <c r="ACE48" s="27"/>
-      <c r="ACF48" s="27"/>
-      <c r="ACG48" s="27"/>
-      <c r="ACH48" s="27"/>
-      <c r="ACI48" s="27"/>
-      <c r="ACJ48" s="27"/>
-      <c r="ACK48" s="27"/>
-      <c r="ACL48" s="27"/>
-      <c r="ACM48" s="27"/>
-      <c r="ACN48" s="27"/>
-      <c r="ACO48" s="27"/>
-      <c r="ACP48" s="27"/>
-      <c r="ACQ48" s="27"/>
-      <c r="ACR48" s="27"/>
-      <c r="ACS48" s="27"/>
-      <c r="ACT48" s="27"/>
-      <c r="ACU48" s="27"/>
-      <c r="ACV48" s="27"/>
-      <c r="ACW48" s="27"/>
-      <c r="ACX48" s="27"/>
-      <c r="ACY48" s="27"/>
-      <c r="ACZ48" s="27"/>
-      <c r="ADA48" s="27"/>
-      <c r="ADB48" s="27"/>
-      <c r="ADC48" s="27"/>
-      <c r="ADD48" s="27"/>
-      <c r="ADE48" s="27"/>
-      <c r="ADF48" s="27"/>
-      <c r="ADG48" s="27"/>
-      <c r="ADH48" s="27"/>
-      <c r="ADI48" s="27"/>
-      <c r="ADJ48" s="27"/>
-      <c r="ADK48" s="27"/>
-      <c r="ADL48" s="27"/>
-      <c r="ADM48" s="27"/>
-      <c r="ADN48" s="27"/>
-      <c r="ADO48" s="27"/>
-      <c r="ADP48" s="27"/>
-      <c r="ADQ48" s="27"/>
-      <c r="ADR48" s="27"/>
-      <c r="ADS48" s="27"/>
-      <c r="ADT48" s="27"/>
-      <c r="ADU48" s="27"/>
-      <c r="ADV48" s="27"/>
-      <c r="ADW48" s="27"/>
-      <c r="ADX48" s="27"/>
-      <c r="ADY48" s="27"/>
-      <c r="ADZ48" s="27"/>
-      <c r="AEA48" s="27"/>
-      <c r="AEB48" s="27"/>
-      <c r="AEC48" s="27"/>
-      <c r="AED48" s="27"/>
-      <c r="AEE48" s="27"/>
-      <c r="AEF48" s="27"/>
-      <c r="AEG48" s="27"/>
-      <c r="AEH48" s="27"/>
-      <c r="AEI48" s="27"/>
-      <c r="AEJ48" s="27"/>
-      <c r="AEK48" s="27"/>
-      <c r="AEL48" s="27"/>
-      <c r="AEM48" s="27"/>
-      <c r="AEN48" s="27"/>
-      <c r="AEO48" s="27"/>
-      <c r="AEP48" s="27"/>
-      <c r="AEQ48" s="27"/>
-      <c r="AER48" s="27"/>
-      <c r="AES48" s="27"/>
-      <c r="AET48" s="27"/>
-      <c r="AEU48" s="27"/>
-      <c r="AEV48" s="27"/>
-      <c r="AEW48" s="27"/>
-      <c r="AEX48" s="27"/>
-      <c r="AEY48" s="27"/>
-      <c r="AEZ48" s="27"/>
-      <c r="AFA48" s="27"/>
-      <c r="AFB48" s="27"/>
-      <c r="AFC48" s="27"/>
-      <c r="AFD48" s="27"/>
-      <c r="AFE48" s="27"/>
-      <c r="AFF48" s="27"/>
-      <c r="AFG48" s="27"/>
-      <c r="AFH48" s="27"/>
-      <c r="AFI48" s="27"/>
-      <c r="AFJ48" s="27"/>
-      <c r="AFK48" s="27"/>
-      <c r="AFL48" s="27"/>
-      <c r="AFM48" s="27"/>
-      <c r="AFN48" s="27"/>
-      <c r="AFO48" s="27"/>
-      <c r="AFP48" s="27"/>
-      <c r="AFQ48" s="27"/>
-      <c r="AFR48" s="27"/>
-      <c r="AFS48" s="27"/>
-      <c r="AFT48" s="27"/>
-      <c r="AFU48" s="27"/>
-      <c r="AFV48" s="27"/>
-      <c r="AFW48" s="27"/>
-      <c r="AFX48" s="27"/>
-      <c r="AFY48" s="27"/>
-      <c r="AFZ48" s="27"/>
-      <c r="AGA48" s="27"/>
-      <c r="AGB48" s="27"/>
-      <c r="AGC48" s="27"/>
-      <c r="AGD48" s="27"/>
-      <c r="AGE48" s="27"/>
-      <c r="AGF48" s="27"/>
-      <c r="AGG48" s="27"/>
-      <c r="AGH48" s="27"/>
-      <c r="AGI48" s="27"/>
-      <c r="AGJ48" s="27"/>
-      <c r="AGK48" s="27"/>
-      <c r="AGL48" s="27"/>
-      <c r="AGM48" s="27"/>
-      <c r="AGN48" s="27"/>
-      <c r="AGO48" s="27"/>
-      <c r="AGP48" s="27"/>
-      <c r="AGQ48" s="27"/>
-      <c r="AGR48" s="27"/>
-      <c r="AGS48" s="27"/>
-      <c r="AGT48" s="27"/>
-      <c r="AGU48" s="27"/>
-      <c r="AGV48" s="27"/>
-      <c r="AGW48" s="27"/>
-      <c r="AGX48" s="27"/>
-      <c r="AGY48" s="27"/>
-      <c r="AGZ48" s="27"/>
-      <c r="AHA48" s="27"/>
-      <c r="AHB48" s="27"/>
-      <c r="AHC48" s="27"/>
-      <c r="AHD48" s="27"/>
-      <c r="AHE48" s="27"/>
-      <c r="AHF48" s="27"/>
-      <c r="AHG48" s="27"/>
-      <c r="AHH48" s="27"/>
-      <c r="AHI48" s="27"/>
-      <c r="AHJ48" s="27"/>
-      <c r="AHK48" s="27"/>
-      <c r="AHL48" s="27"/>
-      <c r="AHM48" s="27"/>
-      <c r="AHN48" s="27"/>
-      <c r="AHO48" s="27"/>
-      <c r="AHP48" s="27"/>
-      <c r="AHQ48" s="27"/>
-      <c r="AHR48" s="27"/>
-      <c r="AHS48" s="27"/>
-      <c r="AHT48" s="27"/>
-      <c r="AHU48" s="27"/>
-      <c r="AHV48" s="27"/>
-      <c r="AHW48" s="27"/>
-      <c r="AHX48" s="27"/>
-      <c r="AHY48" s="27"/>
-      <c r="AHZ48" s="27"/>
-      <c r="AIA48" s="27"/>
-      <c r="AIB48" s="27"/>
-      <c r="AIC48" s="27"/>
-      <c r="AID48" s="27"/>
-      <c r="AIE48" s="27"/>
-      <c r="AIF48" s="27"/>
-      <c r="AIG48" s="27"/>
-      <c r="AIH48" s="27"/>
-      <c r="AII48" s="27"/>
-      <c r="AIJ48" s="27"/>
-      <c r="AIK48" s="27"/>
-      <c r="AIL48" s="27"/>
-      <c r="AIM48" s="27"/>
-      <c r="AIN48" s="27"/>
-      <c r="AIO48" s="27"/>
-      <c r="AIP48" s="27"/>
-      <c r="AIQ48" s="27"/>
-      <c r="AIR48" s="27"/>
-      <c r="AIS48" s="27"/>
-      <c r="AIT48" s="27"/>
-      <c r="AIU48" s="27"/>
-      <c r="AIV48" s="27"/>
-      <c r="AIW48" s="27"/>
-      <c r="AIX48" s="27"/>
-      <c r="AIY48" s="27"/>
-      <c r="AIZ48" s="27"/>
-      <c r="AJA48" s="27"/>
-      <c r="AJB48" s="27"/>
-      <c r="AJC48" s="27"/>
-      <c r="AJD48" s="27"/>
-      <c r="AJE48" s="27"/>
-      <c r="AJF48" s="27"/>
-      <c r="AJG48" s="27"/>
-      <c r="AJH48" s="27"/>
-      <c r="AJI48" s="27"/>
-      <c r="AJJ48" s="27"/>
-      <c r="AJK48" s="27"/>
-      <c r="AJL48" s="27"/>
-      <c r="AJM48" s="27"/>
-      <c r="AJN48" s="27"/>
-      <c r="AJO48" s="27"/>
-      <c r="AJP48" s="27"/>
-      <c r="AJQ48" s="27"/>
-      <c r="AJR48" s="27"/>
-      <c r="AJS48" s="27"/>
-      <c r="AJT48" s="27"/>
-      <c r="AJU48" s="27"/>
-      <c r="AJV48" s="27"/>
-      <c r="AJW48" s="27"/>
-      <c r="AJX48" s="27"/>
-      <c r="AJY48" s="27"/>
-      <c r="AJZ48" s="27"/>
-      <c r="AKA48" s="27"/>
-      <c r="AKB48" s="27"/>
-      <c r="AKC48" s="27"/>
-      <c r="AKD48" s="27"/>
-      <c r="AKE48" s="27"/>
-      <c r="AKF48" s="27"/>
-      <c r="AKG48" s="27"/>
-      <c r="AKH48" s="27"/>
-      <c r="AKI48" s="27"/>
-      <c r="AKJ48" s="27"/>
-      <c r="AKK48" s="27"/>
-      <c r="AKL48" s="27"/>
-      <c r="AKM48" s="27"/>
-      <c r="AKN48" s="27"/>
-      <c r="AKO48" s="27"/>
-      <c r="AKP48" s="27"/>
-      <c r="AKQ48" s="27"/>
-      <c r="AKR48" s="27"/>
-      <c r="AKS48" s="27"/>
-      <c r="AKT48" s="27"/>
-      <c r="AKU48" s="27"/>
-      <c r="AKV48" s="27"/>
-      <c r="AKW48" s="27"/>
-      <c r="AKX48" s="27"/>
-      <c r="AKY48" s="27"/>
-      <c r="AKZ48" s="27"/>
-      <c r="ALA48" s="27"/>
-      <c r="ALB48" s="27"/>
-      <c r="ALC48" s="27"/>
-      <c r="ALD48" s="27"/>
-      <c r="ALE48" s="27"/>
-      <c r="ALF48" s="27"/>
-      <c r="ALG48" s="27"/>
-      <c r="ALH48" s="27"/>
-      <c r="ALI48" s="27"/>
-      <c r="ALJ48" s="27"/>
-      <c r="ALK48" s="27"/>
-      <c r="ALL48" s="27"/>
-      <c r="ALM48" s="27"/>
-      <c r="ALN48" s="27"/>
-      <c r="ALO48" s="27"/>
-      <c r="ALP48" s="27"/>
-      <c r="ALQ48" s="27"/>
-      <c r="ALR48" s="27"/>
-      <c r="ALS48" s="27"/>
-      <c r="ALT48" s="27"/>
-      <c r="ALU48" s="27"/>
-      <c r="ALV48" s="27"/>
-      <c r="ALW48" s="27"/>
-      <c r="ALX48" s="27"/>
-      <c r="ALY48" s="27"/>
-      <c r="ALZ48" s="27"/>
-      <c r="AMA48" s="27"/>
-      <c r="AMB48" s="27"/>
-      <c r="AMC48" s="27"/>
-      <c r="AMD48" s="27"/>
-      <c r="AME48" s="27"/>
-      <c r="AMF48" s="27"/>
-      <c r="AMG48" s="27"/>
-      <c r="AMH48" s="27"/>
-      <c r="AMI48" s="27"/>
-      <c r="AMJ48" s="27"/>
-      <c r="AMK48" s="27"/>
-    </row>
-    <row r="49" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
         <v>210</v>
       </c>
@@ -6114,10 +4105,8 @@
       <c r="T49" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="U49" s="23"/>
-    </row>
-    <row r="50" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="23"/>
+    </row>
+    <row r="50" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="5" t="s">
         <v>279</v>
       </c>
@@ -6163,7 +4152,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="5" t="s">
         <v>214</v>
       </c>
@@ -6209,7 +4198,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="5" t="s">
         <v>245</v>
       </c>
@@ -6255,7 +4244,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:20" ht="32" x14ac:dyDescent="0.2">
       <c r="B53" s="5" t="s">
         <v>242</v>
       </c>
@@ -6301,7 +4290,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:20" ht="32" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="s">
         <v>235</v>
       </c>
@@ -6348,8 +4337,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="2:20" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="s">
         <v>186</v>
       </c>
@@ -6388,1072 +4377,49 @@
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="32" t="s">
+    <row r="60" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="C62" s="32"/>
-    </row>
-    <row r="63" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="33" t="s">
+      <c r="C62" s="30"/>
+    </row>
+    <row r="63" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="C63" s="33"/>
-    </row>
-    <row r="64" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="33" t="s">
+      <c r="C63" s="31"/>
+    </row>
+    <row r="64" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="C64" s="33"/>
-    </row>
-    <row r="65" spans="1:1025" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="34" t="s">
+      <c r="C64" s="31"/>
+    </row>
+    <row r="65" spans="2:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="C65" s="34"/>
-    </row>
-    <row r="66" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="B66" s="34" t="s">
+      <c r="C65" s="32"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B66" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="C66" s="34"/>
-    </row>
-    <row r="67" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="A67" s="26"/>
-      <c r="B67" s="34" t="s">
+      <c r="C66" s="32"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B67" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="C67" s="34"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="26"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="26"/>
-      <c r="K67" s="26"/>
-      <c r="L67" s="26"/>
-      <c r="M67" s="26"/>
-      <c r="N67" s="26"/>
-      <c r="O67" s="26"/>
-      <c r="P67" s="26"/>
-      <c r="Q67" s="26"/>
-      <c r="R67" s="26"/>
-      <c r="S67" s="26"/>
-      <c r="T67" s="26"/>
-      <c r="U67" s="26"/>
-      <c r="V67" s="26"/>
-      <c r="W67" s="26"/>
-      <c r="X67" s="26"/>
-      <c r="Y67" s="26"/>
-      <c r="Z67" s="26"/>
-      <c r="AA67" s="26"/>
-      <c r="AB67" s="26"/>
-      <c r="AC67" s="26"/>
-      <c r="AD67" s="26"/>
-      <c r="AE67" s="26"/>
-      <c r="AF67" s="26"/>
-      <c r="AG67" s="26"/>
-      <c r="AH67" s="26"/>
-      <c r="AI67" s="26"/>
-      <c r="AJ67" s="26"/>
-      <c r="AK67" s="26"/>
-      <c r="AL67" s="26"/>
-      <c r="AM67" s="26"/>
-      <c r="AN67" s="26"/>
-      <c r="AO67" s="26"/>
-      <c r="AP67" s="26"/>
-      <c r="AQ67" s="26"/>
-      <c r="AR67" s="26"/>
-      <c r="AS67" s="26"/>
-      <c r="AT67" s="26"/>
-      <c r="AU67" s="26"/>
-      <c r="AV67" s="26"/>
-      <c r="AW67" s="26"/>
-      <c r="AX67" s="26"/>
-      <c r="AY67" s="26"/>
-      <c r="AZ67" s="26"/>
-      <c r="BA67" s="26"/>
-      <c r="BB67" s="26"/>
-      <c r="BC67" s="26"/>
-      <c r="BD67" s="26"/>
-      <c r="BE67" s="26"/>
-      <c r="BF67" s="26"/>
-      <c r="BG67" s="26"/>
-      <c r="BH67" s="26"/>
-      <c r="BI67" s="26"/>
-      <c r="BJ67" s="26"/>
-      <c r="BK67" s="26"/>
-      <c r="BL67" s="26"/>
-      <c r="BM67" s="26"/>
-      <c r="BN67" s="26"/>
-      <c r="BO67" s="26"/>
-      <c r="BP67" s="26"/>
-      <c r="BQ67" s="26"/>
-      <c r="BR67" s="26"/>
-      <c r="BS67" s="26"/>
-      <c r="BT67" s="26"/>
-      <c r="BU67" s="26"/>
-      <c r="BV67" s="26"/>
-      <c r="BW67" s="26"/>
-      <c r="BX67" s="26"/>
-      <c r="BY67" s="26"/>
-      <c r="BZ67" s="26"/>
-      <c r="CA67" s="26"/>
-      <c r="CB67" s="26"/>
-      <c r="CC67" s="26"/>
-      <c r="CD67" s="26"/>
-      <c r="CE67" s="26"/>
-      <c r="CF67" s="26"/>
-      <c r="CG67" s="26"/>
-      <c r="CH67" s="26"/>
-      <c r="CI67" s="26"/>
-      <c r="CJ67" s="26"/>
-      <c r="CK67" s="26"/>
-      <c r="CL67" s="26"/>
-      <c r="CM67" s="26"/>
-      <c r="CN67" s="26"/>
-      <c r="CO67" s="26"/>
-      <c r="CP67" s="26"/>
-      <c r="CQ67" s="26"/>
-      <c r="CR67" s="26"/>
-      <c r="CS67" s="26"/>
-      <c r="CT67" s="26"/>
-      <c r="CU67" s="26"/>
-      <c r="CV67" s="26"/>
-      <c r="CW67" s="26"/>
-      <c r="CX67" s="26"/>
-      <c r="CY67" s="26"/>
-      <c r="CZ67" s="26"/>
-      <c r="DA67" s="26"/>
-      <c r="DB67" s="26"/>
-      <c r="DC67" s="26"/>
-      <c r="DD67" s="26"/>
-      <c r="DE67" s="26"/>
-      <c r="DF67" s="26"/>
-      <c r="DG67" s="26"/>
-      <c r="DH67" s="26"/>
-      <c r="DI67" s="26"/>
-      <c r="DJ67" s="26"/>
-      <c r="DK67" s="26"/>
-      <c r="DL67" s="26"/>
-      <c r="DM67" s="26"/>
-      <c r="DN67" s="26"/>
-      <c r="DO67" s="26"/>
-      <c r="DP67" s="26"/>
-      <c r="DQ67" s="26"/>
-      <c r="DR67" s="26"/>
-      <c r="DS67" s="26"/>
-      <c r="DT67" s="26"/>
-      <c r="DU67" s="26"/>
-      <c r="DV67" s="26"/>
-      <c r="DW67" s="26"/>
-      <c r="DX67" s="26"/>
-      <c r="DY67" s="26"/>
-      <c r="DZ67" s="26"/>
-      <c r="EA67" s="26"/>
-      <c r="EB67" s="26"/>
-      <c r="EC67" s="26"/>
-      <c r="ED67" s="26"/>
-      <c r="EE67" s="26"/>
-      <c r="EF67" s="26"/>
-      <c r="EG67" s="26"/>
-      <c r="EH67" s="26"/>
-      <c r="EI67" s="26"/>
-      <c r="EJ67" s="26"/>
-      <c r="EK67" s="26"/>
-      <c r="EL67" s="26"/>
-      <c r="EM67" s="26"/>
-      <c r="EN67" s="26"/>
-      <c r="EO67" s="26"/>
-      <c r="EP67" s="26"/>
-      <c r="EQ67" s="26"/>
-      <c r="ER67" s="26"/>
-      <c r="ES67" s="26"/>
-      <c r="ET67" s="26"/>
-      <c r="EU67" s="26"/>
-      <c r="EV67" s="26"/>
-      <c r="EW67" s="26"/>
-      <c r="EX67" s="26"/>
-      <c r="EY67" s="26"/>
-      <c r="EZ67" s="26"/>
-      <c r="FA67" s="26"/>
-      <c r="FB67" s="26"/>
-      <c r="FC67" s="26"/>
-      <c r="FD67" s="26"/>
-      <c r="FE67" s="26"/>
-      <c r="FF67" s="26"/>
-      <c r="FG67" s="26"/>
-      <c r="FH67" s="26"/>
-      <c r="FI67" s="26"/>
-      <c r="FJ67" s="26"/>
-      <c r="FK67" s="26"/>
-      <c r="FL67" s="26"/>
-      <c r="FM67" s="26"/>
-      <c r="FN67" s="26"/>
-      <c r="FO67" s="26"/>
-      <c r="FP67" s="26"/>
-      <c r="FQ67" s="26"/>
-      <c r="FR67" s="26"/>
-      <c r="FS67" s="26"/>
-      <c r="FT67" s="26"/>
-      <c r="FU67" s="26"/>
-      <c r="FV67" s="26"/>
-      <c r="FW67" s="26"/>
-      <c r="FX67" s="26"/>
-      <c r="FY67" s="26"/>
-      <c r="FZ67" s="26"/>
-      <c r="GA67" s="26"/>
-      <c r="GB67" s="26"/>
-      <c r="GC67" s="26"/>
-      <c r="GD67" s="26"/>
-      <c r="GE67" s="26"/>
-      <c r="GF67" s="26"/>
-      <c r="GG67" s="26"/>
-      <c r="GH67" s="26"/>
-      <c r="GI67" s="26"/>
-      <c r="GJ67" s="26"/>
-      <c r="GK67" s="26"/>
-      <c r="GL67" s="26"/>
-      <c r="GM67" s="26"/>
-      <c r="GN67" s="26"/>
-      <c r="GO67" s="26"/>
-      <c r="GP67" s="26"/>
-      <c r="GQ67" s="26"/>
-      <c r="GR67" s="26"/>
-      <c r="GS67" s="26"/>
-      <c r="GT67" s="26"/>
-      <c r="GU67" s="26"/>
-      <c r="GV67" s="26"/>
-      <c r="GW67" s="26"/>
-      <c r="GX67" s="26"/>
-      <c r="GY67" s="26"/>
-      <c r="GZ67" s="26"/>
-      <c r="HA67" s="26"/>
-      <c r="HB67" s="26"/>
-      <c r="HC67" s="26"/>
-      <c r="HD67" s="26"/>
-      <c r="HE67" s="26"/>
-      <c r="HF67" s="26"/>
-      <c r="HG67" s="26"/>
-      <c r="HH67" s="26"/>
-      <c r="HI67" s="26"/>
-      <c r="HJ67" s="26"/>
-      <c r="HK67" s="26"/>
-      <c r="HL67" s="26"/>
-      <c r="HM67" s="26"/>
-      <c r="HN67" s="26"/>
-      <c r="HO67" s="26"/>
-      <c r="HP67" s="26"/>
-      <c r="HQ67" s="26"/>
-      <c r="HR67" s="26"/>
-      <c r="HS67" s="26"/>
-      <c r="HT67" s="26"/>
-      <c r="HU67" s="26"/>
-      <c r="HV67" s="26"/>
-      <c r="HW67" s="26"/>
-      <c r="HX67" s="26"/>
-      <c r="HY67" s="26"/>
-      <c r="HZ67" s="26"/>
-      <c r="IA67" s="26"/>
-      <c r="IB67" s="26"/>
-      <c r="IC67" s="26"/>
-      <c r="ID67" s="26"/>
-      <c r="IE67" s="26"/>
-      <c r="IF67" s="26"/>
-      <c r="IG67" s="26"/>
-      <c r="IH67" s="26"/>
-      <c r="II67" s="26"/>
-      <c r="IJ67" s="26"/>
-      <c r="IK67" s="26"/>
-      <c r="IL67" s="26"/>
-      <c r="IM67" s="26"/>
-      <c r="IN67" s="26"/>
-      <c r="IO67" s="26"/>
-      <c r="IP67" s="26"/>
-      <c r="IQ67" s="26"/>
-      <c r="IR67" s="26"/>
-      <c r="IS67" s="26"/>
-      <c r="IT67" s="26"/>
-      <c r="IU67" s="26"/>
-      <c r="IV67" s="26"/>
-      <c r="IW67" s="26"/>
-      <c r="IX67" s="26"/>
-      <c r="IY67" s="26"/>
-      <c r="IZ67" s="26"/>
-      <c r="JA67" s="26"/>
-      <c r="JB67" s="26"/>
-      <c r="JC67" s="26"/>
-      <c r="JD67" s="26"/>
-      <c r="JE67" s="26"/>
-      <c r="JF67" s="26"/>
-      <c r="JG67" s="26"/>
-      <c r="JH67" s="26"/>
-      <c r="JI67" s="26"/>
-      <c r="JJ67" s="26"/>
-      <c r="JK67" s="26"/>
-      <c r="JL67" s="26"/>
-      <c r="JM67" s="26"/>
-      <c r="JN67" s="26"/>
-      <c r="JO67" s="26"/>
-      <c r="JP67" s="26"/>
-      <c r="JQ67" s="26"/>
-      <c r="JR67" s="26"/>
-      <c r="JS67" s="26"/>
-      <c r="JT67" s="26"/>
-      <c r="JU67" s="26"/>
-      <c r="JV67" s="26"/>
-      <c r="JW67" s="26"/>
-      <c r="JX67" s="26"/>
-      <c r="JY67" s="26"/>
-      <c r="JZ67" s="26"/>
-      <c r="KA67" s="26"/>
-      <c r="KB67" s="26"/>
-      <c r="KC67" s="26"/>
-      <c r="KD67" s="26"/>
-      <c r="KE67" s="26"/>
-      <c r="KF67" s="26"/>
-      <c r="KG67" s="26"/>
-      <c r="KH67" s="26"/>
-      <c r="KI67" s="26"/>
-      <c r="KJ67" s="26"/>
-      <c r="KK67" s="26"/>
-      <c r="KL67" s="26"/>
-      <c r="KM67" s="26"/>
-      <c r="KN67" s="26"/>
-      <c r="KO67" s="26"/>
-      <c r="KP67" s="26"/>
-      <c r="KQ67" s="26"/>
-      <c r="KR67" s="26"/>
-      <c r="KS67" s="26"/>
-      <c r="KT67" s="26"/>
-      <c r="KU67" s="26"/>
-      <c r="KV67" s="26"/>
-      <c r="KW67" s="26"/>
-      <c r="KX67" s="26"/>
-      <c r="KY67" s="26"/>
-      <c r="KZ67" s="26"/>
-      <c r="LA67" s="26"/>
-      <c r="LB67" s="26"/>
-      <c r="LC67" s="26"/>
-      <c r="LD67" s="26"/>
-      <c r="LE67" s="26"/>
-      <c r="LF67" s="26"/>
-      <c r="LG67" s="26"/>
-      <c r="LH67" s="26"/>
-      <c r="LI67" s="26"/>
-      <c r="LJ67" s="26"/>
-      <c r="LK67" s="26"/>
-      <c r="LL67" s="26"/>
-      <c r="LM67" s="26"/>
-      <c r="LN67" s="26"/>
-      <c r="LO67" s="26"/>
-      <c r="LP67" s="26"/>
-      <c r="LQ67" s="26"/>
-      <c r="LR67" s="26"/>
-      <c r="LS67" s="26"/>
-      <c r="LT67" s="26"/>
-      <c r="LU67" s="26"/>
-      <c r="LV67" s="26"/>
-      <c r="LW67" s="26"/>
-      <c r="LX67" s="26"/>
-      <c r="LY67" s="26"/>
-      <c r="LZ67" s="26"/>
-      <c r="MA67" s="26"/>
-      <c r="MB67" s="26"/>
-      <c r="MC67" s="26"/>
-      <c r="MD67" s="26"/>
-      <c r="ME67" s="26"/>
-      <c r="MF67" s="26"/>
-      <c r="MG67" s="26"/>
-      <c r="MH67" s="26"/>
-      <c r="MI67" s="26"/>
-      <c r="MJ67" s="26"/>
-      <c r="MK67" s="26"/>
-      <c r="ML67" s="26"/>
-      <c r="MM67" s="26"/>
-      <c r="MN67" s="26"/>
-      <c r="MO67" s="26"/>
-      <c r="MP67" s="26"/>
-      <c r="MQ67" s="26"/>
-      <c r="MR67" s="26"/>
-      <c r="MS67" s="26"/>
-      <c r="MT67" s="26"/>
-      <c r="MU67" s="26"/>
-      <c r="MV67" s="26"/>
-      <c r="MW67" s="26"/>
-      <c r="MX67" s="26"/>
-      <c r="MY67" s="26"/>
-      <c r="MZ67" s="26"/>
-      <c r="NA67" s="26"/>
-      <c r="NB67" s="26"/>
-      <c r="NC67" s="26"/>
-      <c r="ND67" s="26"/>
-      <c r="NE67" s="26"/>
-      <c r="NF67" s="26"/>
-      <c r="NG67" s="26"/>
-      <c r="NH67" s="26"/>
-      <c r="NI67" s="26"/>
-      <c r="NJ67" s="26"/>
-      <c r="NK67" s="26"/>
-      <c r="NL67" s="26"/>
-      <c r="NM67" s="26"/>
-      <c r="NN67" s="26"/>
-      <c r="NO67" s="26"/>
-      <c r="NP67" s="26"/>
-      <c r="NQ67" s="26"/>
-      <c r="NR67" s="26"/>
-      <c r="NS67" s="26"/>
-      <c r="NT67" s="26"/>
-      <c r="NU67" s="26"/>
-      <c r="NV67" s="26"/>
-      <c r="NW67" s="26"/>
-      <c r="NX67" s="26"/>
-      <c r="NY67" s="26"/>
-      <c r="NZ67" s="26"/>
-      <c r="OA67" s="26"/>
-      <c r="OB67" s="26"/>
-      <c r="OC67" s="26"/>
-      <c r="OD67" s="26"/>
-      <c r="OE67" s="26"/>
-      <c r="OF67" s="26"/>
-      <c r="OG67" s="26"/>
-      <c r="OH67" s="26"/>
-      <c r="OI67" s="26"/>
-      <c r="OJ67" s="26"/>
-      <c r="OK67" s="26"/>
-      <c r="OL67" s="26"/>
-      <c r="OM67" s="26"/>
-      <c r="ON67" s="26"/>
-      <c r="OO67" s="26"/>
-      <c r="OP67" s="26"/>
-      <c r="OQ67" s="26"/>
-      <c r="OR67" s="26"/>
-      <c r="OS67" s="26"/>
-      <c r="OT67" s="26"/>
-      <c r="OU67" s="26"/>
-      <c r="OV67" s="26"/>
-      <c r="OW67" s="26"/>
-      <c r="OX67" s="26"/>
-      <c r="OY67" s="26"/>
-      <c r="OZ67" s="26"/>
-      <c r="PA67" s="26"/>
-      <c r="PB67" s="26"/>
-      <c r="PC67" s="26"/>
-      <c r="PD67" s="26"/>
-      <c r="PE67" s="26"/>
-      <c r="PF67" s="26"/>
-      <c r="PG67" s="26"/>
-      <c r="PH67" s="26"/>
-      <c r="PI67" s="26"/>
-      <c r="PJ67" s="26"/>
-      <c r="PK67" s="26"/>
-      <c r="PL67" s="26"/>
-      <c r="PM67" s="26"/>
-      <c r="PN67" s="26"/>
-      <c r="PO67" s="26"/>
-      <c r="PP67" s="26"/>
-      <c r="PQ67" s="26"/>
-      <c r="PR67" s="26"/>
-      <c r="PS67" s="26"/>
-      <c r="PT67" s="26"/>
-      <c r="PU67" s="26"/>
-      <c r="PV67" s="26"/>
-      <c r="PW67" s="26"/>
-      <c r="PX67" s="26"/>
-      <c r="PY67" s="26"/>
-      <c r="PZ67" s="26"/>
-      <c r="QA67" s="26"/>
-      <c r="QB67" s="26"/>
-      <c r="QC67" s="26"/>
-      <c r="QD67" s="26"/>
-      <c r="QE67" s="26"/>
-      <c r="QF67" s="26"/>
-      <c r="QG67" s="26"/>
-      <c r="QH67" s="26"/>
-      <c r="QI67" s="26"/>
-      <c r="QJ67" s="26"/>
-      <c r="QK67" s="26"/>
-      <c r="QL67" s="26"/>
-      <c r="QM67" s="26"/>
-      <c r="QN67" s="26"/>
-      <c r="QO67" s="26"/>
-      <c r="QP67" s="26"/>
-      <c r="QQ67" s="26"/>
-      <c r="QR67" s="26"/>
-      <c r="QS67" s="26"/>
-      <c r="QT67" s="26"/>
-      <c r="QU67" s="26"/>
-      <c r="QV67" s="26"/>
-      <c r="QW67" s="26"/>
-      <c r="QX67" s="26"/>
-      <c r="QY67" s="26"/>
-      <c r="QZ67" s="26"/>
-      <c r="RA67" s="26"/>
-      <c r="RB67" s="26"/>
-      <c r="RC67" s="26"/>
-      <c r="RD67" s="26"/>
-      <c r="RE67" s="26"/>
-      <c r="RF67" s="26"/>
-      <c r="RG67" s="26"/>
-      <c r="RH67" s="26"/>
-      <c r="RI67" s="26"/>
-      <c r="RJ67" s="26"/>
-      <c r="RK67" s="26"/>
-      <c r="RL67" s="26"/>
-      <c r="RM67" s="26"/>
-      <c r="RN67" s="26"/>
-      <c r="RO67" s="26"/>
-      <c r="RP67" s="26"/>
-      <c r="RQ67" s="26"/>
-      <c r="RR67" s="26"/>
-      <c r="RS67" s="26"/>
-      <c r="RT67" s="26"/>
-      <c r="RU67" s="26"/>
-      <c r="RV67" s="26"/>
-      <c r="RW67" s="26"/>
-      <c r="RX67" s="26"/>
-      <c r="RY67" s="26"/>
-      <c r="RZ67" s="26"/>
-      <c r="SA67" s="26"/>
-      <c r="SB67" s="26"/>
-      <c r="SC67" s="26"/>
-      <c r="SD67" s="26"/>
-      <c r="SE67" s="26"/>
-      <c r="SF67" s="26"/>
-      <c r="SG67" s="26"/>
-      <c r="SH67" s="26"/>
-      <c r="SI67" s="26"/>
-      <c r="SJ67" s="26"/>
-      <c r="SK67" s="26"/>
-      <c r="SL67" s="26"/>
-      <c r="SM67" s="26"/>
-      <c r="SN67" s="26"/>
-      <c r="SO67" s="26"/>
-      <c r="SP67" s="26"/>
-      <c r="SQ67" s="26"/>
-      <c r="SR67" s="26"/>
-      <c r="SS67" s="26"/>
-      <c r="ST67" s="26"/>
-      <c r="SU67" s="26"/>
-      <c r="SV67" s="26"/>
-      <c r="SW67" s="26"/>
-      <c r="SX67" s="26"/>
-      <c r="SY67" s="26"/>
-      <c r="SZ67" s="26"/>
-      <c r="TA67" s="26"/>
-      <c r="TB67" s="26"/>
-      <c r="TC67" s="26"/>
-      <c r="TD67" s="26"/>
-      <c r="TE67" s="26"/>
-      <c r="TF67" s="26"/>
-      <c r="TG67" s="26"/>
-      <c r="TH67" s="26"/>
-      <c r="TI67" s="26"/>
-      <c r="TJ67" s="26"/>
-      <c r="TK67" s="26"/>
-      <c r="TL67" s="26"/>
-      <c r="TM67" s="26"/>
-      <c r="TN67" s="26"/>
-      <c r="TO67" s="26"/>
-      <c r="TP67" s="26"/>
-      <c r="TQ67" s="26"/>
-      <c r="TR67" s="26"/>
-      <c r="TS67" s="26"/>
-      <c r="TT67" s="26"/>
-      <c r="TU67" s="26"/>
-      <c r="TV67" s="26"/>
-      <c r="TW67" s="26"/>
-      <c r="TX67" s="26"/>
-      <c r="TY67" s="26"/>
-      <c r="TZ67" s="26"/>
-      <c r="UA67" s="26"/>
-      <c r="UB67" s="26"/>
-      <c r="UC67" s="26"/>
-      <c r="UD67" s="26"/>
-      <c r="UE67" s="26"/>
-      <c r="UF67" s="26"/>
-      <c r="UG67" s="26"/>
-      <c r="UH67" s="26"/>
-      <c r="UI67" s="26"/>
-      <c r="UJ67" s="26"/>
-      <c r="UK67" s="26"/>
-      <c r="UL67" s="26"/>
-      <c r="UM67" s="26"/>
-      <c r="UN67" s="26"/>
-      <c r="UO67" s="26"/>
-      <c r="UP67" s="26"/>
-      <c r="UQ67" s="26"/>
-      <c r="UR67" s="26"/>
-      <c r="US67" s="26"/>
-      <c r="UT67" s="26"/>
-      <c r="UU67" s="26"/>
-      <c r="UV67" s="26"/>
-      <c r="UW67" s="26"/>
-      <c r="UX67" s="26"/>
-      <c r="UY67" s="26"/>
-      <c r="UZ67" s="26"/>
-      <c r="VA67" s="26"/>
-      <c r="VB67" s="26"/>
-      <c r="VC67" s="26"/>
-      <c r="VD67" s="26"/>
-      <c r="VE67" s="26"/>
-      <c r="VF67" s="26"/>
-      <c r="VG67" s="26"/>
-      <c r="VH67" s="26"/>
-      <c r="VI67" s="26"/>
-      <c r="VJ67" s="26"/>
-      <c r="VK67" s="26"/>
-      <c r="VL67" s="26"/>
-      <c r="VM67" s="26"/>
-      <c r="VN67" s="26"/>
-      <c r="VO67" s="26"/>
-      <c r="VP67" s="26"/>
-      <c r="VQ67" s="26"/>
-      <c r="VR67" s="26"/>
-      <c r="VS67" s="26"/>
-      <c r="VT67" s="26"/>
-      <c r="VU67" s="26"/>
-      <c r="VV67" s="26"/>
-      <c r="VW67" s="26"/>
-      <c r="VX67" s="26"/>
-      <c r="VY67" s="26"/>
-      <c r="VZ67" s="26"/>
-      <c r="WA67" s="26"/>
-      <c r="WB67" s="26"/>
-      <c r="WC67" s="26"/>
-      <c r="WD67" s="26"/>
-      <c r="WE67" s="26"/>
-      <c r="WF67" s="26"/>
-      <c r="WG67" s="26"/>
-      <c r="WH67" s="26"/>
-      <c r="WI67" s="26"/>
-      <c r="WJ67" s="26"/>
-      <c r="WK67" s="26"/>
-      <c r="WL67" s="26"/>
-      <c r="WM67" s="26"/>
-      <c r="WN67" s="26"/>
-      <c r="WO67" s="26"/>
-      <c r="WP67" s="26"/>
-      <c r="WQ67" s="26"/>
-      <c r="WR67" s="26"/>
-      <c r="WS67" s="26"/>
-      <c r="WT67" s="26"/>
-      <c r="WU67" s="26"/>
-      <c r="WV67" s="26"/>
-      <c r="WW67" s="26"/>
-      <c r="WX67" s="26"/>
-      <c r="WY67" s="26"/>
-      <c r="WZ67" s="26"/>
-      <c r="XA67" s="26"/>
-      <c r="XB67" s="26"/>
-      <c r="XC67" s="26"/>
-      <c r="XD67" s="26"/>
-      <c r="XE67" s="26"/>
-      <c r="XF67" s="26"/>
-      <c r="XG67" s="26"/>
-      <c r="XH67" s="26"/>
-      <c r="XI67" s="26"/>
-      <c r="XJ67" s="26"/>
-      <c r="XK67" s="26"/>
-      <c r="XL67" s="26"/>
-      <c r="XM67" s="26"/>
-      <c r="XN67" s="26"/>
-      <c r="XO67" s="26"/>
-      <c r="XP67" s="26"/>
-      <c r="XQ67" s="26"/>
-      <c r="XR67" s="26"/>
-      <c r="XS67" s="26"/>
-      <c r="XT67" s="26"/>
-      <c r="XU67" s="26"/>
-      <c r="XV67" s="26"/>
-      <c r="XW67" s="26"/>
-      <c r="XX67" s="26"/>
-      <c r="XY67" s="26"/>
-      <c r="XZ67" s="26"/>
-      <c r="YA67" s="26"/>
-      <c r="YB67" s="26"/>
-      <c r="YC67" s="26"/>
-      <c r="YD67" s="26"/>
-      <c r="YE67" s="26"/>
-      <c r="YF67" s="26"/>
-      <c r="YG67" s="26"/>
-      <c r="YH67" s="26"/>
-      <c r="YI67" s="26"/>
-      <c r="YJ67" s="26"/>
-      <c r="YK67" s="26"/>
-      <c r="YL67" s="26"/>
-      <c r="YM67" s="26"/>
-      <c r="YN67" s="26"/>
-      <c r="YO67" s="26"/>
-      <c r="YP67" s="26"/>
-      <c r="YQ67" s="26"/>
-      <c r="YR67" s="26"/>
-      <c r="YS67" s="26"/>
-      <c r="YT67" s="26"/>
-      <c r="YU67" s="26"/>
-      <c r="YV67" s="26"/>
-      <c r="YW67" s="26"/>
-      <c r="YX67" s="26"/>
-      <c r="YY67" s="26"/>
-      <c r="YZ67" s="26"/>
-      <c r="ZA67" s="26"/>
-      <c r="ZB67" s="26"/>
-      <c r="ZC67" s="26"/>
-      <c r="ZD67" s="26"/>
-      <c r="ZE67" s="26"/>
-      <c r="ZF67" s="26"/>
-      <c r="ZG67" s="26"/>
-      <c r="ZH67" s="26"/>
-      <c r="ZI67" s="26"/>
-      <c r="ZJ67" s="26"/>
-      <c r="ZK67" s="26"/>
-      <c r="ZL67" s="26"/>
-      <c r="ZM67" s="26"/>
-      <c r="ZN67" s="26"/>
-      <c r="ZO67" s="26"/>
-      <c r="ZP67" s="26"/>
-      <c r="ZQ67" s="26"/>
-      <c r="ZR67" s="26"/>
-      <c r="ZS67" s="26"/>
-      <c r="ZT67" s="26"/>
-      <c r="ZU67" s="26"/>
-      <c r="ZV67" s="26"/>
-      <c r="ZW67" s="26"/>
-      <c r="ZX67" s="26"/>
-      <c r="ZY67" s="26"/>
-      <c r="ZZ67" s="26"/>
-      <c r="AAA67" s="26"/>
-      <c r="AAB67" s="26"/>
-      <c r="AAC67" s="26"/>
-      <c r="AAD67" s="26"/>
-      <c r="AAE67" s="26"/>
-      <c r="AAF67" s="26"/>
-      <c r="AAG67" s="26"/>
-      <c r="AAH67" s="26"/>
-      <c r="AAI67" s="26"/>
-      <c r="AAJ67" s="26"/>
-      <c r="AAK67" s="26"/>
-      <c r="AAL67" s="26"/>
-      <c r="AAM67" s="26"/>
-      <c r="AAN67" s="26"/>
-      <c r="AAO67" s="26"/>
-      <c r="AAP67" s="26"/>
-      <c r="AAQ67" s="26"/>
-      <c r="AAR67" s="26"/>
-      <c r="AAS67" s="26"/>
-      <c r="AAT67" s="26"/>
-      <c r="AAU67" s="26"/>
-      <c r="AAV67" s="26"/>
-      <c r="AAW67" s="26"/>
-      <c r="AAX67" s="26"/>
-      <c r="AAY67" s="26"/>
-      <c r="AAZ67" s="26"/>
-      <c r="ABA67" s="26"/>
-      <c r="ABB67" s="26"/>
-      <c r="ABC67" s="26"/>
-      <c r="ABD67" s="26"/>
-      <c r="ABE67" s="26"/>
-      <c r="ABF67" s="26"/>
-      <c r="ABG67" s="26"/>
-      <c r="ABH67" s="26"/>
-      <c r="ABI67" s="26"/>
-      <c r="ABJ67" s="26"/>
-      <c r="ABK67" s="26"/>
-      <c r="ABL67" s="26"/>
-      <c r="ABM67" s="26"/>
-      <c r="ABN67" s="26"/>
-      <c r="ABO67" s="26"/>
-      <c r="ABP67" s="26"/>
-      <c r="ABQ67" s="26"/>
-      <c r="ABR67" s="26"/>
-      <c r="ABS67" s="26"/>
-      <c r="ABT67" s="26"/>
-      <c r="ABU67" s="26"/>
-      <c r="ABV67" s="26"/>
-      <c r="ABW67" s="26"/>
-      <c r="ABX67" s="26"/>
-      <c r="ABY67" s="26"/>
-      <c r="ABZ67" s="26"/>
-      <c r="ACA67" s="26"/>
-      <c r="ACB67" s="26"/>
-      <c r="ACC67" s="26"/>
-      <c r="ACD67" s="26"/>
-      <c r="ACE67" s="26"/>
-      <c r="ACF67" s="26"/>
-      <c r="ACG67" s="26"/>
-      <c r="ACH67" s="26"/>
-      <c r="ACI67" s="26"/>
-      <c r="ACJ67" s="26"/>
-      <c r="ACK67" s="26"/>
-      <c r="ACL67" s="26"/>
-      <c r="ACM67" s="26"/>
-      <c r="ACN67" s="26"/>
-      <c r="ACO67" s="26"/>
-      <c r="ACP67" s="26"/>
-      <c r="ACQ67" s="26"/>
-      <c r="ACR67" s="26"/>
-      <c r="ACS67" s="26"/>
-      <c r="ACT67" s="26"/>
-      <c r="ACU67" s="26"/>
-      <c r="ACV67" s="26"/>
-      <c r="ACW67" s="26"/>
-      <c r="ACX67" s="26"/>
-      <c r="ACY67" s="26"/>
-      <c r="ACZ67" s="26"/>
-      <c r="ADA67" s="26"/>
-      <c r="ADB67" s="26"/>
-      <c r="ADC67" s="26"/>
-      <c r="ADD67" s="26"/>
-      <c r="ADE67" s="26"/>
-      <c r="ADF67" s="26"/>
-      <c r="ADG67" s="26"/>
-      <c r="ADH67" s="26"/>
-      <c r="ADI67" s="26"/>
-      <c r="ADJ67" s="26"/>
-      <c r="ADK67" s="26"/>
-      <c r="ADL67" s="26"/>
-      <c r="ADM67" s="26"/>
-      <c r="ADN67" s="26"/>
-      <c r="ADO67" s="26"/>
-      <c r="ADP67" s="26"/>
-      <c r="ADQ67" s="26"/>
-      <c r="ADR67" s="26"/>
-      <c r="ADS67" s="26"/>
-      <c r="ADT67" s="26"/>
-      <c r="ADU67" s="26"/>
-      <c r="ADV67" s="26"/>
-      <c r="ADW67" s="26"/>
-      <c r="ADX67" s="26"/>
-      <c r="ADY67" s="26"/>
-      <c r="ADZ67" s="26"/>
-      <c r="AEA67" s="26"/>
-      <c r="AEB67" s="26"/>
-      <c r="AEC67" s="26"/>
-      <c r="AED67" s="26"/>
-      <c r="AEE67" s="26"/>
-      <c r="AEF67" s="26"/>
-      <c r="AEG67" s="26"/>
-      <c r="AEH67" s="26"/>
-      <c r="AEI67" s="26"/>
-      <c r="AEJ67" s="26"/>
-      <c r="AEK67" s="26"/>
-      <c r="AEL67" s="26"/>
-      <c r="AEM67" s="26"/>
-      <c r="AEN67" s="26"/>
-      <c r="AEO67" s="26"/>
-      <c r="AEP67" s="26"/>
-      <c r="AEQ67" s="26"/>
-      <c r="AER67" s="26"/>
-      <c r="AES67" s="26"/>
-      <c r="AET67" s="26"/>
-      <c r="AEU67" s="26"/>
-      <c r="AEV67" s="26"/>
-      <c r="AEW67" s="26"/>
-      <c r="AEX67" s="26"/>
-      <c r="AEY67" s="26"/>
-      <c r="AEZ67" s="26"/>
-      <c r="AFA67" s="26"/>
-      <c r="AFB67" s="26"/>
-      <c r="AFC67" s="26"/>
-      <c r="AFD67" s="26"/>
-      <c r="AFE67" s="26"/>
-      <c r="AFF67" s="26"/>
-      <c r="AFG67" s="26"/>
-      <c r="AFH67" s="26"/>
-      <c r="AFI67" s="26"/>
-      <c r="AFJ67" s="26"/>
-      <c r="AFK67" s="26"/>
-      <c r="AFL67" s="26"/>
-      <c r="AFM67" s="26"/>
-      <c r="AFN67" s="26"/>
-      <c r="AFO67" s="26"/>
-      <c r="AFP67" s="26"/>
-      <c r="AFQ67" s="26"/>
-      <c r="AFR67" s="26"/>
-      <c r="AFS67" s="26"/>
-      <c r="AFT67" s="26"/>
-      <c r="AFU67" s="26"/>
-      <c r="AFV67" s="26"/>
-      <c r="AFW67" s="26"/>
-      <c r="AFX67" s="26"/>
-      <c r="AFY67" s="26"/>
-      <c r="AFZ67" s="26"/>
-      <c r="AGA67" s="26"/>
-      <c r="AGB67" s="26"/>
-      <c r="AGC67" s="26"/>
-      <c r="AGD67" s="26"/>
-      <c r="AGE67" s="26"/>
-      <c r="AGF67" s="26"/>
-      <c r="AGG67" s="26"/>
-      <c r="AGH67" s="26"/>
-      <c r="AGI67" s="26"/>
-      <c r="AGJ67" s="26"/>
-      <c r="AGK67" s="26"/>
-      <c r="AGL67" s="26"/>
-      <c r="AGM67" s="26"/>
-      <c r="AGN67" s="26"/>
-      <c r="AGO67" s="26"/>
-      <c r="AGP67" s="26"/>
-      <c r="AGQ67" s="26"/>
-      <c r="AGR67" s="26"/>
-      <c r="AGS67" s="26"/>
-      <c r="AGT67" s="26"/>
-      <c r="AGU67" s="26"/>
-      <c r="AGV67" s="26"/>
-      <c r="AGW67" s="26"/>
-      <c r="AGX67" s="26"/>
-      <c r="AGY67" s="26"/>
-      <c r="AGZ67" s="26"/>
-      <c r="AHA67" s="26"/>
-      <c r="AHB67" s="26"/>
-      <c r="AHC67" s="26"/>
-      <c r="AHD67" s="26"/>
-      <c r="AHE67" s="26"/>
-      <c r="AHF67" s="26"/>
-      <c r="AHG67" s="26"/>
-      <c r="AHH67" s="26"/>
-      <c r="AHI67" s="26"/>
-      <c r="AHJ67" s="26"/>
-      <c r="AHK67" s="26"/>
-      <c r="AHL67" s="26"/>
-      <c r="AHM67" s="26"/>
-      <c r="AHN67" s="26"/>
-      <c r="AHO67" s="26"/>
-      <c r="AHP67" s="26"/>
-      <c r="AHQ67" s="26"/>
-      <c r="AHR67" s="26"/>
-      <c r="AHS67" s="26"/>
-      <c r="AHT67" s="26"/>
-      <c r="AHU67" s="26"/>
-      <c r="AHV67" s="26"/>
-      <c r="AHW67" s="26"/>
-      <c r="AHX67" s="26"/>
-      <c r="AHY67" s="26"/>
-      <c r="AHZ67" s="26"/>
-      <c r="AIA67" s="26"/>
-      <c r="AIB67" s="26"/>
-      <c r="AIC67" s="26"/>
-      <c r="AID67" s="26"/>
-      <c r="AIE67" s="26"/>
-      <c r="AIF67" s="26"/>
-      <c r="AIG67" s="26"/>
-      <c r="AIH67" s="26"/>
-      <c r="AII67" s="26"/>
-      <c r="AIJ67" s="26"/>
-      <c r="AIK67" s="26"/>
-      <c r="AIL67" s="26"/>
-      <c r="AIM67" s="26"/>
-      <c r="AIN67" s="26"/>
-      <c r="AIO67" s="26"/>
-      <c r="AIP67" s="26"/>
-      <c r="AIQ67" s="26"/>
-      <c r="AIR67" s="26"/>
-      <c r="AIS67" s="26"/>
-      <c r="AIT67" s="26"/>
-      <c r="AIU67" s="26"/>
-      <c r="AIV67" s="26"/>
-      <c r="AIW67" s="26"/>
-      <c r="AIX67" s="26"/>
-      <c r="AIY67" s="26"/>
-      <c r="AIZ67" s="26"/>
-      <c r="AJA67" s="26"/>
-      <c r="AJB67" s="26"/>
-      <c r="AJC67" s="26"/>
-      <c r="AJD67" s="26"/>
-      <c r="AJE67" s="26"/>
-      <c r="AJF67" s="26"/>
-      <c r="AJG67" s="26"/>
-      <c r="AJH67" s="26"/>
-      <c r="AJI67" s="26"/>
-      <c r="AJJ67" s="26"/>
-      <c r="AJK67" s="26"/>
-      <c r="AJL67" s="26"/>
-      <c r="AJM67" s="26"/>
-      <c r="AJN67" s="26"/>
-      <c r="AJO67" s="26"/>
-      <c r="AJP67" s="26"/>
-      <c r="AJQ67" s="26"/>
-      <c r="AJR67" s="26"/>
-      <c r="AJS67" s="26"/>
-      <c r="AJT67" s="26"/>
-      <c r="AJU67" s="26"/>
-      <c r="AJV67" s="26"/>
-      <c r="AJW67" s="26"/>
-      <c r="AJX67" s="26"/>
-      <c r="AJY67" s="26"/>
-      <c r="AJZ67" s="26"/>
-      <c r="AKA67" s="26"/>
-      <c r="AKB67" s="26"/>
-      <c r="AKC67" s="26"/>
-      <c r="AKD67" s="26"/>
-      <c r="AKE67" s="26"/>
-      <c r="AKF67" s="26"/>
-      <c r="AKG67" s="26"/>
-      <c r="AKH67" s="26"/>
-      <c r="AKI67" s="26"/>
-      <c r="AKJ67" s="26"/>
-      <c r="AKK67" s="26"/>
-      <c r="AKL67" s="26"/>
-      <c r="AKM67" s="26"/>
-      <c r="AKN67" s="26"/>
-      <c r="AKO67" s="26"/>
-      <c r="AKP67" s="26"/>
-      <c r="AKQ67" s="26"/>
-      <c r="AKR67" s="26"/>
-      <c r="AKS67" s="26"/>
-      <c r="AKT67" s="26"/>
-      <c r="AKU67" s="26"/>
-      <c r="AKV67" s="26"/>
-      <c r="AKW67" s="26"/>
-      <c r="AKX67" s="26"/>
-      <c r="AKY67" s="26"/>
-      <c r="AKZ67" s="26"/>
-      <c r="ALA67" s="26"/>
-      <c r="ALB67" s="26"/>
-      <c r="ALC67" s="26"/>
-      <c r="ALD67" s="26"/>
-      <c r="ALE67" s="26"/>
-      <c r="ALF67" s="26"/>
-      <c r="ALG67" s="26"/>
-      <c r="ALH67" s="26"/>
-      <c r="ALI67" s="26"/>
-      <c r="ALJ67" s="26"/>
-      <c r="ALK67" s="26"/>
-      <c r="ALL67" s="26"/>
-      <c r="ALM67" s="26"/>
-      <c r="ALN67" s="26"/>
-      <c r="ALO67" s="26"/>
-      <c r="ALP67" s="26"/>
-      <c r="ALQ67" s="26"/>
-      <c r="ALR67" s="26"/>
-      <c r="ALS67" s="26"/>
-      <c r="ALT67" s="26"/>
-      <c r="ALU67" s="26"/>
-      <c r="ALV67" s="26"/>
-      <c r="ALW67" s="26"/>
-      <c r="ALX67" s="26"/>
-      <c r="ALY67" s="26"/>
-      <c r="ALZ67" s="26"/>
-      <c r="AMA67" s="26"/>
-      <c r="AMB67" s="26"/>
-      <c r="AMC67" s="26"/>
-      <c r="AMD67" s="26"/>
-      <c r="AME67" s="26"/>
-      <c r="AMF67" s="26"/>
-      <c r="AMG67" s="26"/>
-      <c r="AMH67" s="26"/>
-      <c r="AMI67" s="26"/>
-      <c r="AMJ67" s="26"/>
-      <c r="AMK67" s="26"/>
-    </row>
-    <row r="68" spans="1:1025" x14ac:dyDescent="0.2">
-      <c r="B68" s="35" t="s">
+      <c r="C67" s="32"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B68" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="C68" s="35"/>
+      <c r="C68" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -7496,16 +4462,16 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>196</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -7516,7 +4482,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="37"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="8" t="s">
         <v>198</v>
       </c>
@@ -7525,7 +4491,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="37"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="8" t="s">
         <v>199</v>
       </c>
@@ -7534,7 +4500,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="37"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="8" t="s">
         <v>200</v>
       </c>
@@ -7543,13 +4509,13 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7569,10 +4535,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:D17"/>
+  <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7584,11 +4550,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
@@ -7744,14 +4710,25 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B17" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B18" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C18" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D18" s="22" t="s">
         <v>289</v>
       </c>
     </row>

</xml_diff>